<commit_message>
LGHUB 2025/5/20 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
</commit_message>
<xml_diff>
--- a/Documents/Graph_PC.xlsx
+++ b/Documents/Graph_PC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FDBA520-1711-400E-80F6-DD725E0FF5D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DE437E3-8D04-418E-9551-F33C2AAB79C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,10 +574,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>13</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>12</c:v>
@@ -958,7 +958,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>374</c:v>
+                  <c:v>379</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>365</c:v>
@@ -1286,8 +1286,8 @@
         <c:axId val="1374569007"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="385"/>
-          <c:min val="290"/>
+          <c:max val="390"/>
+          <c:min val="295"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1794,10 +1794,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>13</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>12</c:v>
@@ -4811,8 +4811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C82" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="J83" sqref="J83"/>
+    <sheetView tabSelected="1" topLeftCell="C87" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="K85" sqref="K85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -4836,7 +4836,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
@@ -4844,7 +4844,7 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
@@ -4860,7 +4860,7 @@
         <v>45796</v>
       </c>
       <c r="D19">
-        <v>374</v>
+        <v>379</v>
       </c>
       <c r="F19" s="1">
         <v>45796</v>

</xml_diff>

<commit_message>
LGHUB 2025/6/2 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
</commit_message>
<xml_diff>
--- a/Documents/Graph_PC.xlsx
+++ b/Documents/Graph_PC.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DE437E3-8D04-418E-9551-F33C2AAB79C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{126E140D-8758-4E77-A676-65F4CAB03EF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,13 +574,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>16</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -917,72 +917,72 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$19:$C$27</c:f>
+              <c:f>Sheet1!$C$17:$C$25</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45810</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45803</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>45796</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>45789</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>45782</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>45775</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>45768</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>45761</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>45754</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>45747</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45740</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$19:$D$27</c:f>
+              <c:f>Sheet1!$D$17:$D$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>391</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>386</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>379</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>365</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>356</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>348</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>343</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>334</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>330</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>325</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>316</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1086,72 +1086,72 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$19:$C$27</c:f>
+              <c:f>Sheet1!$C$17:$C$25</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45810</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45803</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>45796</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>45789</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>45782</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>45775</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>45768</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>45761</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>45754</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>45747</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45740</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$19:$G$27</c:f>
+              <c:f>Sheet1!$G$17:$G$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>349</c:v>
+                  <c:v>354</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>320</c:v>
+                  <c:v>354</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>320</c:v>
+                  <c:v>349</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>320</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>319</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>303</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>302</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>302</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>296</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1286,8 +1286,8 @@
         <c:axId val="1374569007"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="390"/>
-          <c:min val="295"/>
+          <c:max val="400"/>
+          <c:min val="300"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1794,13 +1794,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>16</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4222,9 +4222,9 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>119063</xdr:colOff>
+      <xdr:colOff>106422</xdr:colOff>
       <xdr:row>86</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:rowOff>165023</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
@@ -4260,11 +4260,11 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>190501</xdr:colOff>
       <xdr:row>86</xdr:row>
-      <xdr:rowOff>161926</xdr:rowOff>
+      <xdr:rowOff>162248</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>114299</xdr:colOff>
+      <xdr:colOff>124495</xdr:colOff>
       <xdr:row>101</xdr:row>
       <xdr:rowOff>163286</xdr:rowOff>
     </xdr:to>
@@ -4811,8 +4811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C87" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="K85" sqref="K85"/>
+    <sheetView tabSelected="1" topLeftCell="C85" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="M85" sqref="M85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -4836,7 +4836,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
@@ -4852,7 +4852,35 @@
         <v>4</v>
       </c>
       <c r="C7">
-        <v>12</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C17" s="1">
+        <v>45810</v>
+      </c>
+      <c r="D17">
+        <v>391</v>
+      </c>
+      <c r="F17" s="1">
+        <v>45810</v>
+      </c>
+      <c r="G17">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C18" s="1">
+        <v>45803</v>
+      </c>
+      <c r="D18">
+        <v>386</v>
+      </c>
+      <c r="F18" s="1">
+        <v>45803</v>
+      </c>
+      <c r="G18">
+        <v>354</v>
       </c>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
LGHUB 2025/6/4 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
</commit_message>
<xml_diff>
--- a/Documents/Graph_PC.xlsx
+++ b/Documents/Graph_PC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{126E140D-8758-4E77-A676-65F4CAB03EF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCF46369-AA93-4840-AD75-8E4B60D797FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="2" r:id="rId1"/>
@@ -574,7 +574,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>23</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4</c:v>
@@ -958,7 +958,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>391</c:v>
+                  <c:v>395</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>386</c:v>
@@ -1794,7 +1794,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>23</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4</c:v>
@@ -4811,35 +4811,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C85" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="M85" sqref="M85"/>
+    <sheetView tabSelected="1" topLeftCell="D84" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L85" sqref="L85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -4847,7 +4847,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>4</v>
       </c>
@@ -4855,12 +4855,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C17" s="1">
         <v>45810</v>
       </c>
       <c r="D17">
-        <v>391</v>
+        <v>395</v>
       </c>
       <c r="F17" s="1">
         <v>45810</v>
@@ -4869,7 +4869,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C18" s="1">
         <v>45803</v>
       </c>
@@ -4883,7 +4883,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C19" s="1">
         <v>45796</v>
       </c>
@@ -4897,7 +4897,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C20" s="1">
         <v>45789</v>
       </c>
@@ -4911,7 +4911,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C21" s="1">
         <v>45782</v>
       </c>
@@ -4925,7 +4925,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C22" s="1">
         <v>45775</v>
       </c>
@@ -4939,7 +4939,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C23" s="1">
         <v>45768</v>
       </c>
@@ -4953,7 +4953,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C24" s="1">
         <v>45761</v>
       </c>
@@ -4967,7 +4967,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C25" s="1">
         <v>45754</v>
       </c>
@@ -4981,7 +4981,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C26" s="1">
         <v>45747</v>
       </c>
@@ -4995,7 +4995,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C27" s="1">
         <v>45740</v>
       </c>
@@ -5009,7 +5009,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C28" s="1">
         <v>45733</v>
       </c>
@@ -5023,7 +5023,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C29" s="1">
         <v>45726</v>
       </c>
@@ -5037,7 +5037,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C30" s="1">
         <v>45719</v>
       </c>
@@ -5051,7 +5051,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C31" s="1">
         <v>45712</v>
       </c>
@@ -5065,7 +5065,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C32" s="1">
         <v>45705</v>
       </c>
@@ -5079,7 +5079,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C33" s="1">
         <v>45698</v>
       </c>
@@ -5093,7 +5093,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C34" s="1">
         <v>45691</v>
       </c>
@@ -5107,7 +5107,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C35" s="1">
         <v>45684</v>
       </c>
@@ -5121,7 +5121,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C36" s="1">
         <v>45677</v>
       </c>
@@ -5135,7 +5135,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="37" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C37" s="1">
         <v>45670</v>
       </c>
@@ -5149,7 +5149,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="38" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C38" s="1">
         <v>45663</v>
       </c>
@@ -5163,7 +5163,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="39" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C39" s="1">
         <v>45642</v>
       </c>
@@ -5177,7 +5177,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="40" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C40" s="1">
         <v>45635</v>
       </c>
@@ -5191,7 +5191,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="41" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C41" s="1">
         <v>45628</v>
       </c>
@@ -5205,7 +5205,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="42" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C42" s="1">
         <v>45621</v>
       </c>
@@ -5219,7 +5219,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="43" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C43" s="1">
         <v>45614</v>
       </c>
@@ -5233,7 +5233,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="44" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C44" s="1">
         <v>45607</v>
       </c>
@@ -5247,7 +5247,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="45" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C45" s="1">
         <v>45600</v>
       </c>
@@ -5261,7 +5261,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="46" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C46" s="1">
         <v>45579</v>
       </c>
@@ -5275,7 +5275,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="47" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C47" s="1">
         <v>45572</v>
       </c>
@@ -5289,7 +5289,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="48" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C48" s="1">
         <v>45565</v>
       </c>
@@ -5303,7 +5303,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="49" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C49" s="1">
         <v>45537</v>
       </c>
@@ -5317,7 +5317,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="50" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C50" s="1">
         <v>45530</v>
       </c>
@@ -5331,7 +5331,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="51" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C51" s="1">
         <v>45523</v>
       </c>
@@ -5345,7 +5345,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="52" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C52" s="1">
         <v>45516</v>
       </c>
@@ -5359,7 +5359,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="53" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C53" s="1">
         <v>45509</v>
       </c>
@@ -5373,7 +5373,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="54" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C54" s="1">
         <v>45502</v>
       </c>
@@ -5387,7 +5387,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="55" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C55" s="1">
         <v>45495</v>
       </c>
@@ -5401,7 +5401,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="56" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C56" s="1">
         <v>45488</v>
       </c>
@@ -5415,7 +5415,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="57" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C57" s="1">
         <v>45481</v>
       </c>
@@ -5429,7 +5429,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="58" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C58" s="1">
         <v>45474</v>
       </c>
@@ -5443,7 +5443,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="59" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C59" s="1">
         <v>45467</v>
       </c>
@@ -5457,7 +5457,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="60" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C60" s="1">
         <v>45460</v>
       </c>
@@ -5471,7 +5471,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="61" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C61" s="1">
         <v>45453</v>
       </c>
@@ -5485,7 +5485,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="62" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C62" s="1">
         <v>45446</v>
       </c>
@@ -5499,7 +5499,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="63" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C63" s="1">
         <v>45439</v>
       </c>
@@ -5513,7 +5513,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="64" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C64" s="1">
         <v>45432</v>
       </c>
@@ -5527,7 +5527,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="65" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C65" s="1">
         <v>45425</v>
       </c>
@@ -5541,7 +5541,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="66" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C66" s="1">
         <v>45418</v>
       </c>
@@ -5555,7 +5555,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="67" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C67" s="1">
         <v>45411</v>
       </c>
@@ -5569,7 +5569,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="68" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C68" s="1">
         <v>45404</v>
       </c>
@@ -5583,7 +5583,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="69" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C69" s="1">
         <v>45397</v>
       </c>
@@ -5597,7 +5597,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="70" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C70" s="1">
         <v>45390</v>
       </c>
@@ -5611,7 +5611,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="71" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C71" s="1">
         <v>45383</v>
       </c>
@@ -5625,7 +5625,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="72" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C72" s="1">
         <v>45376</v>
       </c>
@@ -5639,7 +5639,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="73" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C73" s="1">
         <v>45369</v>
       </c>
@@ -5653,7 +5653,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="74" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C74" s="1">
         <v>45362</v>
       </c>
@@ -5662,7 +5662,7 @@
       </c>
       <c r="F74" s="1"/>
     </row>
-    <row r="75" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C75" s="1">
         <v>45355</v>
       </c>
@@ -5670,7 +5670,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="76" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C76" s="1">
         <v>45348</v>
       </c>
@@ -5678,7 +5678,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="77" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C77" s="1">
         <v>45341</v>
       </c>
@@ -5686,7 +5686,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="78" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C78" s="1">
         <v>45334</v>
       </c>
@@ -5694,7 +5694,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="79" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C79" s="1">
         <v>45327</v>
       </c>
@@ -5702,7 +5702,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="80" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C80" s="1">
         <v>45320</v>
       </c>
@@ -5710,7 +5710,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="81" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="81" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C81" s="1">
         <v>45313</v>
       </c>
@@ -5718,7 +5718,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="82" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="82" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C82" s="1">
         <v>45306</v>
       </c>
@@ -5726,7 +5726,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="86" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="86" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D86" s="2"/>
       <c r="E86" s="2"/>
       <c r="F86" s="2"/>
@@ -5742,7 +5742,7 @@
       <c r="P86" s="2"/>
       <c r="Q86" s="2"/>
     </row>
-    <row r="87" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="87" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D87" s="2"/>
       <c r="E87" s="2"/>
       <c r="F87" s="2"/>
@@ -5758,7 +5758,7 @@
       <c r="P87" s="2"/>
       <c r="Q87" s="2"/>
     </row>
-    <row r="88" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="88" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D88" s="2"/>
       <c r="E88" s="2"/>
       <c r="F88" s="2"/>
@@ -5774,7 +5774,7 @@
       <c r="P88" s="2"/>
       <c r="Q88" s="2"/>
     </row>
-    <row r="89" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="89" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D89" s="2"/>
       <c r="E89" s="2"/>
       <c r="F89" s="2"/>
@@ -5790,7 +5790,7 @@
       <c r="P89" s="2"/>
       <c r="Q89" s="2"/>
     </row>
-    <row r="90" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="90" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D90" s="2"/>
       <c r="E90" s="2"/>
       <c r="F90" s="2"/>
@@ -5806,7 +5806,7 @@
       <c r="P90" s="2"/>
       <c r="Q90" s="2"/>
     </row>
-    <row r="91" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="91" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D91" s="2"/>
       <c r="E91" s="2"/>
       <c r="F91" s="2"/>
@@ -5822,7 +5822,7 @@
       <c r="P91" s="2"/>
       <c r="Q91" s="2"/>
     </row>
-    <row r="92" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="92" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D92" s="2"/>
       <c r="E92" s="2"/>
       <c r="F92" s="2"/>
@@ -5838,7 +5838,7 @@
       <c r="P92" s="2"/>
       <c r="Q92" s="2"/>
     </row>
-    <row r="93" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="93" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D93" s="2"/>
       <c r="E93" s="2"/>
       <c r="F93" s="2"/>
@@ -5854,7 +5854,7 @@
       <c r="P93" s="2"/>
       <c r="Q93" s="2"/>
     </row>
-    <row r="94" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="94" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D94" s="2"/>
       <c r="E94" s="2"/>
       <c r="F94" s="2"/>
@@ -5870,7 +5870,7 @@
       <c r="P94" s="2"/>
       <c r="Q94" s="2"/>
     </row>
-    <row r="95" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="95" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D95" s="2"/>
       <c r="E95" s="2"/>
       <c r="F95" s="2"/>
@@ -5886,7 +5886,7 @@
       <c r="P95" s="2"/>
       <c r="Q95" s="2"/>
     </row>
-    <row r="96" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="96" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D96" s="2"/>
       <c r="E96" s="2"/>
       <c r="F96" s="2"/>
@@ -5902,7 +5902,7 @@
       <c r="P96" s="2"/>
       <c r="Q96" s="2"/>
     </row>
-    <row r="97" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="97" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D97" s="2"/>
       <c r="E97" s="2"/>
       <c r="F97" s="2"/>
@@ -5918,7 +5918,7 @@
       <c r="P97" s="2"/>
       <c r="Q97" s="2"/>
     </row>
-    <row r="98" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="98" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D98" s="2"/>
       <c r="E98" s="2"/>
       <c r="F98" s="2"/>
@@ -5934,7 +5934,7 @@
       <c r="P98" s="2"/>
       <c r="Q98" s="2"/>
     </row>
-    <row r="99" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="99" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D99" s="2"/>
       <c r="E99" s="2"/>
       <c r="F99" s="2"/>
@@ -5950,7 +5950,7 @@
       <c r="P99" s="2"/>
       <c r="Q99" s="2"/>
     </row>
-    <row r="100" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="100" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D100" s="2"/>
       <c r="E100" s="2"/>
       <c r="F100" s="2"/>
@@ -5966,7 +5966,7 @@
       <c r="P100" s="2"/>
       <c r="Q100" s="2"/>
     </row>
-    <row r="101" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="101" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D101" s="2"/>
       <c r="E101" s="2"/>
       <c r="F101" s="2"/>
@@ -5982,7 +5982,7 @@
       <c r="P101" s="2"/>
       <c r="Q101" s="2"/>
     </row>
-    <row r="102" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="102" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D102" s="2"/>
       <c r="E102" s="2"/>
       <c r="F102" s="2"/>
@@ -5998,7 +5998,7 @@
       <c r="P102" s="2"/>
       <c r="Q102" s="2"/>
     </row>
-    <row r="103" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="103" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D103" s="2"/>
       <c r="E103" s="2"/>
       <c r="F103" s="2"/>
@@ -6014,7 +6014,7 @@
       <c r="P103" s="2"/>
       <c r="Q103" s="2"/>
     </row>
-    <row r="104" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="104" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D104" s="2"/>
       <c r="E104" s="2"/>
       <c r="F104" s="2"/>
@@ -6030,7 +6030,7 @@
       <c r="P104" s="2"/>
       <c r="Q104" s="2"/>
     </row>
-    <row r="105" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="105" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D105" s="2"/>
       <c r="E105" s="2"/>
       <c r="F105" s="2"/>
@@ -6046,7 +6046,7 @@
       <c r="P105" s="2"/>
       <c r="Q105" s="2"/>
     </row>
-    <row r="106" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="106" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D106" s="2"/>
       <c r="E106" s="2"/>
       <c r="F106" s="2"/>
@@ -6062,7 +6062,7 @@
       <c r="P106" s="2"/>
       <c r="Q106" s="2"/>
     </row>
-    <row r="107" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="107" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D107" s="2"/>
       <c r="E107" s="2"/>
       <c r="F107" s="2"/>
@@ -6078,7 +6078,7 @@
       <c r="P107" s="2"/>
       <c r="Q107" s="2"/>
     </row>
-    <row r="108" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="108" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D108" s="2"/>
       <c r="E108" s="2"/>
       <c r="F108" s="2"/>
@@ -6094,7 +6094,7 @@
       <c r="P108" s="2"/>
       <c r="Q108" s="2"/>
     </row>
-    <row r="109" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="109" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D109" s="2"/>
       <c r="E109" s="2"/>
       <c r="F109" s="2"/>
@@ -6110,7 +6110,7 @@
       <c r="P109" s="2"/>
       <c r="Q109" s="2"/>
     </row>
-    <row r="110" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="110" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D110" s="2"/>
       <c r="E110" s="2"/>
       <c r="F110" s="2"/>
@@ -6126,7 +6126,7 @@
       <c r="P110" s="2"/>
       <c r="Q110" s="2"/>
     </row>
-    <row r="111" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="111" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D111" s="2"/>
       <c r="E111" s="2"/>
       <c r="F111" s="2"/>

</xml_diff>

<commit_message>
LGHUB 2025/6/5 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
</commit_message>
<xml_diff>
--- a/Documents/Graph_PC.xlsx
+++ b/Documents/Graph_PC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCF46369-AA93-4840-AD75-8E4B60D797FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F43B56A-AE49-4E2F-A8FE-DEF56B0DC77E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="2" r:id="rId1"/>
@@ -574,13 +574,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>27</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1127,7 +1127,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>354</c:v>
+                  <c:v>360</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>354</c:v>
@@ -1794,13 +1794,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>27</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4811,51 +4811,51 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D84" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L85" sqref="L85"/>
+    <sheetView tabSelected="1" topLeftCell="C85" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="M85" sqref="M85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C17" s="1">
         <v>45810</v>
       </c>
@@ -4866,10 +4866,10 @@
         <v>45810</v>
       </c>
       <c r="G17">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.35">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C18" s="1">
         <v>45803</v>
       </c>
@@ -4883,7 +4883,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C19" s="1">
         <v>45796</v>
       </c>
@@ -4897,7 +4897,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C20" s="1">
         <v>45789</v>
       </c>
@@ -4911,7 +4911,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C21" s="1">
         <v>45782</v>
       </c>
@@ -4925,7 +4925,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C22" s="1">
         <v>45775</v>
       </c>
@@ -4939,7 +4939,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C23" s="1">
         <v>45768</v>
       </c>
@@ -4953,7 +4953,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C24" s="1">
         <v>45761</v>
       </c>
@@ -4967,7 +4967,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C25" s="1">
         <v>45754</v>
       </c>
@@ -4981,7 +4981,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C26" s="1">
         <v>45747</v>
       </c>
@@ -4995,7 +4995,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C27" s="1">
         <v>45740</v>
       </c>
@@ -5009,7 +5009,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C28" s="1">
         <v>45733</v>
       </c>
@@ -5023,7 +5023,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C29" s="1">
         <v>45726</v>
       </c>
@@ -5037,7 +5037,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C30" s="1">
         <v>45719</v>
       </c>
@@ -5051,7 +5051,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C31" s="1">
         <v>45712</v>
       </c>
@@ -5065,7 +5065,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C32" s="1">
         <v>45705</v>
       </c>
@@ -5079,7 +5079,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C33" s="1">
         <v>45698</v>
       </c>
@@ -5093,7 +5093,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="34" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C34" s="1">
         <v>45691</v>
       </c>
@@ -5107,7 +5107,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="35" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C35" s="1">
         <v>45684</v>
       </c>
@@ -5121,7 +5121,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="36" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C36" s="1">
         <v>45677</v>
       </c>
@@ -5135,7 +5135,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="37" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C37" s="1">
         <v>45670</v>
       </c>
@@ -5149,7 +5149,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="38" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C38" s="1">
         <v>45663</v>
       </c>
@@ -5163,7 +5163,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="39" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C39" s="1">
         <v>45642</v>
       </c>
@@ -5177,7 +5177,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="40" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C40" s="1">
         <v>45635</v>
       </c>
@@ -5191,7 +5191,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="41" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C41" s="1">
         <v>45628</v>
       </c>
@@ -5205,7 +5205,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="42" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C42" s="1">
         <v>45621</v>
       </c>
@@ -5219,7 +5219,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="43" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C43" s="1">
         <v>45614</v>
       </c>
@@ -5233,7 +5233,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="44" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C44" s="1">
         <v>45607</v>
       </c>
@@ -5247,7 +5247,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="45" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C45" s="1">
         <v>45600</v>
       </c>
@@ -5261,7 +5261,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="46" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C46" s="1">
         <v>45579</v>
       </c>
@@ -5275,7 +5275,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="47" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C47" s="1">
         <v>45572</v>
       </c>
@@ -5289,7 +5289,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="48" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C48" s="1">
         <v>45565</v>
       </c>
@@ -5303,7 +5303,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="49" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="49" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C49" s="1">
         <v>45537</v>
       </c>
@@ -5317,7 +5317,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="50" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="50" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C50" s="1">
         <v>45530</v>
       </c>
@@ -5331,7 +5331,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="51" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="51" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C51" s="1">
         <v>45523</v>
       </c>
@@ -5345,7 +5345,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="52" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="52" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C52" s="1">
         <v>45516</v>
       </c>
@@ -5359,7 +5359,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="53" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="53" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C53" s="1">
         <v>45509</v>
       </c>
@@ -5373,7 +5373,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="54" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="54" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C54" s="1">
         <v>45502</v>
       </c>
@@ -5387,7 +5387,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="55" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="55" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C55" s="1">
         <v>45495</v>
       </c>
@@ -5401,7 +5401,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="56" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="56" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C56" s="1">
         <v>45488</v>
       </c>
@@ -5415,7 +5415,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="57" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="57" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C57" s="1">
         <v>45481</v>
       </c>
@@ -5429,7 +5429,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="58" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="58" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C58" s="1">
         <v>45474</v>
       </c>
@@ -5443,7 +5443,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="59" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="59" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C59" s="1">
         <v>45467</v>
       </c>
@@ -5457,7 +5457,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="60" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="60" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C60" s="1">
         <v>45460</v>
       </c>
@@ -5471,7 +5471,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="61" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="61" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C61" s="1">
         <v>45453</v>
       </c>
@@ -5485,7 +5485,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="62" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="62" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C62" s="1">
         <v>45446</v>
       </c>
@@ -5499,7 +5499,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="63" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="63" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C63" s="1">
         <v>45439</v>
       </c>
@@ -5513,7 +5513,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="64" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="64" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C64" s="1">
         <v>45432</v>
       </c>
@@ -5527,7 +5527,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="65" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="65" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C65" s="1">
         <v>45425</v>
       </c>
@@ -5541,7 +5541,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="66" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="66" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C66" s="1">
         <v>45418</v>
       </c>
@@ -5555,7 +5555,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="67" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="67" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C67" s="1">
         <v>45411</v>
       </c>
@@ -5569,7 +5569,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="68" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="68" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C68" s="1">
         <v>45404</v>
       </c>
@@ -5583,7 +5583,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="69" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="69" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C69" s="1">
         <v>45397</v>
       </c>
@@ -5597,7 +5597,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="70" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="70" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C70" s="1">
         <v>45390</v>
       </c>
@@ -5611,7 +5611,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="71" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="71" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C71" s="1">
         <v>45383</v>
       </c>
@@ -5625,7 +5625,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="72" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="72" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C72" s="1">
         <v>45376</v>
       </c>
@@ -5639,7 +5639,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="73" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="73" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C73" s="1">
         <v>45369</v>
       </c>
@@ -5653,7 +5653,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="74" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="74" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C74" s="1">
         <v>45362</v>
       </c>
@@ -5662,7 +5662,7 @@
       </c>
       <c r="F74" s="1"/>
     </row>
-    <row r="75" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="75" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C75" s="1">
         <v>45355</v>
       </c>
@@ -5670,7 +5670,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="76" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="76" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C76" s="1">
         <v>45348</v>
       </c>
@@ -5678,7 +5678,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="77" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="77" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C77" s="1">
         <v>45341</v>
       </c>
@@ -5686,7 +5686,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="78" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="78" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C78" s="1">
         <v>45334</v>
       </c>
@@ -5694,7 +5694,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="79" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="79" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C79" s="1">
         <v>45327</v>
       </c>
@@ -5702,7 +5702,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="80" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="80" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C80" s="1">
         <v>45320</v>
       </c>
@@ -5710,7 +5710,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="81" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="81" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C81" s="1">
         <v>45313</v>
       </c>
@@ -5718,7 +5718,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="82" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="82" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C82" s="1">
         <v>45306</v>
       </c>
@@ -5726,7 +5726,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="86" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="86" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D86" s="2"/>
       <c r="E86" s="2"/>
       <c r="F86" s="2"/>
@@ -5742,7 +5742,7 @@
       <c r="P86" s="2"/>
       <c r="Q86" s="2"/>
     </row>
-    <row r="87" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="87" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D87" s="2"/>
       <c r="E87" s="2"/>
       <c r="F87" s="2"/>
@@ -5758,7 +5758,7 @@
       <c r="P87" s="2"/>
       <c r="Q87" s="2"/>
     </row>
-    <row r="88" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="88" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D88" s="2"/>
       <c r="E88" s="2"/>
       <c r="F88" s="2"/>
@@ -5774,7 +5774,7 @@
       <c r="P88" s="2"/>
       <c r="Q88" s="2"/>
     </row>
-    <row r="89" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="89" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D89" s="2"/>
       <c r="E89" s="2"/>
       <c r="F89" s="2"/>
@@ -5790,7 +5790,7 @@
       <c r="P89" s="2"/>
       <c r="Q89" s="2"/>
     </row>
-    <row r="90" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="90" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D90" s="2"/>
       <c r="E90" s="2"/>
       <c r="F90" s="2"/>
@@ -5806,7 +5806,7 @@
       <c r="P90" s="2"/>
       <c r="Q90" s="2"/>
     </row>
-    <row r="91" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="91" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D91" s="2"/>
       <c r="E91" s="2"/>
       <c r="F91" s="2"/>
@@ -5822,7 +5822,7 @@
       <c r="P91" s="2"/>
       <c r="Q91" s="2"/>
     </row>
-    <row r="92" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="92" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D92" s="2"/>
       <c r="E92" s="2"/>
       <c r="F92" s="2"/>
@@ -5838,7 +5838,7 @@
       <c r="P92" s="2"/>
       <c r="Q92" s="2"/>
     </row>
-    <row r="93" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="93" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D93" s="2"/>
       <c r="E93" s="2"/>
       <c r="F93" s="2"/>
@@ -5854,7 +5854,7 @@
       <c r="P93" s="2"/>
       <c r="Q93" s="2"/>
     </row>
-    <row r="94" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="94" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D94" s="2"/>
       <c r="E94" s="2"/>
       <c r="F94" s="2"/>
@@ -5870,7 +5870,7 @@
       <c r="P94" s="2"/>
       <c r="Q94" s="2"/>
     </row>
-    <row r="95" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="95" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D95" s="2"/>
       <c r="E95" s="2"/>
       <c r="F95" s="2"/>
@@ -5886,7 +5886,7 @@
       <c r="P95" s="2"/>
       <c r="Q95" s="2"/>
     </row>
-    <row r="96" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="96" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D96" s="2"/>
       <c r="E96" s="2"/>
       <c r="F96" s="2"/>
@@ -5902,7 +5902,7 @@
       <c r="P96" s="2"/>
       <c r="Q96" s="2"/>
     </row>
-    <row r="97" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="97" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D97" s="2"/>
       <c r="E97" s="2"/>
       <c r="F97" s="2"/>
@@ -5918,7 +5918,7 @@
       <c r="P97" s="2"/>
       <c r="Q97" s="2"/>
     </row>
-    <row r="98" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="98" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D98" s="2"/>
       <c r="E98" s="2"/>
       <c r="F98" s="2"/>
@@ -5934,7 +5934,7 @@
       <c r="P98" s="2"/>
       <c r="Q98" s="2"/>
     </row>
-    <row r="99" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="99" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D99" s="2"/>
       <c r="E99" s="2"/>
       <c r="F99" s="2"/>
@@ -5950,7 +5950,7 @@
       <c r="P99" s="2"/>
       <c r="Q99" s="2"/>
     </row>
-    <row r="100" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="100" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D100" s="2"/>
       <c r="E100" s="2"/>
       <c r="F100" s="2"/>
@@ -5966,7 +5966,7 @@
       <c r="P100" s="2"/>
       <c r="Q100" s="2"/>
     </row>
-    <row r="101" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="101" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D101" s="2"/>
       <c r="E101" s="2"/>
       <c r="F101" s="2"/>
@@ -5982,7 +5982,7 @@
       <c r="P101" s="2"/>
       <c r="Q101" s="2"/>
     </row>
-    <row r="102" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="102" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D102" s="2"/>
       <c r="E102" s="2"/>
       <c r="F102" s="2"/>
@@ -5998,7 +5998,7 @@
       <c r="P102" s="2"/>
       <c r="Q102" s="2"/>
     </row>
-    <row r="103" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="103" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D103" s="2"/>
       <c r="E103" s="2"/>
       <c r="F103" s="2"/>
@@ -6014,7 +6014,7 @@
       <c r="P103" s="2"/>
       <c r="Q103" s="2"/>
     </row>
-    <row r="104" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="104" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D104" s="2"/>
       <c r="E104" s="2"/>
       <c r="F104" s="2"/>
@@ -6030,7 +6030,7 @@
       <c r="P104" s="2"/>
       <c r="Q104" s="2"/>
     </row>
-    <row r="105" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="105" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D105" s="2"/>
       <c r="E105" s="2"/>
       <c r="F105" s="2"/>
@@ -6046,7 +6046,7 @@
       <c r="P105" s="2"/>
       <c r="Q105" s="2"/>
     </row>
-    <row r="106" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="106" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D106" s="2"/>
       <c r="E106" s="2"/>
       <c r="F106" s="2"/>
@@ -6062,7 +6062,7 @@
       <c r="P106" s="2"/>
       <c r="Q106" s="2"/>
     </row>
-    <row r="107" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="107" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D107" s="2"/>
       <c r="E107" s="2"/>
       <c r="F107" s="2"/>
@@ -6078,7 +6078,7 @@
       <c r="P107" s="2"/>
       <c r="Q107" s="2"/>
     </row>
-    <row r="108" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="108" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D108" s="2"/>
       <c r="E108" s="2"/>
       <c r="F108" s="2"/>
@@ -6094,7 +6094,7 @@
       <c r="P108" s="2"/>
       <c r="Q108" s="2"/>
     </row>
-    <row r="109" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="109" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D109" s="2"/>
       <c r="E109" s="2"/>
       <c r="F109" s="2"/>
@@ -6110,7 +6110,7 @@
       <c r="P109" s="2"/>
       <c r="Q109" s="2"/>
     </row>
-    <row r="110" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="110" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D110" s="2"/>
       <c r="E110" s="2"/>
       <c r="F110" s="2"/>
@@ -6126,7 +6126,7 @@
       <c r="P110" s="2"/>
       <c r="Q110" s="2"/>
     </row>
-    <row r="111" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="111" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D111" s="2"/>
       <c r="E111" s="2"/>
       <c r="F111" s="2"/>

</xml_diff>

<commit_message>
LGHUB 2025/6/11 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
- 网站错误 & 本地化问题详见 LGHUB/WebLoc/README.md
</commit_message>
<xml_diff>
--- a/Documents/Graph_PC.xlsx
+++ b/Documents/Graph_PC.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29005"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F43B56A-AE49-4E2F-A8FE-DEF56B0DC77E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE5726C5-4A37-4BEB-9659-7A6334D81DD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,13 +574,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>25</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -917,72 +917,72 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$17:$C$25</c:f>
+              <c:f>Sheet1!$C$16:$C$24</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45817</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45810</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45803</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45796</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45789</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45782</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45775</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45768</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45761</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45754</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$17:$D$25</c:f>
+              <c:f>Sheet1!$D$16:$D$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>395</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>386</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>379</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>365</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>356</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>348</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>343</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>334</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>330</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1086,57 +1086,57 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$17:$C$25</c:f>
+              <c:f>Sheet1!$C$16:$C$24</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45817</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45810</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45803</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45796</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45789</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45782</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45775</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45768</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45761</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45754</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$17:$G$25</c:f>
+              <c:f>Sheet1!$G$16:$G$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>359</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>360</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>354</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>349</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>320</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>320</c:v>
@@ -1145,13 +1145,13 @@
                   <c:v>320</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>319</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>303</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>302</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1794,13 +1794,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>25</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4811,7 +4811,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C85" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B83" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="M85" sqref="M85"/>
     </sheetView>
   </sheetViews>
@@ -4821,38 +4821,52 @@
     <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7">
-        <v>23</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C16" s="1">
+        <v>45817</v>
+      </c>
+      <c r="D16">
+        <v>400</v>
+      </c>
+      <c r="F16" s="1">
+        <v>45817</v>
+      </c>
+      <c r="G16">
+        <v>359</v>
       </c>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
LGHUB 2025/6/14 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
- 网站错误 & 本地化问题详见 LGHUB/WebLoc/README.md
</commit_message>
<xml_diff>
--- a/Documents/Graph_PC.xlsx
+++ b/Documents/Graph_PC.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29005"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29009"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE5726C5-4A37-4BEB-9659-7A6334D81DD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A0D3019-9107-4FEE-9428-2C00E2BEF628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,10 +574,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>30</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>22</c:v>
@@ -958,7 +958,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>400</c:v>
+                  <c:v>404</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>395</c:v>
@@ -1286,7 +1286,7 @@
         <c:axId val="1374569007"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="400"/>
+          <c:max val="410"/>
           <c:min val="300"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1794,10 +1794,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>30</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>22</c:v>
@@ -4811,8 +4811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B83" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="M85" sqref="M85"/>
+    <sheetView tabSelected="1" topLeftCell="C86" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="K85" sqref="K85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -4836,7 +4836,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
@@ -4844,7 +4844,7 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
@@ -4860,7 +4860,7 @@
         <v>45817</v>
       </c>
       <c r="D16">
-        <v>400</v>
+        <v>404</v>
       </c>
       <c r="F16" s="1">
         <v>45817</v>

</xml_diff>

<commit_message>
LGHUB 2025/6/20 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
- 网站错误 & 本地化问题详见 LGHUB/WebLoc/README.md
</commit_message>
<xml_diff>
--- a/Documents/Graph_PC.xlsx
+++ b/Documents/Graph_PC.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29009"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A0D3019-9107-4FEE-9428-2C00E2BEF628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FACE42BF-5F6C-4DCC-902D-61ADE48E0597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,13 +574,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>33</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -917,72 +917,72 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$16:$C$24</c:f>
+              <c:f>Sheet1!$C$20:$C$28</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45824</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45817</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45810</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45803</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45796</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45789</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45782</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45775</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45768</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45761</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$16:$D$24</c:f>
+              <c:f>Sheet1!$D$20:$D$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>407</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>404</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>395</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>386</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>379</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>365</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>356</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>348</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>343</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>334</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1086,60 +1086,60 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$16:$C$24</c:f>
+              <c:f>Sheet1!$C$20:$C$28</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45824</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45817</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45810</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45803</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45796</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45789</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45782</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45775</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45768</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45761</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$16:$G$24</c:f>
+              <c:f>Sheet1!$G$20:$G$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>369</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>359</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>360</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>354</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>349</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>320</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>320</c:v>
@@ -1148,10 +1148,10 @@
                   <c:v>320</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>319</c:v>
+                  <c:v>320</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>303</c:v>
+                  <c:v>319</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1286,8 +1286,8 @@
         <c:axId val="1374569007"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="410"/>
-          <c:min val="300"/>
+          <c:max val="415"/>
+          <c:min val="315"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1794,13 +1794,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>33</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4223,13 +4223,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>106422</xdr:colOff>
-      <xdr:row>86</xdr:row>
+      <xdr:row>91</xdr:row>
       <xdr:rowOff>165023</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>101</xdr:row>
+      <xdr:row>106</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4259,13 +4259,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>190501</xdr:colOff>
-      <xdr:row>86</xdr:row>
+      <xdr:row>91</xdr:row>
       <xdr:rowOff>162248</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>124495</xdr:colOff>
-      <xdr:row>101</xdr:row>
+      <xdr:row>106</xdr:row>
       <xdr:rowOff>163286</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4809,10 +4809,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:Q111"/>
+  <dimension ref="B2:Q116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C86" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="K85" sqref="K85"/>
+    <sheetView tabSelected="1" topLeftCell="B89" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="K90" sqref="K90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -4821,1004 +4821,938 @@
     <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C16" s="1">
-        <v>45817</v>
-      </c>
-      <c r="D16">
-        <v>404</v>
-      </c>
-      <c r="F16" s="1">
-        <v>45817</v>
-      </c>
-      <c r="G16">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C17" s="1">
-        <v>45810</v>
-      </c>
-      <c r="D17">
-        <v>395</v>
-      </c>
-      <c r="F17" s="1">
-        <v>45810</v>
-      </c>
-      <c r="G17">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C18" s="1">
-        <v>45803</v>
-      </c>
-      <c r="D18">
-        <v>386</v>
-      </c>
-      <c r="F18" s="1">
-        <v>45803</v>
-      </c>
-      <c r="G18">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C19" s="1">
-        <v>45796</v>
-      </c>
-      <c r="D19">
-        <v>379</v>
-      </c>
-      <c r="F19" s="1">
-        <v>45796</v>
-      </c>
-      <c r="G19">
-        <v>349</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C20" s="1">
-        <v>45789</v>
+        <v>45824</v>
       </c>
       <c r="D20">
-        <v>365</v>
+        <v>407</v>
       </c>
       <c r="F20" s="1">
-        <v>45789</v>
+        <v>45824</v>
       </c>
       <c r="G20">
-        <v>320</v>
+        <v>369</v>
       </c>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C21" s="1">
-        <v>45782</v>
+        <v>45817</v>
       </c>
       <c r="D21">
-        <v>356</v>
+        <v>404</v>
       </c>
       <c r="F21" s="1">
-        <v>45782</v>
+        <v>45817</v>
       </c>
       <c r="G21">
-        <v>320</v>
+        <v>359</v>
       </c>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C22" s="1">
-        <v>45775</v>
+        <v>45810</v>
       </c>
       <c r="D22">
-        <v>348</v>
+        <v>395</v>
       </c>
       <c r="F22" s="1">
-        <v>45775</v>
+        <v>45810</v>
       </c>
       <c r="G22">
-        <v>320</v>
+        <v>360</v>
       </c>
     </row>
     <row r="23" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C23" s="1">
-        <v>45768</v>
+        <v>45803</v>
       </c>
       <c r="D23">
-        <v>343</v>
+        <v>386</v>
       </c>
       <c r="F23" s="1">
-        <v>45768</v>
+        <v>45803</v>
       </c>
       <c r="G23">
-        <v>319</v>
+        <v>354</v>
       </c>
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C24" s="1">
-        <v>45761</v>
+        <v>45796</v>
       </c>
       <c r="D24">
-        <v>334</v>
+        <v>379</v>
       </c>
       <c r="F24" s="1">
-        <v>45761</v>
+        <v>45796</v>
       </c>
       <c r="G24">
-        <v>303</v>
+        <v>349</v>
       </c>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C25" s="1">
-        <v>45754</v>
+        <v>45789</v>
       </c>
       <c r="D25">
-        <v>330</v>
+        <v>365</v>
       </c>
       <c r="F25" s="1">
-        <v>45754</v>
+        <v>45789</v>
       </c>
       <c r="G25">
-        <v>302</v>
+        <v>320</v>
       </c>
     </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C26" s="1">
-        <v>45747</v>
+        <v>45782</v>
       </c>
       <c r="D26">
-        <v>325</v>
+        <v>356</v>
       </c>
       <c r="F26" s="1">
-        <v>45747</v>
+        <v>45782</v>
       </c>
       <c r="G26">
-        <v>302</v>
+        <v>320</v>
       </c>
     </row>
     <row r="27" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C27" s="1">
-        <v>45740</v>
+        <v>45775</v>
       </c>
       <c r="D27">
-        <v>316</v>
+        <v>348</v>
       </c>
       <c r="F27" s="1">
-        <v>45740</v>
+        <v>45775</v>
       </c>
       <c r="G27">
-        <v>296</v>
+        <v>320</v>
       </c>
     </row>
     <row r="28" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C28" s="1">
-        <v>45733</v>
+        <v>45768</v>
       </c>
       <c r="D28">
-        <v>310</v>
+        <v>343</v>
       </c>
       <c r="F28" s="1">
-        <v>45733</v>
+        <v>45768</v>
       </c>
       <c r="G28">
-        <v>296</v>
+        <v>319</v>
       </c>
     </row>
     <row r="29" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C29" s="1">
-        <v>45726</v>
+        <v>45761</v>
       </c>
       <c r="D29">
-        <v>309</v>
+        <v>334</v>
       </c>
       <c r="F29" s="1">
-        <v>45726</v>
+        <v>45761</v>
       </c>
       <c r="G29">
-        <v>294</v>
+        <v>303</v>
       </c>
     </row>
     <row r="30" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C30" s="1">
-        <v>45719</v>
+        <v>45754</v>
       </c>
       <c r="D30">
-        <v>308</v>
+        <v>330</v>
       </c>
       <c r="F30" s="1">
-        <v>45719</v>
+        <v>45754</v>
       </c>
       <c r="G30">
-        <v>286</v>
+        <v>302</v>
       </c>
     </row>
     <row r="31" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C31" s="1">
-        <v>45712</v>
+        <v>45747</v>
       </c>
       <c r="D31">
-        <v>306</v>
+        <v>325</v>
       </c>
       <c r="F31" s="1">
-        <v>45712</v>
+        <v>45747</v>
       </c>
       <c r="G31">
-        <v>286</v>
+        <v>302</v>
       </c>
     </row>
     <row r="32" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C32" s="1">
-        <v>45705</v>
+        <v>45740</v>
       </c>
       <c r="D32">
-        <v>301</v>
+        <v>316</v>
       </c>
       <c r="F32" s="1">
-        <v>45705</v>
+        <v>45740</v>
       </c>
       <c r="G32">
-        <v>267</v>
+        <v>296</v>
       </c>
     </row>
     <row r="33" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C33" s="1">
-        <v>45698</v>
+        <v>45733</v>
       </c>
       <c r="D33">
-        <v>295</v>
+        <v>310</v>
       </c>
       <c r="F33" s="1">
-        <v>45698</v>
+        <v>45733</v>
       </c>
       <c r="G33">
-        <v>267</v>
+        <v>296</v>
       </c>
     </row>
     <row r="34" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C34" s="1">
-        <v>45691</v>
+        <v>45726</v>
       </c>
       <c r="D34">
-        <v>289</v>
+        <v>309</v>
       </c>
       <c r="F34" s="1">
-        <v>45691</v>
+        <v>45726</v>
       </c>
       <c r="G34">
-        <v>267</v>
+        <v>294</v>
       </c>
     </row>
     <row r="35" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C35" s="1">
-        <v>45684</v>
+        <v>45719</v>
       </c>
       <c r="D35">
-        <v>284</v>
+        <v>308</v>
       </c>
       <c r="F35" s="1">
-        <v>45684</v>
+        <v>45719</v>
       </c>
       <c r="G35">
-        <v>262</v>
+        <v>286</v>
       </c>
     </row>
     <row r="36" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C36" s="1">
-        <v>45677</v>
+        <v>45712</v>
       </c>
       <c r="D36">
-        <v>273</v>
+        <v>306</v>
       </c>
       <c r="F36" s="1">
-        <v>45677</v>
+        <v>45712</v>
       </c>
       <c r="G36">
-        <v>254</v>
+        <v>286</v>
       </c>
     </row>
     <row r="37" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C37" s="1">
-        <v>45670</v>
+        <v>45705</v>
       </c>
       <c r="D37">
-        <v>264</v>
+        <v>301</v>
       </c>
       <c r="F37" s="1">
-        <v>45670</v>
+        <v>45705</v>
       </c>
       <c r="G37">
-        <v>250</v>
+        <v>267</v>
       </c>
     </row>
     <row r="38" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C38" s="1">
-        <v>45663</v>
+        <v>45698</v>
       </c>
       <c r="D38">
-        <v>256</v>
+        <v>295</v>
       </c>
       <c r="F38" s="1">
-        <v>45663</v>
+        <v>45698</v>
       </c>
       <c r="G38">
-        <v>250</v>
+        <v>267</v>
       </c>
     </row>
     <row r="39" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C39" s="1">
-        <v>45642</v>
+        <v>45691</v>
       </c>
       <c r="D39">
-        <v>256</v>
+        <v>289</v>
       </c>
       <c r="F39" s="1">
-        <v>45642</v>
+        <v>45691</v>
       </c>
       <c r="G39">
-        <v>245</v>
+        <v>267</v>
       </c>
     </row>
     <row r="40" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C40" s="1">
-        <v>45635</v>
+        <v>45684</v>
       </c>
       <c r="D40">
-        <v>251</v>
+        <v>284</v>
       </c>
       <c r="F40" s="1">
-        <v>45635</v>
+        <v>45684</v>
       </c>
       <c r="G40">
-        <v>243</v>
+        <v>262</v>
       </c>
     </row>
     <row r="41" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C41" s="1">
-        <v>45628</v>
+        <v>45677</v>
       </c>
       <c r="D41">
-        <v>251</v>
+        <v>273</v>
       </c>
       <c r="F41" s="1">
-        <v>45628</v>
+        <v>45677</v>
       </c>
       <c r="G41">
-        <v>239</v>
+        <v>254</v>
       </c>
     </row>
     <row r="42" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C42" s="1">
-        <v>45621</v>
+        <v>45670</v>
       </c>
       <c r="D42">
-        <v>247</v>
+        <v>264</v>
       </c>
       <c r="F42" s="1">
-        <v>45621</v>
+        <v>45670</v>
       </c>
       <c r="G42">
-        <v>234</v>
+        <v>250</v>
       </c>
     </row>
     <row r="43" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C43" s="1">
-        <v>45614</v>
+        <v>45663</v>
       </c>
       <c r="D43">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="F43" s="1">
-        <v>45614</v>
+        <v>45663</v>
       </c>
       <c r="G43">
-        <v>234</v>
+        <v>250</v>
       </c>
     </row>
     <row r="44" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C44" s="1">
-        <v>45607</v>
+        <v>45642</v>
       </c>
       <c r="D44">
-        <v>239</v>
+        <v>256</v>
       </c>
       <c r="F44" s="1">
-        <v>45607</v>
+        <v>45642</v>
       </c>
       <c r="G44">
-        <v>230</v>
+        <v>245</v>
       </c>
     </row>
     <row r="45" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C45" s="1">
-        <v>45600</v>
+        <v>45635</v>
       </c>
       <c r="D45">
-        <v>232</v>
+        <v>251</v>
       </c>
       <c r="F45" s="1">
-        <v>45600</v>
+        <v>45635</v>
       </c>
       <c r="G45">
-        <v>227</v>
+        <v>243</v>
       </c>
     </row>
     <row r="46" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C46" s="1">
-        <v>45579</v>
+        <v>45628</v>
       </c>
       <c r="D46">
-        <v>231</v>
+        <v>251</v>
       </c>
       <c r="F46" s="1">
-        <v>45579</v>
+        <v>45628</v>
       </c>
       <c r="G46">
-        <v>222</v>
+        <v>239</v>
       </c>
     </row>
     <row r="47" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C47" s="1">
-        <v>45572</v>
+        <v>45621</v>
       </c>
       <c r="D47">
-        <v>227</v>
+        <v>247</v>
       </c>
       <c r="F47" s="1">
-        <v>45572</v>
+        <v>45621</v>
       </c>
       <c r="G47">
-        <v>216</v>
+        <v>234</v>
       </c>
     </row>
     <row r="48" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C48" s="1">
-        <v>45565</v>
+        <v>45614</v>
       </c>
       <c r="D48">
-        <v>223</v>
+        <v>241</v>
       </c>
       <c r="F48" s="1">
-        <v>45565</v>
+        <v>45614</v>
       </c>
       <c r="G48">
-        <v>216</v>
+        <v>234</v>
       </c>
     </row>
     <row r="49" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C49" s="1">
-        <v>45537</v>
+        <v>45607</v>
       </c>
       <c r="D49">
-        <v>218</v>
+        <v>239</v>
       </c>
       <c r="F49" s="1">
-        <v>45537</v>
+        <v>45607</v>
       </c>
       <c r="G49">
-        <v>207</v>
+        <v>230</v>
       </c>
     </row>
     <row r="50" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C50" s="1">
-        <v>45530</v>
+        <v>45600</v>
       </c>
       <c r="D50">
-        <v>217</v>
+        <v>232</v>
       </c>
       <c r="F50" s="1">
-        <v>45530</v>
+        <v>45600</v>
       </c>
       <c r="G50">
-        <v>207</v>
+        <v>227</v>
       </c>
     </row>
     <row r="51" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C51" s="1">
-        <v>45523</v>
+        <v>45579</v>
       </c>
       <c r="D51">
-        <v>216</v>
+        <v>231</v>
       </c>
       <c r="F51" s="1">
-        <v>45523</v>
+        <v>45579</v>
       </c>
       <c r="G51">
-        <v>200</v>
+        <v>222</v>
       </c>
     </row>
     <row r="52" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C52" s="1">
-        <v>45516</v>
+        <v>45572</v>
       </c>
       <c r="D52">
-        <v>212</v>
+        <v>227</v>
       </c>
       <c r="F52" s="1">
-        <v>45516</v>
+        <v>45572</v>
       </c>
       <c r="G52">
-        <v>190</v>
+        <v>216</v>
       </c>
     </row>
     <row r="53" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C53" s="1">
-        <v>45509</v>
+        <v>45565</v>
       </c>
       <c r="D53">
-        <v>210</v>
+        <v>223</v>
       </c>
       <c r="F53" s="1">
-        <v>45509</v>
+        <v>45565</v>
       </c>
       <c r="G53">
-        <v>189</v>
+        <v>216</v>
       </c>
     </row>
     <row r="54" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C54" s="1">
-        <v>45502</v>
+        <v>45537</v>
       </c>
       <c r="D54">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="F54" s="1">
-        <v>45502</v>
+        <v>45537</v>
       </c>
       <c r="G54">
-        <v>189</v>
+        <v>207</v>
       </c>
     </row>
     <row r="55" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C55" s="1">
-        <v>45495</v>
+        <v>45530</v>
       </c>
       <c r="D55">
-        <v>201</v>
+        <v>217</v>
       </c>
       <c r="F55" s="1">
-        <v>45495</v>
+        <v>45530</v>
       </c>
       <c r="G55">
-        <v>183</v>
+        <v>207</v>
       </c>
     </row>
     <row r="56" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C56" s="1">
-        <v>45488</v>
+        <v>45523</v>
       </c>
       <c r="D56">
-        <v>199</v>
+        <v>216</v>
       </c>
       <c r="F56" s="1">
-        <v>45488</v>
+        <v>45523</v>
       </c>
       <c r="G56">
-        <v>182</v>
+        <v>200</v>
       </c>
     </row>
     <row r="57" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C57" s="1">
-        <v>45481</v>
+        <v>45516</v>
       </c>
       <c r="D57">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="F57" s="1">
-        <v>45481</v>
+        <v>45516</v>
       </c>
       <c r="G57">
-        <v>180</v>
+        <v>190</v>
       </c>
     </row>
     <row r="58" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C58" s="1">
-        <v>45474</v>
+        <v>45509</v>
       </c>
       <c r="D58">
-        <v>187</v>
+        <v>210</v>
       </c>
       <c r="F58" s="1">
-        <v>45474</v>
+        <v>45509</v>
       </c>
       <c r="G58">
-        <v>172</v>
+        <v>189</v>
       </c>
     </row>
     <row r="59" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C59" s="1">
-        <v>45467</v>
+        <v>45502</v>
       </c>
       <c r="D59">
-        <v>187</v>
+        <v>210</v>
       </c>
       <c r="F59" s="1">
-        <v>45467</v>
+        <v>45502</v>
       </c>
       <c r="G59">
-        <v>172</v>
+        <v>189</v>
       </c>
     </row>
     <row r="60" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C60" s="1">
-        <v>45460</v>
+        <v>45495</v>
       </c>
       <c r="D60">
-        <v>185</v>
+        <v>201</v>
       </c>
       <c r="F60" s="1">
-        <v>45460</v>
+        <v>45495</v>
       </c>
       <c r="G60">
-        <v>165</v>
+        <v>183</v>
       </c>
     </row>
     <row r="61" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C61" s="1">
-        <v>45453</v>
+        <v>45488</v>
       </c>
       <c r="D61">
-        <v>180</v>
+        <v>199</v>
       </c>
       <c r="F61" s="1">
-        <v>45453</v>
+        <v>45488</v>
       </c>
       <c r="G61">
-        <v>164</v>
+        <v>182</v>
       </c>
     </row>
     <row r="62" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C62" s="1">
-        <v>45446</v>
+        <v>45481</v>
       </c>
       <c r="D62">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="F62" s="1">
-        <v>45446</v>
+        <v>45481</v>
       </c>
       <c r="G62">
-        <v>161</v>
+        <v>180</v>
       </c>
     </row>
     <row r="63" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C63" s="1">
-        <v>45439</v>
+        <v>45474</v>
       </c>
       <c r="D63">
-        <v>174</v>
+        <v>187</v>
       </c>
       <c r="F63" s="1">
-        <v>45439</v>
+        <v>45474</v>
       </c>
       <c r="G63">
-        <v>161</v>
+        <v>172</v>
       </c>
     </row>
     <row r="64" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C64" s="1">
-        <v>45432</v>
+        <v>45467</v>
       </c>
       <c r="D64">
-        <v>173</v>
+        <v>187</v>
       </c>
       <c r="F64" s="1">
-        <v>45432</v>
+        <v>45467</v>
       </c>
       <c r="G64">
-        <v>159</v>
+        <v>172</v>
       </c>
     </row>
     <row r="65" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C65" s="1">
-        <v>45425</v>
+        <v>45460</v>
       </c>
       <c r="D65">
-        <v>170</v>
+        <v>185</v>
       </c>
       <c r="F65" s="1">
-        <v>45425</v>
+        <v>45460</v>
       </c>
       <c r="G65">
-        <v>157</v>
+        <v>165</v>
       </c>
     </row>
     <row r="66" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C66" s="1">
-        <v>45418</v>
+        <v>45453</v>
       </c>
       <c r="D66">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="F66" s="1">
-        <v>45418</v>
+        <v>45453</v>
       </c>
       <c r="G66">
-        <v>141</v>
+        <v>164</v>
       </c>
     </row>
     <row r="67" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C67" s="1">
-        <v>45411</v>
+        <v>45446</v>
       </c>
       <c r="D67">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="F67" s="1">
-        <v>45411</v>
+        <v>45446</v>
       </c>
       <c r="G67">
-        <v>141</v>
+        <v>161</v>
       </c>
     </row>
     <row r="68" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C68" s="1">
-        <v>45404</v>
+        <v>45439</v>
       </c>
       <c r="D68">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="F68" s="1">
-        <v>45404</v>
+        <v>45439</v>
       </c>
       <c r="G68">
-        <v>141</v>
+        <v>161</v>
       </c>
     </row>
     <row r="69" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C69" s="1">
-        <v>45397</v>
+        <v>45432</v>
       </c>
       <c r="D69">
-        <v>157</v>
+        <v>173</v>
       </c>
       <c r="F69" s="1">
-        <v>45397</v>
+        <v>45432</v>
       </c>
       <c r="G69">
-        <v>132</v>
+        <v>159</v>
       </c>
     </row>
     <row r="70" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C70" s="1">
-        <v>45390</v>
+        <v>45425</v>
       </c>
       <c r="D70">
-        <v>146</v>
+        <v>170</v>
       </c>
       <c r="F70" s="1">
-        <v>45390</v>
+        <v>45425</v>
       </c>
       <c r="G70">
-        <v>132</v>
+        <v>157</v>
       </c>
     </row>
     <row r="71" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C71" s="1">
-        <v>45383</v>
+        <v>45418</v>
       </c>
       <c r="D71">
-        <v>138</v>
+        <v>170</v>
       </c>
       <c r="F71" s="1">
-        <v>45383</v>
+        <v>45418</v>
       </c>
       <c r="G71">
-        <v>119</v>
+        <v>141</v>
       </c>
     </row>
     <row r="72" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C72" s="1">
-        <v>45376</v>
+        <v>45411</v>
       </c>
       <c r="D72">
-        <v>129</v>
+        <v>166</v>
       </c>
       <c r="F72" s="1">
-        <v>45376</v>
+        <v>45411</v>
       </c>
       <c r="G72">
-        <v>114</v>
+        <v>141</v>
       </c>
     </row>
     <row r="73" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C73" s="1">
-        <v>45369</v>
+        <v>45404</v>
       </c>
       <c r="D73">
-        <v>123</v>
+        <v>166</v>
       </c>
       <c r="F73" s="1">
-        <v>45369</v>
+        <v>45404</v>
       </c>
       <c r="G73">
-        <v>97</v>
+        <v>141</v>
       </c>
     </row>
     <row r="74" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C74" s="1">
-        <v>45362</v>
+        <v>45397</v>
       </c>
       <c r="D74">
-        <v>113</v>
-      </c>
-      <c r="F74" s="1"/>
+        <v>157</v>
+      </c>
+      <c r="F74" s="1">
+        <v>45397</v>
+      </c>
+      <c r="G74">
+        <v>132</v>
+      </c>
     </row>
     <row r="75" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C75" s="1">
-        <v>45355</v>
+        <v>45390</v>
       </c>
       <c r="D75">
-        <v>108</v>
+        <v>146</v>
+      </c>
+      <c r="F75" s="1">
+        <v>45390</v>
+      </c>
+      <c r="G75">
+        <v>132</v>
       </c>
     </row>
     <row r="76" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C76" s="1">
-        <v>45348</v>
+        <v>45383</v>
       </c>
       <c r="D76">
-        <v>102</v>
+        <v>138</v>
+      </c>
+      <c r="F76" s="1">
+        <v>45383</v>
+      </c>
+      <c r="G76">
+        <v>119</v>
       </c>
     </row>
     <row r="77" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C77" s="1">
-        <v>45341</v>
+        <v>45376</v>
       </c>
       <c r="D77">
-        <v>95</v>
+        <v>129</v>
+      </c>
+      <c r="F77" s="1">
+        <v>45376</v>
+      </c>
+      <c r="G77">
+        <v>114</v>
       </c>
     </row>
     <row r="78" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C78" s="1">
-        <v>45334</v>
+        <v>45369</v>
       </c>
       <c r="D78">
-        <v>80</v>
+        <v>123</v>
+      </c>
+      <c r="F78" s="1">
+        <v>45369</v>
+      </c>
+      <c r="G78">
+        <v>97</v>
       </c>
     </row>
     <row r="79" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C79" s="1">
-        <v>45327</v>
+        <v>45362</v>
       </c>
       <c r="D79">
-        <v>66</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="F79" s="1"/>
     </row>
     <row r="80" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C80" s="1">
-        <v>45320</v>
+        <v>45355</v>
       </c>
       <c r="D80">
-        <v>55</v>
+        <v>108</v>
       </c>
     </row>
     <row r="81" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C81" s="1">
-        <v>45313</v>
+        <v>45348</v>
       </c>
       <c r="D81">
-        <v>53</v>
+        <v>102</v>
       </c>
     </row>
     <row r="82" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C82" s="1">
+        <v>45341</v>
+      </c>
+      <c r="D82">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="83" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C83" s="1">
+        <v>45334</v>
+      </c>
+      <c r="D83">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="84" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C84" s="1">
+        <v>45327</v>
+      </c>
+      <c r="D84">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="85" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C85" s="1">
+        <v>45320</v>
+      </c>
+      <c r="D85">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="86" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C86" s="1">
+        <v>45313</v>
+      </c>
+      <c r="D86">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="87" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C87" s="1">
         <v>45306</v>
       </c>
-      <c r="D82">
+      <c r="D87">
         <v>52</v>
       </c>
-    </row>
-    <row r="86" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="D86" s="2"/>
-      <c r="E86" s="2"/>
-      <c r="F86" s="2"/>
-      <c r="G86" s="2"/>
-      <c r="H86" s="2"/>
-      <c r="I86" s="2"/>
-      <c r="J86" s="2"/>
-      <c r="K86" s="2"/>
-      <c r="L86" s="2"/>
-      <c r="M86" s="2"/>
-      <c r="N86" s="2"/>
-      <c r="O86" s="2"/>
-      <c r="P86" s="2"/>
-      <c r="Q86" s="2"/>
-    </row>
-    <row r="87" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="D87" s="2"/>
-      <c r="E87" s="2"/>
-      <c r="F87" s="2"/>
-      <c r="G87" s="2"/>
-      <c r="H87" s="2"/>
-      <c r="I87" s="2"/>
-      <c r="J87" s="2"/>
-      <c r="K87" s="2"/>
-      <c r="L87" s="2"/>
-      <c r="M87" s="2"/>
-      <c r="N87" s="2"/>
-      <c r="O87" s="2"/>
-      <c r="P87" s="2"/>
-      <c r="Q87" s="2"/>
-    </row>
-    <row r="88" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="D88" s="2"/>
-      <c r="E88" s="2"/>
-      <c r="F88" s="2"/>
-      <c r="G88" s="2"/>
-      <c r="H88" s="2"/>
-      <c r="I88" s="2"/>
-      <c r="J88" s="2"/>
-      <c r="K88" s="2"/>
-      <c r="L88" s="2"/>
-      <c r="M88" s="2"/>
-      <c r="N88" s="2"/>
-      <c r="O88" s="2"/>
-      <c r="P88" s="2"/>
-      <c r="Q88" s="2"/>
-    </row>
-    <row r="89" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="D89" s="2"/>
-      <c r="E89" s="2"/>
-      <c r="F89" s="2"/>
-      <c r="G89" s="2"/>
-      <c r="H89" s="2"/>
-      <c r="I89" s="2"/>
-      <c r="J89" s="2"/>
-      <c r="K89" s="2"/>
-      <c r="L89" s="2"/>
-      <c r="M89" s="2"/>
-      <c r="N89" s="2"/>
-      <c r="O89" s="2"/>
-      <c r="P89" s="2"/>
-      <c r="Q89" s="2"/>
-    </row>
-    <row r="90" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="D90" s="2"/>
-      <c r="E90" s="2"/>
-      <c r="F90" s="2"/>
-      <c r="G90" s="2"/>
-      <c r="H90" s="2"/>
-      <c r="I90" s="2"/>
-      <c r="J90" s="2"/>
-      <c r="K90" s="2"/>
-      <c r="L90" s="2"/>
-      <c r="M90" s="2"/>
-      <c r="N90" s="2"/>
-      <c r="O90" s="2"/>
-      <c r="P90" s="2"/>
-      <c r="Q90" s="2"/>
     </row>
     <row r="91" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D91" s="2"/>
@@ -6156,9 +6090,89 @@
       <c r="P111" s="2"/>
       <c r="Q111" s="2"/>
     </row>
+    <row r="112" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D112" s="2"/>
+      <c r="E112" s="2"/>
+      <c r="F112" s="2"/>
+      <c r="G112" s="2"/>
+      <c r="H112" s="2"/>
+      <c r="I112" s="2"/>
+      <c r="J112" s="2"/>
+      <c r="K112" s="2"/>
+      <c r="L112" s="2"/>
+      <c r="M112" s="2"/>
+      <c r="N112" s="2"/>
+      <c r="O112" s="2"/>
+      <c r="P112" s="2"/>
+      <c r="Q112" s="2"/>
+    </row>
+    <row r="113" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D113" s="2"/>
+      <c r="E113" s="2"/>
+      <c r="F113" s="2"/>
+      <c r="G113" s="2"/>
+      <c r="H113" s="2"/>
+      <c r="I113" s="2"/>
+      <c r="J113" s="2"/>
+      <c r="K113" s="2"/>
+      <c r="L113" s="2"/>
+      <c r="M113" s="2"/>
+      <c r="N113" s="2"/>
+      <c r="O113" s="2"/>
+      <c r="P113" s="2"/>
+      <c r="Q113" s="2"/>
+    </row>
+    <row r="114" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D114" s="2"/>
+      <c r="E114" s="2"/>
+      <c r="F114" s="2"/>
+      <c r="G114" s="2"/>
+      <c r="H114" s="2"/>
+      <c r="I114" s="2"/>
+      <c r="J114" s="2"/>
+      <c r="K114" s="2"/>
+      <c r="L114" s="2"/>
+      <c r="M114" s="2"/>
+      <c r="N114" s="2"/>
+      <c r="O114" s="2"/>
+      <c r="P114" s="2"/>
+      <c r="Q114" s="2"/>
+    </row>
+    <row r="115" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D115" s="2"/>
+      <c r="E115" s="2"/>
+      <c r="F115" s="2"/>
+      <c r="G115" s="2"/>
+      <c r="H115" s="2"/>
+      <c r="I115" s="2"/>
+      <c r="J115" s="2"/>
+      <c r="K115" s="2"/>
+      <c r="L115" s="2"/>
+      <c r="M115" s="2"/>
+      <c r="N115" s="2"/>
+      <c r="O115" s="2"/>
+      <c r="P115" s="2"/>
+      <c r="Q115" s="2"/>
+    </row>
+    <row r="116" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D116" s="2"/>
+      <c r="E116" s="2"/>
+      <c r="F116" s="2"/>
+      <c r="G116" s="2"/>
+      <c r="H116" s="2"/>
+      <c r="I116" s="2"/>
+      <c r="J116" s="2"/>
+      <c r="K116" s="2"/>
+      <c r="L116" s="2"/>
+      <c r="M116" s="2"/>
+      <c r="N116" s="2"/>
+      <c r="O116" s="2"/>
+      <c r="P116" s="2"/>
+      <c r="Q116" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D86:Q111"/>
+    <mergeCell ref="D91:Q116"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
LGHUB 2025/6/25 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
- 网站错误 & 本地化问题详见 LGHUB/WebLoc/README.md
</commit_message>
<xml_diff>
--- a/Documents/Graph_PC.xlsx
+++ b/Documents/Graph_PC.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29022"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FACE42BF-5F6C-4DCC-902D-61ADE48E0597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CEA3B7B-0C4B-493C-B8C1-C6F6236BADE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -293,6 +293,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -300,7 +301,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -574,13 +574,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>25</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>32</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -917,72 +917,72 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$20:$C$28</c:f>
+              <c:f>Sheet1!$C$19:$C$27</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45831</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45824</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45817</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45810</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45803</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45796</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45789</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45782</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45775</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45768</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$20:$D$28</c:f>
+              <c:f>Sheet1!$D$19:$D$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>416</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>407</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>404</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>395</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>386</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>379</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>365</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>356</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>348</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>343</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1086,63 +1086,63 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$20:$C$28</c:f>
+              <c:f>Sheet1!$C$19:$C$27</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45831</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45824</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45817</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45810</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45803</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45796</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45789</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45782</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45775</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45768</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$20:$G$28</c:f>
+              <c:f>Sheet1!$G$19:$G$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>369</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>359</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>360</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>354</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>349</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>320</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>320</c:v>
@@ -1151,7 +1151,7 @@
                   <c:v>320</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>319</c:v>
+                  <c:v>320</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1286,8 +1286,8 @@
         <c:axId val="1374569007"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="415"/>
-          <c:min val="315"/>
+          <c:max val="420"/>
+          <c:min val="320"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1794,13 +1794,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>25</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>32</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1884,6 +1884,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1891,7 +1892,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -4811,8 +4811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B89" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="K90" sqref="K90"/>
+    <sheetView tabSelected="1" topLeftCell="B88" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="L90" sqref="L90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -4836,7 +4836,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
@@ -4852,7 +4852,21 @@
         <v>4</v>
       </c>
       <c r="C7">
-        <v>32</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C19" s="1">
+        <v>45831</v>
+      </c>
+      <c r="D19">
+        <v>416</v>
+      </c>
+      <c r="F19" s="1">
+        <v>45831</v>
+      </c>
+      <c r="G19">
+        <v>370</v>
       </c>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
LGHUB 2025/7/5 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
- 网站错误 & 本地化问题详见 LGHUB/WebLoc/README.md
</commit_message>
<xml_diff>
--- a/Documents/Graph_PC.xlsx
+++ b/Documents/Graph_PC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29022"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CEA3B7B-0C4B-493C-B8C1-C6F6236BADE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{219C7ADC-063B-4BA0-B51A-901A143A9746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="2" r:id="rId1"/>
@@ -293,7 +293,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -301,6 +300,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -574,13 +574,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>33</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>33</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -917,72 +917,72 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$19:$C$27</c:f>
+              <c:f>Sheet1!$C$17:$C$25</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45845</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45838</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>45831</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>45824</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>45817</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>45810</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>45803</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>45796</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>45789</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>45782</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45775</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$19:$D$27</c:f>
+              <c:f>Sheet1!$D$17:$D$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>418</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>416</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
+                  <c:v>416</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>407</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>404</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>395</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>386</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>379</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>365</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>356</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>348</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1086,69 +1086,69 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$19:$C$27</c:f>
+              <c:f>Sheet1!$C$17:$C$25</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45845</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45838</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>45831</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>45824</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>45817</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>45810</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>45803</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>45796</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>45789</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>45782</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45775</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$19:$G$27</c:f>
+              <c:f>Sheet1!$G$17:$G$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>386</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>370</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>369</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>359</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>360</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>354</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>349</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>320</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>320</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>320</c:v>
@@ -1794,13 +1794,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>33</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>33</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1884,7 +1884,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1892,6 +1891,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -4811,51 +4811,79 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B88" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D89" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="L90" sqref="L90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C17" s="1">
+        <v>45845</v>
+      </c>
+      <c r="D17">
+        <v>418</v>
+      </c>
+      <c r="F17" s="1">
+        <v>45845</v>
+      </c>
+      <c r="G17">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C18" s="1">
+        <v>45838</v>
+      </c>
+      <c r="D18">
+        <v>416</v>
+      </c>
+      <c r="F18" s="1">
+        <v>45838</v>
+      </c>
+      <c r="G18">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C19" s="1">
         <v>45831</v>
       </c>
@@ -4869,7 +4897,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C20" s="1">
         <v>45824</v>
       </c>
@@ -4883,7 +4911,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C21" s="1">
         <v>45817</v>
       </c>
@@ -4897,7 +4925,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C22" s="1">
         <v>45810</v>
       </c>
@@ -4911,7 +4939,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C23" s="1">
         <v>45803</v>
       </c>
@@ -4925,7 +4953,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C24" s="1">
         <v>45796</v>
       </c>
@@ -4939,7 +4967,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C25" s="1">
         <v>45789</v>
       </c>
@@ -4953,7 +4981,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C26" s="1">
         <v>45782</v>
       </c>
@@ -4967,7 +4995,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C27" s="1">
         <v>45775</v>
       </c>
@@ -4981,7 +5009,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C28" s="1">
         <v>45768</v>
       </c>
@@ -4995,7 +5023,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C29" s="1">
         <v>45761</v>
       </c>
@@ -5009,7 +5037,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C30" s="1">
         <v>45754</v>
       </c>
@@ -5023,7 +5051,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C31" s="1">
         <v>45747</v>
       </c>
@@ -5037,7 +5065,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C32" s="1">
         <v>45740</v>
       </c>
@@ -5051,7 +5079,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C33" s="1">
         <v>45733</v>
       </c>
@@ -5065,7 +5093,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C34" s="1">
         <v>45726</v>
       </c>
@@ -5079,7 +5107,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C35" s="1">
         <v>45719</v>
       </c>
@@ -5093,7 +5121,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C36" s="1">
         <v>45712</v>
       </c>
@@ -5107,7 +5135,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="37" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C37" s="1">
         <v>45705</v>
       </c>
@@ -5121,7 +5149,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="38" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C38" s="1">
         <v>45698</v>
       </c>
@@ -5135,7 +5163,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="39" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C39" s="1">
         <v>45691</v>
       </c>
@@ -5149,7 +5177,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="40" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C40" s="1">
         <v>45684</v>
       </c>
@@ -5163,7 +5191,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="41" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C41" s="1">
         <v>45677</v>
       </c>
@@ -5177,7 +5205,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="42" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C42" s="1">
         <v>45670</v>
       </c>
@@ -5191,7 +5219,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="43" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C43" s="1">
         <v>45663</v>
       </c>
@@ -5205,7 +5233,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="44" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C44" s="1">
         <v>45642</v>
       </c>
@@ -5219,7 +5247,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="45" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C45" s="1">
         <v>45635</v>
       </c>
@@ -5233,7 +5261,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="46" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C46" s="1">
         <v>45628</v>
       </c>
@@ -5247,7 +5275,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="47" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C47" s="1">
         <v>45621</v>
       </c>
@@ -5261,7 +5289,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="48" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C48" s="1">
         <v>45614</v>
       </c>
@@ -5275,7 +5303,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="49" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C49" s="1">
         <v>45607</v>
       </c>
@@ -5289,7 +5317,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="50" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C50" s="1">
         <v>45600</v>
       </c>
@@ -5303,7 +5331,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="51" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C51" s="1">
         <v>45579</v>
       </c>
@@ -5317,7 +5345,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="52" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C52" s="1">
         <v>45572</v>
       </c>
@@ -5331,7 +5359,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="53" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C53" s="1">
         <v>45565</v>
       </c>
@@ -5345,7 +5373,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="54" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C54" s="1">
         <v>45537</v>
       </c>
@@ -5359,7 +5387,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="55" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C55" s="1">
         <v>45530</v>
       </c>
@@ -5373,7 +5401,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="56" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C56" s="1">
         <v>45523</v>
       </c>
@@ -5387,7 +5415,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="57" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C57" s="1">
         <v>45516</v>
       </c>
@@ -5401,7 +5429,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="58" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C58" s="1">
         <v>45509</v>
       </c>
@@ -5415,7 +5443,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="59" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C59" s="1">
         <v>45502</v>
       </c>
@@ -5429,7 +5457,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="60" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C60" s="1">
         <v>45495</v>
       </c>
@@ -5443,7 +5471,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="61" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C61" s="1">
         <v>45488</v>
       </c>
@@ -5457,7 +5485,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="62" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C62" s="1">
         <v>45481</v>
       </c>
@@ -5471,7 +5499,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="63" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C63" s="1">
         <v>45474</v>
       </c>
@@ -5485,7 +5513,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="64" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C64" s="1">
         <v>45467</v>
       </c>
@@ -5499,7 +5527,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="65" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C65" s="1">
         <v>45460</v>
       </c>
@@ -5513,7 +5541,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="66" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C66" s="1">
         <v>45453</v>
       </c>
@@ -5527,7 +5555,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="67" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C67" s="1">
         <v>45446</v>
       </c>
@@ -5541,7 +5569,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="68" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C68" s="1">
         <v>45439</v>
       </c>
@@ -5555,7 +5583,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="69" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C69" s="1">
         <v>45432</v>
       </c>
@@ -5569,7 +5597,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="70" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C70" s="1">
         <v>45425</v>
       </c>
@@ -5583,7 +5611,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="71" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C71" s="1">
         <v>45418</v>
       </c>
@@ -5597,7 +5625,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="72" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C72" s="1">
         <v>45411</v>
       </c>
@@ -5611,7 +5639,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="73" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C73" s="1">
         <v>45404</v>
       </c>
@@ -5625,7 +5653,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="74" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C74" s="1">
         <v>45397</v>
       </c>
@@ -5639,7 +5667,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="75" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C75" s="1">
         <v>45390</v>
       </c>
@@ -5653,7 +5681,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="76" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C76" s="1">
         <v>45383</v>
       </c>
@@ -5667,7 +5695,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="77" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C77" s="1">
         <v>45376</v>
       </c>
@@ -5681,7 +5709,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="78" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C78" s="1">
         <v>45369</v>
       </c>
@@ -5695,7 +5723,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="79" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C79" s="1">
         <v>45362</v>
       </c>
@@ -5704,7 +5732,7 @@
       </c>
       <c r="F79" s="1"/>
     </row>
-    <row r="80" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C80" s="1">
         <v>45355</v>
       </c>
@@ -5712,7 +5740,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="81" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="81" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C81" s="1">
         <v>45348</v>
       </c>
@@ -5720,7 +5748,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="82" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="82" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C82" s="1">
         <v>45341</v>
       </c>
@@ -5728,7 +5756,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="83" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="83" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C83" s="1">
         <v>45334</v>
       </c>
@@ -5736,7 +5764,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="84" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="84" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C84" s="1">
         <v>45327</v>
       </c>
@@ -5744,7 +5772,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="85" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="85" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C85" s="1">
         <v>45320</v>
       </c>
@@ -5752,7 +5780,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="86" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="86" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C86" s="1">
         <v>45313</v>
       </c>
@@ -5760,7 +5788,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="87" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="87" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C87" s="1">
         <v>45306</v>
       </c>
@@ -5768,7 +5796,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="91" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="91" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D91" s="2"/>
       <c r="E91" s="2"/>
       <c r="F91" s="2"/>
@@ -5784,7 +5812,7 @@
       <c r="P91" s="2"/>
       <c r="Q91" s="2"/>
     </row>
-    <row r="92" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="92" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D92" s="2"/>
       <c r="E92" s="2"/>
       <c r="F92" s="2"/>
@@ -5800,7 +5828,7 @@
       <c r="P92" s="2"/>
       <c r="Q92" s="2"/>
     </row>
-    <row r="93" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="93" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D93" s="2"/>
       <c r="E93" s="2"/>
       <c r="F93" s="2"/>
@@ -5816,7 +5844,7 @@
       <c r="P93" s="2"/>
       <c r="Q93" s="2"/>
     </row>
-    <row r="94" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="94" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D94" s="2"/>
       <c r="E94" s="2"/>
       <c r="F94" s="2"/>
@@ -5832,7 +5860,7 @@
       <c r="P94" s="2"/>
       <c r="Q94" s="2"/>
     </row>
-    <row r="95" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="95" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D95" s="2"/>
       <c r="E95" s="2"/>
       <c r="F95" s="2"/>
@@ -5848,7 +5876,7 @@
       <c r="P95" s="2"/>
       <c r="Q95" s="2"/>
     </row>
-    <row r="96" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="96" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D96" s="2"/>
       <c r="E96" s="2"/>
       <c r="F96" s="2"/>
@@ -5864,7 +5892,7 @@
       <c r="P96" s="2"/>
       <c r="Q96" s="2"/>
     </row>
-    <row r="97" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="97" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D97" s="2"/>
       <c r="E97" s="2"/>
       <c r="F97" s="2"/>
@@ -5880,7 +5908,7 @@
       <c r="P97" s="2"/>
       <c r="Q97" s="2"/>
     </row>
-    <row r="98" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="98" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D98" s="2"/>
       <c r="E98" s="2"/>
       <c r="F98" s="2"/>
@@ -5896,7 +5924,7 @@
       <c r="P98" s="2"/>
       <c r="Q98" s="2"/>
     </row>
-    <row r="99" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="99" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D99" s="2"/>
       <c r="E99" s="2"/>
       <c r="F99" s="2"/>
@@ -5912,7 +5940,7 @@
       <c r="P99" s="2"/>
       <c r="Q99" s="2"/>
     </row>
-    <row r="100" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="100" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D100" s="2"/>
       <c r="E100" s="2"/>
       <c r="F100" s="2"/>
@@ -5928,7 +5956,7 @@
       <c r="P100" s="2"/>
       <c r="Q100" s="2"/>
     </row>
-    <row r="101" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="101" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D101" s="2"/>
       <c r="E101" s="2"/>
       <c r="F101" s="2"/>
@@ -5944,7 +5972,7 @@
       <c r="P101" s="2"/>
       <c r="Q101" s="2"/>
     </row>
-    <row r="102" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="102" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D102" s="2"/>
       <c r="E102" s="2"/>
       <c r="F102" s="2"/>
@@ -5960,7 +5988,7 @@
       <c r="P102" s="2"/>
       <c r="Q102" s="2"/>
     </row>
-    <row r="103" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="103" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D103" s="2"/>
       <c r="E103" s="2"/>
       <c r="F103" s="2"/>
@@ -5976,7 +6004,7 @@
       <c r="P103" s="2"/>
       <c r="Q103" s="2"/>
     </row>
-    <row r="104" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="104" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D104" s="2"/>
       <c r="E104" s="2"/>
       <c r="F104" s="2"/>
@@ -5992,7 +6020,7 @@
       <c r="P104" s="2"/>
       <c r="Q104" s="2"/>
     </row>
-    <row r="105" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="105" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D105" s="2"/>
       <c r="E105" s="2"/>
       <c r="F105" s="2"/>
@@ -6008,7 +6036,7 @@
       <c r="P105" s="2"/>
       <c r="Q105" s="2"/>
     </row>
-    <row r="106" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="106" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D106" s="2"/>
       <c r="E106" s="2"/>
       <c r="F106" s="2"/>
@@ -6024,7 +6052,7 @@
       <c r="P106" s="2"/>
       <c r="Q106" s="2"/>
     </row>
-    <row r="107" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="107" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D107" s="2"/>
       <c r="E107" s="2"/>
       <c r="F107" s="2"/>
@@ -6040,7 +6068,7 @@
       <c r="P107" s="2"/>
       <c r="Q107" s="2"/>
     </row>
-    <row r="108" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="108" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D108" s="2"/>
       <c r="E108" s="2"/>
       <c r="F108" s="2"/>
@@ -6056,7 +6084,7 @@
       <c r="P108" s="2"/>
       <c r="Q108" s="2"/>
     </row>
-    <row r="109" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="109" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D109" s="2"/>
       <c r="E109" s="2"/>
       <c r="F109" s="2"/>
@@ -6072,7 +6100,7 @@
       <c r="P109" s="2"/>
       <c r="Q109" s="2"/>
     </row>
-    <row r="110" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="110" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D110" s="2"/>
       <c r="E110" s="2"/>
       <c r="F110" s="2"/>
@@ -6088,7 +6116,7 @@
       <c r="P110" s="2"/>
       <c r="Q110" s="2"/>
     </row>
-    <row r="111" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="111" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D111" s="2"/>
       <c r="E111" s="2"/>
       <c r="F111" s="2"/>
@@ -6104,7 +6132,7 @@
       <c r="P111" s="2"/>
       <c r="Q111" s="2"/>
     </row>
-    <row r="112" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="112" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D112" s="2"/>
       <c r="E112" s="2"/>
       <c r="F112" s="2"/>
@@ -6120,7 +6148,7 @@
       <c r="P112" s="2"/>
       <c r="Q112" s="2"/>
     </row>
-    <row r="113" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="113" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D113" s="2"/>
       <c r="E113" s="2"/>
       <c r="F113" s="2"/>
@@ -6136,7 +6164,7 @@
       <c r="P113" s="2"/>
       <c r="Q113" s="2"/>
     </row>
-    <row r="114" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="114" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D114" s="2"/>
       <c r="E114" s="2"/>
       <c r="F114" s="2"/>
@@ -6152,7 +6180,7 @@
       <c r="P114" s="2"/>
       <c r="Q114" s="2"/>
     </row>
-    <row r="115" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="115" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D115" s="2"/>
       <c r="E115" s="2"/>
       <c r="F115" s="2"/>
@@ -6168,7 +6196,7 @@
       <c r="P115" s="2"/>
       <c r="Q115" s="2"/>
     </row>
-    <row r="116" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="116" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D116" s="2"/>
       <c r="E116" s="2"/>
       <c r="F116" s="2"/>

</xml_diff>

<commit_message>
LGHUB 2025/7/12 更新 2
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
- 网站错误 & 本地化问题详见 LGHUB/WebLoc/README.md
</commit_message>
<xml_diff>
--- a/Documents/Graph_PC.xlsx
+++ b/Documents/Graph_PC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{219C7ADC-063B-4BA0-B51A-901A143A9746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C51C6B7-8274-4C65-B034-34C344B5C21E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -577,7 +577,7 @@
                   <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>49</c:v>
@@ -917,72 +917,72 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$17:$C$25</c:f>
+              <c:f>Sheet1!$C$20:$C$28</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45852</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45845</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45838</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45831</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45824</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45817</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45810</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45803</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45796</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45789</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$17:$D$25</c:f>
+              <c:f>Sheet1!$D$20:$D$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>418</c:v>
+                  <c:v>419</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>416</c:v>
+                  <c:v>418</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>416</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>416</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>407</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>404</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>395</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>386</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>379</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>365</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1086,43 +1086,43 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$17:$C$25</c:f>
+              <c:f>Sheet1!$C$20:$C$28</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45852</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45845</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45838</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45831</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45824</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45817</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45810</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45803</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45796</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45789</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$17:$G$25</c:f>
+              <c:f>Sheet1!$G$20:$G$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1130,28 +1130,28 @@
                   <c:v>386</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>370</c:v>
+                  <c:v>386</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>370</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>369</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>359</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>360</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>354</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>349</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>320</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1286,8 +1286,8 @@
         <c:axId val="1374569007"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="420"/>
-          <c:min val="320"/>
+          <c:max val="430"/>
+          <c:min val="340"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1797,7 +1797,7 @@
                   <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>49</c:v>
@@ -4223,13 +4223,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>106422</xdr:colOff>
-      <xdr:row>91</xdr:row>
+      <xdr:row>95</xdr:row>
       <xdr:rowOff>165023</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>106</xdr:row>
+      <xdr:row>110</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4259,13 +4259,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>190501</xdr:colOff>
-      <xdr:row>91</xdr:row>
+      <xdr:row>95</xdr:row>
       <xdr:rowOff>162248</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>124495</xdr:colOff>
-      <xdr:row>106</xdr:row>
+      <xdr:row>110</xdr:row>
       <xdr:rowOff>163286</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4809,10 +4809,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:Q116"/>
+  <dimension ref="B2:Q120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D89" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L90" sqref="L90"/>
+    <sheetView tabSelected="1" topLeftCell="D92" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L94" sqref="L94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -4844,7 +4844,7 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.35">
@@ -4855,1010 +4855,960 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C17" s="1">
-        <v>45845</v>
-      </c>
-      <c r="D17">
-        <v>418</v>
-      </c>
-      <c r="F17" s="1">
-        <v>45845</v>
-      </c>
-      <c r="G17">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C18" s="1">
-        <v>45838</v>
-      </c>
-      <c r="D18">
-        <v>416</v>
-      </c>
-      <c r="F18" s="1">
-        <v>45838</v>
-      </c>
-      <c r="G18">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C19" s="1">
-        <v>45831</v>
-      </c>
-      <c r="D19">
-        <v>416</v>
-      </c>
-      <c r="F19" s="1">
-        <v>45831</v>
-      </c>
-      <c r="G19">
-        <v>370</v>
-      </c>
-    </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C20" s="1">
-        <v>45824</v>
+        <v>45852</v>
       </c>
       <c r="D20">
-        <v>407</v>
+        <v>419</v>
       </c>
       <c r="F20" s="1">
-        <v>45824</v>
+        <v>45852</v>
       </c>
       <c r="G20">
-        <v>369</v>
+        <v>386</v>
       </c>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C21" s="1">
-        <v>45817</v>
+        <v>45845</v>
       </c>
       <c r="D21">
-        <v>404</v>
+        <v>418</v>
       </c>
       <c r="F21" s="1">
-        <v>45817</v>
+        <v>45845</v>
       </c>
       <c r="G21">
-        <v>359</v>
+        <v>386</v>
       </c>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C22" s="1">
-        <v>45810</v>
+        <v>45838</v>
       </c>
       <c r="D22">
-        <v>395</v>
+        <v>416</v>
       </c>
       <c r="F22" s="1">
-        <v>45810</v>
+        <v>45838</v>
       </c>
       <c r="G22">
-        <v>360</v>
+        <v>370</v>
       </c>
     </row>
     <row r="23" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C23" s="1">
-        <v>45803</v>
+        <v>45831</v>
       </c>
       <c r="D23">
-        <v>386</v>
+        <v>416</v>
       </c>
       <c r="F23" s="1">
-        <v>45803</v>
+        <v>45831</v>
       </c>
       <c r="G23">
-        <v>354</v>
+        <v>370</v>
       </c>
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C24" s="1">
-        <v>45796</v>
+        <v>45824</v>
       </c>
       <c r="D24">
-        <v>379</v>
+        <v>407</v>
       </c>
       <c r="F24" s="1">
-        <v>45796</v>
+        <v>45824</v>
       </c>
       <c r="G24">
-        <v>349</v>
+        <v>369</v>
       </c>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C25" s="1">
-        <v>45789</v>
+        <v>45817</v>
       </c>
       <c r="D25">
-        <v>365</v>
+        <v>404</v>
       </c>
       <c r="F25" s="1">
-        <v>45789</v>
+        <v>45817</v>
       </c>
       <c r="G25">
-        <v>320</v>
+        <v>359</v>
       </c>
     </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C26" s="1">
-        <v>45782</v>
+        <v>45810</v>
       </c>
       <c r="D26">
-        <v>356</v>
+        <v>395</v>
       </c>
       <c r="F26" s="1">
-        <v>45782</v>
+        <v>45810</v>
       </c>
       <c r="G26">
-        <v>320</v>
+        <v>360</v>
       </c>
     </row>
     <row r="27" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C27" s="1">
-        <v>45775</v>
+        <v>45803</v>
       </c>
       <c r="D27">
-        <v>348</v>
+        <v>386</v>
       </c>
       <c r="F27" s="1">
-        <v>45775</v>
+        <v>45803</v>
       </c>
       <c r="G27">
-        <v>320</v>
+        <v>354</v>
       </c>
     </row>
     <row r="28" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C28" s="1">
-        <v>45768</v>
+        <v>45796</v>
       </c>
       <c r="D28">
-        <v>343</v>
+        <v>379</v>
       </c>
       <c r="F28" s="1">
-        <v>45768</v>
+        <v>45796</v>
       </c>
       <c r="G28">
-        <v>319</v>
+        <v>349</v>
       </c>
     </row>
     <row r="29" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C29" s="1">
-        <v>45761</v>
+        <v>45789</v>
       </c>
       <c r="D29">
-        <v>334</v>
+        <v>365</v>
       </c>
       <c r="F29" s="1">
-        <v>45761</v>
+        <v>45789</v>
       </c>
       <c r="G29">
-        <v>303</v>
+        <v>320</v>
       </c>
     </row>
     <row r="30" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C30" s="1">
-        <v>45754</v>
+        <v>45782</v>
       </c>
       <c r="D30">
-        <v>330</v>
+        <v>356</v>
       </c>
       <c r="F30" s="1">
-        <v>45754</v>
+        <v>45782</v>
       </c>
       <c r="G30">
-        <v>302</v>
+        <v>320</v>
       </c>
     </row>
     <row r="31" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C31" s="1">
-        <v>45747</v>
+        <v>45775</v>
       </c>
       <c r="D31">
-        <v>325</v>
+        <v>348</v>
       </c>
       <c r="F31" s="1">
-        <v>45747</v>
+        <v>45775</v>
       </c>
       <c r="G31">
-        <v>302</v>
+        <v>320</v>
       </c>
     </row>
     <row r="32" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C32" s="1">
-        <v>45740</v>
+        <v>45768</v>
       </c>
       <c r="D32">
-        <v>316</v>
+        <v>343</v>
       </c>
       <c r="F32" s="1">
-        <v>45740</v>
+        <v>45768</v>
       </c>
       <c r="G32">
-        <v>296</v>
+        <v>319</v>
       </c>
     </row>
     <row r="33" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C33" s="1">
-        <v>45733</v>
+        <v>45761</v>
       </c>
       <c r="D33">
-        <v>310</v>
+        <v>334</v>
       </c>
       <c r="F33" s="1">
-        <v>45733</v>
+        <v>45761</v>
       </c>
       <c r="G33">
-        <v>296</v>
+        <v>303</v>
       </c>
     </row>
     <row r="34" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C34" s="1">
-        <v>45726</v>
+        <v>45754</v>
       </c>
       <c r="D34">
-        <v>309</v>
+        <v>330</v>
       </c>
       <c r="F34" s="1">
-        <v>45726</v>
+        <v>45754</v>
       </c>
       <c r="G34">
-        <v>294</v>
+        <v>302</v>
       </c>
     </row>
     <row r="35" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C35" s="1">
-        <v>45719</v>
+        <v>45747</v>
       </c>
       <c r="D35">
-        <v>308</v>
+        <v>325</v>
       </c>
       <c r="F35" s="1">
-        <v>45719</v>
+        <v>45747</v>
       </c>
       <c r="G35">
-        <v>286</v>
+        <v>302</v>
       </c>
     </row>
     <row r="36" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C36" s="1">
-        <v>45712</v>
+        <v>45740</v>
       </c>
       <c r="D36">
-        <v>306</v>
+        <v>316</v>
       </c>
       <c r="F36" s="1">
-        <v>45712</v>
+        <v>45740</v>
       </c>
       <c r="G36">
-        <v>286</v>
+        <v>296</v>
       </c>
     </row>
     <row r="37" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C37" s="1">
-        <v>45705</v>
+        <v>45733</v>
       </c>
       <c r="D37">
-        <v>301</v>
+        <v>310</v>
       </c>
       <c r="F37" s="1">
-        <v>45705</v>
+        <v>45733</v>
       </c>
       <c r="G37">
-        <v>267</v>
+        <v>296</v>
       </c>
     </row>
     <row r="38" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C38" s="1">
-        <v>45698</v>
+        <v>45726</v>
       </c>
       <c r="D38">
-        <v>295</v>
+        <v>309</v>
       </c>
       <c r="F38" s="1">
-        <v>45698</v>
+        <v>45726</v>
       </c>
       <c r="G38">
-        <v>267</v>
+        <v>294</v>
       </c>
     </row>
     <row r="39" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C39" s="1">
-        <v>45691</v>
+        <v>45719</v>
       </c>
       <c r="D39">
-        <v>289</v>
+        <v>308</v>
       </c>
       <c r="F39" s="1">
-        <v>45691</v>
+        <v>45719</v>
       </c>
       <c r="G39">
-        <v>267</v>
+        <v>286</v>
       </c>
     </row>
     <row r="40" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C40" s="1">
-        <v>45684</v>
+        <v>45712</v>
       </c>
       <c r="D40">
-        <v>284</v>
+        <v>306</v>
       </c>
       <c r="F40" s="1">
-        <v>45684</v>
+        <v>45712</v>
       </c>
       <c r="G40">
-        <v>262</v>
+        <v>286</v>
       </c>
     </row>
     <row r="41" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C41" s="1">
-        <v>45677</v>
+        <v>45705</v>
       </c>
       <c r="D41">
-        <v>273</v>
+        <v>301</v>
       </c>
       <c r="F41" s="1">
-        <v>45677</v>
+        <v>45705</v>
       </c>
       <c r="G41">
-        <v>254</v>
+        <v>267</v>
       </c>
     </row>
     <row r="42" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C42" s="1">
-        <v>45670</v>
+        <v>45698</v>
       </c>
       <c r="D42">
-        <v>264</v>
+        <v>295</v>
       </c>
       <c r="F42" s="1">
-        <v>45670</v>
+        <v>45698</v>
       </c>
       <c r="G42">
-        <v>250</v>
+        <v>267</v>
       </c>
     </row>
     <row r="43" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C43" s="1">
-        <v>45663</v>
+        <v>45691</v>
       </c>
       <c r="D43">
-        <v>256</v>
+        <v>289</v>
       </c>
       <c r="F43" s="1">
-        <v>45663</v>
+        <v>45691</v>
       </c>
       <c r="G43">
-        <v>250</v>
+        <v>267</v>
       </c>
     </row>
     <row r="44" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C44" s="1">
-        <v>45642</v>
+        <v>45684</v>
       </c>
       <c r="D44">
-        <v>256</v>
+        <v>284</v>
       </c>
       <c r="F44" s="1">
-        <v>45642</v>
+        <v>45684</v>
       </c>
       <c r="G44">
-        <v>245</v>
+        <v>262</v>
       </c>
     </row>
     <row r="45" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C45" s="1">
-        <v>45635</v>
+        <v>45677</v>
       </c>
       <c r="D45">
-        <v>251</v>
+        <v>273</v>
       </c>
       <c r="F45" s="1">
-        <v>45635</v>
+        <v>45677</v>
       </c>
       <c r="G45">
-        <v>243</v>
+        <v>254</v>
       </c>
     </row>
     <row r="46" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C46" s="1">
-        <v>45628</v>
+        <v>45670</v>
       </c>
       <c r="D46">
-        <v>251</v>
+        <v>264</v>
       </c>
       <c r="F46" s="1">
-        <v>45628</v>
+        <v>45670</v>
       </c>
       <c r="G46">
-        <v>239</v>
+        <v>250</v>
       </c>
     </row>
     <row r="47" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C47" s="1">
-        <v>45621</v>
+        <v>45663</v>
       </c>
       <c r="D47">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="F47" s="1">
-        <v>45621</v>
+        <v>45663</v>
       </c>
       <c r="G47">
-        <v>234</v>
+        <v>250</v>
       </c>
     </row>
     <row r="48" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C48" s="1">
-        <v>45614</v>
+        <v>45642</v>
       </c>
       <c r="D48">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="F48" s="1">
-        <v>45614</v>
+        <v>45642</v>
       </c>
       <c r="G48">
-        <v>234</v>
+        <v>245</v>
       </c>
     </row>
     <row r="49" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C49" s="1">
-        <v>45607</v>
+        <v>45635</v>
       </c>
       <c r="D49">
-        <v>239</v>
+        <v>251</v>
       </c>
       <c r="F49" s="1">
-        <v>45607</v>
+        <v>45635</v>
       </c>
       <c r="G49">
-        <v>230</v>
+        <v>243</v>
       </c>
     </row>
     <row r="50" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C50" s="1">
-        <v>45600</v>
+        <v>45628</v>
       </c>
       <c r="D50">
-        <v>232</v>
+        <v>251</v>
       </c>
       <c r="F50" s="1">
-        <v>45600</v>
+        <v>45628</v>
       </c>
       <c r="G50">
-        <v>227</v>
+        <v>239</v>
       </c>
     </row>
     <row r="51" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C51" s="1">
-        <v>45579</v>
+        <v>45621</v>
       </c>
       <c r="D51">
-        <v>231</v>
+        <v>247</v>
       </c>
       <c r="F51" s="1">
-        <v>45579</v>
+        <v>45621</v>
       </c>
       <c r="G51">
-        <v>222</v>
+        <v>234</v>
       </c>
     </row>
     <row r="52" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C52" s="1">
-        <v>45572</v>
+        <v>45614</v>
       </c>
       <c r="D52">
-        <v>227</v>
+        <v>241</v>
       </c>
       <c r="F52" s="1">
-        <v>45572</v>
+        <v>45614</v>
       </c>
       <c r="G52">
-        <v>216</v>
+        <v>234</v>
       </c>
     </row>
     <row r="53" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C53" s="1">
-        <v>45565</v>
+        <v>45607</v>
       </c>
       <c r="D53">
-        <v>223</v>
+        <v>239</v>
       </c>
       <c r="F53" s="1">
-        <v>45565</v>
+        <v>45607</v>
       </c>
       <c r="G53">
-        <v>216</v>
+        <v>230</v>
       </c>
     </row>
     <row r="54" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C54" s="1">
-        <v>45537</v>
+        <v>45600</v>
       </c>
       <c r="D54">
-        <v>218</v>
+        <v>232</v>
       </c>
       <c r="F54" s="1">
-        <v>45537</v>
+        <v>45600</v>
       </c>
       <c r="G54">
-        <v>207</v>
+        <v>227</v>
       </c>
     </row>
     <row r="55" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C55" s="1">
-        <v>45530</v>
+        <v>45579</v>
       </c>
       <c r="D55">
-        <v>217</v>
+        <v>231</v>
       </c>
       <c r="F55" s="1">
-        <v>45530</v>
+        <v>45579</v>
       </c>
       <c r="G55">
-        <v>207</v>
+        <v>222</v>
       </c>
     </row>
     <row r="56" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C56" s="1">
-        <v>45523</v>
+        <v>45572</v>
       </c>
       <c r="D56">
+        <v>227</v>
+      </c>
+      <c r="F56" s="1">
+        <v>45572</v>
+      </c>
+      <c r="G56">
         <v>216</v>
-      </c>
-      <c r="F56" s="1">
-        <v>45523</v>
-      </c>
-      <c r="G56">
-        <v>200</v>
       </c>
     </row>
     <row r="57" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C57" s="1">
-        <v>45516</v>
+        <v>45565</v>
       </c>
       <c r="D57">
-        <v>212</v>
+        <v>223</v>
       </c>
       <c r="F57" s="1">
-        <v>45516</v>
+        <v>45565</v>
       </c>
       <c r="G57">
-        <v>190</v>
+        <v>216</v>
       </c>
     </row>
     <row r="58" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C58" s="1">
-        <v>45509</v>
+        <v>45537</v>
       </c>
       <c r="D58">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="F58" s="1">
-        <v>45509</v>
+        <v>45537</v>
       </c>
       <c r="G58">
-        <v>189</v>
+        <v>207</v>
       </c>
     </row>
     <row r="59" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C59" s="1">
-        <v>45502</v>
+        <v>45530</v>
       </c>
       <c r="D59">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="F59" s="1">
-        <v>45502</v>
+        <v>45530</v>
       </c>
       <c r="G59">
-        <v>189</v>
+        <v>207</v>
       </c>
     </row>
     <row r="60" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C60" s="1">
-        <v>45495</v>
+        <v>45523</v>
       </c>
       <c r="D60">
-        <v>201</v>
+        <v>216</v>
       </c>
       <c r="F60" s="1">
-        <v>45495</v>
+        <v>45523</v>
       </c>
       <c r="G60">
-        <v>183</v>
+        <v>200</v>
       </c>
     </row>
     <row r="61" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C61" s="1">
-        <v>45488</v>
+        <v>45516</v>
       </c>
       <c r="D61">
-        <v>199</v>
+        <v>212</v>
       </c>
       <c r="F61" s="1">
-        <v>45488</v>
+        <v>45516</v>
       </c>
       <c r="G61">
-        <v>182</v>
+        <v>190</v>
       </c>
     </row>
     <row r="62" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C62" s="1">
-        <v>45481</v>
+        <v>45509</v>
       </c>
       <c r="D62">
-        <v>188</v>
+        <v>210</v>
       </c>
       <c r="F62" s="1">
-        <v>45481</v>
+        <v>45509</v>
       </c>
       <c r="G62">
-        <v>180</v>
+        <v>189</v>
       </c>
     </row>
     <row r="63" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C63" s="1">
-        <v>45474</v>
+        <v>45502</v>
       </c>
       <c r="D63">
-        <v>187</v>
+        <v>210</v>
       </c>
       <c r="F63" s="1">
-        <v>45474</v>
+        <v>45502</v>
       </c>
       <c r="G63">
-        <v>172</v>
+        <v>189</v>
       </c>
     </row>
     <row r="64" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C64" s="1">
-        <v>45467</v>
+        <v>45495</v>
       </c>
       <c r="D64">
-        <v>187</v>
+        <v>201</v>
       </c>
       <c r="F64" s="1">
-        <v>45467</v>
+        <v>45495</v>
       </c>
       <c r="G64">
-        <v>172</v>
+        <v>183</v>
       </c>
     </row>
     <row r="65" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C65" s="1">
-        <v>45460</v>
+        <v>45488</v>
       </c>
       <c r="D65">
-        <v>185</v>
+        <v>199</v>
       </c>
       <c r="F65" s="1">
-        <v>45460</v>
+        <v>45488</v>
       </c>
       <c r="G65">
-        <v>165</v>
+        <v>182</v>
       </c>
     </row>
     <row r="66" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C66" s="1">
-        <v>45453</v>
+        <v>45481</v>
       </c>
       <c r="D66">
+        <v>188</v>
+      </c>
+      <c r="F66" s="1">
+        <v>45481</v>
+      </c>
+      <c r="G66">
         <v>180</v>
-      </c>
-      <c r="F66" s="1">
-        <v>45453</v>
-      </c>
-      <c r="G66">
-        <v>164</v>
       </c>
     </row>
     <row r="67" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C67" s="1">
-        <v>45446</v>
+        <v>45474</v>
       </c>
       <c r="D67">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="F67" s="1">
-        <v>45446</v>
+        <v>45474</v>
       </c>
       <c r="G67">
-        <v>161</v>
+        <v>172</v>
       </c>
     </row>
     <row r="68" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C68" s="1">
-        <v>45439</v>
+        <v>45467</v>
       </c>
       <c r="D68">
-        <v>174</v>
+        <v>187</v>
       </c>
       <c r="F68" s="1">
-        <v>45439</v>
+        <v>45467</v>
       </c>
       <c r="G68">
-        <v>161</v>
+        <v>172</v>
       </c>
     </row>
     <row r="69" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C69" s="1">
-        <v>45432</v>
+        <v>45460</v>
       </c>
       <c r="D69">
-        <v>173</v>
+        <v>185</v>
       </c>
       <c r="F69" s="1">
-        <v>45432</v>
+        <v>45460</v>
       </c>
       <c r="G69">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row r="70" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C70" s="1">
-        <v>45425</v>
+        <v>45453</v>
       </c>
       <c r="D70">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="F70" s="1">
-        <v>45425</v>
+        <v>45453</v>
       </c>
       <c r="G70">
-        <v>157</v>
+        <v>164</v>
       </c>
     </row>
     <row r="71" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C71" s="1">
-        <v>45418</v>
+        <v>45446</v>
       </c>
       <c r="D71">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="F71" s="1">
-        <v>45418</v>
+        <v>45446</v>
       </c>
       <c r="G71">
-        <v>141</v>
+        <v>161</v>
       </c>
     </row>
     <row r="72" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C72" s="1">
-        <v>45411</v>
+        <v>45439</v>
       </c>
       <c r="D72">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="F72" s="1">
-        <v>45411</v>
+        <v>45439</v>
       </c>
       <c r="G72">
-        <v>141</v>
+        <v>161</v>
       </c>
     </row>
     <row r="73" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C73" s="1">
-        <v>45404</v>
+        <v>45432</v>
       </c>
       <c r="D73">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="F73" s="1">
-        <v>45404</v>
+        <v>45432</v>
       </c>
       <c r="G73">
-        <v>141</v>
+        <v>159</v>
       </c>
     </row>
     <row r="74" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C74" s="1">
-        <v>45397</v>
+        <v>45425</v>
       </c>
       <c r="D74">
+        <v>170</v>
+      </c>
+      <c r="F74" s="1">
+        <v>45425</v>
+      </c>
+      <c r="G74">
         <v>157</v>
-      </c>
-      <c r="F74" s="1">
-        <v>45397</v>
-      </c>
-      <c r="G74">
-        <v>132</v>
       </c>
     </row>
     <row r="75" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C75" s="1">
-        <v>45390</v>
+        <v>45418</v>
       </c>
       <c r="D75">
-        <v>146</v>
+        <v>170</v>
       </c>
       <c r="F75" s="1">
-        <v>45390</v>
+        <v>45418</v>
       </c>
       <c r="G75">
-        <v>132</v>
+        <v>141</v>
       </c>
     </row>
     <row r="76" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C76" s="1">
-        <v>45383</v>
+        <v>45411</v>
       </c>
       <c r="D76">
-        <v>138</v>
+        <v>166</v>
       </c>
       <c r="F76" s="1">
-        <v>45383</v>
+        <v>45411</v>
       </c>
       <c r="G76">
-        <v>119</v>
+        <v>141</v>
       </c>
     </row>
     <row r="77" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C77" s="1">
-        <v>45376</v>
+        <v>45404</v>
       </c>
       <c r="D77">
-        <v>129</v>
+        <v>166</v>
       </c>
       <c r="F77" s="1">
-        <v>45376</v>
+        <v>45404</v>
       </c>
       <c r="G77">
-        <v>114</v>
+        <v>141</v>
       </c>
     </row>
     <row r="78" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C78" s="1">
-        <v>45369</v>
+        <v>45397</v>
       </c>
       <c r="D78">
-        <v>123</v>
+        <v>157</v>
       </c>
       <c r="F78" s="1">
-        <v>45369</v>
+        <v>45397</v>
       </c>
       <c r="G78">
-        <v>97</v>
+        <v>132</v>
       </c>
     </row>
     <row r="79" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C79" s="1">
-        <v>45362</v>
+        <v>45390</v>
       </c>
       <c r="D79">
-        <v>113</v>
-      </c>
-      <c r="F79" s="1"/>
+        <v>146</v>
+      </c>
+      <c r="F79" s="1">
+        <v>45390</v>
+      </c>
+      <c r="G79">
+        <v>132</v>
+      </c>
     </row>
     <row r="80" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C80" s="1">
-        <v>45355</v>
+        <v>45383</v>
       </c>
       <c r="D80">
-        <v>108</v>
+        <v>138</v>
+      </c>
+      <c r="F80" s="1">
+        <v>45383</v>
+      </c>
+      <c r="G80">
+        <v>119</v>
       </c>
     </row>
     <row r="81" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C81" s="1">
-        <v>45348</v>
+        <v>45376</v>
       </c>
       <c r="D81">
-        <v>102</v>
+        <v>129</v>
+      </c>
+      <c r="F81" s="1">
+        <v>45376</v>
+      </c>
+      <c r="G81">
+        <v>114</v>
       </c>
     </row>
     <row r="82" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C82" s="1">
-        <v>45341</v>
+        <v>45369</v>
       </c>
       <c r="D82">
-        <v>95</v>
+        <v>123</v>
+      </c>
+      <c r="F82" s="1">
+        <v>45369</v>
+      </c>
+      <c r="G82">
+        <v>97</v>
       </c>
     </row>
     <row r="83" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C83" s="1">
-        <v>45334</v>
+        <v>45362</v>
       </c>
       <c r="D83">
-        <v>80</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="F83" s="1"/>
     </row>
     <row r="84" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C84" s="1">
-        <v>45327</v>
+        <v>45355</v>
       </c>
       <c r="D84">
-        <v>66</v>
+        <v>108</v>
       </c>
     </row>
     <row r="85" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C85" s="1">
-        <v>45320</v>
+        <v>45348</v>
       </c>
       <c r="D85">
-        <v>55</v>
+        <v>102</v>
       </c>
     </row>
     <row r="86" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C86" s="1">
-        <v>45313</v>
+        <v>45341</v>
       </c>
       <c r="D86">
-        <v>53</v>
+        <v>95</v>
       </c>
     </row>
     <row r="87" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C87" s="1">
+        <v>45334</v>
+      </c>
+      <c r="D87">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="88" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C88" s="1">
+        <v>45327</v>
+      </c>
+      <c r="D88">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="89" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C89" s="1">
+        <v>45320</v>
+      </c>
+      <c r="D89">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="90" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C90" s="1">
+        <v>45313</v>
+      </c>
+      <c r="D90">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="91" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C91" s="1">
         <v>45306</v>
       </c>
-      <c r="D87">
+      <c r="D91">
         <v>52</v>
       </c>
-    </row>
-    <row r="91" spans="3:17" x14ac:dyDescent="0.35">
-      <c r="D91" s="2"/>
-      <c r="E91" s="2"/>
-      <c r="F91" s="2"/>
-      <c r="G91" s="2"/>
-      <c r="H91" s="2"/>
-      <c r="I91" s="2"/>
-      <c r="J91" s="2"/>
-      <c r="K91" s="2"/>
-      <c r="L91" s="2"/>
-      <c r="M91" s="2"/>
-      <c r="N91" s="2"/>
-      <c r="O91" s="2"/>
-      <c r="P91" s="2"/>
-      <c r="Q91" s="2"/>
-    </row>
-    <row r="92" spans="3:17" x14ac:dyDescent="0.35">
-      <c r="D92" s="2"/>
-      <c r="E92" s="2"/>
-      <c r="F92" s="2"/>
-      <c r="G92" s="2"/>
-      <c r="H92" s="2"/>
-      <c r="I92" s="2"/>
-      <c r="J92" s="2"/>
-      <c r="K92" s="2"/>
-      <c r="L92" s="2"/>
-      <c r="M92" s="2"/>
-      <c r="N92" s="2"/>
-      <c r="O92" s="2"/>
-      <c r="P92" s="2"/>
-      <c r="Q92" s="2"/>
-    </row>
-    <row r="93" spans="3:17" x14ac:dyDescent="0.35">
-      <c r="D93" s="2"/>
-      <c r="E93" s="2"/>
-      <c r="F93" s="2"/>
-      <c r="G93" s="2"/>
-      <c r="H93" s="2"/>
-      <c r="I93" s="2"/>
-      <c r="J93" s="2"/>
-      <c r="K93" s="2"/>
-      <c r="L93" s="2"/>
-      <c r="M93" s="2"/>
-      <c r="N93" s="2"/>
-      <c r="O93" s="2"/>
-      <c r="P93" s="2"/>
-      <c r="Q93" s="2"/>
-    </row>
-    <row r="94" spans="3:17" x14ac:dyDescent="0.35">
-      <c r="D94" s="2"/>
-      <c r="E94" s="2"/>
-      <c r="F94" s="2"/>
-      <c r="G94" s="2"/>
-      <c r="H94" s="2"/>
-      <c r="I94" s="2"/>
-      <c r="J94" s="2"/>
-      <c r="K94" s="2"/>
-      <c r="L94" s="2"/>
-      <c r="M94" s="2"/>
-      <c r="N94" s="2"/>
-      <c r="O94" s="2"/>
-      <c r="P94" s="2"/>
-      <c r="Q94" s="2"/>
     </row>
     <row r="95" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D95" s="2"/>
@@ -6212,9 +6162,73 @@
       <c r="P116" s="2"/>
       <c r="Q116" s="2"/>
     </row>
+    <row r="117" spans="4:17" x14ac:dyDescent="0.35">
+      <c r="D117" s="2"/>
+      <c r="E117" s="2"/>
+      <c r="F117" s="2"/>
+      <c r="G117" s="2"/>
+      <c r="H117" s="2"/>
+      <c r="I117" s="2"/>
+      <c r="J117" s="2"/>
+      <c r="K117" s="2"/>
+      <c r="L117" s="2"/>
+      <c r="M117" s="2"/>
+      <c r="N117" s="2"/>
+      <c r="O117" s="2"/>
+      <c r="P117" s="2"/>
+      <c r="Q117" s="2"/>
+    </row>
+    <row r="118" spans="4:17" x14ac:dyDescent="0.35">
+      <c r="D118" s="2"/>
+      <c r="E118" s="2"/>
+      <c r="F118" s="2"/>
+      <c r="G118" s="2"/>
+      <c r="H118" s="2"/>
+      <c r="I118" s="2"/>
+      <c r="J118" s="2"/>
+      <c r="K118" s="2"/>
+      <c r="L118" s="2"/>
+      <c r="M118" s="2"/>
+      <c r="N118" s="2"/>
+      <c r="O118" s="2"/>
+      <c r="P118" s="2"/>
+      <c r="Q118" s="2"/>
+    </row>
+    <row r="119" spans="4:17" x14ac:dyDescent="0.35">
+      <c r="D119" s="2"/>
+      <c r="E119" s="2"/>
+      <c r="F119" s="2"/>
+      <c r="G119" s="2"/>
+      <c r="H119" s="2"/>
+      <c r="I119" s="2"/>
+      <c r="J119" s="2"/>
+      <c r="K119" s="2"/>
+      <c r="L119" s="2"/>
+      <c r="M119" s="2"/>
+      <c r="N119" s="2"/>
+      <c r="O119" s="2"/>
+      <c r="P119" s="2"/>
+      <c r="Q119" s="2"/>
+    </row>
+    <row r="120" spans="4:17" x14ac:dyDescent="0.35">
+      <c r="D120" s="2"/>
+      <c r="E120" s="2"/>
+      <c r="F120" s="2"/>
+      <c r="G120" s="2"/>
+      <c r="H120" s="2"/>
+      <c r="I120" s="2"/>
+      <c r="J120" s="2"/>
+      <c r="K120" s="2"/>
+      <c r="L120" s="2"/>
+      <c r="M120" s="2"/>
+      <c r="N120" s="2"/>
+      <c r="O120" s="2"/>
+      <c r="P120" s="2"/>
+      <c r="Q120" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D91:Q116"/>
+    <mergeCell ref="D95:Q120"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
LGHUB 2025/7/19 更新 2
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
- 网站错误 & 本地化问题详见 LGHUB/WebLoc/README.md
</commit_message>
<xml_diff>
--- a/Documents/Graph_PC.xlsx
+++ b/Documents/Graph_PC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C51C6B7-8274-4C65-B034-34C344B5C21E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB252C37-EEAA-416F-ABD5-8594DD5726CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,13 +574,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>21</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>49</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -917,72 +917,72 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$20:$C$28</c:f>
+              <c:f>Sheet1!$C$19:$C$27</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45859</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45852</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45845</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45838</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45831</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45824</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45817</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45810</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45803</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45796</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$20:$D$28</c:f>
+              <c:f>Sheet1!$D$19:$D$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>430</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>419</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>418</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>416</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>416</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>416</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>407</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>404</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>395</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>386</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>379</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1086,72 +1086,72 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$20:$C$28</c:f>
+              <c:f>Sheet1!$C$19:$C$27</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45859</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45852</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45845</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45838</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45831</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45824</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45817</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45810</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45803</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45796</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$20:$G$28</c:f>
+              <c:f>Sheet1!$G$19:$G$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>386</c:v>
+                  <c:v>389</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>386</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>370</c:v>
+                  <c:v>386</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>370</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>369</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>359</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>360</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>354</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>349</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1286,8 +1286,8 @@
         <c:axId val="1374569007"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="430"/>
-          <c:min val="340"/>
+          <c:max val="440"/>
+          <c:min val="350"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1794,13 +1794,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>21</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>49</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4811,8 +4811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D92" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L94" sqref="L94"/>
+    <sheetView tabSelected="1" topLeftCell="D94" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M94" sqref="M94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -4836,7 +4836,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.35">
@@ -4844,7 +4844,7 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.35">
@@ -4852,7 +4852,21 @@
         <v>4</v>
       </c>
       <c r="C7">
-        <v>49</v>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C19" s="1">
+        <v>45859</v>
+      </c>
+      <c r="D19">
+        <v>430</v>
+      </c>
+      <c r="F19" s="1">
+        <v>45859</v>
+      </c>
+      <c r="G19">
+        <v>389</v>
       </c>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
LGHUB 2025/7/26 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
- 网站错误 & 本地化问题详见 LGHUB/WebLoc/README.md
</commit_message>
<xml_diff>
--- a/Documents/Graph_PC.xlsx
+++ b/Documents/Graph_PC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29119"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB252C37-EEAA-416F-ABD5-8594DD5726CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0BDC6DA-6736-419A-9ADF-6CE8773A638F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="2" r:id="rId1"/>
@@ -293,6 +293,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -300,7 +301,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -574,13 +574,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>27</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>52</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -917,72 +917,72 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$19:$C$27</c:f>
+              <c:f>Sheet1!$C$18:$C$26</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45866</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45859</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45852</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45845</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45838</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45831</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45824</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45817</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45810</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45803</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$19:$D$27</c:f>
+              <c:f>Sheet1!$D$18:$D$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>431</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>430</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>419</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>418</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>416</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>416</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>416</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>407</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>404</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>395</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>386</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1086,72 +1086,72 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$19:$C$27</c:f>
+              <c:f>Sheet1!$C$18:$C$26</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45866</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45859</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45852</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45845</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45838</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45831</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45824</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45817</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45810</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45803</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$19:$G$27</c:f>
+              <c:f>Sheet1!$G$18:$G$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>389</c:v>
+                  <c:v>399</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>386</c:v>
+                  <c:v>389</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>386</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>370</c:v>
+                  <c:v>386</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>370</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>369</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>359</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>360</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>354</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1286,7 +1286,7 @@
         <c:axId val="1374569007"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="440"/>
+          <c:max val="450"/>
           <c:min val="350"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1794,13 +1794,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>27</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>52</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1884,6 +1884,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1891,7 +1892,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -4811,51 +4811,65 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D94" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M94" sqref="M94"/>
+    <sheetView tabSelected="1" topLeftCell="C94" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="J94" sqref="J94"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C18" s="1">
+        <v>45866</v>
+      </c>
+      <c r="D18">
+        <v>431</v>
+      </c>
+      <c r="F18" s="1">
+        <v>45866</v>
+      </c>
+      <c r="G18">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C19" s="1">
         <v>45859</v>
       </c>
@@ -4869,7 +4883,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C20" s="1">
         <v>45852</v>
       </c>
@@ -4883,7 +4897,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C21" s="1">
         <v>45845</v>
       </c>
@@ -4897,7 +4911,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C22" s="1">
         <v>45838</v>
       </c>
@@ -4911,7 +4925,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C23" s="1">
         <v>45831</v>
       </c>
@@ -4925,7 +4939,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C24" s="1">
         <v>45824</v>
       </c>
@@ -4939,7 +4953,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C25" s="1">
         <v>45817</v>
       </c>
@@ -4953,7 +4967,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C26" s="1">
         <v>45810</v>
       </c>
@@ -4967,7 +4981,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C27" s="1">
         <v>45803</v>
       </c>
@@ -4981,7 +4995,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C28" s="1">
         <v>45796</v>
       </c>
@@ -4995,7 +5009,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C29" s="1">
         <v>45789</v>
       </c>
@@ -5009,7 +5023,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C30" s="1">
         <v>45782</v>
       </c>
@@ -5023,7 +5037,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C31" s="1">
         <v>45775</v>
       </c>
@@ -5037,7 +5051,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C32" s="1">
         <v>45768</v>
       </c>
@@ -5051,7 +5065,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C33" s="1">
         <v>45761</v>
       </c>
@@ -5065,7 +5079,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="34" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C34" s="1">
         <v>45754</v>
       </c>
@@ -5079,7 +5093,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="35" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C35" s="1">
         <v>45747</v>
       </c>
@@ -5093,7 +5107,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="36" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C36" s="1">
         <v>45740</v>
       </c>
@@ -5107,7 +5121,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="37" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C37" s="1">
         <v>45733</v>
       </c>
@@ -5121,7 +5135,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="38" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C38" s="1">
         <v>45726</v>
       </c>
@@ -5135,7 +5149,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="39" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C39" s="1">
         <v>45719</v>
       </c>
@@ -5149,7 +5163,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="40" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C40" s="1">
         <v>45712</v>
       </c>
@@ -5163,7 +5177,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="41" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C41" s="1">
         <v>45705</v>
       </c>
@@ -5177,7 +5191,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="42" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C42" s="1">
         <v>45698</v>
       </c>
@@ -5191,7 +5205,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="43" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C43" s="1">
         <v>45691</v>
       </c>
@@ -5205,7 +5219,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="44" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C44" s="1">
         <v>45684</v>
       </c>
@@ -5219,7 +5233,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="45" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C45" s="1">
         <v>45677</v>
       </c>
@@ -5233,7 +5247,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="46" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C46" s="1">
         <v>45670</v>
       </c>
@@ -5247,7 +5261,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="47" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C47" s="1">
         <v>45663</v>
       </c>
@@ -5261,7 +5275,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="48" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C48" s="1">
         <v>45642</v>
       </c>
@@ -5275,7 +5289,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="49" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="49" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C49" s="1">
         <v>45635</v>
       </c>
@@ -5289,7 +5303,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="50" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="50" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C50" s="1">
         <v>45628</v>
       </c>
@@ -5303,7 +5317,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="51" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="51" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C51" s="1">
         <v>45621</v>
       </c>
@@ -5317,7 +5331,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="52" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="52" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C52" s="1">
         <v>45614</v>
       </c>
@@ -5331,7 +5345,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="53" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="53" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C53" s="1">
         <v>45607</v>
       </c>
@@ -5345,7 +5359,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="54" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="54" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C54" s="1">
         <v>45600</v>
       </c>
@@ -5359,7 +5373,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="55" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="55" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C55" s="1">
         <v>45579</v>
       </c>
@@ -5373,7 +5387,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="56" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="56" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C56" s="1">
         <v>45572</v>
       </c>
@@ -5387,7 +5401,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="57" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="57" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C57" s="1">
         <v>45565</v>
       </c>
@@ -5401,7 +5415,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="58" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="58" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C58" s="1">
         <v>45537</v>
       </c>
@@ -5415,7 +5429,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="59" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="59" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C59" s="1">
         <v>45530</v>
       </c>
@@ -5429,7 +5443,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="60" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="60" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C60" s="1">
         <v>45523</v>
       </c>
@@ -5443,7 +5457,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="61" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="61" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C61" s="1">
         <v>45516</v>
       </c>
@@ -5457,7 +5471,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="62" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="62" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C62" s="1">
         <v>45509</v>
       </c>
@@ -5471,7 +5485,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="63" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="63" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C63" s="1">
         <v>45502</v>
       </c>
@@ -5485,7 +5499,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="64" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="64" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C64" s="1">
         <v>45495</v>
       </c>
@@ -5499,7 +5513,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="65" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="65" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C65" s="1">
         <v>45488</v>
       </c>
@@ -5513,7 +5527,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="66" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="66" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C66" s="1">
         <v>45481</v>
       </c>
@@ -5527,7 +5541,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="67" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="67" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C67" s="1">
         <v>45474</v>
       </c>
@@ -5541,7 +5555,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="68" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="68" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C68" s="1">
         <v>45467</v>
       </c>
@@ -5555,7 +5569,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="69" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="69" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C69" s="1">
         <v>45460</v>
       </c>
@@ -5569,7 +5583,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="70" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="70" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C70" s="1">
         <v>45453</v>
       </c>
@@ -5583,7 +5597,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="71" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="71" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C71" s="1">
         <v>45446</v>
       </c>
@@ -5597,7 +5611,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="72" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="72" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C72" s="1">
         <v>45439</v>
       </c>
@@ -5611,7 +5625,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="73" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="73" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C73" s="1">
         <v>45432</v>
       </c>
@@ -5625,7 +5639,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="74" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="74" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C74" s="1">
         <v>45425</v>
       </c>
@@ -5639,7 +5653,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="75" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="75" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C75" s="1">
         <v>45418</v>
       </c>
@@ -5653,7 +5667,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="76" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="76" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C76" s="1">
         <v>45411</v>
       </c>
@@ -5667,7 +5681,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="77" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="77" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C77" s="1">
         <v>45404</v>
       </c>
@@ -5681,7 +5695,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="78" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="78" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C78" s="1">
         <v>45397</v>
       </c>
@@ -5695,7 +5709,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="79" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="79" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C79" s="1">
         <v>45390</v>
       </c>
@@ -5709,7 +5723,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="80" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="80" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C80" s="1">
         <v>45383</v>
       </c>
@@ -5723,7 +5737,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="81" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="81" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C81" s="1">
         <v>45376</v>
       </c>
@@ -5737,7 +5751,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="82" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="82" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C82" s="1">
         <v>45369</v>
       </c>
@@ -5751,7 +5765,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="83" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="83" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C83" s="1">
         <v>45362</v>
       </c>
@@ -5760,7 +5774,7 @@
       </c>
       <c r="F83" s="1"/>
     </row>
-    <row r="84" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="84" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C84" s="1">
         <v>45355</v>
       </c>
@@ -5768,7 +5782,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="85" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="85" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C85" s="1">
         <v>45348</v>
       </c>
@@ -5776,7 +5790,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="86" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="86" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C86" s="1">
         <v>45341</v>
       </c>
@@ -5784,7 +5798,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="87" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="87" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C87" s="1">
         <v>45334</v>
       </c>
@@ -5792,7 +5806,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="88" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="88" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C88" s="1">
         <v>45327</v>
       </c>
@@ -5800,7 +5814,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="89" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="89" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C89" s="1">
         <v>45320</v>
       </c>
@@ -5808,7 +5822,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="90" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="90" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C90" s="1">
         <v>45313</v>
       </c>
@@ -5816,7 +5830,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="91" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="91" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C91" s="1">
         <v>45306</v>
       </c>
@@ -5824,7 +5838,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="95" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="95" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D95" s="2"/>
       <c r="E95" s="2"/>
       <c r="F95" s="2"/>
@@ -5840,7 +5854,7 @@
       <c r="P95" s="2"/>
       <c r="Q95" s="2"/>
     </row>
-    <row r="96" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="96" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D96" s="2"/>
       <c r="E96" s="2"/>
       <c r="F96" s="2"/>
@@ -5856,7 +5870,7 @@
       <c r="P96" s="2"/>
       <c r="Q96" s="2"/>
     </row>
-    <row r="97" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="97" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D97" s="2"/>
       <c r="E97" s="2"/>
       <c r="F97" s="2"/>
@@ -5872,7 +5886,7 @@
       <c r="P97" s="2"/>
       <c r="Q97" s="2"/>
     </row>
-    <row r="98" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="98" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D98" s="2"/>
       <c r="E98" s="2"/>
       <c r="F98" s="2"/>
@@ -5888,7 +5902,7 @@
       <c r="P98" s="2"/>
       <c r="Q98" s="2"/>
     </row>
-    <row r="99" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="99" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D99" s="2"/>
       <c r="E99" s="2"/>
       <c r="F99" s="2"/>
@@ -5904,7 +5918,7 @@
       <c r="P99" s="2"/>
       <c r="Q99" s="2"/>
     </row>
-    <row r="100" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="100" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D100" s="2"/>
       <c r="E100" s="2"/>
       <c r="F100" s="2"/>
@@ -5920,7 +5934,7 @@
       <c r="P100" s="2"/>
       <c r="Q100" s="2"/>
     </row>
-    <row r="101" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="101" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D101" s="2"/>
       <c r="E101" s="2"/>
       <c r="F101" s="2"/>
@@ -5936,7 +5950,7 @@
       <c r="P101" s="2"/>
       <c r="Q101" s="2"/>
     </row>
-    <row r="102" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="102" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D102" s="2"/>
       <c r="E102" s="2"/>
       <c r="F102" s="2"/>
@@ -5952,7 +5966,7 @@
       <c r="P102" s="2"/>
       <c r="Q102" s="2"/>
     </row>
-    <row r="103" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="103" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D103" s="2"/>
       <c r="E103" s="2"/>
       <c r="F103" s="2"/>
@@ -5968,7 +5982,7 @@
       <c r="P103" s="2"/>
       <c r="Q103" s="2"/>
     </row>
-    <row r="104" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="104" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D104" s="2"/>
       <c r="E104" s="2"/>
       <c r="F104" s="2"/>
@@ -5984,7 +5998,7 @@
       <c r="P104" s="2"/>
       <c r="Q104" s="2"/>
     </row>
-    <row r="105" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="105" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D105" s="2"/>
       <c r="E105" s="2"/>
       <c r="F105" s="2"/>
@@ -6000,7 +6014,7 @@
       <c r="P105" s="2"/>
       <c r="Q105" s="2"/>
     </row>
-    <row r="106" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="106" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D106" s="2"/>
       <c r="E106" s="2"/>
       <c r="F106" s="2"/>
@@ -6016,7 +6030,7 @@
       <c r="P106" s="2"/>
       <c r="Q106" s="2"/>
     </row>
-    <row r="107" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="107" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D107" s="2"/>
       <c r="E107" s="2"/>
       <c r="F107" s="2"/>
@@ -6032,7 +6046,7 @@
       <c r="P107" s="2"/>
       <c r="Q107" s="2"/>
     </row>
-    <row r="108" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="108" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D108" s="2"/>
       <c r="E108" s="2"/>
       <c r="F108" s="2"/>
@@ -6048,7 +6062,7 @@
       <c r="P108" s="2"/>
       <c r="Q108" s="2"/>
     </row>
-    <row r="109" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="109" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D109" s="2"/>
       <c r="E109" s="2"/>
       <c r="F109" s="2"/>
@@ -6064,7 +6078,7 @@
       <c r="P109" s="2"/>
       <c r="Q109" s="2"/>
     </row>
-    <row r="110" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="110" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D110" s="2"/>
       <c r="E110" s="2"/>
       <c r="F110" s="2"/>
@@ -6080,7 +6094,7 @@
       <c r="P110" s="2"/>
       <c r="Q110" s="2"/>
     </row>
-    <row r="111" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="111" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D111" s="2"/>
       <c r="E111" s="2"/>
       <c r="F111" s="2"/>
@@ -6096,7 +6110,7 @@
       <c r="P111" s="2"/>
       <c r="Q111" s="2"/>
     </row>
-    <row r="112" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="112" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D112" s="2"/>
       <c r="E112" s="2"/>
       <c r="F112" s="2"/>
@@ -6112,7 +6126,7 @@
       <c r="P112" s="2"/>
       <c r="Q112" s="2"/>
     </row>
-    <row r="113" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="113" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D113" s="2"/>
       <c r="E113" s="2"/>
       <c r="F113" s="2"/>
@@ -6128,7 +6142,7 @@
       <c r="P113" s="2"/>
       <c r="Q113" s="2"/>
     </row>
-    <row r="114" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="114" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D114" s="2"/>
       <c r="E114" s="2"/>
       <c r="F114" s="2"/>
@@ -6144,7 +6158,7 @@
       <c r="P114" s="2"/>
       <c r="Q114" s="2"/>
     </row>
-    <row r="115" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="115" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D115" s="2"/>
       <c r="E115" s="2"/>
       <c r="F115" s="2"/>
@@ -6160,7 +6174,7 @@
       <c r="P115" s="2"/>
       <c r="Q115" s="2"/>
     </row>
-    <row r="116" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="116" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D116" s="2"/>
       <c r="E116" s="2"/>
       <c r="F116" s="2"/>
@@ -6176,7 +6190,7 @@
       <c r="P116" s="2"/>
       <c r="Q116" s="2"/>
     </row>
-    <row r="117" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="117" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D117" s="2"/>
       <c r="E117" s="2"/>
       <c r="F117" s="2"/>
@@ -6192,7 +6206,7 @@
       <c r="P117" s="2"/>
       <c r="Q117" s="2"/>
     </row>
-    <row r="118" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="118" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D118" s="2"/>
       <c r="E118" s="2"/>
       <c r="F118" s="2"/>
@@ -6208,7 +6222,7 @@
       <c r="P118" s="2"/>
       <c r="Q118" s="2"/>
     </row>
-    <row r="119" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="119" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D119" s="2"/>
       <c r="E119" s="2"/>
       <c r="F119" s="2"/>
@@ -6224,7 +6238,7 @@
       <c r="P119" s="2"/>
       <c r="Q119" s="2"/>
     </row>
-    <row r="120" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="120" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D120" s="2"/>
       <c r="E120" s="2"/>
       <c r="F120" s="2"/>

</xml_diff>

<commit_message>
LGHUB 2025/7/31 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
- 网站错误 & 本地化问题详见 LGHUB/WebLoc/README.md
</commit_message>
<xml_diff>
--- a/Documents/Graph_PC.xlsx
+++ b/Documents/Graph_PC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0BDC6DA-6736-419A-9ADF-6CE8773A638F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A47FE92-03B8-47B5-BB75-38A879C4DFBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,13 +574,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>19</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>62</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -958,7 +958,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>431</c:v>
+                  <c:v>432</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>430</c:v>
@@ -1127,7 +1127,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>399</c:v>
+                  <c:v>406</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>389</c:v>
@@ -1794,13 +1794,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>19</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>62</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4811,8 +4811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C94" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J94" sqref="J94"/>
+    <sheetView tabSelected="1" topLeftCell="C93" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="L94" sqref="L94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -4836,7 +4836,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
@@ -4844,7 +4844,7 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
@@ -4852,7 +4852,7 @@
         <v>4</v>
       </c>
       <c r="C7">
-        <v>62</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.25">
@@ -4860,13 +4860,13 @@
         <v>45866</v>
       </c>
       <c r="D18">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="F18" s="1">
         <v>45866</v>
       </c>
       <c r="G18">
-        <v>399</v>
+        <v>406</v>
       </c>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
LGHUB 2025/8/5 更新 2
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
- 网站错误 & 本地化问题详见 LGHUB/WebLoc/README.md
</commit_message>
<xml_diff>
--- a/Documents/Graph_PC.xlsx
+++ b/Documents/Graph_PC.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A47FE92-03B8-47B5-BB75-38A879C4DFBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE9B856-DB52-4FC4-96B1-459E44EE57F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,13 +574,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>16</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>69</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -917,72 +917,72 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$18:$C$26</c:f>
+              <c:f>Sheet1!$C$17:$C$25</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45873</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45866</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45859</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45852</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45845</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45838</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45831</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45824</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45817</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45810</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$18:$D$26</c:f>
+              <c:f>Sheet1!$D$17:$D$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>432</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>430</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>419</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>418</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>416</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>416</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>416</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>407</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>404</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>395</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1086,72 +1086,72 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$18:$C$26</c:f>
+              <c:f>Sheet1!$C$17:$C$25</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45873</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45866</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45859</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45852</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45845</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45838</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45831</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45824</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45817</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45810</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$18:$G$26</c:f>
+              <c:f>Sheet1!$G$17:$G$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>405</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>406</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>389</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>386</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>386</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>370</c:v>
+                  <c:v>386</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>370</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>369</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>359</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>360</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1794,13 +1794,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>16</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>69</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4811,8 +4811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C93" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="L94" sqref="L94"/>
+    <sheetView tabSelected="1" topLeftCell="B95" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="K94" sqref="K94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -4836,7 +4836,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
@@ -4844,7 +4844,7 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
@@ -4852,7 +4852,21 @@
         <v>4</v>
       </c>
       <c r="C7">
-        <v>69</v>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C17" s="1">
+        <v>45873</v>
+      </c>
+      <c r="D17">
+        <v>440</v>
+      </c>
+      <c r="F17" s="1">
+        <v>45873</v>
+      </c>
+      <c r="G17">
+        <v>405</v>
       </c>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
LGHUB 2025/8/9 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
- 网站错误 & 本地化问题详见 LGHUB/WebLoc/README.md
</commit_message>
<xml_diff>
--- a/Documents/Graph_PC.xlsx
+++ b/Documents/Graph_PC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE9B856-DB52-4FC4-96B1-459E44EE57F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDBB65BB-C429-45E3-889C-C168B55A6F36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,13 +574,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>23</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>68</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -917,72 +917,72 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$17:$C$25</c:f>
+              <c:f>Sheet1!$C$16:$C$24</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45880</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45873</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45866</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45859</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45852</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45845</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45838</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45831</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45824</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45817</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$17:$D$25</c:f>
+              <c:f>Sheet1!$D$16:$D$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>443</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>440</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>432</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>430</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>419</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>418</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>416</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>416</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>407</c:v>
+                  <c:v>416</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>404</c:v>
+                  <c:v>407</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1086,72 +1086,72 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$17:$C$25</c:f>
+              <c:f>Sheet1!$C$16:$C$24</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45880</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45873</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45866</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45859</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45852</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45845</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45838</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45831</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45824</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45817</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$17:$G$25</c:f>
+              <c:f>Sheet1!$G$16:$G$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>406</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>405</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>406</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>389</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>386</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>386</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>370</c:v>
+                  <c:v>386</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>370</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>369</c:v>
+                  <c:v>370</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>359</c:v>
+                  <c:v>369</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1794,13 +1794,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>23</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>68</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4811,7 +4811,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B95" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B94" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="K94" sqref="K94"/>
     </sheetView>
   </sheetViews>
@@ -4821,38 +4821,52 @@
     <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7">
-        <v>68</v>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C16" s="1">
+        <v>45880</v>
+      </c>
+      <c r="D16">
+        <v>443</v>
+      </c>
+      <c r="F16" s="1">
+        <v>45880</v>
+      </c>
+      <c r="G16">
+        <v>406</v>
       </c>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
LGHUB 2025/8/16 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
- 网站错误 & 本地化问题详见 LGHUB/WebLoc/README.md
</commit_message>
<xml_diff>
--- a/Documents/Graph_PC.xlsx
+++ b/Documents/Graph_PC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDBB65BB-C429-45E3-889C-C168B55A6F36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8CE8366-2973-4A64-A3CD-20F6E8C4B9C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="2" r:id="rId1"/>
@@ -574,13 +574,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>22</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>69</c:v>
+                  <c:v>78</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -917,72 +917,72 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$16:$C$24</c:f>
+              <c:f>Sheet1!$C$20:$C$28</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45887</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45880</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45873</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45866</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45859</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45852</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45845</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45838</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45831</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45824</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$16:$D$24</c:f>
+              <c:f>Sheet1!$D$20:$D$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>446</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>443</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>440</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>432</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>430</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>419</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>418</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>416</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>416</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>407</c:v>
+                  <c:v>416</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1086,72 +1086,72 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$16:$C$24</c:f>
+              <c:f>Sheet1!$C$20:$C$28</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45887</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45880</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45873</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45866</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45859</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45852</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45845</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45838</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45831</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45824</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$16:$G$24</c:f>
+              <c:f>Sheet1!$G$20:$G$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>415</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>406</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>405</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>406</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>389</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>386</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>386</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>370</c:v>
+                  <c:v>386</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>370</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>369</c:v>
+                  <c:v>370</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1794,13 +1794,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>22</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>69</c:v>
+                  <c:v>78</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4223,13 +4223,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>106422</xdr:colOff>
-      <xdr:row>95</xdr:row>
+      <xdr:row>100</xdr:row>
       <xdr:rowOff>165023</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>110</xdr:row>
+      <xdr:row>115</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4259,13 +4259,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>190501</xdr:colOff>
-      <xdr:row>95</xdr:row>
+      <xdr:row>100</xdr:row>
       <xdr:rowOff>162248</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>124495</xdr:colOff>
-      <xdr:row>110</xdr:row>
+      <xdr:row>115</xdr:row>
       <xdr:rowOff>163286</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4809,37 +4809,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:Q120"/>
+  <dimension ref="B2:Q125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B94" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="K94" sqref="K94"/>
+    <sheetView tabSelected="1" topLeftCell="D98" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L99" sqref="L99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -4847,1106 +4847,1040 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C16" s="1">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C20" s="1">
+        <v>45887</v>
+      </c>
+      <c r="D20">
+        <v>446</v>
+      </c>
+      <c r="F20" s="1">
+        <v>45887</v>
+      </c>
+      <c r="G20">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C21" s="1">
         <v>45880</v>
       </c>
-      <c r="D16">
+      <c r="D21">
         <v>443</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F21" s="1">
         <v>45880</v>
       </c>
-      <c r="G16">
+      <c r="G21">
         <v>406</v>
       </c>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C17" s="1">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C22" s="1">
         <v>45873</v>
       </c>
-      <c r="D17">
+      <c r="D22">
         <v>440</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F22" s="1">
         <v>45873</v>
       </c>
-      <c r="G17">
+      <c r="G22">
         <v>405</v>
       </c>
     </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C18" s="1">
+    <row r="23" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C23" s="1">
         <v>45866</v>
       </c>
-      <c r="D18">
+      <c r="D23">
         <v>432</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F23" s="1">
         <v>45866</v>
       </c>
-      <c r="G18">
+      <c r="G23">
         <v>406</v>
       </c>
     </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C19" s="1">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C24" s="1">
         <v>45859</v>
       </c>
-      <c r="D19">
+      <c r="D24">
         <v>430</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F24" s="1">
         <v>45859</v>
       </c>
-      <c r="G19">
+      <c r="G24">
         <v>389</v>
       </c>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C20" s="1">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C25" s="1">
         <v>45852</v>
       </c>
-      <c r="D20">
+      <c r="D25">
         <v>419</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F25" s="1">
         <v>45852</v>
       </c>
-      <c r="G20">
+      <c r="G25">
         <v>386</v>
       </c>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C21" s="1">
+    <row r="26" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C26" s="1">
         <v>45845</v>
       </c>
-      <c r="D21">
+      <c r="D26">
         <v>418</v>
       </c>
-      <c r="F21" s="1">
+      <c r="F26" s="1">
         <v>45845</v>
       </c>
-      <c r="G21">
+      <c r="G26">
         <v>386</v>
       </c>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C22" s="1">
+    <row r="27" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C27" s="1">
         <v>45838</v>
       </c>
-      <c r="D22">
+      <c r="D27">
         <v>416</v>
       </c>
-      <c r="F22" s="1">
+      <c r="F27" s="1">
         <v>45838</v>
       </c>
-      <c r="G22">
+      <c r="G27">
         <v>370</v>
       </c>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C23" s="1">
+    <row r="28" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C28" s="1">
         <v>45831</v>
       </c>
-      <c r="D23">
+      <c r="D28">
         <v>416</v>
       </c>
-      <c r="F23" s="1">
+      <c r="F28" s="1">
         <v>45831</v>
       </c>
-      <c r="G23">
+      <c r="G28">
         <v>370</v>
       </c>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C24" s="1">
+    <row r="29" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C29" s="1">
         <v>45824</v>
       </c>
-      <c r="D24">
+      <c r="D29">
         <v>407</v>
       </c>
-      <c r="F24" s="1">
+      <c r="F29" s="1">
         <v>45824</v>
       </c>
-      <c r="G24">
+      <c r="G29">
         <v>369</v>
       </c>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C25" s="1">
+    <row r="30" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C30" s="1">
         <v>45817</v>
       </c>
-      <c r="D25">
+      <c r="D30">
         <v>404</v>
       </c>
-      <c r="F25" s="1">
+      <c r="F30" s="1">
         <v>45817</v>
       </c>
-      <c r="G25">
+      <c r="G30">
         <v>359</v>
       </c>
     </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C26" s="1">
+    <row r="31" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C31" s="1">
         <v>45810</v>
       </c>
-      <c r="D26">
+      <c r="D31">
         <v>395</v>
       </c>
-      <c r="F26" s="1">
+      <c r="F31" s="1">
         <v>45810</v>
       </c>
-      <c r="G26">
+      <c r="G31">
         <v>360</v>
       </c>
     </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C27" s="1">
+    <row r="32" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C32" s="1">
         <v>45803</v>
       </c>
-      <c r="D27">
+      <c r="D32">
         <v>386</v>
       </c>
-      <c r="F27" s="1">
+      <c r="F32" s="1">
         <v>45803</v>
       </c>
-      <c r="G27">
+      <c r="G32">
         <v>354</v>
       </c>
     </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C28" s="1">
+    <row r="33" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C33" s="1">
         <v>45796</v>
       </c>
-      <c r="D28">
+      <c r="D33">
         <v>379</v>
       </c>
-      <c r="F28" s="1">
+      <c r="F33" s="1">
         <v>45796</v>
       </c>
-      <c r="G28">
+      <c r="G33">
         <v>349</v>
       </c>
     </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C29" s="1">
+    <row r="34" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C34" s="1">
         <v>45789</v>
       </c>
-      <c r="D29">
+      <c r="D34">
         <v>365</v>
       </c>
-      <c r="F29" s="1">
+      <c r="F34" s="1">
         <v>45789</v>
       </c>
-      <c r="G29">
+      <c r="G34">
         <v>320</v>
       </c>
     </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C30" s="1">
+    <row r="35" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C35" s="1">
         <v>45782</v>
       </c>
-      <c r="D30">
+      <c r="D35">
         <v>356</v>
       </c>
-      <c r="F30" s="1">
+      <c r="F35" s="1">
         <v>45782</v>
       </c>
-      <c r="G30">
+      <c r="G35">
         <v>320</v>
       </c>
     </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C31" s="1">
+    <row r="36" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C36" s="1">
         <v>45775</v>
       </c>
-      <c r="D31">
+      <c r="D36">
         <v>348</v>
       </c>
-      <c r="F31" s="1">
+      <c r="F36" s="1">
         <v>45775</v>
       </c>
-      <c r="G31">
+      <c r="G36">
         <v>320</v>
       </c>
     </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C32" s="1">
+    <row r="37" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C37" s="1">
         <v>45768</v>
       </c>
-      <c r="D32">
+      <c r="D37">
         <v>343</v>
       </c>
-      <c r="F32" s="1">
+      <c r="F37" s="1">
         <v>45768</v>
       </c>
-      <c r="G32">
+      <c r="G37">
         <v>319</v>
       </c>
     </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C33" s="1">
+    <row r="38" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C38" s="1">
         <v>45761</v>
       </c>
-      <c r="D33">
+      <c r="D38">
         <v>334</v>
       </c>
-      <c r="F33" s="1">
+      <c r="F38" s="1">
         <v>45761</v>
       </c>
-      <c r="G33">
+      <c r="G38">
         <v>303</v>
       </c>
     </row>
-    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C34" s="1">
+    <row r="39" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C39" s="1">
         <v>45754</v>
       </c>
-      <c r="D34">
+      <c r="D39">
         <v>330</v>
       </c>
-      <c r="F34" s="1">
+      <c r="F39" s="1">
         <v>45754</v>
       </c>
-      <c r="G34">
+      <c r="G39">
         <v>302</v>
       </c>
     </row>
-    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C35" s="1">
+    <row r="40" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C40" s="1">
         <v>45747</v>
       </c>
-      <c r="D35">
+      <c r="D40">
         <v>325</v>
       </c>
-      <c r="F35" s="1">
+      <c r="F40" s="1">
         <v>45747</v>
       </c>
-      <c r="G35">
+      <c r="G40">
         <v>302</v>
       </c>
     </row>
-    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C36" s="1">
+    <row r="41" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C41" s="1">
         <v>45740</v>
       </c>
-      <c r="D36">
+      <c r="D41">
         <v>316</v>
       </c>
-      <c r="F36" s="1">
+      <c r="F41" s="1">
         <v>45740</v>
       </c>
-      <c r="G36">
+      <c r="G41">
         <v>296</v>
       </c>
     </row>
-    <row r="37" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C37" s="1">
+    <row r="42" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C42" s="1">
         <v>45733</v>
       </c>
-      <c r="D37">
+      <c r="D42">
         <v>310</v>
       </c>
-      <c r="F37" s="1">
+      <c r="F42" s="1">
         <v>45733</v>
       </c>
-      <c r="G37">
+      <c r="G42">
         <v>296</v>
       </c>
     </row>
-    <row r="38" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C38" s="1">
+    <row r="43" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C43" s="1">
         <v>45726</v>
       </c>
-      <c r="D38">
+      <c r="D43">
         <v>309</v>
       </c>
-      <c r="F38" s="1">
+      <c r="F43" s="1">
         <v>45726</v>
       </c>
-      <c r="G38">
+      <c r="G43">
         <v>294</v>
       </c>
     </row>
-    <row r="39" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C39" s="1">
+    <row r="44" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C44" s="1">
         <v>45719</v>
       </c>
-      <c r="D39">
+      <c r="D44">
         <v>308</v>
       </c>
-      <c r="F39" s="1">
+      <c r="F44" s="1">
         <v>45719</v>
       </c>
-      <c r="G39">
+      <c r="G44">
         <v>286</v>
       </c>
     </row>
-    <row r="40" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C40" s="1">
+    <row r="45" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C45" s="1">
         <v>45712</v>
       </c>
-      <c r="D40">
+      <c r="D45">
         <v>306</v>
       </c>
-      <c r="F40" s="1">
+      <c r="F45" s="1">
         <v>45712</v>
       </c>
-      <c r="G40">
+      <c r="G45">
         <v>286</v>
       </c>
     </row>
-    <row r="41" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C41" s="1">
+    <row r="46" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C46" s="1">
         <v>45705</v>
       </c>
-      <c r="D41">
+      <c r="D46">
         <v>301</v>
       </c>
-      <c r="F41" s="1">
+      <c r="F46" s="1">
         <v>45705</v>
       </c>
-      <c r="G41">
+      <c r="G46">
         <v>267</v>
       </c>
     </row>
-    <row r="42" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C42" s="1">
+    <row r="47" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C47" s="1">
         <v>45698</v>
       </c>
-      <c r="D42">
+      <c r="D47">
         <v>295</v>
       </c>
-      <c r="F42" s="1">
+      <c r="F47" s="1">
         <v>45698</v>
       </c>
-      <c r="G42">
+      <c r="G47">
         <v>267</v>
       </c>
     </row>
-    <row r="43" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C43" s="1">
+    <row r="48" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C48" s="1">
         <v>45691</v>
       </c>
-      <c r="D43">
+      <c r="D48">
         <v>289</v>
       </c>
-      <c r="F43" s="1">
+      <c r="F48" s="1">
         <v>45691</v>
       </c>
-      <c r="G43">
+      <c r="G48">
         <v>267</v>
       </c>
     </row>
-    <row r="44" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C44" s="1">
+    <row r="49" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C49" s="1">
         <v>45684</v>
       </c>
-      <c r="D44">
+      <c r="D49">
         <v>284</v>
       </c>
-      <c r="F44" s="1">
+      <c r="F49" s="1">
         <v>45684</v>
       </c>
-      <c r="G44">
+      <c r="G49">
         <v>262</v>
       </c>
     </row>
-    <row r="45" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C45" s="1">
+    <row r="50" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C50" s="1">
         <v>45677</v>
       </c>
-      <c r="D45">
+      <c r="D50">
         <v>273</v>
       </c>
-      <c r="F45" s="1">
+      <c r="F50" s="1">
         <v>45677</v>
       </c>
-      <c r="G45">
+      <c r="G50">
         <v>254</v>
       </c>
     </row>
-    <row r="46" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C46" s="1">
+    <row r="51" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C51" s="1">
         <v>45670</v>
       </c>
-      <c r="D46">
+      <c r="D51">
         <v>264</v>
       </c>
-      <c r="F46" s="1">
+      <c r="F51" s="1">
         <v>45670</v>
       </c>
-      <c r="G46">
+      <c r="G51">
         <v>250</v>
       </c>
     </row>
-    <row r="47" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C47" s="1">
+    <row r="52" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C52" s="1">
         <v>45663</v>
       </c>
-      <c r="D47">
+      <c r="D52">
         <v>256</v>
       </c>
-      <c r="F47" s="1">
+      <c r="F52" s="1">
         <v>45663</v>
       </c>
-      <c r="G47">
+      <c r="G52">
         <v>250</v>
       </c>
     </row>
-    <row r="48" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C48" s="1">
+    <row r="53" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C53" s="1">
         <v>45642</v>
       </c>
-      <c r="D48">
+      <c r="D53">
         <v>256</v>
       </c>
-      <c r="F48" s="1">
+      <c r="F53" s="1">
         <v>45642</v>
       </c>
-      <c r="G48">
+      <c r="G53">
         <v>245</v>
       </c>
     </row>
-    <row r="49" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C49" s="1">
+    <row r="54" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C54" s="1">
         <v>45635</v>
       </c>
-      <c r="D49">
+      <c r="D54">
         <v>251</v>
       </c>
-      <c r="F49" s="1">
+      <c r="F54" s="1">
         <v>45635</v>
       </c>
-      <c r="G49">
+      <c r="G54">
         <v>243</v>
       </c>
     </row>
-    <row r="50" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C50" s="1">
+    <row r="55" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C55" s="1">
         <v>45628</v>
       </c>
-      <c r="D50">
+      <c r="D55">
         <v>251</v>
       </c>
-      <c r="F50" s="1">
+      <c r="F55" s="1">
         <v>45628</v>
       </c>
-      <c r="G50">
+      <c r="G55">
         <v>239</v>
       </c>
     </row>
-    <row r="51" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C51" s="1">
+    <row r="56" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C56" s="1">
         <v>45621</v>
       </c>
-      <c r="D51">
+      <c r="D56">
         <v>247</v>
       </c>
-      <c r="F51" s="1">
+      <c r="F56" s="1">
         <v>45621</v>
       </c>
-      <c r="G51">
+      <c r="G56">
         <v>234</v>
       </c>
     </row>
-    <row r="52" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C52" s="1">
+    <row r="57" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C57" s="1">
         <v>45614</v>
       </c>
-      <c r="D52">
+      <c r="D57">
         <v>241</v>
       </c>
-      <c r="F52" s="1">
+      <c r="F57" s="1">
         <v>45614</v>
       </c>
-      <c r="G52">
+      <c r="G57">
         <v>234</v>
       </c>
     </row>
-    <row r="53" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C53" s="1">
+    <row r="58" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C58" s="1">
         <v>45607</v>
       </c>
-      <c r="D53">
+      <c r="D58">
         <v>239</v>
       </c>
-      <c r="F53" s="1">
+      <c r="F58" s="1">
         <v>45607</v>
       </c>
-      <c r="G53">
+      <c r="G58">
         <v>230</v>
       </c>
     </row>
-    <row r="54" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C54" s="1">
+    <row r="59" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C59" s="1">
         <v>45600</v>
       </c>
-      <c r="D54">
+      <c r="D59">
         <v>232</v>
       </c>
-      <c r="F54" s="1">
+      <c r="F59" s="1">
         <v>45600</v>
       </c>
-      <c r="G54">
+      <c r="G59">
         <v>227</v>
       </c>
     </row>
-    <row r="55" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C55" s="1">
+    <row r="60" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C60" s="1">
         <v>45579</v>
       </c>
-      <c r="D55">
+      <c r="D60">
         <v>231</v>
       </c>
-      <c r="F55" s="1">
+      <c r="F60" s="1">
         <v>45579</v>
       </c>
-      <c r="G55">
+      <c r="G60">
         <v>222</v>
       </c>
     </row>
-    <row r="56" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C56" s="1">
+    <row r="61" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C61" s="1">
         <v>45572</v>
       </c>
-      <c r="D56">
+      <c r="D61">
         <v>227</v>
       </c>
-      <c r="F56" s="1">
+      <c r="F61" s="1">
         <v>45572</v>
       </c>
-      <c r="G56">
+      <c r="G61">
         <v>216</v>
       </c>
     </row>
-    <row r="57" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C57" s="1">
+    <row r="62" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C62" s="1">
         <v>45565</v>
       </c>
-      <c r="D57">
+      <c r="D62">
         <v>223</v>
       </c>
-      <c r="F57" s="1">
+      <c r="F62" s="1">
         <v>45565</v>
       </c>
-      <c r="G57">
+      <c r="G62">
         <v>216</v>
       </c>
     </row>
-    <row r="58" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C58" s="1">
+    <row r="63" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C63" s="1">
         <v>45537</v>
       </c>
-      <c r="D58">
+      <c r="D63">
         <v>218</v>
       </c>
-      <c r="F58" s="1">
+      <c r="F63" s="1">
         <v>45537</v>
       </c>
-      <c r="G58">
+      <c r="G63">
         <v>207</v>
       </c>
     </row>
-    <row r="59" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C59" s="1">
+    <row r="64" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C64" s="1">
         <v>45530</v>
       </c>
-      <c r="D59">
+      <c r="D64">
         <v>217</v>
       </c>
-      <c r="F59" s="1">
+      <c r="F64" s="1">
         <v>45530</v>
       </c>
-      <c r="G59">
+      <c r="G64">
         <v>207</v>
       </c>
     </row>
-    <row r="60" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C60" s="1">
+    <row r="65" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C65" s="1">
         <v>45523</v>
       </c>
-      <c r="D60">
+      <c r="D65">
         <v>216</v>
       </c>
-      <c r="F60" s="1">
+      <c r="F65" s="1">
         <v>45523</v>
       </c>
-      <c r="G60">
+      <c r="G65">
         <v>200</v>
       </c>
     </row>
-    <row r="61" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C61" s="1">
+    <row r="66" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C66" s="1">
         <v>45516</v>
       </c>
-      <c r="D61">
+      <c r="D66">
         <v>212</v>
       </c>
-      <c r="F61" s="1">
+      <c r="F66" s="1">
         <v>45516</v>
       </c>
-      <c r="G61">
+      <c r="G66">
         <v>190</v>
       </c>
     </row>
-    <row r="62" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C62" s="1">
+    <row r="67" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C67" s="1">
         <v>45509</v>
       </c>
-      <c r="D62">
+      <c r="D67">
         <v>210</v>
       </c>
-      <c r="F62" s="1">
+      <c r="F67" s="1">
         <v>45509</v>
       </c>
-      <c r="G62">
+      <c r="G67">
         <v>189</v>
       </c>
     </row>
-    <row r="63" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C63" s="1">
+    <row r="68" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C68" s="1">
         <v>45502</v>
       </c>
-      <c r="D63">
+      <c r="D68">
         <v>210</v>
       </c>
-      <c r="F63" s="1">
+      <c r="F68" s="1">
         <v>45502</v>
       </c>
-      <c r="G63">
+      <c r="G68">
         <v>189</v>
       </c>
     </row>
-    <row r="64" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C64" s="1">
+    <row r="69" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C69" s="1">
         <v>45495</v>
       </c>
-      <c r="D64">
+      <c r="D69">
         <v>201</v>
       </c>
-      <c r="F64" s="1">
+      <c r="F69" s="1">
         <v>45495</v>
       </c>
-      <c r="G64">
+      <c r="G69">
         <v>183</v>
       </c>
     </row>
-    <row r="65" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C65" s="1">
+    <row r="70" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C70" s="1">
         <v>45488</v>
       </c>
-      <c r="D65">
+      <c r="D70">
         <v>199</v>
       </c>
-      <c r="F65" s="1">
+      <c r="F70" s="1">
         <v>45488</v>
       </c>
-      <c r="G65">
+      <c r="G70">
         <v>182</v>
       </c>
     </row>
-    <row r="66" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C66" s="1">
+    <row r="71" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C71" s="1">
         <v>45481</v>
       </c>
-      <c r="D66">
+      <c r="D71">
         <v>188</v>
       </c>
-      <c r="F66" s="1">
+      <c r="F71" s="1">
         <v>45481</v>
       </c>
-      <c r="G66">
+      <c r="G71">
         <v>180</v>
       </c>
     </row>
-    <row r="67" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C67" s="1">
+    <row r="72" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C72" s="1">
         <v>45474</v>
       </c>
-      <c r="D67">
+      <c r="D72">
         <v>187</v>
       </c>
-      <c r="F67" s="1">
+      <c r="F72" s="1">
         <v>45474</v>
       </c>
-      <c r="G67">
+      <c r="G72">
         <v>172</v>
       </c>
     </row>
-    <row r="68" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C68" s="1">
+    <row r="73" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C73" s="1">
         <v>45467</v>
       </c>
-      <c r="D68">
+      <c r="D73">
         <v>187</v>
       </c>
-      <c r="F68" s="1">
+      <c r="F73" s="1">
         <v>45467</v>
       </c>
-      <c r="G68">
+      <c r="G73">
         <v>172</v>
       </c>
     </row>
-    <row r="69" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C69" s="1">
+    <row r="74" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C74" s="1">
         <v>45460</v>
       </c>
-      <c r="D69">
+      <c r="D74">
         <v>185</v>
       </c>
-      <c r="F69" s="1">
+      <c r="F74" s="1">
         <v>45460</v>
       </c>
-      <c r="G69">
+      <c r="G74">
         <v>165</v>
       </c>
     </row>
-    <row r="70" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C70" s="1">
+    <row r="75" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C75" s="1">
         <v>45453</v>
       </c>
-      <c r="D70">
+      <c r="D75">
         <v>180</v>
       </c>
-      <c r="F70" s="1">
+      <c r="F75" s="1">
         <v>45453</v>
       </c>
-      <c r="G70">
+      <c r="G75">
         <v>164</v>
       </c>
     </row>
-    <row r="71" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C71" s="1">
+    <row r="76" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C76" s="1">
         <v>45446</v>
       </c>
-      <c r="D71">
+      <c r="D76">
         <v>177</v>
       </c>
-      <c r="F71" s="1">
+      <c r="F76" s="1">
         <v>45446</v>
       </c>
-      <c r="G71">
+      <c r="G76">
         <v>161</v>
       </c>
     </row>
-    <row r="72" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C72" s="1">
+    <row r="77" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C77" s="1">
         <v>45439</v>
       </c>
-      <c r="D72">
+      <c r="D77">
         <v>174</v>
       </c>
-      <c r="F72" s="1">
+      <c r="F77" s="1">
         <v>45439</v>
       </c>
-      <c r="G72">
+      <c r="G77">
         <v>161</v>
       </c>
     </row>
-    <row r="73" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C73" s="1">
+    <row r="78" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C78" s="1">
         <v>45432</v>
       </c>
-      <c r="D73">
+      <c r="D78">
         <v>173</v>
       </c>
-      <c r="F73" s="1">
+      <c r="F78" s="1">
         <v>45432</v>
       </c>
-      <c r="G73">
+      <c r="G78">
         <v>159</v>
       </c>
     </row>
-    <row r="74" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C74" s="1">
+    <row r="79" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C79" s="1">
         <v>45425</v>
       </c>
-      <c r="D74">
+      <c r="D79">
         <v>170</v>
       </c>
-      <c r="F74" s="1">
+      <c r="F79" s="1">
         <v>45425</v>
       </c>
-      <c r="G74">
+      <c r="G79">
         <v>157</v>
       </c>
     </row>
-    <row r="75" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C75" s="1">
+    <row r="80" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C80" s="1">
         <v>45418</v>
       </c>
-      <c r="D75">
+      <c r="D80">
         <v>170</v>
       </c>
-      <c r="F75" s="1">
+      <c r="F80" s="1">
         <v>45418</v>
       </c>
-      <c r="G75">
+      <c r="G80">
         <v>141</v>
       </c>
     </row>
-    <row r="76" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C76" s="1">
+    <row r="81" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C81" s="1">
         <v>45411</v>
       </c>
-      <c r="D76">
+      <c r="D81">
         <v>166</v>
       </c>
-      <c r="F76" s="1">
+      <c r="F81" s="1">
         <v>45411</v>
       </c>
-      <c r="G76">
+      <c r="G81">
         <v>141</v>
       </c>
     </row>
-    <row r="77" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C77" s="1">
+    <row r="82" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C82" s="1">
         <v>45404</v>
       </c>
-      <c r="D77">
+      <c r="D82">
         <v>166</v>
       </c>
-      <c r="F77" s="1">
+      <c r="F82" s="1">
         <v>45404</v>
       </c>
-      <c r="G77">
+      <c r="G82">
         <v>141</v>
       </c>
     </row>
-    <row r="78" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C78" s="1">
+    <row r="83" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C83" s="1">
         <v>45397</v>
       </c>
-      <c r="D78">
+      <c r="D83">
         <v>157</v>
       </c>
-      <c r="F78" s="1">
+      <c r="F83" s="1">
         <v>45397</v>
       </c>
-      <c r="G78">
+      <c r="G83">
         <v>132</v>
       </c>
     </row>
-    <row r="79" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C79" s="1">
+    <row r="84" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C84" s="1">
         <v>45390</v>
       </c>
-      <c r="D79">
+      <c r="D84">
         <v>146</v>
       </c>
-      <c r="F79" s="1">
+      <c r="F84" s="1">
         <v>45390</v>
       </c>
-      <c r="G79">
+      <c r="G84">
         <v>132</v>
       </c>
     </row>
-    <row r="80" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C80" s="1">
+    <row r="85" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C85" s="1">
         <v>45383</v>
       </c>
-      <c r="D80">
+      <c r="D85">
         <v>138</v>
       </c>
-      <c r="F80" s="1">
+      <c r="F85" s="1">
         <v>45383</v>
       </c>
-      <c r="G80">
+      <c r="G85">
         <v>119</v>
       </c>
     </row>
-    <row r="81" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C81" s="1">
+    <row r="86" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C86" s="1">
         <v>45376</v>
       </c>
-      <c r="D81">
+      <c r="D86">
         <v>129</v>
       </c>
-      <c r="F81" s="1">
+      <c r="F86" s="1">
         <v>45376</v>
       </c>
-      <c r="G81">
+      <c r="G86">
         <v>114</v>
       </c>
     </row>
-    <row r="82" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C82" s="1">
+    <row r="87" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C87" s="1">
         <v>45369</v>
       </c>
-      <c r="D82">
+      <c r="D87">
         <v>123</v>
       </c>
-      <c r="F82" s="1">
+      <c r="F87" s="1">
         <v>45369</v>
       </c>
-      <c r="G82">
+      <c r="G87">
         <v>97</v>
       </c>
     </row>
-    <row r="83" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C83" s="1">
+    <row r="88" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C88" s="1">
         <v>45362</v>
       </c>
-      <c r="D83">
+      <c r="D88">
         <v>113</v>
       </c>
-      <c r="F83" s="1"/>
-    </row>
-    <row r="84" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C84" s="1">
+      <c r="F88" s="1"/>
+    </row>
+    <row r="89" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C89" s="1">
         <v>45355</v>
       </c>
-      <c r="D84">
+      <c r="D89">
         <v>108</v>
       </c>
     </row>
-    <row r="85" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C85" s="1">
+    <row r="90" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C90" s="1">
         <v>45348</v>
       </c>
-      <c r="D85">
+      <c r="D90">
         <v>102</v>
       </c>
     </row>
-    <row r="86" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C86" s="1">
+    <row r="91" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C91" s="1">
         <v>45341</v>
       </c>
-      <c r="D86">
+      <c r="D91">
         <v>95</v>
       </c>
     </row>
-    <row r="87" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C87" s="1">
+    <row r="92" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C92" s="1">
         <v>45334</v>
       </c>
-      <c r="D87">
+      <c r="D92">
         <v>80</v>
       </c>
     </row>
-    <row r="88" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C88" s="1">
+    <row r="93" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C93" s="1">
         <v>45327</v>
       </c>
-      <c r="D88">
+      <c r="D93">
         <v>66</v>
       </c>
     </row>
-    <row r="89" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C89" s="1">
+    <row r="94" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C94" s="1">
         <v>45320</v>
       </c>
-      <c r="D89">
+      <c r="D94">
         <v>55</v>
       </c>
     </row>
-    <row r="90" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C90" s="1">
+    <row r="95" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C95" s="1">
         <v>45313</v>
       </c>
-      <c r="D90">
+      <c r="D95">
         <v>53</v>
       </c>
     </row>
-    <row r="91" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C91" s="1">
+    <row r="96" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C96" s="1">
         <v>45306</v>
       </c>
-      <c r="D91">
+      <c r="D96">
         <v>52</v>
       </c>
     </row>
-    <row r="95" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="D95" s="2"/>
-      <c r="E95" s="2"/>
-      <c r="F95" s="2"/>
-      <c r="G95" s="2"/>
-      <c r="H95" s="2"/>
-      <c r="I95" s="2"/>
-      <c r="J95" s="2"/>
-      <c r="K95" s="2"/>
-      <c r="L95" s="2"/>
-      <c r="M95" s="2"/>
-      <c r="N95" s="2"/>
-      <c r="O95" s="2"/>
-      <c r="P95" s="2"/>
-      <c r="Q95" s="2"/>
-    </row>
-    <row r="96" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="D96" s="2"/>
-      <c r="E96" s="2"/>
-      <c r="F96" s="2"/>
-      <c r="G96" s="2"/>
-      <c r="H96" s="2"/>
-      <c r="I96" s="2"/>
-      <c r="J96" s="2"/>
-      <c r="K96" s="2"/>
-      <c r="L96" s="2"/>
-      <c r="M96" s="2"/>
-      <c r="N96" s="2"/>
-      <c r="O96" s="2"/>
-      <c r="P96" s="2"/>
-      <c r="Q96" s="2"/>
-    </row>
-    <row r="97" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D97" s="2"/>
-      <c r="E97" s="2"/>
-      <c r="F97" s="2"/>
-      <c r="G97" s="2"/>
-      <c r="H97" s="2"/>
-      <c r="I97" s="2"/>
-      <c r="J97" s="2"/>
-      <c r="K97" s="2"/>
-      <c r="L97" s="2"/>
-      <c r="M97" s="2"/>
-      <c r="N97" s="2"/>
-      <c r="O97" s="2"/>
-      <c r="P97" s="2"/>
-      <c r="Q97" s="2"/>
-    </row>
-    <row r="98" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D98" s="2"/>
-      <c r="E98" s="2"/>
-      <c r="F98" s="2"/>
-      <c r="G98" s="2"/>
-      <c r="H98" s="2"/>
-      <c r="I98" s="2"/>
-      <c r="J98" s="2"/>
-      <c r="K98" s="2"/>
-      <c r="L98" s="2"/>
-      <c r="M98" s="2"/>
-      <c r="N98" s="2"/>
-      <c r="O98" s="2"/>
-      <c r="P98" s="2"/>
-      <c r="Q98" s="2"/>
-    </row>
-    <row r="99" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D99" s="2"/>
-      <c r="E99" s="2"/>
-      <c r="F99" s="2"/>
-      <c r="G99" s="2"/>
-      <c r="H99" s="2"/>
-      <c r="I99" s="2"/>
-      <c r="J99" s="2"/>
-      <c r="K99" s="2"/>
-      <c r="L99" s="2"/>
-      <c r="M99" s="2"/>
-      <c r="N99" s="2"/>
-      <c r="O99" s="2"/>
-      <c r="P99" s="2"/>
-      <c r="Q99" s="2"/>
-    </row>
-    <row r="100" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="100" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D100" s="2"/>
       <c r="E100" s="2"/>
       <c r="F100" s="2"/>
@@ -5962,7 +5896,7 @@
       <c r="P100" s="2"/>
       <c r="Q100" s="2"/>
     </row>
-    <row r="101" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="101" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D101" s="2"/>
       <c r="E101" s="2"/>
       <c r="F101" s="2"/>
@@ -5978,7 +5912,7 @@
       <c r="P101" s="2"/>
       <c r="Q101" s="2"/>
     </row>
-    <row r="102" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="102" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D102" s="2"/>
       <c r="E102" s="2"/>
       <c r="F102" s="2"/>
@@ -5994,7 +5928,7 @@
       <c r="P102" s="2"/>
       <c r="Q102" s="2"/>
     </row>
-    <row r="103" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="103" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D103" s="2"/>
       <c r="E103" s="2"/>
       <c r="F103" s="2"/>
@@ -6010,7 +5944,7 @@
       <c r="P103" s="2"/>
       <c r="Q103" s="2"/>
     </row>
-    <row r="104" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="104" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D104" s="2"/>
       <c r="E104" s="2"/>
       <c r="F104" s="2"/>
@@ -6026,7 +5960,7 @@
       <c r="P104" s="2"/>
       <c r="Q104" s="2"/>
     </row>
-    <row r="105" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="105" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D105" s="2"/>
       <c r="E105" s="2"/>
       <c r="F105" s="2"/>
@@ -6042,7 +5976,7 @@
       <c r="P105" s="2"/>
       <c r="Q105" s="2"/>
     </row>
-    <row r="106" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="106" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D106" s="2"/>
       <c r="E106" s="2"/>
       <c r="F106" s="2"/>
@@ -6058,7 +5992,7 @@
       <c r="P106" s="2"/>
       <c r="Q106" s="2"/>
     </row>
-    <row r="107" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="107" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D107" s="2"/>
       <c r="E107" s="2"/>
       <c r="F107" s="2"/>
@@ -6074,7 +6008,7 @@
       <c r="P107" s="2"/>
       <c r="Q107" s="2"/>
     </row>
-    <row r="108" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="108" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D108" s="2"/>
       <c r="E108" s="2"/>
       <c r="F108" s="2"/>
@@ -6090,7 +6024,7 @@
       <c r="P108" s="2"/>
       <c r="Q108" s="2"/>
     </row>
-    <row r="109" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="109" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D109" s="2"/>
       <c r="E109" s="2"/>
       <c r="F109" s="2"/>
@@ -6106,7 +6040,7 @@
       <c r="P109" s="2"/>
       <c r="Q109" s="2"/>
     </row>
-    <row r="110" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="110" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D110" s="2"/>
       <c r="E110" s="2"/>
       <c r="F110" s="2"/>
@@ -6122,7 +6056,7 @@
       <c r="P110" s="2"/>
       <c r="Q110" s="2"/>
     </row>
-    <row r="111" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="111" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D111" s="2"/>
       <c r="E111" s="2"/>
       <c r="F111" s="2"/>
@@ -6138,7 +6072,7 @@
       <c r="P111" s="2"/>
       <c r="Q111" s="2"/>
     </row>
-    <row r="112" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="112" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D112" s="2"/>
       <c r="E112" s="2"/>
       <c r="F112" s="2"/>
@@ -6154,7 +6088,7 @@
       <c r="P112" s="2"/>
       <c r="Q112" s="2"/>
     </row>
-    <row r="113" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="113" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D113" s="2"/>
       <c r="E113" s="2"/>
       <c r="F113" s="2"/>
@@ -6170,7 +6104,7 @@
       <c r="P113" s="2"/>
       <c r="Q113" s="2"/>
     </row>
-    <row r="114" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="114" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D114" s="2"/>
       <c r="E114" s="2"/>
       <c r="F114" s="2"/>
@@ -6186,7 +6120,7 @@
       <c r="P114" s="2"/>
       <c r="Q114" s="2"/>
     </row>
-    <row r="115" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="115" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D115" s="2"/>
       <c r="E115" s="2"/>
       <c r="F115" s="2"/>
@@ -6202,7 +6136,7 @@
       <c r="P115" s="2"/>
       <c r="Q115" s="2"/>
     </row>
-    <row r="116" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="116" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D116" s="2"/>
       <c r="E116" s="2"/>
       <c r="F116" s="2"/>
@@ -6218,7 +6152,7 @@
       <c r="P116" s="2"/>
       <c r="Q116" s="2"/>
     </row>
-    <row r="117" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="117" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D117" s="2"/>
       <c r="E117" s="2"/>
       <c r="F117" s="2"/>
@@ -6234,7 +6168,7 @@
       <c r="P117" s="2"/>
       <c r="Q117" s="2"/>
     </row>
-    <row r="118" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="118" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D118" s="2"/>
       <c r="E118" s="2"/>
       <c r="F118" s="2"/>
@@ -6250,7 +6184,7 @@
       <c r="P118" s="2"/>
       <c r="Q118" s="2"/>
     </row>
-    <row r="119" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="119" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D119" s="2"/>
       <c r="E119" s="2"/>
       <c r="F119" s="2"/>
@@ -6266,7 +6200,7 @@
       <c r="P119" s="2"/>
       <c r="Q119" s="2"/>
     </row>
-    <row r="120" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="120" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D120" s="2"/>
       <c r="E120" s="2"/>
       <c r="F120" s="2"/>
@@ -6282,9 +6216,89 @@
       <c r="P120" s="2"/>
       <c r="Q120" s="2"/>
     </row>
+    <row r="121" spans="4:17" x14ac:dyDescent="0.35">
+      <c r="D121" s="2"/>
+      <c r="E121" s="2"/>
+      <c r="F121" s="2"/>
+      <c r="G121" s="2"/>
+      <c r="H121" s="2"/>
+      <c r="I121" s="2"/>
+      <c r="J121" s="2"/>
+      <c r="K121" s="2"/>
+      <c r="L121" s="2"/>
+      <c r="M121" s="2"/>
+      <c r="N121" s="2"/>
+      <c r="O121" s="2"/>
+      <c r="P121" s="2"/>
+      <c r="Q121" s="2"/>
+    </row>
+    <row r="122" spans="4:17" x14ac:dyDescent="0.35">
+      <c r="D122" s="2"/>
+      <c r="E122" s="2"/>
+      <c r="F122" s="2"/>
+      <c r="G122" s="2"/>
+      <c r="H122" s="2"/>
+      <c r="I122" s="2"/>
+      <c r="J122" s="2"/>
+      <c r="K122" s="2"/>
+      <c r="L122" s="2"/>
+      <c r="M122" s="2"/>
+      <c r="N122" s="2"/>
+      <c r="O122" s="2"/>
+      <c r="P122" s="2"/>
+      <c r="Q122" s="2"/>
+    </row>
+    <row r="123" spans="4:17" x14ac:dyDescent="0.35">
+      <c r="D123" s="2"/>
+      <c r="E123" s="2"/>
+      <c r="F123" s="2"/>
+      <c r="G123" s="2"/>
+      <c r="H123" s="2"/>
+      <c r="I123" s="2"/>
+      <c r="J123" s="2"/>
+      <c r="K123" s="2"/>
+      <c r="L123" s="2"/>
+      <c r="M123" s="2"/>
+      <c r="N123" s="2"/>
+      <c r="O123" s="2"/>
+      <c r="P123" s="2"/>
+      <c r="Q123" s="2"/>
+    </row>
+    <row r="124" spans="4:17" x14ac:dyDescent="0.35">
+      <c r="D124" s="2"/>
+      <c r="E124" s="2"/>
+      <c r="F124" s="2"/>
+      <c r="G124" s="2"/>
+      <c r="H124" s="2"/>
+      <c r="I124" s="2"/>
+      <c r="J124" s="2"/>
+      <c r="K124" s="2"/>
+      <c r="L124" s="2"/>
+      <c r="M124" s="2"/>
+      <c r="N124" s="2"/>
+      <c r="O124" s="2"/>
+      <c r="P124" s="2"/>
+      <c r="Q124" s="2"/>
+    </row>
+    <row r="125" spans="4:17" x14ac:dyDescent="0.35">
+      <c r="D125" s="2"/>
+      <c r="E125" s="2"/>
+      <c r="F125" s="2"/>
+      <c r="G125" s="2"/>
+      <c r="H125" s="2"/>
+      <c r="I125" s="2"/>
+      <c r="J125" s="2"/>
+      <c r="K125" s="2"/>
+      <c r="L125" s="2"/>
+      <c r="M125" s="2"/>
+      <c r="N125" s="2"/>
+      <c r="O125" s="2"/>
+      <c r="P125" s="2"/>
+      <c r="Q125" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D95:Q120"/>
+    <mergeCell ref="D100:Q125"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
LGHUB 2025/8/24 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
- 网站错误 & 本地化问题详见 LGHUB/WebLoc/README.md
</commit_message>
<xml_diff>
--- a/Documents/Graph_PC.xlsx
+++ b/Documents/Graph_PC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29220"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8CE8366-2973-4A64-A3CD-20F6E8C4B9C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BE25974-DC44-4BC9-A00F-9870910B0B1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="2" r:id="rId1"/>
@@ -574,13 +574,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>16</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>78</c:v>
+                  <c:v>84</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -917,69 +917,69 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$20:$C$28</c:f>
+              <c:f>Sheet1!$C$19:$C$27</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45894</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45887</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45880</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45873</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45866</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45859</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45852</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45845</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45838</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45831</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$20:$D$28</c:f>
+              <c:f>Sheet1!$D$19:$D$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>456</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>446</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>443</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>440</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>432</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>430</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>419</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>418</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>416</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>416</c:v>
@@ -1086,69 +1086,69 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$20:$C$28</c:f>
+              <c:f>Sheet1!$C$19:$C$27</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45894</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45887</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45880</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45873</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45866</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45859</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45852</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45845</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45838</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45831</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$20:$G$28</c:f>
+              <c:f>Sheet1!$G$19:$G$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>421</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>415</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>406</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>405</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>406</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>389</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>386</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>386</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>370</c:v>
+                  <c:v>386</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>370</c:v>
@@ -1286,8 +1286,8 @@
         <c:axId val="1374569007"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="450"/>
-          <c:min val="350"/>
+          <c:max val="460"/>
+          <c:min val="360"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1794,13 +1794,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>16</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>78</c:v>
+                  <c:v>84</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4811,51 +4811,65 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D98" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L99" sqref="L99"/>
+    <sheetView tabSelected="1" topLeftCell="B97" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="R107" sqref="R107"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.35">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C19" s="1">
+        <v>45894</v>
+      </c>
+      <c r="D19">
+        <v>456</v>
+      </c>
+      <c r="F19" s="1">
+        <v>45894</v>
+      </c>
+      <c r="G19">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C20" s="1">
         <v>45887</v>
       </c>
@@ -4869,7 +4883,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C21" s="1">
         <v>45880</v>
       </c>
@@ -4883,7 +4897,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C22" s="1">
         <v>45873</v>
       </c>
@@ -4897,7 +4911,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C23" s="1">
         <v>45866</v>
       </c>
@@ -4911,7 +4925,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C24" s="1">
         <v>45859</v>
       </c>
@@ -4925,7 +4939,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C25" s="1">
         <v>45852</v>
       </c>
@@ -4939,7 +4953,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C26" s="1">
         <v>45845</v>
       </c>
@@ -4953,7 +4967,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C27" s="1">
         <v>45838</v>
       </c>
@@ -4967,7 +4981,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C28" s="1">
         <v>45831</v>
       </c>
@@ -4981,7 +4995,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C29" s="1">
         <v>45824</v>
       </c>
@@ -4995,7 +5009,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C30" s="1">
         <v>45817</v>
       </c>
@@ -5009,7 +5023,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C31" s="1">
         <v>45810</v>
       </c>
@@ -5023,7 +5037,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C32" s="1">
         <v>45803</v>
       </c>
@@ -5037,7 +5051,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C33" s="1">
         <v>45796</v>
       </c>
@@ -5051,7 +5065,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="34" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C34" s="1">
         <v>45789</v>
       </c>
@@ -5065,7 +5079,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="35" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C35" s="1">
         <v>45782</v>
       </c>
@@ -5079,7 +5093,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="36" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C36" s="1">
         <v>45775</v>
       </c>
@@ -5093,7 +5107,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="37" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C37" s="1">
         <v>45768</v>
       </c>
@@ -5107,7 +5121,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="38" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C38" s="1">
         <v>45761</v>
       </c>
@@ -5121,7 +5135,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="39" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C39" s="1">
         <v>45754</v>
       </c>
@@ -5135,7 +5149,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="40" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C40" s="1">
         <v>45747</v>
       </c>
@@ -5149,7 +5163,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="41" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C41" s="1">
         <v>45740</v>
       </c>
@@ -5163,7 +5177,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="42" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C42" s="1">
         <v>45733</v>
       </c>
@@ -5177,7 +5191,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="43" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C43" s="1">
         <v>45726</v>
       </c>
@@ -5191,7 +5205,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="44" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C44" s="1">
         <v>45719</v>
       </c>
@@ -5205,7 +5219,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="45" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C45" s="1">
         <v>45712</v>
       </c>
@@ -5219,7 +5233,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="46" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C46" s="1">
         <v>45705</v>
       </c>
@@ -5233,7 +5247,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="47" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C47" s="1">
         <v>45698</v>
       </c>
@@ -5247,7 +5261,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="48" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C48" s="1">
         <v>45691</v>
       </c>
@@ -5261,7 +5275,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="49" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="49" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C49" s="1">
         <v>45684</v>
       </c>
@@ -5275,7 +5289,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="50" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="50" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C50" s="1">
         <v>45677</v>
       </c>
@@ -5289,7 +5303,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="51" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="51" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C51" s="1">
         <v>45670</v>
       </c>
@@ -5303,7 +5317,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="52" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="52" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C52" s="1">
         <v>45663</v>
       </c>
@@ -5317,7 +5331,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="53" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="53" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C53" s="1">
         <v>45642</v>
       </c>
@@ -5331,7 +5345,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="54" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="54" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C54" s="1">
         <v>45635</v>
       </c>
@@ -5345,7 +5359,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="55" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="55" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C55" s="1">
         <v>45628</v>
       </c>
@@ -5359,7 +5373,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="56" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="56" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C56" s="1">
         <v>45621</v>
       </c>
@@ -5373,7 +5387,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="57" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="57" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C57" s="1">
         <v>45614</v>
       </c>
@@ -5387,7 +5401,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="58" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="58" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C58" s="1">
         <v>45607</v>
       </c>
@@ -5401,7 +5415,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="59" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="59" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C59" s="1">
         <v>45600</v>
       </c>
@@ -5415,7 +5429,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="60" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="60" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C60" s="1">
         <v>45579</v>
       </c>
@@ -5429,7 +5443,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="61" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="61" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C61" s="1">
         <v>45572</v>
       </c>
@@ -5443,7 +5457,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="62" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="62" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C62" s="1">
         <v>45565</v>
       </c>
@@ -5457,7 +5471,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="63" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="63" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C63" s="1">
         <v>45537</v>
       </c>
@@ -5471,7 +5485,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="64" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="64" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C64" s="1">
         <v>45530</v>
       </c>
@@ -5485,7 +5499,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="65" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="65" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C65" s="1">
         <v>45523</v>
       </c>
@@ -5499,7 +5513,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="66" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="66" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C66" s="1">
         <v>45516</v>
       </c>
@@ -5513,7 +5527,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="67" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="67" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C67" s="1">
         <v>45509</v>
       </c>
@@ -5527,7 +5541,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="68" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="68" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C68" s="1">
         <v>45502</v>
       </c>
@@ -5541,7 +5555,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="69" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="69" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C69" s="1">
         <v>45495</v>
       </c>
@@ -5555,7 +5569,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="70" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="70" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C70" s="1">
         <v>45488</v>
       </c>
@@ -5569,7 +5583,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="71" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="71" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C71" s="1">
         <v>45481</v>
       </c>
@@ -5583,7 +5597,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="72" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="72" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C72" s="1">
         <v>45474</v>
       </c>
@@ -5597,7 +5611,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="73" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="73" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C73" s="1">
         <v>45467</v>
       </c>
@@ -5611,7 +5625,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="74" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="74" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C74" s="1">
         <v>45460</v>
       </c>
@@ -5625,7 +5639,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="75" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="75" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C75" s="1">
         <v>45453</v>
       </c>
@@ -5639,7 +5653,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="76" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="76" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C76" s="1">
         <v>45446</v>
       </c>
@@ -5653,7 +5667,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="77" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="77" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C77" s="1">
         <v>45439</v>
       </c>
@@ -5667,7 +5681,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="78" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="78" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C78" s="1">
         <v>45432</v>
       </c>
@@ -5681,7 +5695,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="79" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="79" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C79" s="1">
         <v>45425</v>
       </c>
@@ -5695,7 +5709,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="80" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="80" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C80" s="1">
         <v>45418</v>
       </c>
@@ -5709,7 +5723,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="81" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="81" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C81" s="1">
         <v>45411</v>
       </c>
@@ -5723,7 +5737,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="82" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="82" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C82" s="1">
         <v>45404</v>
       </c>
@@ -5737,7 +5751,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="83" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="83" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C83" s="1">
         <v>45397</v>
       </c>
@@ -5751,7 +5765,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="84" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="84" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C84" s="1">
         <v>45390</v>
       </c>
@@ -5765,7 +5779,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="85" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="85" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C85" s="1">
         <v>45383</v>
       </c>
@@ -5779,7 +5793,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="86" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="86" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C86" s="1">
         <v>45376</v>
       </c>
@@ -5793,7 +5807,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="87" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="87" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C87" s="1">
         <v>45369</v>
       </c>
@@ -5807,7 +5821,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="88" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="88" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C88" s="1">
         <v>45362</v>
       </c>
@@ -5816,7 +5830,7 @@
       </c>
       <c r="F88" s="1"/>
     </row>
-    <row r="89" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="89" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C89" s="1">
         <v>45355</v>
       </c>
@@ -5824,7 +5838,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="90" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="90" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C90" s="1">
         <v>45348</v>
       </c>
@@ -5832,7 +5846,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="91" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="91" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C91" s="1">
         <v>45341</v>
       </c>
@@ -5840,7 +5854,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="92" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="92" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C92" s="1">
         <v>45334</v>
       </c>
@@ -5848,7 +5862,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="93" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="93" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C93" s="1">
         <v>45327</v>
       </c>
@@ -5856,7 +5870,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="94" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="94" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C94" s="1">
         <v>45320</v>
       </c>
@@ -5864,7 +5878,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="95" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="95" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C95" s="1">
         <v>45313</v>
       </c>
@@ -5872,7 +5886,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="96" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="96" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C96" s="1">
         <v>45306</v>
       </c>
@@ -5880,7 +5894,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="100" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="100" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D100" s="2"/>
       <c r="E100" s="2"/>
       <c r="F100" s="2"/>
@@ -5896,7 +5910,7 @@
       <c r="P100" s="2"/>
       <c r="Q100" s="2"/>
     </row>
-    <row r="101" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="101" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D101" s="2"/>
       <c r="E101" s="2"/>
       <c r="F101" s="2"/>
@@ -5912,7 +5926,7 @@
       <c r="P101" s="2"/>
       <c r="Q101" s="2"/>
     </row>
-    <row r="102" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="102" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D102" s="2"/>
       <c r="E102" s="2"/>
       <c r="F102" s="2"/>
@@ -5928,7 +5942,7 @@
       <c r="P102" s="2"/>
       <c r="Q102" s="2"/>
     </row>
-    <row r="103" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="103" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D103" s="2"/>
       <c r="E103" s="2"/>
       <c r="F103" s="2"/>
@@ -5944,7 +5958,7 @@
       <c r="P103" s="2"/>
       <c r="Q103" s="2"/>
     </row>
-    <row r="104" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="104" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D104" s="2"/>
       <c r="E104" s="2"/>
       <c r="F104" s="2"/>
@@ -5960,7 +5974,7 @@
       <c r="P104" s="2"/>
       <c r="Q104" s="2"/>
     </row>
-    <row r="105" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="105" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D105" s="2"/>
       <c r="E105" s="2"/>
       <c r="F105" s="2"/>
@@ -5976,7 +5990,7 @@
       <c r="P105" s="2"/>
       <c r="Q105" s="2"/>
     </row>
-    <row r="106" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="106" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D106" s="2"/>
       <c r="E106" s="2"/>
       <c r="F106" s="2"/>
@@ -5992,7 +6006,7 @@
       <c r="P106" s="2"/>
       <c r="Q106" s="2"/>
     </row>
-    <row r="107" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="107" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D107" s="2"/>
       <c r="E107" s="2"/>
       <c r="F107" s="2"/>
@@ -6008,7 +6022,7 @@
       <c r="P107" s="2"/>
       <c r="Q107" s="2"/>
     </row>
-    <row r="108" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="108" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D108" s="2"/>
       <c r="E108" s="2"/>
       <c r="F108" s="2"/>
@@ -6024,7 +6038,7 @@
       <c r="P108" s="2"/>
       <c r="Q108" s="2"/>
     </row>
-    <row r="109" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="109" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D109" s="2"/>
       <c r="E109" s="2"/>
       <c r="F109" s="2"/>
@@ -6040,7 +6054,7 @@
       <c r="P109" s="2"/>
       <c r="Q109" s="2"/>
     </row>
-    <row r="110" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="110" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D110" s="2"/>
       <c r="E110" s="2"/>
       <c r="F110" s="2"/>
@@ -6056,7 +6070,7 @@
       <c r="P110" s="2"/>
       <c r="Q110" s="2"/>
     </row>
-    <row r="111" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="111" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D111" s="2"/>
       <c r="E111" s="2"/>
       <c r="F111" s="2"/>
@@ -6072,7 +6086,7 @@
       <c r="P111" s="2"/>
       <c r="Q111" s="2"/>
     </row>
-    <row r="112" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="112" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D112" s="2"/>
       <c r="E112" s="2"/>
       <c r="F112" s="2"/>
@@ -6088,7 +6102,7 @@
       <c r="P112" s="2"/>
       <c r="Q112" s="2"/>
     </row>
-    <row r="113" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="113" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D113" s="2"/>
       <c r="E113" s="2"/>
       <c r="F113" s="2"/>
@@ -6104,7 +6118,7 @@
       <c r="P113" s="2"/>
       <c r="Q113" s="2"/>
     </row>
-    <row r="114" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="114" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D114" s="2"/>
       <c r="E114" s="2"/>
       <c r="F114" s="2"/>
@@ -6120,7 +6134,7 @@
       <c r="P114" s="2"/>
       <c r="Q114" s="2"/>
     </row>
-    <row r="115" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="115" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D115" s="2"/>
       <c r="E115" s="2"/>
       <c r="F115" s="2"/>
@@ -6136,7 +6150,7 @@
       <c r="P115" s="2"/>
       <c r="Q115" s="2"/>
     </row>
-    <row r="116" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="116" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D116" s="2"/>
       <c r="E116" s="2"/>
       <c r="F116" s="2"/>
@@ -6152,7 +6166,7 @@
       <c r="P116" s="2"/>
       <c r="Q116" s="2"/>
     </row>
-    <row r="117" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="117" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D117" s="2"/>
       <c r="E117" s="2"/>
       <c r="F117" s="2"/>
@@ -6168,7 +6182,7 @@
       <c r="P117" s="2"/>
       <c r="Q117" s="2"/>
     </row>
-    <row r="118" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="118" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D118" s="2"/>
       <c r="E118" s="2"/>
       <c r="F118" s="2"/>
@@ -6184,7 +6198,7 @@
       <c r="P118" s="2"/>
       <c r="Q118" s="2"/>
     </row>
-    <row r="119" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="119" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D119" s="2"/>
       <c r="E119" s="2"/>
       <c r="F119" s="2"/>
@@ -6200,7 +6214,7 @@
       <c r="P119" s="2"/>
       <c r="Q119" s="2"/>
     </row>
-    <row r="120" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="120" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D120" s="2"/>
       <c r="E120" s="2"/>
       <c r="F120" s="2"/>
@@ -6216,7 +6230,7 @@
       <c r="P120" s="2"/>
       <c r="Q120" s="2"/>
     </row>
-    <row r="121" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="121" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D121" s="2"/>
       <c r="E121" s="2"/>
       <c r="F121" s="2"/>
@@ -6232,7 +6246,7 @@
       <c r="P121" s="2"/>
       <c r="Q121" s="2"/>
     </row>
-    <row r="122" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="122" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D122" s="2"/>
       <c r="E122" s="2"/>
       <c r="F122" s="2"/>
@@ -6248,7 +6262,7 @@
       <c r="P122" s="2"/>
       <c r="Q122" s="2"/>
     </row>
-    <row r="123" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="123" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D123" s="2"/>
       <c r="E123" s="2"/>
       <c r="F123" s="2"/>
@@ -6264,7 +6278,7 @@
       <c r="P123" s="2"/>
       <c r="Q123" s="2"/>
     </row>
-    <row r="124" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="124" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D124" s="2"/>
       <c r="E124" s="2"/>
       <c r="F124" s="2"/>
@@ -6280,7 +6294,7 @@
       <c r="P124" s="2"/>
       <c r="Q124" s="2"/>
     </row>
-    <row r="125" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="125" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D125" s="2"/>
       <c r="E125" s="2"/>
       <c r="F125" s="2"/>

</xml_diff>

<commit_message>
LGHUB 2025/9/2 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
- 网站错误 & 本地化问题详见 LGHUB/WebLoc/README.md
</commit_message>
<xml_diff>
--- a/Documents/Graph_PC.xlsx
+++ b/Documents/Graph_PC.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29220"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29221"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BE25974-DC44-4BC9-A00F-9870910B0B1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CC8225C-5BDC-409A-8515-F1A53346920D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,13 +574,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>21</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>84</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -917,72 +917,72 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$19:$C$27</c:f>
+              <c:f>Sheet1!$C$18:$C$26</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45901</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45894</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45887</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45880</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45873</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45866</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45859</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45852</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45845</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45838</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$19:$D$27</c:f>
+              <c:f>Sheet1!$D$18:$D$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>465</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>456</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>446</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>443</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>440</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>432</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>430</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>419</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>418</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>416</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1086,72 +1086,72 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$19:$C$27</c:f>
+              <c:f>Sheet1!$C$18:$C$26</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45901</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45894</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45887</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45880</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45873</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45866</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45859</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45852</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45845</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45838</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$19:$G$27</c:f>
+              <c:f>Sheet1!$G$18:$G$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>426</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>421</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>415</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>406</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>405</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>406</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>389</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>386</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>386</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>370</c:v>
+                  <c:v>386</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1286,8 +1286,8 @@
         <c:axId val="1374569007"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="460"/>
-          <c:min val="360"/>
+          <c:max val="470"/>
+          <c:min val="380"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1529,7 +1529,7 @@
                 <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
                 <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
               </a:rPr>
-              <a:t>(5</a:t>
+              <a:t>(9</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="zh-CN" altLang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
@@ -1555,7 +1555,7 @@
                 <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
                 <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
               </a:rPr>
-              <a:t>- 8</a:t>
+              <a:t>- 12</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="zh-CN" altLang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
@@ -1794,13 +1794,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>21</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>84</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4811,8 +4811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B97" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="R107" sqref="R107"/>
+    <sheetView tabSelected="1" topLeftCell="C99" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="L99" sqref="L99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -4836,7 +4836,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>21</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
@@ -4844,7 +4844,7 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
@@ -4852,7 +4852,21 @@
         <v>4</v>
       </c>
       <c r="C7">
-        <v>84</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C18" s="1">
+        <v>45901</v>
+      </c>
+      <c r="D18">
+        <v>465</v>
+      </c>
+      <c r="F18" s="1">
+        <v>45901</v>
+      </c>
+      <c r="G18">
+        <v>426</v>
       </c>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
LGHUB 2025/9/5 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
- 网站错误 & 本地化问题详见 LGHUB/WebLoc/README.md
</commit_message>
<xml_diff>
--- a/Documents/Graph_PC.xlsx
+++ b/Documents/Graph_PC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29221"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CC8225C-5BDC-409A-8515-F1A53346920D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D37339B-9B19-4426-9F69-9357A87EDFEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="2" r:id="rId1"/>
@@ -574,10 +574,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>6</c:v>
@@ -958,7 +958,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>465</c:v>
+                  <c:v>471</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>456</c:v>
@@ -1286,7 +1286,7 @@
         <c:axId val="1374569007"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="470"/>
+          <c:max val="480"/>
           <c:min val="380"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1794,10 +1794,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>6</c:v>
@@ -4811,43 +4811,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C99" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="L99" sqref="L99"/>
+    <sheetView tabSelected="1" topLeftCell="D97" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K99" sqref="K99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>4</v>
       </c>
@@ -4855,12 +4855,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C18" s="1">
         <v>45901</v>
       </c>
       <c r="D18">
-        <v>465</v>
+        <v>471</v>
       </c>
       <c r="F18" s="1">
         <v>45901</v>
@@ -4869,7 +4869,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C19" s="1">
         <v>45894</v>
       </c>
@@ -4883,7 +4883,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C20" s="1">
         <v>45887</v>
       </c>
@@ -4897,7 +4897,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C21" s="1">
         <v>45880</v>
       </c>
@@ -4911,7 +4911,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C22" s="1">
         <v>45873</v>
       </c>
@@ -4925,7 +4925,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C23" s="1">
         <v>45866</v>
       </c>
@@ -4939,7 +4939,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C24" s="1">
         <v>45859</v>
       </c>
@@ -4953,7 +4953,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C25" s="1">
         <v>45852</v>
       </c>
@@ -4967,7 +4967,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C26" s="1">
         <v>45845</v>
       </c>
@@ -4981,7 +4981,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C27" s="1">
         <v>45838</v>
       </c>
@@ -4995,7 +4995,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C28" s="1">
         <v>45831</v>
       </c>
@@ -5009,7 +5009,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C29" s="1">
         <v>45824</v>
       </c>
@@ -5023,7 +5023,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C30" s="1">
         <v>45817</v>
       </c>
@@ -5037,7 +5037,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C31" s="1">
         <v>45810</v>
       </c>
@@ -5051,7 +5051,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C32" s="1">
         <v>45803</v>
       </c>
@@ -5065,7 +5065,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C33" s="1">
         <v>45796</v>
       </c>
@@ -5079,7 +5079,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C34" s="1">
         <v>45789</v>
       </c>
@@ -5093,7 +5093,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C35" s="1">
         <v>45782</v>
       </c>
@@ -5107,7 +5107,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C36" s="1">
         <v>45775</v>
       </c>
@@ -5121,7 +5121,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="37" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C37" s="1">
         <v>45768</v>
       </c>
@@ -5135,7 +5135,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="38" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C38" s="1">
         <v>45761</v>
       </c>
@@ -5149,7 +5149,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="39" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C39" s="1">
         <v>45754</v>
       </c>
@@ -5163,7 +5163,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="40" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C40" s="1">
         <v>45747</v>
       </c>
@@ -5177,7 +5177,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="41" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C41" s="1">
         <v>45740</v>
       </c>
@@ -5191,7 +5191,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="42" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C42" s="1">
         <v>45733</v>
       </c>
@@ -5205,7 +5205,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="43" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C43" s="1">
         <v>45726</v>
       </c>
@@ -5219,7 +5219,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="44" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C44" s="1">
         <v>45719</v>
       </c>
@@ -5233,7 +5233,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="45" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C45" s="1">
         <v>45712</v>
       </c>
@@ -5247,7 +5247,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="46" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C46" s="1">
         <v>45705</v>
       </c>
@@ -5261,7 +5261,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="47" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C47" s="1">
         <v>45698</v>
       </c>
@@ -5275,7 +5275,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="48" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C48" s="1">
         <v>45691</v>
       </c>
@@ -5289,7 +5289,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="49" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C49" s="1">
         <v>45684</v>
       </c>
@@ -5303,7 +5303,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="50" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C50" s="1">
         <v>45677</v>
       </c>
@@ -5317,7 +5317,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="51" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C51" s="1">
         <v>45670</v>
       </c>
@@ -5331,7 +5331,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="52" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C52" s="1">
         <v>45663</v>
       </c>
@@ -5345,7 +5345,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="53" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C53" s="1">
         <v>45642</v>
       </c>
@@ -5359,7 +5359,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="54" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C54" s="1">
         <v>45635</v>
       </c>
@@ -5373,7 +5373,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="55" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C55" s="1">
         <v>45628</v>
       </c>
@@ -5387,7 +5387,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="56" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C56" s="1">
         <v>45621</v>
       </c>
@@ -5401,7 +5401,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="57" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C57" s="1">
         <v>45614</v>
       </c>
@@ -5415,7 +5415,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="58" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C58" s="1">
         <v>45607</v>
       </c>
@@ -5429,7 +5429,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="59" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C59" s="1">
         <v>45600</v>
       </c>
@@ -5443,7 +5443,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="60" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C60" s="1">
         <v>45579</v>
       </c>
@@ -5457,7 +5457,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="61" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C61" s="1">
         <v>45572</v>
       </c>
@@ -5471,7 +5471,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="62" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C62" s="1">
         <v>45565</v>
       </c>
@@ -5485,7 +5485,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="63" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C63" s="1">
         <v>45537</v>
       </c>
@@ -5499,7 +5499,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="64" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C64" s="1">
         <v>45530</v>
       </c>
@@ -5513,7 +5513,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="65" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C65" s="1">
         <v>45523</v>
       </c>
@@ -5527,7 +5527,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="66" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C66" s="1">
         <v>45516</v>
       </c>
@@ -5541,7 +5541,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="67" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C67" s="1">
         <v>45509</v>
       </c>
@@ -5555,7 +5555,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="68" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C68" s="1">
         <v>45502</v>
       </c>
@@ -5569,7 +5569,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="69" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C69" s="1">
         <v>45495</v>
       </c>
@@ -5583,7 +5583,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="70" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C70" s="1">
         <v>45488</v>
       </c>
@@ -5597,7 +5597,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="71" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C71" s="1">
         <v>45481</v>
       </c>
@@ -5611,7 +5611,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="72" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C72" s="1">
         <v>45474</v>
       </c>
@@ -5625,7 +5625,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="73" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C73" s="1">
         <v>45467</v>
       </c>
@@ -5639,7 +5639,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="74" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C74" s="1">
         <v>45460</v>
       </c>
@@ -5653,7 +5653,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="75" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C75" s="1">
         <v>45453</v>
       </c>
@@ -5667,7 +5667,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="76" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C76" s="1">
         <v>45446</v>
       </c>
@@ -5681,7 +5681,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="77" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C77" s="1">
         <v>45439</v>
       </c>
@@ -5695,7 +5695,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="78" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C78" s="1">
         <v>45432</v>
       </c>
@@ -5709,7 +5709,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="79" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C79" s="1">
         <v>45425</v>
       </c>
@@ -5723,7 +5723,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="80" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C80" s="1">
         <v>45418</v>
       </c>
@@ -5737,7 +5737,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="81" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C81" s="1">
         <v>45411</v>
       </c>
@@ -5751,7 +5751,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="82" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C82" s="1">
         <v>45404</v>
       </c>
@@ -5765,7 +5765,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="83" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C83" s="1">
         <v>45397</v>
       </c>
@@ -5779,7 +5779,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="84" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C84" s="1">
         <v>45390</v>
       </c>
@@ -5793,7 +5793,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="85" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C85" s="1">
         <v>45383</v>
       </c>
@@ -5807,7 +5807,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="86" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C86" s="1">
         <v>45376</v>
       </c>
@@ -5821,7 +5821,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="87" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C87" s="1">
         <v>45369</v>
       </c>
@@ -5835,7 +5835,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="88" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C88" s="1">
         <v>45362</v>
       </c>
@@ -5844,7 +5844,7 @@
       </c>
       <c r="F88" s="1"/>
     </row>
-    <row r="89" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C89" s="1">
         <v>45355</v>
       </c>
@@ -5852,7 +5852,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="90" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C90" s="1">
         <v>45348</v>
       </c>
@@ -5860,7 +5860,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="91" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C91" s="1">
         <v>45341</v>
       </c>
@@ -5868,7 +5868,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="92" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C92" s="1">
         <v>45334</v>
       </c>
@@ -5876,7 +5876,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="93" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C93" s="1">
         <v>45327</v>
       </c>
@@ -5884,7 +5884,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="94" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C94" s="1">
         <v>45320</v>
       </c>
@@ -5892,7 +5892,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="95" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C95" s="1">
         <v>45313</v>
       </c>
@@ -5900,7 +5900,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="96" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C96" s="1">
         <v>45306</v>
       </c>
@@ -5908,7 +5908,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="100" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="100" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D100" s="2"/>
       <c r="E100" s="2"/>
       <c r="F100" s="2"/>
@@ -5924,7 +5924,7 @@
       <c r="P100" s="2"/>
       <c r="Q100" s="2"/>
     </row>
-    <row r="101" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="101" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D101" s="2"/>
       <c r="E101" s="2"/>
       <c r="F101" s="2"/>
@@ -5940,7 +5940,7 @@
       <c r="P101" s="2"/>
       <c r="Q101" s="2"/>
     </row>
-    <row r="102" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="102" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D102" s="2"/>
       <c r="E102" s="2"/>
       <c r="F102" s="2"/>
@@ -5956,7 +5956,7 @@
       <c r="P102" s="2"/>
       <c r="Q102" s="2"/>
     </row>
-    <row r="103" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="103" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D103" s="2"/>
       <c r="E103" s="2"/>
       <c r="F103" s="2"/>
@@ -5972,7 +5972,7 @@
       <c r="P103" s="2"/>
       <c r="Q103" s="2"/>
     </row>
-    <row r="104" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="104" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D104" s="2"/>
       <c r="E104" s="2"/>
       <c r="F104" s="2"/>
@@ -5988,7 +5988,7 @@
       <c r="P104" s="2"/>
       <c r="Q104" s="2"/>
     </row>
-    <row r="105" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="105" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D105" s="2"/>
       <c r="E105" s="2"/>
       <c r="F105" s="2"/>
@@ -6004,7 +6004,7 @@
       <c r="P105" s="2"/>
       <c r="Q105" s="2"/>
     </row>
-    <row r="106" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="106" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D106" s="2"/>
       <c r="E106" s="2"/>
       <c r="F106" s="2"/>
@@ -6020,7 +6020,7 @@
       <c r="P106" s="2"/>
       <c r="Q106" s="2"/>
     </row>
-    <row r="107" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="107" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D107" s="2"/>
       <c r="E107" s="2"/>
       <c r="F107" s="2"/>
@@ -6036,7 +6036,7 @@
       <c r="P107" s="2"/>
       <c r="Q107" s="2"/>
     </row>
-    <row r="108" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="108" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D108" s="2"/>
       <c r="E108" s="2"/>
       <c r="F108" s="2"/>
@@ -6052,7 +6052,7 @@
       <c r="P108" s="2"/>
       <c r="Q108" s="2"/>
     </row>
-    <row r="109" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="109" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D109" s="2"/>
       <c r="E109" s="2"/>
       <c r="F109" s="2"/>
@@ -6068,7 +6068,7 @@
       <c r="P109" s="2"/>
       <c r="Q109" s="2"/>
     </row>
-    <row r="110" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="110" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D110" s="2"/>
       <c r="E110" s="2"/>
       <c r="F110" s="2"/>
@@ -6084,7 +6084,7 @@
       <c r="P110" s="2"/>
       <c r="Q110" s="2"/>
     </row>
-    <row r="111" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="111" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D111" s="2"/>
       <c r="E111" s="2"/>
       <c r="F111" s="2"/>
@@ -6100,7 +6100,7 @@
       <c r="P111" s="2"/>
       <c r="Q111" s="2"/>
     </row>
-    <row r="112" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="112" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D112" s="2"/>
       <c r="E112" s="2"/>
       <c r="F112" s="2"/>
@@ -6116,7 +6116,7 @@
       <c r="P112" s="2"/>
       <c r="Q112" s="2"/>
     </row>
-    <row r="113" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="113" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D113" s="2"/>
       <c r="E113" s="2"/>
       <c r="F113" s="2"/>
@@ -6132,7 +6132,7 @@
       <c r="P113" s="2"/>
       <c r="Q113" s="2"/>
     </row>
-    <row r="114" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="114" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D114" s="2"/>
       <c r="E114" s="2"/>
       <c r="F114" s="2"/>
@@ -6148,7 +6148,7 @@
       <c r="P114" s="2"/>
       <c r="Q114" s="2"/>
     </row>
-    <row r="115" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="115" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D115" s="2"/>
       <c r="E115" s="2"/>
       <c r="F115" s="2"/>
@@ -6164,7 +6164,7 @@
       <c r="P115" s="2"/>
       <c r="Q115" s="2"/>
     </row>
-    <row r="116" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="116" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D116" s="2"/>
       <c r="E116" s="2"/>
       <c r="F116" s="2"/>
@@ -6180,7 +6180,7 @@
       <c r="P116" s="2"/>
       <c r="Q116" s="2"/>
     </row>
-    <row r="117" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="117" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D117" s="2"/>
       <c r="E117" s="2"/>
       <c r="F117" s="2"/>
@@ -6196,7 +6196,7 @@
       <c r="P117" s="2"/>
       <c r="Q117" s="2"/>
     </row>
-    <row r="118" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="118" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D118" s="2"/>
       <c r="E118" s="2"/>
       <c r="F118" s="2"/>
@@ -6212,7 +6212,7 @@
       <c r="P118" s="2"/>
       <c r="Q118" s="2"/>
     </row>
-    <row r="119" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="119" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D119" s="2"/>
       <c r="E119" s="2"/>
       <c r="F119" s="2"/>
@@ -6228,7 +6228,7 @@
       <c r="P119" s="2"/>
       <c r="Q119" s="2"/>
     </row>
-    <row r="120" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="120" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D120" s="2"/>
       <c r="E120" s="2"/>
       <c r="F120" s="2"/>
@@ -6244,7 +6244,7 @@
       <c r="P120" s="2"/>
       <c r="Q120" s="2"/>
     </row>
-    <row r="121" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="121" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D121" s="2"/>
       <c r="E121" s="2"/>
       <c r="F121" s="2"/>
@@ -6260,7 +6260,7 @@
       <c r="P121" s="2"/>
       <c r="Q121" s="2"/>
     </row>
-    <row r="122" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="122" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D122" s="2"/>
       <c r="E122" s="2"/>
       <c r="F122" s="2"/>
@@ -6276,7 +6276,7 @@
       <c r="P122" s="2"/>
       <c r="Q122" s="2"/>
     </row>
-    <row r="123" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="123" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D123" s="2"/>
       <c r="E123" s="2"/>
       <c r="F123" s="2"/>
@@ -6292,7 +6292,7 @@
       <c r="P123" s="2"/>
       <c r="Q123" s="2"/>
     </row>
-    <row r="124" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="124" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D124" s="2"/>
       <c r="E124" s="2"/>
       <c r="F124" s="2"/>
@@ -6308,7 +6308,7 @@
       <c r="P124" s="2"/>
       <c r="Q124" s="2"/>
     </row>
-    <row r="125" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="125" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D125" s="2"/>
       <c r="E125" s="2"/>
       <c r="F125" s="2"/>

</xml_diff>

<commit_message>
LGHUB 2025/9/8 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
- 网站错误 & 本地化问题详见 LGHUB/WebLoc/README.md
</commit_message>
<xml_diff>
--- a/Documents/Graph_PC.xlsx
+++ b/Documents/Graph_PC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29230"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D37339B-9B19-4426-9F69-9357A87EDFEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AB41DDC-9024-4F47-A98F-994A9DDC32F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="2" r:id="rId1"/>
@@ -574,7 +574,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>9</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>6</c:v>
@@ -917,72 +917,72 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$18:$C$26</c:f>
+              <c:f>Sheet1!$C$17:$C$25</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45908</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45901</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45894</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45887</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45880</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45873</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45866</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45859</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45852</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45845</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$18:$D$26</c:f>
+              <c:f>Sheet1!$D$17:$D$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>477</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>471</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>456</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>446</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>443</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>440</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>432</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>430</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>419</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>418</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1086,43 +1086,43 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$18:$C$26</c:f>
+              <c:f>Sheet1!$C$17:$C$25</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45908</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45901</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45894</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45887</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45880</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45873</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45866</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45859</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45852</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45845</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$18:$G$26</c:f>
+              <c:f>Sheet1!$G$17:$G$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1130,25 +1130,25 @@
                   <c:v>426</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>426</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>421</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>415</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>406</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>405</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>406</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>389</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>386</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>386</c:v>
@@ -1794,7 +1794,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>9</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>6</c:v>
@@ -4811,35 +4811,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D97" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C99" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="K99" sqref="K99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -4847,7 +4847,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>4</v>
       </c>
@@ -4855,7 +4855,21 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C17" s="1">
+        <v>45908</v>
+      </c>
+      <c r="D17">
+        <v>477</v>
+      </c>
+      <c r="F17" s="1">
+        <v>45908</v>
+      </c>
+      <c r="G17">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C18" s="1">
         <v>45901</v>
       </c>
@@ -4869,7 +4883,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C19" s="1">
         <v>45894</v>
       </c>
@@ -4883,7 +4897,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C20" s="1">
         <v>45887</v>
       </c>
@@ -4897,7 +4911,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C21" s="1">
         <v>45880</v>
       </c>
@@ -4911,7 +4925,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C22" s="1">
         <v>45873</v>
       </c>
@@ -4925,7 +4939,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C23" s="1">
         <v>45866</v>
       </c>
@@ -4939,7 +4953,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C24" s="1">
         <v>45859</v>
       </c>
@@ -4953,7 +4967,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C25" s="1">
         <v>45852</v>
       </c>
@@ -4967,7 +4981,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C26" s="1">
         <v>45845</v>
       </c>
@@ -4981,7 +4995,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C27" s="1">
         <v>45838</v>
       </c>
@@ -4995,7 +5009,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C28" s="1">
         <v>45831</v>
       </c>
@@ -5009,7 +5023,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C29" s="1">
         <v>45824</v>
       </c>
@@ -5023,7 +5037,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C30" s="1">
         <v>45817</v>
       </c>
@@ -5037,7 +5051,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C31" s="1">
         <v>45810</v>
       </c>
@@ -5051,7 +5065,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C32" s="1">
         <v>45803</v>
       </c>
@@ -5065,7 +5079,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C33" s="1">
         <v>45796</v>
       </c>
@@ -5079,7 +5093,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="34" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C34" s="1">
         <v>45789</v>
       </c>
@@ -5093,7 +5107,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="35" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C35" s="1">
         <v>45782</v>
       </c>
@@ -5107,7 +5121,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="36" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C36" s="1">
         <v>45775</v>
       </c>
@@ -5121,7 +5135,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="37" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C37" s="1">
         <v>45768</v>
       </c>
@@ -5135,7 +5149,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="38" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C38" s="1">
         <v>45761</v>
       </c>
@@ -5149,7 +5163,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="39" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C39" s="1">
         <v>45754</v>
       </c>
@@ -5163,7 +5177,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="40" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C40" s="1">
         <v>45747</v>
       </c>
@@ -5177,7 +5191,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="41" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C41" s="1">
         <v>45740</v>
       </c>
@@ -5191,7 +5205,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="42" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C42" s="1">
         <v>45733</v>
       </c>
@@ -5205,7 +5219,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="43" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C43" s="1">
         <v>45726</v>
       </c>
@@ -5219,7 +5233,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="44" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C44" s="1">
         <v>45719</v>
       </c>
@@ -5233,7 +5247,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="45" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C45" s="1">
         <v>45712</v>
       </c>
@@ -5247,7 +5261,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="46" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C46" s="1">
         <v>45705</v>
       </c>
@@ -5261,7 +5275,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="47" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C47" s="1">
         <v>45698</v>
       </c>
@@ -5275,7 +5289,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="48" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C48" s="1">
         <v>45691</v>
       </c>
@@ -5289,7 +5303,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="49" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="49" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C49" s="1">
         <v>45684</v>
       </c>
@@ -5303,7 +5317,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="50" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="50" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C50" s="1">
         <v>45677</v>
       </c>
@@ -5317,7 +5331,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="51" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="51" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C51" s="1">
         <v>45670</v>
       </c>
@@ -5331,7 +5345,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="52" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="52" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C52" s="1">
         <v>45663</v>
       </c>
@@ -5345,7 +5359,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="53" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="53" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C53" s="1">
         <v>45642</v>
       </c>
@@ -5359,7 +5373,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="54" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="54" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C54" s="1">
         <v>45635</v>
       </c>
@@ -5373,7 +5387,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="55" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="55" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C55" s="1">
         <v>45628</v>
       </c>
@@ -5387,7 +5401,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="56" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="56" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C56" s="1">
         <v>45621</v>
       </c>
@@ -5401,7 +5415,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="57" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="57" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C57" s="1">
         <v>45614</v>
       </c>
@@ -5415,7 +5429,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="58" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="58" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C58" s="1">
         <v>45607</v>
       </c>
@@ -5429,7 +5443,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="59" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="59" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C59" s="1">
         <v>45600</v>
       </c>
@@ -5443,7 +5457,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="60" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="60" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C60" s="1">
         <v>45579</v>
       </c>
@@ -5457,7 +5471,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="61" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="61" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C61" s="1">
         <v>45572</v>
       </c>
@@ -5471,7 +5485,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="62" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="62" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C62" s="1">
         <v>45565</v>
       </c>
@@ -5485,7 +5499,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="63" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="63" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C63" s="1">
         <v>45537</v>
       </c>
@@ -5499,7 +5513,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="64" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="64" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C64" s="1">
         <v>45530</v>
       </c>
@@ -5513,7 +5527,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="65" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="65" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C65" s="1">
         <v>45523</v>
       </c>
@@ -5527,7 +5541,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="66" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="66" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C66" s="1">
         <v>45516</v>
       </c>
@@ -5541,7 +5555,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="67" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="67" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C67" s="1">
         <v>45509</v>
       </c>
@@ -5555,7 +5569,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="68" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="68" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C68" s="1">
         <v>45502</v>
       </c>
@@ -5569,7 +5583,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="69" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="69" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C69" s="1">
         <v>45495</v>
       </c>
@@ -5583,7 +5597,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="70" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="70" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C70" s="1">
         <v>45488</v>
       </c>
@@ -5597,7 +5611,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="71" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="71" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C71" s="1">
         <v>45481</v>
       </c>
@@ -5611,7 +5625,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="72" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="72" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C72" s="1">
         <v>45474</v>
       </c>
@@ -5625,7 +5639,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="73" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="73" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C73" s="1">
         <v>45467</v>
       </c>
@@ -5639,7 +5653,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="74" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="74" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C74" s="1">
         <v>45460</v>
       </c>
@@ -5653,7 +5667,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="75" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="75" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C75" s="1">
         <v>45453</v>
       </c>
@@ -5667,7 +5681,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="76" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="76" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C76" s="1">
         <v>45446</v>
       </c>
@@ -5681,7 +5695,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="77" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="77" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C77" s="1">
         <v>45439</v>
       </c>
@@ -5695,7 +5709,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="78" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="78" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C78" s="1">
         <v>45432</v>
       </c>
@@ -5709,7 +5723,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="79" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="79" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C79" s="1">
         <v>45425</v>
       </c>
@@ -5723,7 +5737,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="80" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="80" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C80" s="1">
         <v>45418</v>
       </c>
@@ -5737,7 +5751,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="81" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="81" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C81" s="1">
         <v>45411</v>
       </c>
@@ -5751,7 +5765,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="82" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="82" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C82" s="1">
         <v>45404</v>
       </c>
@@ -5765,7 +5779,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="83" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="83" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C83" s="1">
         <v>45397</v>
       </c>
@@ -5779,7 +5793,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="84" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="84" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C84" s="1">
         <v>45390</v>
       </c>
@@ -5793,7 +5807,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="85" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="85" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C85" s="1">
         <v>45383</v>
       </c>
@@ -5807,7 +5821,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="86" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="86" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C86" s="1">
         <v>45376</v>
       </c>
@@ -5821,7 +5835,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="87" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="87" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C87" s="1">
         <v>45369</v>
       </c>
@@ -5835,7 +5849,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="88" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="88" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C88" s="1">
         <v>45362</v>
       </c>
@@ -5844,7 +5858,7 @@
       </c>
       <c r="F88" s="1"/>
     </row>
-    <row r="89" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="89" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C89" s="1">
         <v>45355</v>
       </c>
@@ -5852,7 +5866,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="90" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="90" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C90" s="1">
         <v>45348</v>
       </c>
@@ -5860,7 +5874,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="91" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="91" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C91" s="1">
         <v>45341</v>
       </c>
@@ -5868,7 +5882,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="92" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="92" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C92" s="1">
         <v>45334</v>
       </c>
@@ -5876,7 +5890,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="93" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="93" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C93" s="1">
         <v>45327</v>
       </c>
@@ -5884,7 +5898,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="94" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="94" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C94" s="1">
         <v>45320</v>
       </c>
@@ -5892,7 +5906,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="95" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="95" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C95" s="1">
         <v>45313</v>
       </c>
@@ -5900,7 +5914,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="96" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="96" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C96" s="1">
         <v>45306</v>
       </c>
@@ -5908,7 +5922,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="100" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="100" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D100" s="2"/>
       <c r="E100" s="2"/>
       <c r="F100" s="2"/>
@@ -5924,7 +5938,7 @@
       <c r="P100" s="2"/>
       <c r="Q100" s="2"/>
     </row>
-    <row r="101" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="101" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D101" s="2"/>
       <c r="E101" s="2"/>
       <c r="F101" s="2"/>
@@ -5940,7 +5954,7 @@
       <c r="P101" s="2"/>
       <c r="Q101" s="2"/>
     </row>
-    <row r="102" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="102" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D102" s="2"/>
       <c r="E102" s="2"/>
       <c r="F102" s="2"/>
@@ -5956,7 +5970,7 @@
       <c r="P102" s="2"/>
       <c r="Q102" s="2"/>
     </row>
-    <row r="103" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="103" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D103" s="2"/>
       <c r="E103" s="2"/>
       <c r="F103" s="2"/>
@@ -5972,7 +5986,7 @@
       <c r="P103" s="2"/>
       <c r="Q103" s="2"/>
     </row>
-    <row r="104" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="104" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D104" s="2"/>
       <c r="E104" s="2"/>
       <c r="F104" s="2"/>
@@ -5988,7 +6002,7 @@
       <c r="P104" s="2"/>
       <c r="Q104" s="2"/>
     </row>
-    <row r="105" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="105" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D105" s="2"/>
       <c r="E105" s="2"/>
       <c r="F105" s="2"/>
@@ -6004,7 +6018,7 @@
       <c r="P105" s="2"/>
       <c r="Q105" s="2"/>
     </row>
-    <row r="106" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="106" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D106" s="2"/>
       <c r="E106" s="2"/>
       <c r="F106" s="2"/>
@@ -6020,7 +6034,7 @@
       <c r="P106" s="2"/>
       <c r="Q106" s="2"/>
     </row>
-    <row r="107" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="107" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D107" s="2"/>
       <c r="E107" s="2"/>
       <c r="F107" s="2"/>
@@ -6036,7 +6050,7 @@
       <c r="P107" s="2"/>
       <c r="Q107" s="2"/>
     </row>
-    <row r="108" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="108" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D108" s="2"/>
       <c r="E108" s="2"/>
       <c r="F108" s="2"/>
@@ -6052,7 +6066,7 @@
       <c r="P108" s="2"/>
       <c r="Q108" s="2"/>
     </row>
-    <row r="109" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="109" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D109" s="2"/>
       <c r="E109" s="2"/>
       <c r="F109" s="2"/>
@@ -6068,7 +6082,7 @@
       <c r="P109" s="2"/>
       <c r="Q109" s="2"/>
     </row>
-    <row r="110" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="110" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D110" s="2"/>
       <c r="E110" s="2"/>
       <c r="F110" s="2"/>
@@ -6084,7 +6098,7 @@
       <c r="P110" s="2"/>
       <c r="Q110" s="2"/>
     </row>
-    <row r="111" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="111" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D111" s="2"/>
       <c r="E111" s="2"/>
       <c r="F111" s="2"/>
@@ -6100,7 +6114,7 @@
       <c r="P111" s="2"/>
       <c r="Q111" s="2"/>
     </row>
-    <row r="112" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="112" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D112" s="2"/>
       <c r="E112" s="2"/>
       <c r="F112" s="2"/>
@@ -6116,7 +6130,7 @@
       <c r="P112" s="2"/>
       <c r="Q112" s="2"/>
     </row>
-    <row r="113" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="113" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D113" s="2"/>
       <c r="E113" s="2"/>
       <c r="F113" s="2"/>
@@ -6132,7 +6146,7 @@
       <c r="P113" s="2"/>
       <c r="Q113" s="2"/>
     </row>
-    <row r="114" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="114" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D114" s="2"/>
       <c r="E114" s="2"/>
       <c r="F114" s="2"/>
@@ -6148,7 +6162,7 @@
       <c r="P114" s="2"/>
       <c r="Q114" s="2"/>
     </row>
-    <row r="115" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="115" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D115" s="2"/>
       <c r="E115" s="2"/>
       <c r="F115" s="2"/>
@@ -6164,7 +6178,7 @@
       <c r="P115" s="2"/>
       <c r="Q115" s="2"/>
     </row>
-    <row r="116" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="116" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D116" s="2"/>
       <c r="E116" s="2"/>
       <c r="F116" s="2"/>
@@ -6180,7 +6194,7 @@
       <c r="P116" s="2"/>
       <c r="Q116" s="2"/>
     </row>
-    <row r="117" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="117" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D117" s="2"/>
       <c r="E117" s="2"/>
       <c r="F117" s="2"/>
@@ -6196,7 +6210,7 @@
       <c r="P117" s="2"/>
       <c r="Q117" s="2"/>
     </row>
-    <row r="118" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="118" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D118" s="2"/>
       <c r="E118" s="2"/>
       <c r="F118" s="2"/>
@@ -6212,7 +6226,7 @@
       <c r="P118" s="2"/>
       <c r="Q118" s="2"/>
     </row>
-    <row r="119" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="119" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D119" s="2"/>
       <c r="E119" s="2"/>
       <c r="F119" s="2"/>
@@ -6228,7 +6242,7 @@
       <c r="P119" s="2"/>
       <c r="Q119" s="2"/>
     </row>
-    <row r="120" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="120" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D120" s="2"/>
       <c r="E120" s="2"/>
       <c r="F120" s="2"/>
@@ -6244,7 +6258,7 @@
       <c r="P120" s="2"/>
       <c r="Q120" s="2"/>
     </row>
-    <row r="121" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="121" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D121" s="2"/>
       <c r="E121" s="2"/>
       <c r="F121" s="2"/>
@@ -6260,7 +6274,7 @@
       <c r="P121" s="2"/>
       <c r="Q121" s="2"/>
     </row>
-    <row r="122" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="122" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D122" s="2"/>
       <c r="E122" s="2"/>
       <c r="F122" s="2"/>
@@ -6276,7 +6290,7 @@
       <c r="P122" s="2"/>
       <c r="Q122" s="2"/>
     </row>
-    <row r="123" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="123" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D123" s="2"/>
       <c r="E123" s="2"/>
       <c r="F123" s="2"/>
@@ -6292,7 +6306,7 @@
       <c r="P123" s="2"/>
       <c r="Q123" s="2"/>
     </row>
-    <row r="124" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="124" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D124" s="2"/>
       <c r="E124" s="2"/>
       <c r="F124" s="2"/>
@@ -6308,7 +6322,7 @@
       <c r="P124" s="2"/>
       <c r="Q124" s="2"/>
     </row>
-    <row r="125" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="125" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D125" s="2"/>
       <c r="E125" s="2"/>
       <c r="F125" s="2"/>

</xml_diff>

<commit_message>
LGHUB 2025/9/9 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
- 网站错误 & 本地化问题详见 LGHUB/WebLoc/README.md
</commit_message>
<xml_diff>
--- a/Documents/Graph_PC.xlsx
+++ b/Documents/Graph_PC.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29230"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AB41DDC-9024-4F47-A98F-994A9DDC32F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55D77131-C848-410A-90D9-363A9A1629BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,13 +574,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>15</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -958,7 +958,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>477</c:v>
+                  <c:v>481</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>471</c:v>
@@ -1127,7 +1127,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>426</c:v>
+                  <c:v>439</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>426</c:v>
@@ -1286,7 +1286,7 @@
         <c:axId val="1374569007"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="480"/>
+          <c:max val="490"/>
           <c:min val="380"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1794,13 +1794,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>15</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4811,8 +4811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C99" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="K99" sqref="K99"/>
+    <sheetView tabSelected="1" topLeftCell="C100" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="L99" sqref="L99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -4836,7 +4836,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
@@ -4844,7 +4844,7 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
@@ -4852,7 +4852,7 @@
         <v>4</v>
       </c>
       <c r="C7">
-        <v>6</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.25">
@@ -4860,13 +4860,13 @@
         <v>45908</v>
       </c>
       <c r="D17">
-        <v>477</v>
+        <v>481</v>
       </c>
       <c r="F17" s="1">
         <v>45908</v>
       </c>
       <c r="G17">
-        <v>426</v>
+        <v>439</v>
       </c>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
LGHUB 2025/9/13 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
- 网站错误 & 本地化问题详见 LGHUB/WebLoc/README.md
</commit_message>
<xml_diff>
--- a/Documents/Graph_PC.xlsx
+++ b/Documents/Graph_PC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55D77131-C848-410A-90D9-363A9A1629BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F0B2C58-DCEF-49F2-9A2E-D8976985E348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="2" r:id="rId1"/>
@@ -577,10 +577,10 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -958,7 +958,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>481</c:v>
+                  <c:v>485</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>471</c:v>
@@ -1127,7 +1127,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>439</c:v>
+                  <c:v>444</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>426</c:v>
@@ -1797,10 +1797,10 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4811,27 +4811,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C100" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D99" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="L99" sqref="L99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -4839,37 +4839,37 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C17" s="1">
         <v>45908</v>
       </c>
       <c r="D17">
-        <v>481</v>
+        <v>485</v>
       </c>
       <c r="F17" s="1">
         <v>45908</v>
       </c>
       <c r="G17">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C18" s="1">
         <v>45901</v>
       </c>
@@ -4883,7 +4883,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C19" s="1">
         <v>45894</v>
       </c>
@@ -4897,7 +4897,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C20" s="1">
         <v>45887</v>
       </c>
@@ -4911,7 +4911,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C21" s="1">
         <v>45880</v>
       </c>
@@ -4925,7 +4925,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C22" s="1">
         <v>45873</v>
       </c>
@@ -4939,7 +4939,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C23" s="1">
         <v>45866</v>
       </c>
@@ -4953,7 +4953,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C24" s="1">
         <v>45859</v>
       </c>
@@ -4967,7 +4967,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C25" s="1">
         <v>45852</v>
       </c>
@@ -4981,7 +4981,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C26" s="1">
         <v>45845</v>
       </c>
@@ -4995,7 +4995,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C27" s="1">
         <v>45838</v>
       </c>
@@ -5009,7 +5009,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C28" s="1">
         <v>45831</v>
       </c>
@@ -5023,7 +5023,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C29" s="1">
         <v>45824</v>
       </c>
@@ -5037,7 +5037,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C30" s="1">
         <v>45817</v>
       </c>
@@ -5051,7 +5051,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C31" s="1">
         <v>45810</v>
       </c>
@@ -5065,7 +5065,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C32" s="1">
         <v>45803</v>
       </c>
@@ -5079,7 +5079,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C33" s="1">
         <v>45796</v>
       </c>
@@ -5093,7 +5093,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C34" s="1">
         <v>45789</v>
       </c>
@@ -5107,7 +5107,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C35" s="1">
         <v>45782</v>
       </c>
@@ -5121,7 +5121,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C36" s="1">
         <v>45775</v>
       </c>
@@ -5135,7 +5135,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="37" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C37" s="1">
         <v>45768</v>
       </c>
@@ -5149,7 +5149,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="38" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C38" s="1">
         <v>45761</v>
       </c>
@@ -5163,7 +5163,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="39" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C39" s="1">
         <v>45754</v>
       </c>
@@ -5177,7 +5177,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="40" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C40" s="1">
         <v>45747</v>
       </c>
@@ -5191,7 +5191,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="41" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C41" s="1">
         <v>45740</v>
       </c>
@@ -5205,7 +5205,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="42" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C42" s="1">
         <v>45733</v>
       </c>
@@ -5219,7 +5219,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="43" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C43" s="1">
         <v>45726</v>
       </c>
@@ -5233,7 +5233,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="44" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C44" s="1">
         <v>45719</v>
       </c>
@@ -5247,7 +5247,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="45" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C45" s="1">
         <v>45712</v>
       </c>
@@ -5261,7 +5261,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="46" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C46" s="1">
         <v>45705</v>
       </c>
@@ -5275,7 +5275,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="47" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C47" s="1">
         <v>45698</v>
       </c>
@@ -5289,7 +5289,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="48" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C48" s="1">
         <v>45691</v>
       </c>
@@ -5303,7 +5303,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="49" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C49" s="1">
         <v>45684</v>
       </c>
@@ -5317,7 +5317,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="50" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C50" s="1">
         <v>45677</v>
       </c>
@@ -5331,7 +5331,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="51" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C51" s="1">
         <v>45670</v>
       </c>
@@ -5345,7 +5345,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="52" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C52" s="1">
         <v>45663</v>
       </c>
@@ -5359,7 +5359,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="53" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C53" s="1">
         <v>45642</v>
       </c>
@@ -5373,7 +5373,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="54" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C54" s="1">
         <v>45635</v>
       </c>
@@ -5387,7 +5387,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="55" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C55" s="1">
         <v>45628</v>
       </c>
@@ -5401,7 +5401,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="56" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C56" s="1">
         <v>45621</v>
       </c>
@@ -5415,7 +5415,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="57" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C57" s="1">
         <v>45614</v>
       </c>
@@ -5429,7 +5429,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="58" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C58" s="1">
         <v>45607</v>
       </c>
@@ -5443,7 +5443,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="59" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C59" s="1">
         <v>45600</v>
       </c>
@@ -5457,7 +5457,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="60" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C60" s="1">
         <v>45579</v>
       </c>
@@ -5471,7 +5471,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="61" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C61" s="1">
         <v>45572</v>
       </c>
@@ -5485,7 +5485,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="62" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C62" s="1">
         <v>45565</v>
       </c>
@@ -5499,7 +5499,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="63" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C63" s="1">
         <v>45537</v>
       </c>
@@ -5513,7 +5513,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="64" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C64" s="1">
         <v>45530</v>
       </c>
@@ -5527,7 +5527,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="65" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C65" s="1">
         <v>45523</v>
       </c>
@@ -5541,7 +5541,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="66" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C66" s="1">
         <v>45516</v>
       </c>
@@ -5555,7 +5555,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="67" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C67" s="1">
         <v>45509</v>
       </c>
@@ -5569,7 +5569,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="68" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C68" s="1">
         <v>45502</v>
       </c>
@@ -5583,7 +5583,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="69" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C69" s="1">
         <v>45495</v>
       </c>
@@ -5597,7 +5597,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="70" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C70" s="1">
         <v>45488</v>
       </c>
@@ -5611,7 +5611,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="71" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C71" s="1">
         <v>45481</v>
       </c>
@@ -5625,7 +5625,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="72" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C72" s="1">
         <v>45474</v>
       </c>
@@ -5639,7 +5639,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="73" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C73" s="1">
         <v>45467</v>
       </c>
@@ -5653,7 +5653,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="74" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C74" s="1">
         <v>45460</v>
       </c>
@@ -5667,7 +5667,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="75" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C75" s="1">
         <v>45453</v>
       </c>
@@ -5681,7 +5681,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="76" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C76" s="1">
         <v>45446</v>
       </c>
@@ -5695,7 +5695,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="77" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C77" s="1">
         <v>45439</v>
       </c>
@@ -5709,7 +5709,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="78" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C78" s="1">
         <v>45432</v>
       </c>
@@ -5723,7 +5723,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="79" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C79" s="1">
         <v>45425</v>
       </c>
@@ -5737,7 +5737,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="80" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C80" s="1">
         <v>45418</v>
       </c>
@@ -5751,7 +5751,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="81" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C81" s="1">
         <v>45411</v>
       </c>
@@ -5765,7 +5765,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="82" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C82" s="1">
         <v>45404</v>
       </c>
@@ -5779,7 +5779,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="83" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C83" s="1">
         <v>45397</v>
       </c>
@@ -5793,7 +5793,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="84" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C84" s="1">
         <v>45390</v>
       </c>
@@ -5807,7 +5807,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="85" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C85" s="1">
         <v>45383</v>
       </c>
@@ -5821,7 +5821,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="86" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C86" s="1">
         <v>45376</v>
       </c>
@@ -5835,7 +5835,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="87" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C87" s="1">
         <v>45369</v>
       </c>
@@ -5849,7 +5849,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="88" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C88" s="1">
         <v>45362</v>
       </c>
@@ -5858,7 +5858,7 @@
       </c>
       <c r="F88" s="1"/>
     </row>
-    <row r="89" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C89" s="1">
         <v>45355</v>
       </c>
@@ -5866,7 +5866,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="90" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C90" s="1">
         <v>45348</v>
       </c>
@@ -5874,7 +5874,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="91" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C91" s="1">
         <v>45341</v>
       </c>
@@ -5882,7 +5882,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="92" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C92" s="1">
         <v>45334</v>
       </c>
@@ -5890,7 +5890,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="93" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C93" s="1">
         <v>45327</v>
       </c>
@@ -5898,7 +5898,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="94" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C94" s="1">
         <v>45320</v>
       </c>
@@ -5906,7 +5906,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="95" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C95" s="1">
         <v>45313</v>
       </c>
@@ -5914,7 +5914,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="96" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C96" s="1">
         <v>45306</v>
       </c>
@@ -5922,7 +5922,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="100" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="100" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D100" s="2"/>
       <c r="E100" s="2"/>
       <c r="F100" s="2"/>
@@ -5938,7 +5938,7 @@
       <c r="P100" s="2"/>
       <c r="Q100" s="2"/>
     </row>
-    <row r="101" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="101" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D101" s="2"/>
       <c r="E101" s="2"/>
       <c r="F101" s="2"/>
@@ -5954,7 +5954,7 @@
       <c r="P101" s="2"/>
       <c r="Q101" s="2"/>
     </row>
-    <row r="102" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="102" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D102" s="2"/>
       <c r="E102" s="2"/>
       <c r="F102" s="2"/>
@@ -5970,7 +5970,7 @@
       <c r="P102" s="2"/>
       <c r="Q102" s="2"/>
     </row>
-    <row r="103" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="103" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D103" s="2"/>
       <c r="E103" s="2"/>
       <c r="F103" s="2"/>
@@ -5986,7 +5986,7 @@
       <c r="P103" s="2"/>
       <c r="Q103" s="2"/>
     </row>
-    <row r="104" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="104" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D104" s="2"/>
       <c r="E104" s="2"/>
       <c r="F104" s="2"/>
@@ -6002,7 +6002,7 @@
       <c r="P104" s="2"/>
       <c r="Q104" s="2"/>
     </row>
-    <row r="105" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="105" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D105" s="2"/>
       <c r="E105" s="2"/>
       <c r="F105" s="2"/>
@@ -6018,7 +6018,7 @@
       <c r="P105" s="2"/>
       <c r="Q105" s="2"/>
     </row>
-    <row r="106" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="106" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D106" s="2"/>
       <c r="E106" s="2"/>
       <c r="F106" s="2"/>
@@ -6034,7 +6034,7 @@
       <c r="P106" s="2"/>
       <c r="Q106" s="2"/>
     </row>
-    <row r="107" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="107" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D107" s="2"/>
       <c r="E107" s="2"/>
       <c r="F107" s="2"/>
@@ -6050,7 +6050,7 @@
       <c r="P107" s="2"/>
       <c r="Q107" s="2"/>
     </row>
-    <row r="108" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="108" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D108" s="2"/>
       <c r="E108" s="2"/>
       <c r="F108" s="2"/>
@@ -6066,7 +6066,7 @@
       <c r="P108" s="2"/>
       <c r="Q108" s="2"/>
     </row>
-    <row r="109" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="109" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D109" s="2"/>
       <c r="E109" s="2"/>
       <c r="F109" s="2"/>
@@ -6082,7 +6082,7 @@
       <c r="P109" s="2"/>
       <c r="Q109" s="2"/>
     </row>
-    <row r="110" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="110" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D110" s="2"/>
       <c r="E110" s="2"/>
       <c r="F110" s="2"/>
@@ -6098,7 +6098,7 @@
       <c r="P110" s="2"/>
       <c r="Q110" s="2"/>
     </row>
-    <row r="111" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="111" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D111" s="2"/>
       <c r="E111" s="2"/>
       <c r="F111" s="2"/>
@@ -6114,7 +6114,7 @@
       <c r="P111" s="2"/>
       <c r="Q111" s="2"/>
     </row>
-    <row r="112" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="112" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D112" s="2"/>
       <c r="E112" s="2"/>
       <c r="F112" s="2"/>
@@ -6130,7 +6130,7 @@
       <c r="P112" s="2"/>
       <c r="Q112" s="2"/>
     </row>
-    <row r="113" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="113" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D113" s="2"/>
       <c r="E113" s="2"/>
       <c r="F113" s="2"/>
@@ -6146,7 +6146,7 @@
       <c r="P113" s="2"/>
       <c r="Q113" s="2"/>
     </row>
-    <row r="114" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="114" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D114" s="2"/>
       <c r="E114" s="2"/>
       <c r="F114" s="2"/>
@@ -6162,7 +6162,7 @@
       <c r="P114" s="2"/>
       <c r="Q114" s="2"/>
     </row>
-    <row r="115" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="115" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D115" s="2"/>
       <c r="E115" s="2"/>
       <c r="F115" s="2"/>
@@ -6178,7 +6178,7 @@
       <c r="P115" s="2"/>
       <c r="Q115" s="2"/>
     </row>
-    <row r="116" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="116" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D116" s="2"/>
       <c r="E116" s="2"/>
       <c r="F116" s="2"/>
@@ -6194,7 +6194,7 @@
       <c r="P116" s="2"/>
       <c r="Q116" s="2"/>
     </row>
-    <row r="117" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="117" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D117" s="2"/>
       <c r="E117" s="2"/>
       <c r="F117" s="2"/>
@@ -6210,7 +6210,7 @@
       <c r="P117" s="2"/>
       <c r="Q117" s="2"/>
     </row>
-    <row r="118" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="118" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D118" s="2"/>
       <c r="E118" s="2"/>
       <c r="F118" s="2"/>
@@ -6226,7 +6226,7 @@
       <c r="P118" s="2"/>
       <c r="Q118" s="2"/>
     </row>
-    <row r="119" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="119" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D119" s="2"/>
       <c r="E119" s="2"/>
       <c r="F119" s="2"/>
@@ -6242,7 +6242,7 @@
       <c r="P119" s="2"/>
       <c r="Q119" s="2"/>
     </row>
-    <row r="120" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="120" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D120" s="2"/>
       <c r="E120" s="2"/>
       <c r="F120" s="2"/>
@@ -6258,7 +6258,7 @@
       <c r="P120" s="2"/>
       <c r="Q120" s="2"/>
     </row>
-    <row r="121" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="121" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D121" s="2"/>
       <c r="E121" s="2"/>
       <c r="F121" s="2"/>
@@ -6274,7 +6274,7 @@
       <c r="P121" s="2"/>
       <c r="Q121" s="2"/>
     </row>
-    <row r="122" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="122" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D122" s="2"/>
       <c r="E122" s="2"/>
       <c r="F122" s="2"/>
@@ -6290,7 +6290,7 @@
       <c r="P122" s="2"/>
       <c r="Q122" s="2"/>
     </row>
-    <row r="123" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="123" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D123" s="2"/>
       <c r="E123" s="2"/>
       <c r="F123" s="2"/>
@@ -6306,7 +6306,7 @@
       <c r="P123" s="2"/>
       <c r="Q123" s="2"/>
     </row>
-    <row r="124" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="124" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D124" s="2"/>
       <c r="E124" s="2"/>
       <c r="F124" s="2"/>
@@ -6322,7 +6322,7 @@
       <c r="P124" s="2"/>
       <c r="Q124" s="2"/>
     </row>
-    <row r="125" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="125" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D125" s="2"/>
       <c r="E125" s="2"/>
       <c r="F125" s="2"/>

</xml_diff>

<commit_message>
LGHUB 2025/9/19 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
- 网站错误 & 本地化问题详见 LGHUB/WebLoc/README.md
</commit_message>
<xml_diff>
--- a/Documents/Graph_PC.xlsx
+++ b/Documents/Graph_PC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F0B2C58-DCEF-49F2-9A2E-D8976985E348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14DF824E-0FF0-4EB5-B163-F0CFD2BD9237}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,7 +574,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4</c:v>
@@ -917,72 +917,72 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$17:$C$25</c:f>
+              <c:f>Sheet1!$C$16:$C$24</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45915</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45908</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45901</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45894</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45887</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45880</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45873</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45866</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45859</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45852</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$17:$D$25</c:f>
+              <c:f>Sheet1!$D$16:$D$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>488</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>485</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>471</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>456</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>446</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>443</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>440</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>432</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>430</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>419</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1086,43 +1086,43 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$17:$C$25</c:f>
+              <c:f>Sheet1!$C$16:$C$24</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45915</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45908</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45901</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45894</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45887</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45880</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45873</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45866</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45859</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45852</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$17:$G$25</c:f>
+              <c:f>Sheet1!$G$16:$G$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1130,28 +1130,28 @@
                   <c:v>444</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>444</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>426</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>421</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>415</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>406</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>405</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>406</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>389</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>386</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1794,7 +1794,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4</c:v>
@@ -4811,8 +4811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D99" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L99" sqref="L99"/>
+    <sheetView tabSelected="1" topLeftCell="D97" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K99" sqref="K99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -4821,25 +4821,25 @@
     <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -4847,12 +4847,26 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7">
         <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C16" s="1">
+        <v>45915</v>
+      </c>
+      <c r="D16">
+        <v>488</v>
+      </c>
+      <c r="F16" s="1">
+        <v>45915</v>
+      </c>
+      <c r="G16">
+        <v>444</v>
       </c>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
LGHUB 2025/9/20 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
- 网站错误 & 本地化问题详见 LGHUB/WebLoc/README.md
</commit_message>
<xml_diff>
--- a/Documents/Graph_PC.xlsx
+++ b/Documents/Graph_PC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14DF824E-0FF0-4EB5-B163-F0CFD2BD9237}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52FA5F7D-8467-4CD0-95A4-F6B89B45E131}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,13 +574,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -917,7 +917,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$16:$C$24</c:f>
+              <c:f>Sheet1!$C$21:$C$29</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
@@ -953,7 +953,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$16:$D$24</c:f>
+              <c:f>Sheet1!$D$21:$D$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1086,7 +1086,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$16:$C$24</c:f>
+              <c:f>Sheet1!$C$21:$C$29</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1122,12 +1122,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$16:$G$24</c:f>
+              <c:f>Sheet1!$G$21:$G$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>444</c:v>
+                  <c:v>450</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>444</c:v>
@@ -1286,7 +1286,7 @@
         <c:axId val="1374569007"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="490"/>
+          <c:max val="500"/>
           <c:min val="380"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1794,13 +1794,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4223,13 +4223,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>106422</xdr:colOff>
-      <xdr:row>100</xdr:row>
+      <xdr:row>105</xdr:row>
       <xdr:rowOff>165023</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>115</xdr:row>
+      <xdr:row>120</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4259,13 +4259,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>190501</xdr:colOff>
-      <xdr:row>100</xdr:row>
+      <xdr:row>105</xdr:row>
       <xdr:rowOff>162248</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>124495</xdr:colOff>
-      <xdr:row>115</xdr:row>
+      <xdr:row>120</xdr:row>
       <xdr:rowOff>163286</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4809,10 +4809,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:Q125"/>
+  <dimension ref="B2:Q130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D97" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K99" sqref="K99"/>
+    <sheetView tabSelected="1" topLeftCell="D103" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L104" sqref="L104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -4821,1202 +4821,1122 @@
     <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C16" s="1">
-        <v>45915</v>
-      </c>
-      <c r="D16">
-        <v>488</v>
-      </c>
-      <c r="F16" s="1">
-        <v>45915</v>
-      </c>
-      <c r="G16">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C17" s="1">
-        <v>45908</v>
-      </c>
-      <c r="D17">
-        <v>485</v>
-      </c>
-      <c r="F17" s="1">
-        <v>45908</v>
-      </c>
-      <c r="G17">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C18" s="1">
-        <v>45901</v>
-      </c>
-      <c r="D18">
-        <v>471</v>
-      </c>
-      <c r="F18" s="1">
-        <v>45901</v>
-      </c>
-      <c r="G18">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C19" s="1">
-        <v>45894</v>
-      </c>
-      <c r="D19">
-        <v>456</v>
-      </c>
-      <c r="F19" s="1">
-        <v>45894</v>
-      </c>
-      <c r="G19">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C20" s="1">
-        <v>45887</v>
-      </c>
-      <c r="D20">
-        <v>446</v>
-      </c>
-      <c r="F20" s="1">
-        <v>45887</v>
-      </c>
-      <c r="G20">
-        <v>415</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C21" s="1">
-        <v>45880</v>
+        <v>45915</v>
       </c>
       <c r="D21">
-        <v>443</v>
+        <v>488</v>
       </c>
       <c r="F21" s="1">
-        <v>45880</v>
+        <v>45915</v>
       </c>
       <c r="G21">
-        <v>406</v>
+        <v>450</v>
       </c>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C22" s="1">
-        <v>45873</v>
+        <v>45908</v>
       </c>
       <c r="D22">
-        <v>440</v>
+        <v>485</v>
       </c>
       <c r="F22" s="1">
-        <v>45873</v>
+        <v>45908</v>
       </c>
       <c r="G22">
-        <v>405</v>
+        <v>444</v>
       </c>
     </row>
     <row r="23" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C23" s="1">
-        <v>45866</v>
+        <v>45901</v>
       </c>
       <c r="D23">
-        <v>432</v>
+        <v>471</v>
       </c>
       <c r="F23" s="1">
-        <v>45866</v>
+        <v>45901</v>
       </c>
       <c r="G23">
-        <v>406</v>
+        <v>426</v>
       </c>
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C24" s="1">
-        <v>45859</v>
+        <v>45894</v>
       </c>
       <c r="D24">
-        <v>430</v>
+        <v>456</v>
       </c>
       <c r="F24" s="1">
-        <v>45859</v>
+        <v>45894</v>
       </c>
       <c r="G24">
-        <v>389</v>
+        <v>421</v>
       </c>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C25" s="1">
-        <v>45852</v>
+        <v>45887</v>
       </c>
       <c r="D25">
-        <v>419</v>
+        <v>446</v>
       </c>
       <c r="F25" s="1">
-        <v>45852</v>
+        <v>45887</v>
       </c>
       <c r="G25">
-        <v>386</v>
+        <v>415</v>
       </c>
     </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C26" s="1">
-        <v>45845</v>
+        <v>45880</v>
       </c>
       <c r="D26">
-        <v>418</v>
+        <v>443</v>
       </c>
       <c r="F26" s="1">
-        <v>45845</v>
+        <v>45880</v>
       </c>
       <c r="G26">
-        <v>386</v>
+        <v>406</v>
       </c>
     </row>
     <row r="27" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C27" s="1">
-        <v>45838</v>
+        <v>45873</v>
       </c>
       <c r="D27">
-        <v>416</v>
+        <v>440</v>
       </c>
       <c r="F27" s="1">
-        <v>45838</v>
+        <v>45873</v>
       </c>
       <c r="G27">
-        <v>370</v>
+        <v>405</v>
       </c>
     </row>
     <row r="28" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C28" s="1">
-        <v>45831</v>
+        <v>45866</v>
       </c>
       <c r="D28">
-        <v>416</v>
+        <v>432</v>
       </c>
       <c r="F28" s="1">
-        <v>45831</v>
+        <v>45866</v>
       </c>
       <c r="G28">
-        <v>370</v>
+        <v>406</v>
       </c>
     </row>
     <row r="29" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C29" s="1">
-        <v>45824</v>
+        <v>45859</v>
       </c>
       <c r="D29">
-        <v>407</v>
+        <v>430</v>
       </c>
       <c r="F29" s="1">
-        <v>45824</v>
+        <v>45859</v>
       </c>
       <c r="G29">
-        <v>369</v>
+        <v>389</v>
       </c>
     </row>
     <row r="30" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C30" s="1">
-        <v>45817</v>
+        <v>45852</v>
       </c>
       <c r="D30">
-        <v>404</v>
+        <v>419</v>
       </c>
       <c r="F30" s="1">
-        <v>45817</v>
+        <v>45852</v>
       </c>
       <c r="G30">
-        <v>359</v>
+        <v>386</v>
       </c>
     </row>
     <row r="31" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C31" s="1">
-        <v>45810</v>
+        <v>45845</v>
       </c>
       <c r="D31">
-        <v>395</v>
+        <v>418</v>
       </c>
       <c r="F31" s="1">
-        <v>45810</v>
+        <v>45845</v>
       </c>
       <c r="G31">
-        <v>360</v>
+        <v>386</v>
       </c>
     </row>
     <row r="32" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C32" s="1">
-        <v>45803</v>
+        <v>45838</v>
       </c>
       <c r="D32">
-        <v>386</v>
+        <v>416</v>
       </c>
       <c r="F32" s="1">
-        <v>45803</v>
+        <v>45838</v>
       </c>
       <c r="G32">
-        <v>354</v>
+        <v>370</v>
       </c>
     </row>
     <row r="33" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C33" s="1">
-        <v>45796</v>
+        <v>45831</v>
       </c>
       <c r="D33">
-        <v>379</v>
+        <v>416</v>
       </c>
       <c r="F33" s="1">
-        <v>45796</v>
+        <v>45831</v>
       </c>
       <c r="G33">
-        <v>349</v>
+        <v>370</v>
       </c>
     </row>
     <row r="34" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C34" s="1">
-        <v>45789</v>
+        <v>45824</v>
       </c>
       <c r="D34">
-        <v>365</v>
+        <v>407</v>
       </c>
       <c r="F34" s="1">
-        <v>45789</v>
+        <v>45824</v>
       </c>
       <c r="G34">
-        <v>320</v>
+        <v>369</v>
       </c>
     </row>
     <row r="35" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C35" s="1">
-        <v>45782</v>
+        <v>45817</v>
       </c>
       <c r="D35">
-        <v>356</v>
+        <v>404</v>
       </c>
       <c r="F35" s="1">
-        <v>45782</v>
+        <v>45817</v>
       </c>
       <c r="G35">
-        <v>320</v>
+        <v>359</v>
       </c>
     </row>
     <row r="36" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C36" s="1">
-        <v>45775</v>
+        <v>45810</v>
       </c>
       <c r="D36">
-        <v>348</v>
+        <v>395</v>
       </c>
       <c r="F36" s="1">
-        <v>45775</v>
+        <v>45810</v>
       </c>
       <c r="G36">
-        <v>320</v>
+        <v>360</v>
       </c>
     </row>
     <row r="37" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C37" s="1">
-        <v>45768</v>
+        <v>45803</v>
       </c>
       <c r="D37">
-        <v>343</v>
+        <v>386</v>
       </c>
       <c r="F37" s="1">
-        <v>45768</v>
+        <v>45803</v>
       </c>
       <c r="G37">
-        <v>319</v>
+        <v>354</v>
       </c>
     </row>
     <row r="38" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C38" s="1">
-        <v>45761</v>
+        <v>45796</v>
       </c>
       <c r="D38">
-        <v>334</v>
+        <v>379</v>
       </c>
       <c r="F38" s="1">
-        <v>45761</v>
+        <v>45796</v>
       </c>
       <c r="G38">
-        <v>303</v>
+        <v>349</v>
       </c>
     </row>
     <row r="39" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C39" s="1">
-        <v>45754</v>
+        <v>45789</v>
       </c>
       <c r="D39">
-        <v>330</v>
+        <v>365</v>
       </c>
       <c r="F39" s="1">
-        <v>45754</v>
+        <v>45789</v>
       </c>
       <c r="G39">
-        <v>302</v>
+        <v>320</v>
       </c>
     </row>
     <row r="40" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C40" s="1">
-        <v>45747</v>
+        <v>45782</v>
       </c>
       <c r="D40">
-        <v>325</v>
+        <v>356</v>
       </c>
       <c r="F40" s="1">
-        <v>45747</v>
+        <v>45782</v>
       </c>
       <c r="G40">
-        <v>302</v>
+        <v>320</v>
       </c>
     </row>
     <row r="41" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C41" s="1">
-        <v>45740</v>
+        <v>45775</v>
       </c>
       <c r="D41">
-        <v>316</v>
+        <v>348</v>
       </c>
       <c r="F41" s="1">
-        <v>45740</v>
+        <v>45775</v>
       </c>
       <c r="G41">
-        <v>296</v>
+        <v>320</v>
       </c>
     </row>
     <row r="42" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C42" s="1">
-        <v>45733</v>
+        <v>45768</v>
       </c>
       <c r="D42">
-        <v>310</v>
+        <v>343</v>
       </c>
       <c r="F42" s="1">
-        <v>45733</v>
+        <v>45768</v>
       </c>
       <c r="G42">
-        <v>296</v>
+        <v>319</v>
       </c>
     </row>
     <row r="43" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C43" s="1">
-        <v>45726</v>
+        <v>45761</v>
       </c>
       <c r="D43">
-        <v>309</v>
+        <v>334</v>
       </c>
       <c r="F43" s="1">
-        <v>45726</v>
+        <v>45761</v>
       </c>
       <c r="G43">
-        <v>294</v>
+        <v>303</v>
       </c>
     </row>
     <row r="44" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C44" s="1">
-        <v>45719</v>
+        <v>45754</v>
       </c>
       <c r="D44">
-        <v>308</v>
+        <v>330</v>
       </c>
       <c r="F44" s="1">
-        <v>45719</v>
+        <v>45754</v>
       </c>
       <c r="G44">
-        <v>286</v>
+        <v>302</v>
       </c>
     </row>
     <row r="45" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C45" s="1">
-        <v>45712</v>
+        <v>45747</v>
       </c>
       <c r="D45">
-        <v>306</v>
+        <v>325</v>
       </c>
       <c r="F45" s="1">
-        <v>45712</v>
+        <v>45747</v>
       </c>
       <c r="G45">
-        <v>286</v>
+        <v>302</v>
       </c>
     </row>
     <row r="46" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C46" s="1">
-        <v>45705</v>
+        <v>45740</v>
       </c>
       <c r="D46">
-        <v>301</v>
+        <v>316</v>
       </c>
       <c r="F46" s="1">
-        <v>45705</v>
+        <v>45740</v>
       </c>
       <c r="G46">
-        <v>267</v>
+        <v>296</v>
       </c>
     </row>
     <row r="47" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C47" s="1">
-        <v>45698</v>
+        <v>45733</v>
       </c>
       <c r="D47">
-        <v>295</v>
+        <v>310</v>
       </c>
       <c r="F47" s="1">
-        <v>45698</v>
+        <v>45733</v>
       </c>
       <c r="G47">
-        <v>267</v>
+        <v>296</v>
       </c>
     </row>
     <row r="48" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C48" s="1">
-        <v>45691</v>
+        <v>45726</v>
       </c>
       <c r="D48">
-        <v>289</v>
+        <v>309</v>
       </c>
       <c r="F48" s="1">
-        <v>45691</v>
+        <v>45726</v>
       </c>
       <c r="G48">
-        <v>267</v>
+        <v>294</v>
       </c>
     </row>
     <row r="49" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C49" s="1">
-        <v>45684</v>
+        <v>45719</v>
       </c>
       <c r="D49">
-        <v>284</v>
+        <v>308</v>
       </c>
       <c r="F49" s="1">
-        <v>45684</v>
+        <v>45719</v>
       </c>
       <c r="G49">
-        <v>262</v>
+        <v>286</v>
       </c>
     </row>
     <row r="50" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C50" s="1">
-        <v>45677</v>
+        <v>45712</v>
       </c>
       <c r="D50">
-        <v>273</v>
+        <v>306</v>
       </c>
       <c r="F50" s="1">
-        <v>45677</v>
+        <v>45712</v>
       </c>
       <c r="G50">
-        <v>254</v>
+        <v>286</v>
       </c>
     </row>
     <row r="51" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C51" s="1">
-        <v>45670</v>
+        <v>45705</v>
       </c>
       <c r="D51">
-        <v>264</v>
+        <v>301</v>
       </c>
       <c r="F51" s="1">
-        <v>45670</v>
+        <v>45705</v>
       </c>
       <c r="G51">
-        <v>250</v>
+        <v>267</v>
       </c>
     </row>
     <row r="52" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C52" s="1">
-        <v>45663</v>
+        <v>45698</v>
       </c>
       <c r="D52">
-        <v>256</v>
+        <v>295</v>
       </c>
       <c r="F52" s="1">
-        <v>45663</v>
+        <v>45698</v>
       </c>
       <c r="G52">
-        <v>250</v>
+        <v>267</v>
       </c>
     </row>
     <row r="53" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C53" s="1">
-        <v>45642</v>
+        <v>45691</v>
       </c>
       <c r="D53">
-        <v>256</v>
+        <v>289</v>
       </c>
       <c r="F53" s="1">
-        <v>45642</v>
+        <v>45691</v>
       </c>
       <c r="G53">
-        <v>245</v>
+        <v>267</v>
       </c>
     </row>
     <row r="54" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C54" s="1">
-        <v>45635</v>
+        <v>45684</v>
       </c>
       <c r="D54">
-        <v>251</v>
+        <v>284</v>
       </c>
       <c r="F54" s="1">
-        <v>45635</v>
+        <v>45684</v>
       </c>
       <c r="G54">
-        <v>243</v>
+        <v>262</v>
       </c>
     </row>
     <row r="55" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C55" s="1">
-        <v>45628</v>
+        <v>45677</v>
       </c>
       <c r="D55">
-        <v>251</v>
+        <v>273</v>
       </c>
       <c r="F55" s="1">
-        <v>45628</v>
+        <v>45677</v>
       </c>
       <c r="G55">
-        <v>239</v>
+        <v>254</v>
       </c>
     </row>
     <row r="56" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C56" s="1">
-        <v>45621</v>
+        <v>45670</v>
       </c>
       <c r="D56">
-        <v>247</v>
+        <v>264</v>
       </c>
       <c r="F56" s="1">
-        <v>45621</v>
+        <v>45670</v>
       </c>
       <c r="G56">
-        <v>234</v>
+        <v>250</v>
       </c>
     </row>
     <row r="57" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C57" s="1">
-        <v>45614</v>
+        <v>45663</v>
       </c>
       <c r="D57">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="F57" s="1">
-        <v>45614</v>
+        <v>45663</v>
       </c>
       <c r="G57">
-        <v>234</v>
+        <v>250</v>
       </c>
     </row>
     <row r="58" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C58" s="1">
-        <v>45607</v>
+        <v>45642</v>
       </c>
       <c r="D58">
-        <v>239</v>
+        <v>256</v>
       </c>
       <c r="F58" s="1">
-        <v>45607</v>
+        <v>45642</v>
       </c>
       <c r="G58">
-        <v>230</v>
+        <v>245</v>
       </c>
     </row>
     <row r="59" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C59" s="1">
-        <v>45600</v>
+        <v>45635</v>
       </c>
       <c r="D59">
-        <v>232</v>
+        <v>251</v>
       </c>
       <c r="F59" s="1">
-        <v>45600</v>
+        <v>45635</v>
       </c>
       <c r="G59">
-        <v>227</v>
+        <v>243</v>
       </c>
     </row>
     <row r="60" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C60" s="1">
-        <v>45579</v>
+        <v>45628</v>
       </c>
       <c r="D60">
-        <v>231</v>
+        <v>251</v>
       </c>
       <c r="F60" s="1">
-        <v>45579</v>
+        <v>45628</v>
       </c>
       <c r="G60">
-        <v>222</v>
+        <v>239</v>
       </c>
     </row>
     <row r="61" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C61" s="1">
-        <v>45572</v>
+        <v>45621</v>
       </c>
       <c r="D61">
-        <v>227</v>
+        <v>247</v>
       </c>
       <c r="F61" s="1">
-        <v>45572</v>
+        <v>45621</v>
       </c>
       <c r="G61">
-        <v>216</v>
+        <v>234</v>
       </c>
     </row>
     <row r="62" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C62" s="1">
-        <v>45565</v>
+        <v>45614</v>
       </c>
       <c r="D62">
-        <v>223</v>
+        <v>241</v>
       </c>
       <c r="F62" s="1">
-        <v>45565</v>
+        <v>45614</v>
       </c>
       <c r="G62">
-        <v>216</v>
+        <v>234</v>
       </c>
     </row>
     <row r="63" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C63" s="1">
-        <v>45537</v>
+        <v>45607</v>
       </c>
       <c r="D63">
-        <v>218</v>
+        <v>239</v>
       </c>
       <c r="F63" s="1">
-        <v>45537</v>
+        <v>45607</v>
       </c>
       <c r="G63">
-        <v>207</v>
+        <v>230</v>
       </c>
     </row>
     <row r="64" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C64" s="1">
-        <v>45530</v>
+        <v>45600</v>
       </c>
       <c r="D64">
-        <v>217</v>
+        <v>232</v>
       </c>
       <c r="F64" s="1">
-        <v>45530</v>
+        <v>45600</v>
       </c>
       <c r="G64">
-        <v>207</v>
+        <v>227</v>
       </c>
     </row>
     <row r="65" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C65" s="1">
-        <v>45523</v>
+        <v>45579</v>
       </c>
       <c r="D65">
-        <v>216</v>
+        <v>231</v>
       </c>
       <c r="F65" s="1">
-        <v>45523</v>
+        <v>45579</v>
       </c>
       <c r="G65">
-        <v>200</v>
+        <v>222</v>
       </c>
     </row>
     <row r="66" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C66" s="1">
-        <v>45516</v>
+        <v>45572</v>
       </c>
       <c r="D66">
-        <v>212</v>
+        <v>227</v>
       </c>
       <c r="F66" s="1">
-        <v>45516</v>
+        <v>45572</v>
       </c>
       <c r="G66">
-        <v>190</v>
+        <v>216</v>
       </c>
     </row>
     <row r="67" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C67" s="1">
-        <v>45509</v>
+        <v>45565</v>
       </c>
       <c r="D67">
-        <v>210</v>
+        <v>223</v>
       </c>
       <c r="F67" s="1">
-        <v>45509</v>
+        <v>45565</v>
       </c>
       <c r="G67">
-        <v>189</v>
+        <v>216</v>
       </c>
     </row>
     <row r="68" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C68" s="1">
-        <v>45502</v>
+        <v>45537</v>
       </c>
       <c r="D68">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="F68" s="1">
-        <v>45502</v>
+        <v>45537</v>
       </c>
       <c r="G68">
-        <v>189</v>
+        <v>207</v>
       </c>
     </row>
     <row r="69" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C69" s="1">
-        <v>45495</v>
+        <v>45530</v>
       </c>
       <c r="D69">
-        <v>201</v>
+        <v>217</v>
       </c>
       <c r="F69" s="1">
-        <v>45495</v>
+        <v>45530</v>
       </c>
       <c r="G69">
-        <v>183</v>
+        <v>207</v>
       </c>
     </row>
     <row r="70" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C70" s="1">
-        <v>45488</v>
+        <v>45523</v>
       </c>
       <c r="D70">
-        <v>199</v>
+        <v>216</v>
       </c>
       <c r="F70" s="1">
-        <v>45488</v>
+        <v>45523</v>
       </c>
       <c r="G70">
-        <v>182</v>
+        <v>200</v>
       </c>
     </row>
     <row r="71" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C71" s="1">
-        <v>45481</v>
+        <v>45516</v>
       </c>
       <c r="D71">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="F71" s="1">
-        <v>45481</v>
+        <v>45516</v>
       </c>
       <c r="G71">
-        <v>180</v>
+        <v>190</v>
       </c>
     </row>
     <row r="72" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C72" s="1">
-        <v>45474</v>
+        <v>45509</v>
       </c>
       <c r="D72">
-        <v>187</v>
+        <v>210</v>
       </c>
       <c r="F72" s="1">
-        <v>45474</v>
+        <v>45509</v>
       </c>
       <c r="G72">
-        <v>172</v>
+        <v>189</v>
       </c>
     </row>
     <row r="73" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C73" s="1">
-        <v>45467</v>
+        <v>45502</v>
       </c>
       <c r="D73">
-        <v>187</v>
+        <v>210</v>
       </c>
       <c r="F73" s="1">
-        <v>45467</v>
+        <v>45502</v>
       </c>
       <c r="G73">
-        <v>172</v>
+        <v>189</v>
       </c>
     </row>
     <row r="74" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C74" s="1">
-        <v>45460</v>
+        <v>45495</v>
       </c>
       <c r="D74">
-        <v>185</v>
+        <v>201</v>
       </c>
       <c r="F74" s="1">
-        <v>45460</v>
+        <v>45495</v>
       </c>
       <c r="G74">
-        <v>165</v>
+        <v>183</v>
       </c>
     </row>
     <row r="75" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C75" s="1">
-        <v>45453</v>
+        <v>45488</v>
       </c>
       <c r="D75">
-        <v>180</v>
+        <v>199</v>
       </c>
       <c r="F75" s="1">
-        <v>45453</v>
+        <v>45488</v>
       </c>
       <c r="G75">
-        <v>164</v>
+        <v>182</v>
       </c>
     </row>
     <row r="76" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C76" s="1">
-        <v>45446</v>
+        <v>45481</v>
       </c>
       <c r="D76">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="F76" s="1">
-        <v>45446</v>
+        <v>45481</v>
       </c>
       <c r="G76">
-        <v>161</v>
+        <v>180</v>
       </c>
     </row>
     <row r="77" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C77" s="1">
-        <v>45439</v>
+        <v>45474</v>
       </c>
       <c r="D77">
-        <v>174</v>
+        <v>187</v>
       </c>
       <c r="F77" s="1">
-        <v>45439</v>
+        <v>45474</v>
       </c>
       <c r="G77">
-        <v>161</v>
+        <v>172</v>
       </c>
     </row>
     <row r="78" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C78" s="1">
-        <v>45432</v>
+        <v>45467</v>
       </c>
       <c r="D78">
-        <v>173</v>
+        <v>187</v>
       </c>
       <c r="F78" s="1">
-        <v>45432</v>
+        <v>45467</v>
       </c>
       <c r="G78">
-        <v>159</v>
+        <v>172</v>
       </c>
     </row>
     <row r="79" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C79" s="1">
-        <v>45425</v>
+        <v>45460</v>
       </c>
       <c r="D79">
-        <v>170</v>
+        <v>185</v>
       </c>
       <c r="F79" s="1">
-        <v>45425</v>
+        <v>45460</v>
       </c>
       <c r="G79">
-        <v>157</v>
+        <v>165</v>
       </c>
     </row>
     <row r="80" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C80" s="1">
-        <v>45418</v>
+        <v>45453</v>
       </c>
       <c r="D80">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="F80" s="1">
-        <v>45418</v>
+        <v>45453</v>
       </c>
       <c r="G80">
-        <v>141</v>
+        <v>164</v>
       </c>
     </row>
     <row r="81" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C81" s="1">
-        <v>45411</v>
+        <v>45446</v>
       </c>
       <c r="D81">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="F81" s="1">
-        <v>45411</v>
+        <v>45446</v>
       </c>
       <c r="G81">
-        <v>141</v>
+        <v>161</v>
       </c>
     </row>
     <row r="82" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C82" s="1">
-        <v>45404</v>
+        <v>45439</v>
       </c>
       <c r="D82">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="F82" s="1">
-        <v>45404</v>
+        <v>45439</v>
       </c>
       <c r="G82">
-        <v>141</v>
+        <v>161</v>
       </c>
     </row>
     <row r="83" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C83" s="1">
-        <v>45397</v>
+        <v>45432</v>
       </c>
       <c r="D83">
-        <v>157</v>
+        <v>173</v>
       </c>
       <c r="F83" s="1">
-        <v>45397</v>
+        <v>45432</v>
       </c>
       <c r="G83">
-        <v>132</v>
+        <v>159</v>
       </c>
     </row>
     <row r="84" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C84" s="1">
-        <v>45390</v>
+        <v>45425</v>
       </c>
       <c r="D84">
-        <v>146</v>
+        <v>170</v>
       </c>
       <c r="F84" s="1">
-        <v>45390</v>
+        <v>45425</v>
       </c>
       <c r="G84">
-        <v>132</v>
+        <v>157</v>
       </c>
     </row>
     <row r="85" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C85" s="1">
-        <v>45383</v>
+        <v>45418</v>
       </c>
       <c r="D85">
-        <v>138</v>
+        <v>170</v>
       </c>
       <c r="F85" s="1">
-        <v>45383</v>
+        <v>45418</v>
       </c>
       <c r="G85">
-        <v>119</v>
+        <v>141</v>
       </c>
     </row>
     <row r="86" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C86" s="1">
-        <v>45376</v>
+        <v>45411</v>
       </c>
       <c r="D86">
-        <v>129</v>
+        <v>166</v>
       </c>
       <c r="F86" s="1">
-        <v>45376</v>
+        <v>45411</v>
       </c>
       <c r="G86">
-        <v>114</v>
+        <v>141</v>
       </c>
     </row>
     <row r="87" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C87" s="1">
-        <v>45369</v>
+        <v>45404</v>
       </c>
       <c r="D87">
-        <v>123</v>
+        <v>166</v>
       </c>
       <c r="F87" s="1">
-        <v>45369</v>
+        <v>45404</v>
       </c>
       <c r="G87">
-        <v>97</v>
+        <v>141</v>
       </c>
     </row>
     <row r="88" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C88" s="1">
-        <v>45362</v>
+        <v>45397</v>
       </c>
       <c r="D88">
-        <v>113</v>
-      </c>
-      <c r="F88" s="1"/>
+        <v>157</v>
+      </c>
+      <c r="F88" s="1">
+        <v>45397</v>
+      </c>
+      <c r="G88">
+        <v>132</v>
+      </c>
     </row>
     <row r="89" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C89" s="1">
-        <v>45355</v>
+        <v>45390</v>
       </c>
       <c r="D89">
-        <v>108</v>
+        <v>146</v>
+      </c>
+      <c r="F89" s="1">
+        <v>45390</v>
+      </c>
+      <c r="G89">
+        <v>132</v>
       </c>
     </row>
     <row r="90" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C90" s="1">
-        <v>45348</v>
+        <v>45383</v>
       </c>
       <c r="D90">
-        <v>102</v>
+        <v>138</v>
+      </c>
+      <c r="F90" s="1">
+        <v>45383</v>
+      </c>
+      <c r="G90">
+        <v>119</v>
       </c>
     </row>
     <row r="91" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C91" s="1">
-        <v>45341</v>
+        <v>45376</v>
       </c>
       <c r="D91">
-        <v>95</v>
+        <v>129</v>
+      </c>
+      <c r="F91" s="1">
+        <v>45376</v>
+      </c>
+      <c r="G91">
+        <v>114</v>
       </c>
     </row>
     <row r="92" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C92" s="1">
-        <v>45334</v>
+        <v>45369</v>
       </c>
       <c r="D92">
-        <v>80</v>
+        <v>123</v>
+      </c>
+      <c r="F92" s="1">
+        <v>45369</v>
+      </c>
+      <c r="G92">
+        <v>97</v>
       </c>
     </row>
     <row r="93" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C93" s="1">
-        <v>45327</v>
+        <v>45362</v>
       </c>
       <c r="D93">
-        <v>66</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="F93" s="1"/>
     </row>
     <row r="94" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C94" s="1">
-        <v>45320</v>
+        <v>45355</v>
       </c>
       <c r="D94">
-        <v>55</v>
+        <v>108</v>
       </c>
     </row>
     <row r="95" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C95" s="1">
-        <v>45313</v>
+        <v>45348</v>
       </c>
       <c r="D95">
-        <v>53</v>
+        <v>102</v>
       </c>
     </row>
     <row r="96" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C96" s="1">
+        <v>45341</v>
+      </c>
+      <c r="D96">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C97" s="1">
+        <v>45334</v>
+      </c>
+      <c r="D97">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="98" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C98" s="1">
+        <v>45327</v>
+      </c>
+      <c r="D98">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="99" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C99" s="1">
+        <v>45320</v>
+      </c>
+      <c r="D99">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="100" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C100" s="1">
+        <v>45313</v>
+      </c>
+      <c r="D100">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="101" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C101" s="1">
         <v>45306</v>
       </c>
-      <c r="D96">
+      <c r="D101">
         <v>52</v>
       </c>
     </row>
-    <row r="100" spans="4:17" x14ac:dyDescent="0.35">
-      <c r="D100" s="2"/>
-      <c r="E100" s="2"/>
-      <c r="F100" s="2"/>
-      <c r="G100" s="2"/>
-      <c r="H100" s="2"/>
-      <c r="I100" s="2"/>
-      <c r="J100" s="2"/>
-      <c r="K100" s="2"/>
-      <c r="L100" s="2"/>
-      <c r="M100" s="2"/>
-      <c r="N100" s="2"/>
-      <c r="O100" s="2"/>
-      <c r="P100" s="2"/>
-      <c r="Q100" s="2"/>
-    </row>
-    <row r="101" spans="4:17" x14ac:dyDescent="0.35">
-      <c r="D101" s="2"/>
-      <c r="E101" s="2"/>
-      <c r="F101" s="2"/>
-      <c r="G101" s="2"/>
-      <c r="H101" s="2"/>
-      <c r="I101" s="2"/>
-      <c r="J101" s="2"/>
-      <c r="K101" s="2"/>
-      <c r="L101" s="2"/>
-      <c r="M101" s="2"/>
-      <c r="N101" s="2"/>
-      <c r="O101" s="2"/>
-      <c r="P101" s="2"/>
-      <c r="Q101" s="2"/>
-    </row>
-    <row r="102" spans="4:17" x14ac:dyDescent="0.35">
-      <c r="D102" s="2"/>
-      <c r="E102" s="2"/>
-      <c r="F102" s="2"/>
-      <c r="G102" s="2"/>
-      <c r="H102" s="2"/>
-      <c r="I102" s="2"/>
-      <c r="J102" s="2"/>
-      <c r="K102" s="2"/>
-      <c r="L102" s="2"/>
-      <c r="M102" s="2"/>
-      <c r="N102" s="2"/>
-      <c r="O102" s="2"/>
-      <c r="P102" s="2"/>
-      <c r="Q102" s="2"/>
-    </row>
-    <row r="103" spans="4:17" x14ac:dyDescent="0.35">
-      <c r="D103" s="2"/>
-      <c r="E103" s="2"/>
-      <c r="F103" s="2"/>
-      <c r="G103" s="2"/>
-      <c r="H103" s="2"/>
-      <c r="I103" s="2"/>
-      <c r="J103" s="2"/>
-      <c r="K103" s="2"/>
-      <c r="L103" s="2"/>
-      <c r="M103" s="2"/>
-      <c r="N103" s="2"/>
-      <c r="O103" s="2"/>
-      <c r="P103" s="2"/>
-      <c r="Q103" s="2"/>
-    </row>
-    <row r="104" spans="4:17" x14ac:dyDescent="0.35">
-      <c r="D104" s="2"/>
-      <c r="E104" s="2"/>
-      <c r="F104" s="2"/>
-      <c r="G104" s="2"/>
-      <c r="H104" s="2"/>
-      <c r="I104" s="2"/>
-      <c r="J104" s="2"/>
-      <c r="K104" s="2"/>
-      <c r="L104" s="2"/>
-      <c r="M104" s="2"/>
-      <c r="N104" s="2"/>
-      <c r="O104" s="2"/>
-      <c r="P104" s="2"/>
-      <c r="Q104" s="2"/>
-    </row>
-    <row r="105" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="105" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D105" s="2"/>
       <c r="E105" s="2"/>
       <c r="F105" s="2"/>
@@ -6032,7 +5952,7 @@
       <c r="P105" s="2"/>
       <c r="Q105" s="2"/>
     </row>
-    <row r="106" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="106" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D106" s="2"/>
       <c r="E106" s="2"/>
       <c r="F106" s="2"/>
@@ -6048,7 +5968,7 @@
       <c r="P106" s="2"/>
       <c r="Q106" s="2"/>
     </row>
-    <row r="107" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="107" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D107" s="2"/>
       <c r="E107" s="2"/>
       <c r="F107" s="2"/>
@@ -6064,7 +5984,7 @@
       <c r="P107" s="2"/>
       <c r="Q107" s="2"/>
     </row>
-    <row r="108" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="108" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D108" s="2"/>
       <c r="E108" s="2"/>
       <c r="F108" s="2"/>
@@ -6080,7 +6000,7 @@
       <c r="P108" s="2"/>
       <c r="Q108" s="2"/>
     </row>
-    <row r="109" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="109" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D109" s="2"/>
       <c r="E109" s="2"/>
       <c r="F109" s="2"/>
@@ -6096,7 +6016,7 @@
       <c r="P109" s="2"/>
       <c r="Q109" s="2"/>
     </row>
-    <row r="110" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="110" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D110" s="2"/>
       <c r="E110" s="2"/>
       <c r="F110" s="2"/>
@@ -6112,7 +6032,7 @@
       <c r="P110" s="2"/>
       <c r="Q110" s="2"/>
     </row>
-    <row r="111" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="111" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D111" s="2"/>
       <c r="E111" s="2"/>
       <c r="F111" s="2"/>
@@ -6128,7 +6048,7 @@
       <c r="P111" s="2"/>
       <c r="Q111" s="2"/>
     </row>
-    <row r="112" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="112" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D112" s="2"/>
       <c r="E112" s="2"/>
       <c r="F112" s="2"/>
@@ -6352,9 +6272,89 @@
       <c r="P125" s="2"/>
       <c r="Q125" s="2"/>
     </row>
+    <row r="126" spans="4:17" x14ac:dyDescent="0.35">
+      <c r="D126" s="2"/>
+      <c r="E126" s="2"/>
+      <c r="F126" s="2"/>
+      <c r="G126" s="2"/>
+      <c r="H126" s="2"/>
+      <c r="I126" s="2"/>
+      <c r="J126" s="2"/>
+      <c r="K126" s="2"/>
+      <c r="L126" s="2"/>
+      <c r="M126" s="2"/>
+      <c r="N126" s="2"/>
+      <c r="O126" s="2"/>
+      <c r="P126" s="2"/>
+      <c r="Q126" s="2"/>
+    </row>
+    <row r="127" spans="4:17" x14ac:dyDescent="0.35">
+      <c r="D127" s="2"/>
+      <c r="E127" s="2"/>
+      <c r="F127" s="2"/>
+      <c r="G127" s="2"/>
+      <c r="H127" s="2"/>
+      <c r="I127" s="2"/>
+      <c r="J127" s="2"/>
+      <c r="K127" s="2"/>
+      <c r="L127" s="2"/>
+      <c r="M127" s="2"/>
+      <c r="N127" s="2"/>
+      <c r="O127" s="2"/>
+      <c r="P127" s="2"/>
+      <c r="Q127" s="2"/>
+    </row>
+    <row r="128" spans="4:17" x14ac:dyDescent="0.35">
+      <c r="D128" s="2"/>
+      <c r="E128" s="2"/>
+      <c r="F128" s="2"/>
+      <c r="G128" s="2"/>
+      <c r="H128" s="2"/>
+      <c r="I128" s="2"/>
+      <c r="J128" s="2"/>
+      <c r="K128" s="2"/>
+      <c r="L128" s="2"/>
+      <c r="M128" s="2"/>
+      <c r="N128" s="2"/>
+      <c r="O128" s="2"/>
+      <c r="P128" s="2"/>
+      <c r="Q128" s="2"/>
+    </row>
+    <row r="129" spans="4:17" x14ac:dyDescent="0.35">
+      <c r="D129" s="2"/>
+      <c r="E129" s="2"/>
+      <c r="F129" s="2"/>
+      <c r="G129" s="2"/>
+      <c r="H129" s="2"/>
+      <c r="I129" s="2"/>
+      <c r="J129" s="2"/>
+      <c r="K129" s="2"/>
+      <c r="L129" s="2"/>
+      <c r="M129" s="2"/>
+      <c r="N129" s="2"/>
+      <c r="O129" s="2"/>
+      <c r="P129" s="2"/>
+      <c r="Q129" s="2"/>
+    </row>
+    <row r="130" spans="4:17" x14ac:dyDescent="0.35">
+      <c r="D130" s="2"/>
+      <c r="E130" s="2"/>
+      <c r="F130" s="2"/>
+      <c r="G130" s="2"/>
+      <c r="H130" s="2"/>
+      <c r="I130" s="2"/>
+      <c r="J130" s="2"/>
+      <c r="K130" s="2"/>
+      <c r="L130" s="2"/>
+      <c r="M130" s="2"/>
+      <c r="N130" s="2"/>
+      <c r="O130" s="2"/>
+      <c r="P130" s="2"/>
+      <c r="Q130" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D100:Q125"/>
+    <mergeCell ref="D105:Q130"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
LGHUB 2025/9/23 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
- 网站错误 & 本地化问题详见 LGHUB/WebLoc/README.md
</commit_message>
<xml_diff>
--- a/Documents/Graph_PC.xlsx
+++ b/Documents/Graph_PC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29315"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52FA5F7D-8467-4CD0-95A4-F6B89B45E131}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F13966F-E25D-467B-B423-739C76B785AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="2" r:id="rId1"/>
@@ -574,10 +574,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>28</c:v>
@@ -917,72 +917,72 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$21:$C$29</c:f>
+              <c:f>Sheet1!$C$20:$C$28</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45922</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45915</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45908</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45901</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45894</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45887</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45880</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45873</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45866</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45859</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$21:$D$29</c:f>
+              <c:f>Sheet1!$D$20:$D$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>493</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>488</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>485</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>471</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>456</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>446</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>443</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>440</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>432</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>430</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1086,43 +1086,43 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$21:$C$29</c:f>
+              <c:f>Sheet1!$C$20:$C$28</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45922</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45915</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45908</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45901</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45894</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45887</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45880</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45873</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45866</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45859</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$21:$G$29</c:f>
+              <c:f>Sheet1!$G$20:$G$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1130,28 +1130,28 @@
                   <c:v>450</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>444</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>426</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>421</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>415</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>406</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>405</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>406</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>389</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1287,7 +1287,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="500"/>
-          <c:min val="380"/>
+          <c:min val="400"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1794,10 +1794,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>28</c:v>
@@ -4811,43 +4811,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D103" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L104" sqref="L104"/>
+    <sheetView tabSelected="1" topLeftCell="B105" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="J104" sqref="J104"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>4</v>
       </c>
@@ -4855,7 +4855,21 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C20" s="1">
+        <v>45922</v>
+      </c>
+      <c r="D20">
+        <v>493</v>
+      </c>
+      <c r="F20" s="1">
+        <v>45922</v>
+      </c>
+      <c r="G20">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C21" s="1">
         <v>45915</v>
       </c>
@@ -4869,7 +4883,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C22" s="1">
         <v>45908</v>
       </c>
@@ -4883,7 +4897,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C23" s="1">
         <v>45901</v>
       </c>
@@ -4897,7 +4911,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C24" s="1">
         <v>45894</v>
       </c>
@@ -4911,7 +4925,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C25" s="1">
         <v>45887</v>
       </c>
@@ -4925,7 +4939,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C26" s="1">
         <v>45880</v>
       </c>
@@ -4939,7 +4953,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C27" s="1">
         <v>45873</v>
       </c>
@@ -4953,7 +4967,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C28" s="1">
         <v>45866</v>
       </c>
@@ -4967,7 +4981,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C29" s="1">
         <v>45859</v>
       </c>
@@ -4981,7 +4995,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C30" s="1">
         <v>45852</v>
       </c>
@@ -4995,7 +5009,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C31" s="1">
         <v>45845</v>
       </c>
@@ -5009,7 +5023,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C32" s="1">
         <v>45838</v>
       </c>
@@ -5023,7 +5037,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C33" s="1">
         <v>45831</v>
       </c>
@@ -5037,7 +5051,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="34" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C34" s="1">
         <v>45824</v>
       </c>
@@ -5051,7 +5065,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="35" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C35" s="1">
         <v>45817</v>
       </c>
@@ -5065,7 +5079,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="36" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C36" s="1">
         <v>45810</v>
       </c>
@@ -5079,7 +5093,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="37" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C37" s="1">
         <v>45803</v>
       </c>
@@ -5093,7 +5107,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="38" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C38" s="1">
         <v>45796</v>
       </c>
@@ -5107,7 +5121,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="39" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C39" s="1">
         <v>45789</v>
       </c>
@@ -5121,7 +5135,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="40" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C40" s="1">
         <v>45782</v>
       </c>
@@ -5135,7 +5149,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="41" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C41" s="1">
         <v>45775</v>
       </c>
@@ -5149,7 +5163,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="42" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C42" s="1">
         <v>45768</v>
       </c>
@@ -5163,7 +5177,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="43" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C43" s="1">
         <v>45761</v>
       </c>
@@ -5177,7 +5191,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="44" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C44" s="1">
         <v>45754</v>
       </c>
@@ -5191,7 +5205,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="45" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C45" s="1">
         <v>45747</v>
       </c>
@@ -5205,7 +5219,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="46" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C46" s="1">
         <v>45740</v>
       </c>
@@ -5219,7 +5233,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="47" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C47" s="1">
         <v>45733</v>
       </c>
@@ -5233,7 +5247,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="48" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C48" s="1">
         <v>45726</v>
       </c>
@@ -5247,7 +5261,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="49" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="49" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C49" s="1">
         <v>45719</v>
       </c>
@@ -5261,7 +5275,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="50" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="50" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C50" s="1">
         <v>45712</v>
       </c>
@@ -5275,7 +5289,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="51" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="51" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C51" s="1">
         <v>45705</v>
       </c>
@@ -5289,7 +5303,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="52" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="52" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C52" s="1">
         <v>45698</v>
       </c>
@@ -5303,7 +5317,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="53" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="53" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C53" s="1">
         <v>45691</v>
       </c>
@@ -5317,7 +5331,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="54" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="54" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C54" s="1">
         <v>45684</v>
       </c>
@@ -5331,7 +5345,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="55" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="55" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C55" s="1">
         <v>45677</v>
       </c>
@@ -5345,7 +5359,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="56" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="56" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C56" s="1">
         <v>45670</v>
       </c>
@@ -5359,7 +5373,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="57" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="57" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C57" s="1">
         <v>45663</v>
       </c>
@@ -5373,7 +5387,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="58" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="58" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C58" s="1">
         <v>45642</v>
       </c>
@@ -5387,7 +5401,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="59" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="59" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C59" s="1">
         <v>45635</v>
       </c>
@@ -5401,7 +5415,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="60" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="60" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C60" s="1">
         <v>45628</v>
       </c>
@@ -5415,7 +5429,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="61" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="61" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C61" s="1">
         <v>45621</v>
       </c>
@@ -5429,7 +5443,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="62" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="62" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C62" s="1">
         <v>45614</v>
       </c>
@@ -5443,7 +5457,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="63" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="63" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C63" s="1">
         <v>45607</v>
       </c>
@@ -5457,7 +5471,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="64" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="64" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C64" s="1">
         <v>45600</v>
       </c>
@@ -5471,7 +5485,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="65" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="65" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C65" s="1">
         <v>45579</v>
       </c>
@@ -5485,7 +5499,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="66" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="66" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C66" s="1">
         <v>45572</v>
       </c>
@@ -5499,7 +5513,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="67" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="67" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C67" s="1">
         <v>45565</v>
       </c>
@@ -5513,7 +5527,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="68" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="68" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C68" s="1">
         <v>45537</v>
       </c>
@@ -5527,7 +5541,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="69" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="69" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C69" s="1">
         <v>45530</v>
       </c>
@@ -5541,7 +5555,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="70" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="70" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C70" s="1">
         <v>45523</v>
       </c>
@@ -5555,7 +5569,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="71" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="71" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C71" s="1">
         <v>45516</v>
       </c>
@@ -5569,7 +5583,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="72" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="72" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C72" s="1">
         <v>45509</v>
       </c>
@@ -5583,7 +5597,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="73" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="73" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C73" s="1">
         <v>45502</v>
       </c>
@@ -5597,7 +5611,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="74" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="74" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C74" s="1">
         <v>45495</v>
       </c>
@@ -5611,7 +5625,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="75" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="75" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C75" s="1">
         <v>45488</v>
       </c>
@@ -5625,7 +5639,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="76" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="76" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C76" s="1">
         <v>45481</v>
       </c>
@@ -5639,7 +5653,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="77" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="77" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C77" s="1">
         <v>45474</v>
       </c>
@@ -5653,7 +5667,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="78" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="78" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C78" s="1">
         <v>45467</v>
       </c>
@@ -5667,7 +5681,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="79" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="79" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C79" s="1">
         <v>45460</v>
       </c>
@@ -5681,7 +5695,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="80" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="80" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C80" s="1">
         <v>45453</v>
       </c>
@@ -5695,7 +5709,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="81" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="81" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C81" s="1">
         <v>45446</v>
       </c>
@@ -5709,7 +5723,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="82" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="82" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C82" s="1">
         <v>45439</v>
       </c>
@@ -5723,7 +5737,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="83" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="83" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C83" s="1">
         <v>45432</v>
       </c>
@@ -5737,7 +5751,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="84" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="84" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C84" s="1">
         <v>45425</v>
       </c>
@@ -5751,7 +5765,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="85" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="85" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C85" s="1">
         <v>45418</v>
       </c>
@@ -5765,7 +5779,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="86" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="86" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C86" s="1">
         <v>45411</v>
       </c>
@@ -5779,7 +5793,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="87" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="87" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C87" s="1">
         <v>45404</v>
       </c>
@@ -5793,7 +5807,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="88" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="88" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C88" s="1">
         <v>45397</v>
       </c>
@@ -5807,7 +5821,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="89" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="89" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C89" s="1">
         <v>45390</v>
       </c>
@@ -5821,7 +5835,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="90" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="90" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C90" s="1">
         <v>45383</v>
       </c>
@@ -5835,7 +5849,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="91" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="91" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C91" s="1">
         <v>45376</v>
       </c>
@@ -5849,7 +5863,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="92" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="92" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C92" s="1">
         <v>45369</v>
       </c>
@@ -5863,7 +5877,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="93" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="93" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C93" s="1">
         <v>45362</v>
       </c>
@@ -5872,7 +5886,7 @@
       </c>
       <c r="F93" s="1"/>
     </row>
-    <row r="94" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="94" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C94" s="1">
         <v>45355</v>
       </c>
@@ -5880,7 +5894,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="95" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="95" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C95" s="1">
         <v>45348</v>
       </c>
@@ -5888,7 +5902,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="96" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="96" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C96" s="1">
         <v>45341</v>
       </c>
@@ -5896,7 +5910,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="97" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C97" s="1">
         <v>45334</v>
       </c>
@@ -5904,7 +5918,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="98" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="98" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C98" s="1">
         <v>45327</v>
       </c>
@@ -5912,7 +5926,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="99" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="99" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C99" s="1">
         <v>45320</v>
       </c>
@@ -5920,7 +5934,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="100" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="100" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C100" s="1">
         <v>45313</v>
       </c>
@@ -5928,7 +5942,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="101" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="101" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C101" s="1">
         <v>45306</v>
       </c>
@@ -5936,7 +5950,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="105" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="105" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D105" s="2"/>
       <c r="E105" s="2"/>
       <c r="F105" s="2"/>
@@ -5952,7 +5966,7 @@
       <c r="P105" s="2"/>
       <c r="Q105" s="2"/>
     </row>
-    <row r="106" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="106" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D106" s="2"/>
       <c r="E106" s="2"/>
       <c r="F106" s="2"/>
@@ -5968,7 +5982,7 @@
       <c r="P106" s="2"/>
       <c r="Q106" s="2"/>
     </row>
-    <row r="107" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="107" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D107" s="2"/>
       <c r="E107" s="2"/>
       <c r="F107" s="2"/>
@@ -5984,7 +5998,7 @@
       <c r="P107" s="2"/>
       <c r="Q107" s="2"/>
     </row>
-    <row r="108" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="108" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D108" s="2"/>
       <c r="E108" s="2"/>
       <c r="F108" s="2"/>
@@ -6000,7 +6014,7 @@
       <c r="P108" s="2"/>
       <c r="Q108" s="2"/>
     </row>
-    <row r="109" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="109" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D109" s="2"/>
       <c r="E109" s="2"/>
       <c r="F109" s="2"/>
@@ -6016,7 +6030,7 @@
       <c r="P109" s="2"/>
       <c r="Q109" s="2"/>
     </row>
-    <row r="110" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="110" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D110" s="2"/>
       <c r="E110" s="2"/>
       <c r="F110" s="2"/>
@@ -6032,7 +6046,7 @@
       <c r="P110" s="2"/>
       <c r="Q110" s="2"/>
     </row>
-    <row r="111" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="111" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D111" s="2"/>
       <c r="E111" s="2"/>
       <c r="F111" s="2"/>
@@ -6048,7 +6062,7 @@
       <c r="P111" s="2"/>
       <c r="Q111" s="2"/>
     </row>
-    <row r="112" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="112" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D112" s="2"/>
       <c r="E112" s="2"/>
       <c r="F112" s="2"/>
@@ -6064,7 +6078,7 @@
       <c r="P112" s="2"/>
       <c r="Q112" s="2"/>
     </row>
-    <row r="113" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="113" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D113" s="2"/>
       <c r="E113" s="2"/>
       <c r="F113" s="2"/>
@@ -6080,7 +6094,7 @@
       <c r="P113" s="2"/>
       <c r="Q113" s="2"/>
     </row>
-    <row r="114" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="114" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D114" s="2"/>
       <c r="E114" s="2"/>
       <c r="F114" s="2"/>
@@ -6096,7 +6110,7 @@
       <c r="P114" s="2"/>
       <c r="Q114" s="2"/>
     </row>
-    <row r="115" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="115" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D115" s="2"/>
       <c r="E115" s="2"/>
       <c r="F115" s="2"/>
@@ -6112,7 +6126,7 @@
       <c r="P115" s="2"/>
       <c r="Q115" s="2"/>
     </row>
-    <row r="116" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="116" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D116" s="2"/>
       <c r="E116" s="2"/>
       <c r="F116" s="2"/>
@@ -6128,7 +6142,7 @@
       <c r="P116" s="2"/>
       <c r="Q116" s="2"/>
     </row>
-    <row r="117" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="117" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D117" s="2"/>
       <c r="E117" s="2"/>
       <c r="F117" s="2"/>
@@ -6144,7 +6158,7 @@
       <c r="P117" s="2"/>
       <c r="Q117" s="2"/>
     </row>
-    <row r="118" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="118" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D118" s="2"/>
       <c r="E118" s="2"/>
       <c r="F118" s="2"/>
@@ -6160,7 +6174,7 @@
       <c r="P118" s="2"/>
       <c r="Q118" s="2"/>
     </row>
-    <row r="119" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="119" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D119" s="2"/>
       <c r="E119" s="2"/>
       <c r="F119" s="2"/>
@@ -6176,7 +6190,7 @@
       <c r="P119" s="2"/>
       <c r="Q119" s="2"/>
     </row>
-    <row r="120" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="120" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D120" s="2"/>
       <c r="E120" s="2"/>
       <c r="F120" s="2"/>
@@ -6192,7 +6206,7 @@
       <c r="P120" s="2"/>
       <c r="Q120" s="2"/>
     </row>
-    <row r="121" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="121" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D121" s="2"/>
       <c r="E121" s="2"/>
       <c r="F121" s="2"/>
@@ -6208,7 +6222,7 @@
       <c r="P121" s="2"/>
       <c r="Q121" s="2"/>
     </row>
-    <row r="122" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="122" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D122" s="2"/>
       <c r="E122" s="2"/>
       <c r="F122" s="2"/>
@@ -6224,7 +6238,7 @@
       <c r="P122" s="2"/>
       <c r="Q122" s="2"/>
     </row>
-    <row r="123" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="123" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D123" s="2"/>
       <c r="E123" s="2"/>
       <c r="F123" s="2"/>
@@ -6240,7 +6254,7 @@
       <c r="P123" s="2"/>
       <c r="Q123" s="2"/>
     </row>
-    <row r="124" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="124" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D124" s="2"/>
       <c r="E124" s="2"/>
       <c r="F124" s="2"/>
@@ -6256,7 +6270,7 @@
       <c r="P124" s="2"/>
       <c r="Q124" s="2"/>
     </row>
-    <row r="125" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="125" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D125" s="2"/>
       <c r="E125" s="2"/>
       <c r="F125" s="2"/>
@@ -6272,7 +6286,7 @@
       <c r="P125" s="2"/>
       <c r="Q125" s="2"/>
     </row>
-    <row r="126" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="126" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D126" s="2"/>
       <c r="E126" s="2"/>
       <c r="F126" s="2"/>
@@ -6288,7 +6302,7 @@
       <c r="P126" s="2"/>
       <c r="Q126" s="2"/>
     </row>
-    <row r="127" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="127" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D127" s="2"/>
       <c r="E127" s="2"/>
       <c r="F127" s="2"/>
@@ -6304,7 +6318,7 @@
       <c r="P127" s="2"/>
       <c r="Q127" s="2"/>
     </row>
-    <row r="128" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="128" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D128" s="2"/>
       <c r="E128" s="2"/>
       <c r="F128" s="2"/>
@@ -6320,7 +6334,7 @@
       <c r="P128" s="2"/>
       <c r="Q128" s="2"/>
     </row>
-    <row r="129" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="129" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D129" s="2"/>
       <c r="E129" s="2"/>
       <c r="F129" s="2"/>
@@ -6336,7 +6350,7 @@
       <c r="P129" s="2"/>
       <c r="Q129" s="2"/>
     </row>
-    <row r="130" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="130" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D130" s="2"/>
       <c r="E130" s="2"/>
       <c r="F130" s="2"/>

</xml_diff>

<commit_message>
LGHUB 2025/9/27 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
- 网站错误 & 本地化问题详见 LGHUB/WebLoc/README.md
</commit_message>
<xml_diff>
--- a/Documents/Graph_PC.xlsx
+++ b/Documents/Graph_PC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F13966F-E25D-467B-B423-739C76B785AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4FAA230-B3E9-4621-9D74-905DA1148341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="2" r:id="rId1"/>
@@ -574,13 +574,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -958,7 +958,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>493</c:v>
+                  <c:v>496</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>488</c:v>
@@ -1127,7 +1127,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>450</c:v>
+                  <c:v>455</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>450</c:v>
@@ -1794,13 +1794,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4811,65 +4811,65 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B105" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D103" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="J104" sqref="J104"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C20" s="1">
         <v>45922</v>
       </c>
       <c r="D20">
-        <v>493</v>
+        <v>496</v>
       </c>
       <c r="F20" s="1">
         <v>45922</v>
       </c>
       <c r="G20">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C21" s="1">
         <v>45915</v>
       </c>
@@ -4883,7 +4883,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C22" s="1">
         <v>45908</v>
       </c>
@@ -4897,7 +4897,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C23" s="1">
         <v>45901</v>
       </c>
@@ -4911,7 +4911,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C24" s="1">
         <v>45894</v>
       </c>
@@ -4925,7 +4925,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C25" s="1">
         <v>45887</v>
       </c>
@@ -4939,7 +4939,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C26" s="1">
         <v>45880</v>
       </c>
@@ -4953,7 +4953,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C27" s="1">
         <v>45873</v>
       </c>
@@ -4967,7 +4967,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C28" s="1">
         <v>45866</v>
       </c>
@@ -4981,7 +4981,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C29" s="1">
         <v>45859</v>
       </c>
@@ -4995,7 +4995,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C30" s="1">
         <v>45852</v>
       </c>
@@ -5009,7 +5009,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C31" s="1">
         <v>45845</v>
       </c>
@@ -5023,7 +5023,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C32" s="1">
         <v>45838</v>
       </c>
@@ -5037,7 +5037,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C33" s="1">
         <v>45831</v>
       </c>
@@ -5051,7 +5051,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C34" s="1">
         <v>45824</v>
       </c>
@@ -5065,7 +5065,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C35" s="1">
         <v>45817</v>
       </c>
@@ -5079,7 +5079,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C36" s="1">
         <v>45810</v>
       </c>
@@ -5093,7 +5093,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="37" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C37" s="1">
         <v>45803</v>
       </c>
@@ -5107,7 +5107,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="38" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C38" s="1">
         <v>45796</v>
       </c>
@@ -5121,7 +5121,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="39" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C39" s="1">
         <v>45789</v>
       </c>
@@ -5135,7 +5135,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="40" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C40" s="1">
         <v>45782</v>
       </c>
@@ -5149,7 +5149,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="41" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C41" s="1">
         <v>45775</v>
       </c>
@@ -5163,7 +5163,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="42" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C42" s="1">
         <v>45768</v>
       </c>
@@ -5177,7 +5177,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="43" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C43" s="1">
         <v>45761</v>
       </c>
@@ -5191,7 +5191,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="44" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C44" s="1">
         <v>45754</v>
       </c>
@@ -5205,7 +5205,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="45" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C45" s="1">
         <v>45747</v>
       </c>
@@ -5219,7 +5219,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="46" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C46" s="1">
         <v>45740</v>
       </c>
@@ -5233,7 +5233,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="47" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C47" s="1">
         <v>45733</v>
       </c>
@@ -5247,7 +5247,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="48" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C48" s="1">
         <v>45726</v>
       </c>
@@ -5261,7 +5261,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="49" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C49" s="1">
         <v>45719</v>
       </c>
@@ -5275,7 +5275,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="50" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C50" s="1">
         <v>45712</v>
       </c>
@@ -5289,7 +5289,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="51" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C51" s="1">
         <v>45705</v>
       </c>
@@ -5303,7 +5303,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="52" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C52" s="1">
         <v>45698</v>
       </c>
@@ -5317,7 +5317,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="53" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C53" s="1">
         <v>45691</v>
       </c>
@@ -5331,7 +5331,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="54" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C54" s="1">
         <v>45684</v>
       </c>
@@ -5345,7 +5345,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="55" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C55" s="1">
         <v>45677</v>
       </c>
@@ -5359,7 +5359,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="56" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C56" s="1">
         <v>45670</v>
       </c>
@@ -5373,7 +5373,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="57" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C57" s="1">
         <v>45663</v>
       </c>
@@ -5387,7 +5387,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="58" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C58" s="1">
         <v>45642</v>
       </c>
@@ -5401,7 +5401,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="59" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C59" s="1">
         <v>45635</v>
       </c>
@@ -5415,7 +5415,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="60" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C60" s="1">
         <v>45628</v>
       </c>
@@ -5429,7 +5429,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="61" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C61" s="1">
         <v>45621</v>
       </c>
@@ -5443,7 +5443,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="62" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C62" s="1">
         <v>45614</v>
       </c>
@@ -5457,7 +5457,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="63" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C63" s="1">
         <v>45607</v>
       </c>
@@ -5471,7 +5471,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="64" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C64" s="1">
         <v>45600</v>
       </c>
@@ -5485,7 +5485,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="65" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C65" s="1">
         <v>45579</v>
       </c>
@@ -5499,7 +5499,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="66" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C66" s="1">
         <v>45572</v>
       </c>
@@ -5513,7 +5513,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="67" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C67" s="1">
         <v>45565</v>
       </c>
@@ -5527,7 +5527,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="68" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C68" s="1">
         <v>45537</v>
       </c>
@@ -5541,7 +5541,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="69" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C69" s="1">
         <v>45530</v>
       </c>
@@ -5555,7 +5555,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="70" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C70" s="1">
         <v>45523</v>
       </c>
@@ -5569,7 +5569,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="71" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C71" s="1">
         <v>45516</v>
       </c>
@@ -5583,7 +5583,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="72" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C72" s="1">
         <v>45509</v>
       </c>
@@ -5597,7 +5597,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="73" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C73" s="1">
         <v>45502</v>
       </c>
@@ -5611,7 +5611,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="74" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C74" s="1">
         <v>45495</v>
       </c>
@@ -5625,7 +5625,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="75" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C75" s="1">
         <v>45488</v>
       </c>
@@ -5639,7 +5639,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="76" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C76" s="1">
         <v>45481</v>
       </c>
@@ -5653,7 +5653,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="77" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C77" s="1">
         <v>45474</v>
       </c>
@@ -5667,7 +5667,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="78" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C78" s="1">
         <v>45467</v>
       </c>
@@ -5681,7 +5681,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="79" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C79" s="1">
         <v>45460</v>
       </c>
@@ -5695,7 +5695,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="80" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C80" s="1">
         <v>45453</v>
       </c>
@@ -5709,7 +5709,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="81" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C81" s="1">
         <v>45446</v>
       </c>
@@ -5723,7 +5723,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="82" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C82" s="1">
         <v>45439</v>
       </c>
@@ -5737,7 +5737,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="83" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C83" s="1">
         <v>45432</v>
       </c>
@@ -5751,7 +5751,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="84" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C84" s="1">
         <v>45425</v>
       </c>
@@ -5765,7 +5765,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="85" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C85" s="1">
         <v>45418</v>
       </c>
@@ -5779,7 +5779,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="86" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C86" s="1">
         <v>45411</v>
       </c>
@@ -5793,7 +5793,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="87" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C87" s="1">
         <v>45404</v>
       </c>
@@ -5807,7 +5807,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="88" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C88" s="1">
         <v>45397</v>
       </c>
@@ -5821,7 +5821,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="89" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C89" s="1">
         <v>45390</v>
       </c>
@@ -5835,7 +5835,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="90" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C90" s="1">
         <v>45383</v>
       </c>
@@ -5849,7 +5849,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="91" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C91" s="1">
         <v>45376</v>
       </c>
@@ -5863,7 +5863,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="92" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C92" s="1">
         <v>45369</v>
       </c>
@@ -5877,7 +5877,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="93" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C93" s="1">
         <v>45362</v>
       </c>
@@ -5886,7 +5886,7 @@
       </c>
       <c r="F93" s="1"/>
     </row>
-    <row r="94" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C94" s="1">
         <v>45355</v>
       </c>
@@ -5894,7 +5894,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="95" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C95" s="1">
         <v>45348</v>
       </c>
@@ -5902,7 +5902,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="96" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="3:7" x14ac:dyDescent="0.35">
       <c r="C96" s="1">
         <v>45341</v>
       </c>
@@ -5910,7 +5910,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="97" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C97" s="1">
         <v>45334</v>
       </c>
@@ -5918,7 +5918,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="98" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="98" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C98" s="1">
         <v>45327</v>
       </c>
@@ -5926,7 +5926,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="99" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="99" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C99" s="1">
         <v>45320</v>
       </c>
@@ -5934,7 +5934,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="100" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="100" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C100" s="1">
         <v>45313</v>
       </c>
@@ -5942,7 +5942,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="101" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="101" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C101" s="1">
         <v>45306</v>
       </c>
@@ -5950,7 +5950,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="105" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="105" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D105" s="2"/>
       <c r="E105" s="2"/>
       <c r="F105" s="2"/>
@@ -5966,7 +5966,7 @@
       <c r="P105" s="2"/>
       <c r="Q105" s="2"/>
     </row>
-    <row r="106" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="106" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D106" s="2"/>
       <c r="E106" s="2"/>
       <c r="F106" s="2"/>
@@ -5982,7 +5982,7 @@
       <c r="P106" s="2"/>
       <c r="Q106" s="2"/>
     </row>
-    <row r="107" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="107" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D107" s="2"/>
       <c r="E107" s="2"/>
       <c r="F107" s="2"/>
@@ -5998,7 +5998,7 @@
       <c r="P107" s="2"/>
       <c r="Q107" s="2"/>
     </row>
-    <row r="108" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="108" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D108" s="2"/>
       <c r="E108" s="2"/>
       <c r="F108" s="2"/>
@@ -6014,7 +6014,7 @@
       <c r="P108" s="2"/>
       <c r="Q108" s="2"/>
     </row>
-    <row r="109" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="109" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D109" s="2"/>
       <c r="E109" s="2"/>
       <c r="F109" s="2"/>
@@ -6030,7 +6030,7 @@
       <c r="P109" s="2"/>
       <c r="Q109" s="2"/>
     </row>
-    <row r="110" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="110" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D110" s="2"/>
       <c r="E110" s="2"/>
       <c r="F110" s="2"/>
@@ -6046,7 +6046,7 @@
       <c r="P110" s="2"/>
       <c r="Q110" s="2"/>
     </row>
-    <row r="111" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="111" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D111" s="2"/>
       <c r="E111" s="2"/>
       <c r="F111" s="2"/>
@@ -6062,7 +6062,7 @@
       <c r="P111" s="2"/>
       <c r="Q111" s="2"/>
     </row>
-    <row r="112" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="112" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D112" s="2"/>
       <c r="E112" s="2"/>
       <c r="F112" s="2"/>
@@ -6078,7 +6078,7 @@
       <c r="P112" s="2"/>
       <c r="Q112" s="2"/>
     </row>
-    <row r="113" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="113" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D113" s="2"/>
       <c r="E113" s="2"/>
       <c r="F113" s="2"/>
@@ -6094,7 +6094,7 @@
       <c r="P113" s="2"/>
       <c r="Q113" s="2"/>
     </row>
-    <row r="114" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="114" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D114" s="2"/>
       <c r="E114" s="2"/>
       <c r="F114" s="2"/>
@@ -6110,7 +6110,7 @@
       <c r="P114" s="2"/>
       <c r="Q114" s="2"/>
     </row>
-    <row r="115" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="115" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D115" s="2"/>
       <c r="E115" s="2"/>
       <c r="F115" s="2"/>
@@ -6126,7 +6126,7 @@
       <c r="P115" s="2"/>
       <c r="Q115" s="2"/>
     </row>
-    <row r="116" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="116" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D116" s="2"/>
       <c r="E116" s="2"/>
       <c r="F116" s="2"/>
@@ -6142,7 +6142,7 @@
       <c r="P116" s="2"/>
       <c r="Q116" s="2"/>
     </row>
-    <row r="117" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="117" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D117" s="2"/>
       <c r="E117" s="2"/>
       <c r="F117" s="2"/>
@@ -6158,7 +6158,7 @@
       <c r="P117" s="2"/>
       <c r="Q117" s="2"/>
     </row>
-    <row r="118" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="118" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D118" s="2"/>
       <c r="E118" s="2"/>
       <c r="F118" s="2"/>
@@ -6174,7 +6174,7 @@
       <c r="P118" s="2"/>
       <c r="Q118" s="2"/>
     </row>
-    <row r="119" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="119" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D119" s="2"/>
       <c r="E119" s="2"/>
       <c r="F119" s="2"/>
@@ -6190,7 +6190,7 @@
       <c r="P119" s="2"/>
       <c r="Q119" s="2"/>
     </row>
-    <row r="120" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="120" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D120" s="2"/>
       <c r="E120" s="2"/>
       <c r="F120" s="2"/>
@@ -6206,7 +6206,7 @@
       <c r="P120" s="2"/>
       <c r="Q120" s="2"/>
     </row>
-    <row r="121" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="121" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D121" s="2"/>
       <c r="E121" s="2"/>
       <c r="F121" s="2"/>
@@ -6222,7 +6222,7 @@
       <c r="P121" s="2"/>
       <c r="Q121" s="2"/>
     </row>
-    <row r="122" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="122" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D122" s="2"/>
       <c r="E122" s="2"/>
       <c r="F122" s="2"/>
@@ -6238,7 +6238,7 @@
       <c r="P122" s="2"/>
       <c r="Q122" s="2"/>
     </row>
-    <row r="123" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="123" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D123" s="2"/>
       <c r="E123" s="2"/>
       <c r="F123" s="2"/>
@@ -6254,7 +6254,7 @@
       <c r="P123" s="2"/>
       <c r="Q123" s="2"/>
     </row>
-    <row r="124" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="124" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D124" s="2"/>
       <c r="E124" s="2"/>
       <c r="F124" s="2"/>
@@ -6270,7 +6270,7 @@
       <c r="P124" s="2"/>
       <c r="Q124" s="2"/>
     </row>
-    <row r="125" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="125" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D125" s="2"/>
       <c r="E125" s="2"/>
       <c r="F125" s="2"/>
@@ -6286,7 +6286,7 @@
       <c r="P125" s="2"/>
       <c r="Q125" s="2"/>
     </row>
-    <row r="126" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="126" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D126" s="2"/>
       <c r="E126" s="2"/>
       <c r="F126" s="2"/>
@@ -6302,7 +6302,7 @@
       <c r="P126" s="2"/>
       <c r="Q126" s="2"/>
     </row>
-    <row r="127" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="127" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D127" s="2"/>
       <c r="E127" s="2"/>
       <c r="F127" s="2"/>
@@ -6318,7 +6318,7 @@
       <c r="P127" s="2"/>
       <c r="Q127" s="2"/>
     </row>
-    <row r="128" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="128" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D128" s="2"/>
       <c r="E128" s="2"/>
       <c r="F128" s="2"/>
@@ -6334,7 +6334,7 @@
       <c r="P128" s="2"/>
       <c r="Q128" s="2"/>
     </row>
-    <row r="129" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="129" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D129" s="2"/>
       <c r="E129" s="2"/>
       <c r="F129" s="2"/>
@@ -6350,7 +6350,7 @@
       <c r="P129" s="2"/>
       <c r="Q129" s="2"/>
     </row>
-    <row r="130" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="130" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D130" s="2"/>
       <c r="E130" s="2"/>
       <c r="F130" s="2"/>

</xml_diff>

<commit_message>
LGHUB 2025/9/29 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
- 网站错误 & 本地化问题详见 LGHUB/WebLoc/README.md
</commit_message>
<xml_diff>
--- a/Documents/Graph_PC.xlsx
+++ b/Documents/Graph_PC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4FAA230-B3E9-4621-9D74-905DA1148341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A8B626D-3D2F-4886-BF29-91AA700F1DD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,7 +574,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>9</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4</c:v>
@@ -917,72 +917,72 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$20:$C$28</c:f>
+              <c:f>Sheet1!$C$19:$C$27</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45929</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45922</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45915</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45908</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45901</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45894</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45887</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45880</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45873</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45866</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$20:$D$28</c:f>
+              <c:f>Sheet1!$D$19:$D$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>499</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>496</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>488</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>485</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>471</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>456</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>446</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>443</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>440</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>432</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1086,43 +1086,43 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$20:$C$28</c:f>
+              <c:f>Sheet1!$C$19:$C$27</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45929</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45922</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45915</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45908</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45901</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45894</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45887</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45880</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45873</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45866</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$20:$G$28</c:f>
+              <c:f>Sheet1!$G$19:$G$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1130,28 +1130,28 @@
                   <c:v>455</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>455</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>450</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>444</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>426</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>421</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>415</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>406</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>405</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>406</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1794,7 +1794,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>9</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4</c:v>
@@ -4836,7 +4836,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.35">
@@ -4853,6 +4853,20 @@
       </c>
       <c r="C7">
         <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C19" s="1">
+        <v>45929</v>
+      </c>
+      <c r="D19">
+        <v>499</v>
+      </c>
+      <c r="F19" s="1">
+        <v>45929</v>
+      </c>
+      <c r="G19">
+        <v>455</v>
       </c>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
LGHUB 2025/10/5 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
- 网站错误 & 本地化问题详见 LGHUB/WebLoc/README.md
</commit_message>
<xml_diff>
--- a/Documents/Graph_PC.xlsx
+++ b/Documents/Graph_PC.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A8B626D-3D2F-4886-BF29-91AA700F1DD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D578234-4364-45E1-BE8A-434B9DACE593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,7 +574,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4</c:v>
@@ -917,72 +917,72 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$19:$C$27</c:f>
+              <c:f>Sheet1!$C$18:$C$26</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45936</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45929</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45922</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45915</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45908</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45901</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45894</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45887</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45880</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45873</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$19:$D$27</c:f>
+              <c:f>Sheet1!$D$18:$D$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>507</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>499</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>496</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>488</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>485</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>471</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>456</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>446</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>443</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>440</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1086,43 +1086,43 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$19:$C$27</c:f>
+              <c:f>Sheet1!$C$18:$C$26</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45936</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45929</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45922</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45915</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45908</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45901</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45894</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45887</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45880</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45873</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$19:$G$27</c:f>
+              <c:f>Sheet1!$G$18:$G$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1133,25 +1133,25 @@
                   <c:v>455</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>455</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>450</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>444</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>426</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>421</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>415</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>406</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>405</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1286,7 +1286,7 @@
         <c:axId val="1374569007"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="500"/>
+          <c:max val="520"/>
           <c:min val="400"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1794,7 +1794,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4</c:v>
@@ -4812,7 +4812,7 @@
   <dimension ref="B2:Q130"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D103" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J104" sqref="J104"/>
+      <selection activeCell="K104" sqref="K104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -4836,7 +4836,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.35">
@@ -4853,6 +4853,20 @@
       </c>
       <c r="C7">
         <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C18" s="1">
+        <v>45936</v>
+      </c>
+      <c r="D18">
+        <v>507</v>
+      </c>
+      <c r="F18" s="1">
+        <v>45936</v>
+      </c>
+      <c r="G18">
+        <v>455</v>
       </c>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
LGHUB 2025/10/7 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
- 网站错误 & 本地化问题详见 LGHUB/WebLoc/README.md
</commit_message>
<xml_diff>
--- a/Documents/Graph_PC.xlsx
+++ b/Documents/Graph_PC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D578234-4364-45E1-BE8A-434B9DACE593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59B76FE4-106A-4CF9-BADC-C01055B0E59B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="2" r:id="rId1"/>
@@ -574,13 +574,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>20</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>33</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1127,7 +1127,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>455</c:v>
+                  <c:v>468</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>455</c:v>
@@ -1794,13 +1794,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>20</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>33</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4811,51 +4811,51 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D103" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K104" sqref="K104"/>
+    <sheetView tabSelected="1" topLeftCell="C104" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="J104" sqref="J104"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.35">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C18" s="1">
         <v>45936</v>
       </c>
@@ -4866,10 +4866,10 @@
         <v>45936</v>
       </c>
       <c r="G18">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.35">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C19" s="1">
         <v>45929</v>
       </c>
@@ -4883,7 +4883,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C20" s="1">
         <v>45922</v>
       </c>
@@ -4897,7 +4897,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C21" s="1">
         <v>45915</v>
       </c>
@@ -4911,7 +4911,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C22" s="1">
         <v>45908</v>
       </c>
@@ -4925,7 +4925,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C23" s="1">
         <v>45901</v>
       </c>
@@ -4939,7 +4939,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C24" s="1">
         <v>45894</v>
       </c>
@@ -4953,7 +4953,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C25" s="1">
         <v>45887</v>
       </c>
@@ -4967,7 +4967,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C26" s="1">
         <v>45880</v>
       </c>
@@ -4981,7 +4981,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C27" s="1">
         <v>45873</v>
       </c>
@@ -4995,7 +4995,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C28" s="1">
         <v>45866</v>
       </c>
@@ -5009,7 +5009,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C29" s="1">
         <v>45859</v>
       </c>
@@ -5023,7 +5023,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C30" s="1">
         <v>45852</v>
       </c>
@@ -5037,7 +5037,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C31" s="1">
         <v>45845</v>
       </c>
@@ -5051,7 +5051,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C32" s="1">
         <v>45838</v>
       </c>
@@ -5065,7 +5065,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C33" s="1">
         <v>45831</v>
       </c>
@@ -5079,7 +5079,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="34" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C34" s="1">
         <v>45824</v>
       </c>
@@ -5093,7 +5093,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="35" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C35" s="1">
         <v>45817</v>
       </c>
@@ -5107,7 +5107,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="36" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C36" s="1">
         <v>45810</v>
       </c>
@@ -5121,7 +5121,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="37" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C37" s="1">
         <v>45803</v>
       </c>
@@ -5135,7 +5135,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="38" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C38" s="1">
         <v>45796</v>
       </c>
@@ -5149,7 +5149,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="39" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C39" s="1">
         <v>45789</v>
       </c>
@@ -5163,7 +5163,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="40" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C40" s="1">
         <v>45782</v>
       </c>
@@ -5177,7 +5177,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="41" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C41" s="1">
         <v>45775</v>
       </c>
@@ -5191,7 +5191,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="42" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C42" s="1">
         <v>45768</v>
       </c>
@@ -5205,7 +5205,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="43" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C43" s="1">
         <v>45761</v>
       </c>
@@ -5219,7 +5219,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="44" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C44" s="1">
         <v>45754</v>
       </c>
@@ -5233,7 +5233,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="45" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C45" s="1">
         <v>45747</v>
       </c>
@@ -5247,7 +5247,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="46" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C46" s="1">
         <v>45740</v>
       </c>
@@ -5261,7 +5261,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="47" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C47" s="1">
         <v>45733</v>
       </c>
@@ -5275,7 +5275,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="48" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C48" s="1">
         <v>45726</v>
       </c>
@@ -5289,7 +5289,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="49" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="49" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C49" s="1">
         <v>45719</v>
       </c>
@@ -5303,7 +5303,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="50" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="50" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C50" s="1">
         <v>45712</v>
       </c>
@@ -5317,7 +5317,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="51" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="51" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C51" s="1">
         <v>45705</v>
       </c>
@@ -5331,7 +5331,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="52" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="52" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C52" s="1">
         <v>45698</v>
       </c>
@@ -5345,7 +5345,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="53" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="53" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C53" s="1">
         <v>45691</v>
       </c>
@@ -5359,7 +5359,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="54" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="54" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C54" s="1">
         <v>45684</v>
       </c>
@@ -5373,7 +5373,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="55" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="55" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C55" s="1">
         <v>45677</v>
       </c>
@@ -5387,7 +5387,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="56" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="56" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C56" s="1">
         <v>45670</v>
       </c>
@@ -5401,7 +5401,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="57" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="57" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C57" s="1">
         <v>45663</v>
       </c>
@@ -5415,7 +5415,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="58" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="58" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C58" s="1">
         <v>45642</v>
       </c>
@@ -5429,7 +5429,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="59" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="59" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C59" s="1">
         <v>45635</v>
       </c>
@@ -5443,7 +5443,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="60" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="60" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C60" s="1">
         <v>45628</v>
       </c>
@@ -5457,7 +5457,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="61" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="61" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C61" s="1">
         <v>45621</v>
       </c>
@@ -5471,7 +5471,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="62" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="62" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C62" s="1">
         <v>45614</v>
       </c>
@@ -5485,7 +5485,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="63" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="63" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C63" s="1">
         <v>45607</v>
       </c>
@@ -5499,7 +5499,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="64" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="64" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C64" s="1">
         <v>45600</v>
       </c>
@@ -5513,7 +5513,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="65" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="65" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C65" s="1">
         <v>45579</v>
       </c>
@@ -5527,7 +5527,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="66" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="66" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C66" s="1">
         <v>45572</v>
       </c>
@@ -5541,7 +5541,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="67" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="67" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C67" s="1">
         <v>45565</v>
       </c>
@@ -5555,7 +5555,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="68" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="68" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C68" s="1">
         <v>45537</v>
       </c>
@@ -5569,7 +5569,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="69" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="69" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C69" s="1">
         <v>45530</v>
       </c>
@@ -5583,7 +5583,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="70" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="70" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C70" s="1">
         <v>45523</v>
       </c>
@@ -5597,7 +5597,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="71" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="71" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C71" s="1">
         <v>45516</v>
       </c>
@@ -5611,7 +5611,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="72" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="72" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C72" s="1">
         <v>45509</v>
       </c>
@@ -5625,7 +5625,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="73" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="73" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C73" s="1">
         <v>45502</v>
       </c>
@@ -5639,7 +5639,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="74" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="74" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C74" s="1">
         <v>45495</v>
       </c>
@@ -5653,7 +5653,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="75" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="75" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C75" s="1">
         <v>45488</v>
       </c>
@@ -5667,7 +5667,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="76" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="76" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C76" s="1">
         <v>45481</v>
       </c>
@@ -5681,7 +5681,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="77" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="77" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C77" s="1">
         <v>45474</v>
       </c>
@@ -5695,7 +5695,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="78" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="78" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C78" s="1">
         <v>45467</v>
       </c>
@@ -5709,7 +5709,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="79" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="79" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C79" s="1">
         <v>45460</v>
       </c>
@@ -5723,7 +5723,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="80" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="80" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C80" s="1">
         <v>45453</v>
       </c>
@@ -5737,7 +5737,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="81" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="81" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C81" s="1">
         <v>45446</v>
       </c>
@@ -5751,7 +5751,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="82" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="82" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C82" s="1">
         <v>45439</v>
       </c>
@@ -5765,7 +5765,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="83" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="83" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C83" s="1">
         <v>45432</v>
       </c>
@@ -5779,7 +5779,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="84" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="84" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C84" s="1">
         <v>45425</v>
       </c>
@@ -5793,7 +5793,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="85" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="85" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C85" s="1">
         <v>45418</v>
       </c>
@@ -5807,7 +5807,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="86" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="86" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C86" s="1">
         <v>45411</v>
       </c>
@@ -5821,7 +5821,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="87" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="87" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C87" s="1">
         <v>45404</v>
       </c>
@@ -5835,7 +5835,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="88" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="88" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C88" s="1">
         <v>45397</v>
       </c>
@@ -5849,7 +5849,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="89" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="89" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C89" s="1">
         <v>45390</v>
       </c>
@@ -5863,7 +5863,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="90" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="90" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C90" s="1">
         <v>45383</v>
       </c>
@@ -5877,7 +5877,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="91" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="91" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C91" s="1">
         <v>45376</v>
       </c>
@@ -5891,7 +5891,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="92" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="92" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C92" s="1">
         <v>45369</v>
       </c>
@@ -5905,7 +5905,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="93" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="93" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C93" s="1">
         <v>45362</v>
       </c>
@@ -5914,7 +5914,7 @@
       </c>
       <c r="F93" s="1"/>
     </row>
-    <row r="94" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="94" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C94" s="1">
         <v>45355</v>
       </c>
@@ -5922,7 +5922,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="95" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="95" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C95" s="1">
         <v>45348</v>
       </c>
@@ -5930,7 +5930,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="96" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="96" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C96" s="1">
         <v>45341</v>
       </c>
@@ -5938,7 +5938,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="97" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C97" s="1">
         <v>45334</v>
       </c>
@@ -5946,7 +5946,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="98" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="98" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C98" s="1">
         <v>45327</v>
       </c>
@@ -5954,7 +5954,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="99" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="99" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C99" s="1">
         <v>45320</v>
       </c>
@@ -5962,7 +5962,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="100" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="100" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C100" s="1">
         <v>45313</v>
       </c>
@@ -5970,7 +5970,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="101" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="101" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C101" s="1">
         <v>45306</v>
       </c>
@@ -5978,7 +5978,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="105" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="105" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D105" s="2"/>
       <c r="E105" s="2"/>
       <c r="F105" s="2"/>
@@ -5994,7 +5994,7 @@
       <c r="P105" s="2"/>
       <c r="Q105" s="2"/>
     </row>
-    <row r="106" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="106" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D106" s="2"/>
       <c r="E106" s="2"/>
       <c r="F106" s="2"/>
@@ -6010,7 +6010,7 @@
       <c r="P106" s="2"/>
       <c r="Q106" s="2"/>
     </row>
-    <row r="107" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="107" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D107" s="2"/>
       <c r="E107" s="2"/>
       <c r="F107" s="2"/>
@@ -6026,7 +6026,7 @@
       <c r="P107" s="2"/>
       <c r="Q107" s="2"/>
     </row>
-    <row r="108" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="108" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D108" s="2"/>
       <c r="E108" s="2"/>
       <c r="F108" s="2"/>
@@ -6042,7 +6042,7 @@
       <c r="P108" s="2"/>
       <c r="Q108" s="2"/>
     </row>
-    <row r="109" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="109" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D109" s="2"/>
       <c r="E109" s="2"/>
       <c r="F109" s="2"/>
@@ -6058,7 +6058,7 @@
       <c r="P109" s="2"/>
       <c r="Q109" s="2"/>
     </row>
-    <row r="110" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="110" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D110" s="2"/>
       <c r="E110" s="2"/>
       <c r="F110" s="2"/>
@@ -6074,7 +6074,7 @@
       <c r="P110" s="2"/>
       <c r="Q110" s="2"/>
     </row>
-    <row r="111" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="111" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D111" s="2"/>
       <c r="E111" s="2"/>
       <c r="F111" s="2"/>
@@ -6090,7 +6090,7 @@
       <c r="P111" s="2"/>
       <c r="Q111" s="2"/>
     </row>
-    <row r="112" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="112" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D112" s="2"/>
       <c r="E112" s="2"/>
       <c r="F112" s="2"/>
@@ -6106,7 +6106,7 @@
       <c r="P112" s="2"/>
       <c r="Q112" s="2"/>
     </row>
-    <row r="113" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="113" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D113" s="2"/>
       <c r="E113" s="2"/>
       <c r="F113" s="2"/>
@@ -6122,7 +6122,7 @@
       <c r="P113" s="2"/>
       <c r="Q113" s="2"/>
     </row>
-    <row r="114" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="114" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D114" s="2"/>
       <c r="E114" s="2"/>
       <c r="F114" s="2"/>
@@ -6138,7 +6138,7 @@
       <c r="P114" s="2"/>
       <c r="Q114" s="2"/>
     </row>
-    <row r="115" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="115" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D115" s="2"/>
       <c r="E115" s="2"/>
       <c r="F115" s="2"/>
@@ -6154,7 +6154,7 @@
       <c r="P115" s="2"/>
       <c r="Q115" s="2"/>
     </row>
-    <row r="116" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="116" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D116" s="2"/>
       <c r="E116" s="2"/>
       <c r="F116" s="2"/>
@@ -6170,7 +6170,7 @@
       <c r="P116" s="2"/>
       <c r="Q116" s="2"/>
     </row>
-    <row r="117" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="117" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D117" s="2"/>
       <c r="E117" s="2"/>
       <c r="F117" s="2"/>
@@ -6186,7 +6186,7 @@
       <c r="P117" s="2"/>
       <c r="Q117" s="2"/>
     </row>
-    <row r="118" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="118" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D118" s="2"/>
       <c r="E118" s="2"/>
       <c r="F118" s="2"/>
@@ -6202,7 +6202,7 @@
       <c r="P118" s="2"/>
       <c r="Q118" s="2"/>
     </row>
-    <row r="119" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="119" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D119" s="2"/>
       <c r="E119" s="2"/>
       <c r="F119" s="2"/>
@@ -6218,7 +6218,7 @@
       <c r="P119" s="2"/>
       <c r="Q119" s="2"/>
     </row>
-    <row r="120" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="120" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D120" s="2"/>
       <c r="E120" s="2"/>
       <c r="F120" s="2"/>
@@ -6234,7 +6234,7 @@
       <c r="P120" s="2"/>
       <c r="Q120" s="2"/>
     </row>
-    <row r="121" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="121" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D121" s="2"/>
       <c r="E121" s="2"/>
       <c r="F121" s="2"/>
@@ -6250,7 +6250,7 @@
       <c r="P121" s="2"/>
       <c r="Q121" s="2"/>
     </row>
-    <row r="122" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="122" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D122" s="2"/>
       <c r="E122" s="2"/>
       <c r="F122" s="2"/>
@@ -6266,7 +6266,7 @@
       <c r="P122" s="2"/>
       <c r="Q122" s="2"/>
     </row>
-    <row r="123" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="123" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D123" s="2"/>
       <c r="E123" s="2"/>
       <c r="F123" s="2"/>
@@ -6282,7 +6282,7 @@
       <c r="P123" s="2"/>
       <c r="Q123" s="2"/>
     </row>
-    <row r="124" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="124" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D124" s="2"/>
       <c r="E124" s="2"/>
       <c r="F124" s="2"/>
@@ -6298,7 +6298,7 @@
       <c r="P124" s="2"/>
       <c r="Q124" s="2"/>
     </row>
-    <row r="125" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="125" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D125" s="2"/>
       <c r="E125" s="2"/>
       <c r="F125" s="2"/>
@@ -6314,7 +6314,7 @@
       <c r="P125" s="2"/>
       <c r="Q125" s="2"/>
     </row>
-    <row r="126" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="126" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D126" s="2"/>
       <c r="E126" s="2"/>
       <c r="F126" s="2"/>
@@ -6330,7 +6330,7 @@
       <c r="P126" s="2"/>
       <c r="Q126" s="2"/>
     </row>
-    <row r="127" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="127" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D127" s="2"/>
       <c r="E127" s="2"/>
       <c r="F127" s="2"/>
@@ -6346,7 +6346,7 @@
       <c r="P127" s="2"/>
       <c r="Q127" s="2"/>
     </row>
-    <row r="128" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="128" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D128" s="2"/>
       <c r="E128" s="2"/>
       <c r="F128" s="2"/>
@@ -6362,7 +6362,7 @@
       <c r="P128" s="2"/>
       <c r="Q128" s="2"/>
     </row>
-    <row r="129" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="129" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D129" s="2"/>
       <c r="E129" s="2"/>
       <c r="F129" s="2"/>
@@ -6378,7 +6378,7 @@
       <c r="P129" s="2"/>
       <c r="Q129" s="2"/>
     </row>
-    <row r="130" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="130" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D130" s="2"/>
       <c r="E130" s="2"/>
       <c r="F130" s="2"/>

</xml_diff>

<commit_message>
LGHUB 2025/10/9 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
- 网站错误 & 本地化问题详见 LGHUB/WebLoc/README.md
</commit_message>
<xml_diff>
--- a/Documents/Graph_PC.xlsx
+++ b/Documents/Graph_PC.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59B76FE4-106A-4CF9-BADC-C01055B0E59B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC565FD9-556F-4824-8523-29F73D81166B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,13 +574,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>46</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -958,7 +958,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>507</c:v>
+                  <c:v>509</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>499</c:v>
@@ -1127,7 +1127,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>468</c:v>
+                  <c:v>472</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>455</c:v>
@@ -1794,13 +1794,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>46</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4811,8 +4811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C104" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J104" sqref="J104"/>
+    <sheetView tabSelected="1" topLeftCell="C103" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="K104" sqref="K104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -4836,7 +4836,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
@@ -4844,7 +4844,7 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
@@ -4852,7 +4852,7 @@
         <v>4</v>
       </c>
       <c r="C7">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.25">
@@ -4860,13 +4860,13 @@
         <v>45936</v>
       </c>
       <c r="D18">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="F18" s="1">
         <v>45936</v>
       </c>
       <c r="G18">
-        <v>468</v>
+        <v>472</v>
       </c>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
LGHUB 2025/10/14 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
- 网站错误 & 本地化问题详见 LGHUB/WebLoc/README.md
</commit_message>
<xml_diff>
--- a/Documents/Graph_PC.xlsx
+++ b/Documents/Graph_PC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC565FD9-556F-4824-8523-29F73D81166B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCDD2C56-8BB4-47C0-B92D-896DE86AEBB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,7 +574,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>5</c:v>
@@ -917,72 +917,72 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$18:$C$26</c:f>
+              <c:f>Sheet1!$C$17:$C$25</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45943</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45936</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45929</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45922</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45915</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45908</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45901</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45894</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45887</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45880</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$18:$D$26</c:f>
+              <c:f>Sheet1!$D$17:$D$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>514</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>509</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>499</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>496</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>488</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>485</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>471</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>456</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>446</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>443</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1086,43 +1086,43 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$18:$C$26</c:f>
+              <c:f>Sheet1!$C$17:$C$25</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45943</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45936</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45929</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45922</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45915</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45908</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45901</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45894</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45887</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45880</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$18:$G$26</c:f>
+              <c:f>Sheet1!$G$17:$G$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1130,28 +1130,28 @@
                   <c:v>472</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>455</c:v>
+                  <c:v>472</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>455</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>455</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>450</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>444</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>426</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>421</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>415</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>406</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1286,8 +1286,8 @@
         <c:axId val="1374569007"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="520"/>
-          <c:min val="400"/>
+          <c:max val="530"/>
+          <c:min val="410"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1794,7 +1794,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>5</c:v>
@@ -4811,8 +4811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C103" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="K104" sqref="K104"/>
+    <sheetView tabSelected="1" topLeftCell="B104" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="L104" sqref="L104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -4836,7 +4836,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
@@ -4853,6 +4853,20 @@
       </c>
       <c r="C7">
         <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C17" s="1">
+        <v>45943</v>
+      </c>
+      <c r="D17">
+        <v>514</v>
+      </c>
+      <c r="F17" s="1">
+        <v>45943</v>
+      </c>
+      <c r="G17">
+        <v>472</v>
       </c>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
LGHUB 2025/10/17 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
- 网站错误 & 本地化问题详见 LGHUB/WebLoc/README.md
</commit_message>
<xml_diff>
--- a/Documents/Graph_PC.xlsx
+++ b/Documents/Graph_PC.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29409"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCDD2C56-8BB4-47C0-B92D-896DE86AEBB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B963273E-E1F3-4501-A2F5-E823ECF645A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,13 +574,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1127,7 +1127,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>472</c:v>
+                  <c:v>482</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>472</c:v>
@@ -1794,13 +1794,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4836,7 +4836,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
@@ -4844,7 +4844,7 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
@@ -4852,7 +4852,7 @@
         <v>4</v>
       </c>
       <c r="C7">
-        <v>50</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.25">
@@ -4866,7 +4866,7 @@
         <v>45943</v>
       </c>
       <c r="G17">
-        <v>472</v>
+        <v>482</v>
       </c>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
LGHUB 2025/10/22 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
- 网站错误 & 本地化问题详见 LGHUB/WebLoc/README.md
</commit_message>
<xml_diff>
--- a/Documents/Graph_PC.xlsx
+++ b/Documents/Graph_PC.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29413"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B963273E-E1F3-4501-A2F5-E823ECF645A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E56175E-6A02-4C66-8900-C4781F18B6D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,10 +574,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>60</c:v>
@@ -917,72 +917,72 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$17:$C$25</c:f>
+              <c:f>Sheet1!$C$16:$C$24</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45950</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45943</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45936</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45929</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45922</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45915</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45908</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45901</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45894</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45887</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$17:$D$25</c:f>
+              <c:f>Sheet1!$D$16:$D$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>523</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>514</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>509</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>499</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>496</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>488</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>485</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>471</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>456</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>446</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1086,43 +1086,43 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$17:$C$25</c:f>
+              <c:f>Sheet1!$C$16:$C$24</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45950</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45943</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45936</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45929</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45922</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45915</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45908</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45901</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45894</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45887</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$17:$G$25</c:f>
+              <c:f>Sheet1!$G$16:$G$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -1130,28 +1130,28 @@
                   <c:v>482</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>472</c:v>
+                  <c:v>482</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>455</c:v>
+                  <c:v>472</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>455</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>455</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>450</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>444</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>426</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>421</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>415</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1794,10 +1794,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>60</c:v>
@@ -4811,8 +4811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B104" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="L104" sqref="L104"/>
+    <sheetView tabSelected="1" topLeftCell="C103" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="K104" sqref="K104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -4821,38 +4821,52 @@
     <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7">
         <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C16" s="1">
+        <v>45950</v>
+      </c>
+      <c r="D16">
+        <v>523</v>
+      </c>
+      <c r="F16" s="1">
+        <v>45950</v>
+      </c>
+      <c r="G16">
+        <v>482</v>
       </c>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
LGHUB 2025/10/26 更新 3
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
- 网站错误 & 本地化问题详见 LGHUB/WebLoc/README.md
</commit_message>
<xml_diff>
--- a/Documents/Graph_PC.xlsx
+++ b/Documents/Graph_PC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29417"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E56175E-6A02-4C66-8900-C4781F18B6D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC8AC63B-2553-4096-AE26-327A677FA4AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="2" r:id="rId1"/>
@@ -574,13 +574,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>14</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>60</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -917,43 +917,43 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$16:$C$24</c:f>
+              <c:f>Sheet1!$C$20:$C$28</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45957</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45950</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45943</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45936</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45929</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45922</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45915</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45908</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45901</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45894</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$16:$D$24</c:f>
+              <c:f>Sheet1!$D$20:$D$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -961,28 +961,28 @@
                   <c:v>523</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>523</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>514</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>509</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>499</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>496</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>488</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>485</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>471</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>456</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1086,72 +1086,72 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$16:$C$24</c:f>
+              <c:f>Sheet1!$C$20:$C$28</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45957</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45950</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45943</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45936</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45929</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45922</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45915</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45908</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45901</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45894</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$16:$G$24</c:f>
+              <c:f>Sheet1!$G$20:$G$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>482</c:v>
+                  <c:v>489</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>482</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>472</c:v>
+                  <c:v>482</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>455</c:v>
+                  <c:v>472</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>455</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>455</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>450</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>444</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>426</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>421</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1177,10 +1177,10 @@
         <c:axId val="1374558447"/>
         <c:axId val="1374569007"/>
       </c:lineChart>
-      <c:dateAx>
+      <c:catAx>
         <c:axId val="1374558447"/>
         <c:scaling>
-          <c:orientation val="minMax"/>
+          <c:orientation val="maxMin"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1278,10 +1278,11 @@
         </c:txPr>
         <c:crossAx val="1374569007"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
+        <c:auto val="0"/>
+        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:baseTimeUnit val="days"/>
-      </c:dateAx>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
       <c:valAx>
         <c:axId val="1374569007"/>
         <c:scaling>
@@ -1290,7 +1291,7 @@
           <c:min val="410"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="l"/>
+        <c:axPos val="r"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -1794,13 +1795,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>14</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>60</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4223,13 +4224,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>106422</xdr:colOff>
-      <xdr:row>105</xdr:row>
+      <xdr:row>110</xdr:row>
       <xdr:rowOff>165023</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>120</xdr:row>
+      <xdr:row>125</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4259,13 +4260,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>190501</xdr:colOff>
-      <xdr:row>105</xdr:row>
+      <xdr:row>110</xdr:row>
       <xdr:rowOff>162248</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>124495</xdr:colOff>
-      <xdr:row>120</xdr:row>
+      <xdr:row>125</xdr:row>
       <xdr:rowOff>163286</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4809,1284 +4810,1218 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:Q130"/>
+  <dimension ref="B2:Q135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C103" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="K104" sqref="K104"/>
+    <sheetView tabSelected="1" topLeftCell="D108" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L109" sqref="L109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C16" s="1">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C20" s="1">
+        <v>45957</v>
+      </c>
+      <c r="D20">
+        <v>523</v>
+      </c>
+      <c r="F20" s="1">
+        <v>45957</v>
+      </c>
+      <c r="G20">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C21" s="1">
         <v>45950</v>
       </c>
-      <c r="D16">
+      <c r="D21">
         <v>523</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F21" s="1">
         <v>45950</v>
       </c>
-      <c r="G16">
+      <c r="G21">
         <v>482</v>
       </c>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C17" s="1">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C22" s="1">
         <v>45943</v>
       </c>
-      <c r="D17">
+      <c r="D22">
         <v>514</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F22" s="1">
         <v>45943</v>
       </c>
-      <c r="G17">
+      <c r="G22">
         <v>482</v>
       </c>
     </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C18" s="1">
+    <row r="23" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C23" s="1">
         <v>45936</v>
       </c>
-      <c r="D18">
+      <c r="D23">
         <v>509</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F23" s="1">
         <v>45936</v>
       </c>
-      <c r="G18">
+      <c r="G23">
         <v>472</v>
       </c>
     </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C19" s="1">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C24" s="1">
         <v>45929</v>
       </c>
-      <c r="D19">
+      <c r="D24">
         <v>499</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F24" s="1">
         <v>45929</v>
       </c>
-      <c r="G19">
+      <c r="G24">
         <v>455</v>
       </c>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C20" s="1">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C25" s="1">
         <v>45922</v>
       </c>
-      <c r="D20">
+      <c r="D25">
         <v>496</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F25" s="1">
         <v>45922</v>
       </c>
-      <c r="G20">
+      <c r="G25">
         <v>455</v>
       </c>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C21" s="1">
+    <row r="26" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C26" s="1">
         <v>45915</v>
       </c>
-      <c r="D21">
+      <c r="D26">
         <v>488</v>
       </c>
-      <c r="F21" s="1">
+      <c r="F26" s="1">
         <v>45915</v>
       </c>
-      <c r="G21">
+      <c r="G26">
         <v>450</v>
       </c>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C22" s="1">
+    <row r="27" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C27" s="1">
         <v>45908</v>
       </c>
-      <c r="D22">
+      <c r="D27">
         <v>485</v>
       </c>
-      <c r="F22" s="1">
+      <c r="F27" s="1">
         <v>45908</v>
       </c>
-      <c r="G22">
+      <c r="G27">
         <v>444</v>
       </c>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C23" s="1">
+    <row r="28" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C28" s="1">
         <v>45901</v>
       </c>
-      <c r="D23">
+      <c r="D28">
         <v>471</v>
       </c>
-      <c r="F23" s="1">
+      <c r="F28" s="1">
         <v>45901</v>
       </c>
-      <c r="G23">
+      <c r="G28">
         <v>426</v>
       </c>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C24" s="1">
+    <row r="29" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C29" s="1">
         <v>45894</v>
       </c>
-      <c r="D24">
+      <c r="D29">
         <v>456</v>
       </c>
-      <c r="F24" s="1">
+      <c r="F29" s="1">
         <v>45894</v>
       </c>
-      <c r="G24">
+      <c r="G29">
         <v>421</v>
       </c>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C25" s="1">
+    <row r="30" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C30" s="1">
         <v>45887</v>
       </c>
-      <c r="D25">
+      <c r="D30">
         <v>446</v>
       </c>
-      <c r="F25" s="1">
+      <c r="F30" s="1">
         <v>45887</v>
       </c>
-      <c r="G25">
+      <c r="G30">
         <v>415</v>
       </c>
     </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C26" s="1">
+    <row r="31" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C31" s="1">
         <v>45880</v>
       </c>
-      <c r="D26">
+      <c r="D31">
         <v>443</v>
       </c>
-      <c r="F26" s="1">
+      <c r="F31" s="1">
         <v>45880</v>
       </c>
-      <c r="G26">
+      <c r="G31">
         <v>406</v>
       </c>
     </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C27" s="1">
+    <row r="32" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C32" s="1">
         <v>45873</v>
       </c>
-      <c r="D27">
+      <c r="D32">
         <v>440</v>
       </c>
-      <c r="F27" s="1">
+      <c r="F32" s="1">
         <v>45873</v>
       </c>
-      <c r="G27">
+      <c r="G32">
         <v>405</v>
       </c>
     </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C28" s="1">
+    <row r="33" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C33" s="1">
         <v>45866</v>
       </c>
-      <c r="D28">
+      <c r="D33">
         <v>432</v>
       </c>
-      <c r="F28" s="1">
+      <c r="F33" s="1">
         <v>45866</v>
       </c>
-      <c r="G28">
+      <c r="G33">
         <v>406</v>
       </c>
     </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C29" s="1">
+    <row r="34" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C34" s="1">
         <v>45859</v>
       </c>
-      <c r="D29">
+      <c r="D34">
         <v>430</v>
       </c>
-      <c r="F29" s="1">
+      <c r="F34" s="1">
         <v>45859</v>
       </c>
-      <c r="G29">
+      <c r="G34">
         <v>389</v>
       </c>
     </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C30" s="1">
+    <row r="35" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C35" s="1">
         <v>45852</v>
       </c>
-      <c r="D30">
+      <c r="D35">
         <v>419</v>
       </c>
-      <c r="F30" s="1">
+      <c r="F35" s="1">
         <v>45852</v>
       </c>
-      <c r="G30">
+      <c r="G35">
         <v>386</v>
       </c>
     </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C31" s="1">
+    <row r="36" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C36" s="1">
         <v>45845</v>
       </c>
-      <c r="D31">
+      <c r="D36">
         <v>418</v>
       </c>
-      <c r="F31" s="1">
+      <c r="F36" s="1">
         <v>45845</v>
       </c>
-      <c r="G31">
+      <c r="G36">
         <v>386</v>
       </c>
     </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C32" s="1">
+    <row r="37" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C37" s="1">
         <v>45838</v>
       </c>
-      <c r="D32">
+      <c r="D37">
         <v>416</v>
       </c>
-      <c r="F32" s="1">
+      <c r="F37" s="1">
         <v>45838</v>
       </c>
-      <c r="G32">
+      <c r="G37">
         <v>370</v>
       </c>
     </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C33" s="1">
+    <row r="38" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C38" s="1">
         <v>45831</v>
       </c>
-      <c r="D33">
+      <c r="D38">
         <v>416</v>
       </c>
-      <c r="F33" s="1">
+      <c r="F38" s="1">
         <v>45831</v>
       </c>
-      <c r="G33">
+      <c r="G38">
         <v>370</v>
       </c>
     </row>
-    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C34" s="1">
+    <row r="39" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C39" s="1">
         <v>45824</v>
       </c>
-      <c r="D34">
+      <c r="D39">
         <v>407</v>
       </c>
-      <c r="F34" s="1">
+      <c r="F39" s="1">
         <v>45824</v>
       </c>
-      <c r="G34">
+      <c r="G39">
         <v>369</v>
       </c>
     </row>
-    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C35" s="1">
+    <row r="40" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C40" s="1">
         <v>45817</v>
       </c>
-      <c r="D35">
+      <c r="D40">
         <v>404</v>
       </c>
-      <c r="F35" s="1">
+      <c r="F40" s="1">
         <v>45817</v>
       </c>
-      <c r="G35">
+      <c r="G40">
         <v>359</v>
       </c>
     </row>
-    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C36" s="1">
+    <row r="41" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C41" s="1">
         <v>45810</v>
       </c>
-      <c r="D36">
+      <c r="D41">
         <v>395</v>
       </c>
-      <c r="F36" s="1">
+      <c r="F41" s="1">
         <v>45810</v>
       </c>
-      <c r="G36">
+      <c r="G41">
         <v>360</v>
       </c>
     </row>
-    <row r="37" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C37" s="1">
+    <row r="42" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C42" s="1">
         <v>45803</v>
       </c>
-      <c r="D37">
+      <c r="D42">
         <v>386</v>
       </c>
-      <c r="F37" s="1">
+      <c r="F42" s="1">
         <v>45803</v>
       </c>
-      <c r="G37">
+      <c r="G42">
         <v>354</v>
       </c>
     </row>
-    <row r="38" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C38" s="1">
+    <row r="43" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C43" s="1">
         <v>45796</v>
       </c>
-      <c r="D38">
+      <c r="D43">
         <v>379</v>
       </c>
-      <c r="F38" s="1">
+      <c r="F43" s="1">
         <v>45796</v>
       </c>
-      <c r="G38">
+      <c r="G43">
         <v>349</v>
       </c>
     </row>
-    <row r="39" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C39" s="1">
+    <row r="44" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C44" s="1">
         <v>45789</v>
       </c>
-      <c r="D39">
+      <c r="D44">
         <v>365</v>
       </c>
-      <c r="F39" s="1">
+      <c r="F44" s="1">
         <v>45789</v>
       </c>
-      <c r="G39">
+      <c r="G44">
         <v>320</v>
       </c>
     </row>
-    <row r="40" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C40" s="1">
+    <row r="45" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C45" s="1">
         <v>45782</v>
       </c>
-      <c r="D40">
+      <c r="D45">
         <v>356</v>
       </c>
-      <c r="F40" s="1">
+      <c r="F45" s="1">
         <v>45782</v>
       </c>
-      <c r="G40">
+      <c r="G45">
         <v>320</v>
       </c>
     </row>
-    <row r="41" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C41" s="1">
+    <row r="46" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C46" s="1">
         <v>45775</v>
       </c>
-      <c r="D41">
+      <c r="D46">
         <v>348</v>
       </c>
-      <c r="F41" s="1">
+      <c r="F46" s="1">
         <v>45775</v>
       </c>
-      <c r="G41">
+      <c r="G46">
         <v>320</v>
       </c>
     </row>
-    <row r="42" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C42" s="1">
+    <row r="47" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C47" s="1">
         <v>45768</v>
       </c>
-      <c r="D42">
+      <c r="D47">
         <v>343</v>
       </c>
-      <c r="F42" s="1">
+      <c r="F47" s="1">
         <v>45768</v>
       </c>
-      <c r="G42">
+      <c r="G47">
         <v>319</v>
       </c>
     </row>
-    <row r="43" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C43" s="1">
+    <row r="48" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C48" s="1">
         <v>45761</v>
       </c>
-      <c r="D43">
+      <c r="D48">
         <v>334</v>
       </c>
-      <c r="F43" s="1">
+      <c r="F48" s="1">
         <v>45761</v>
       </c>
-      <c r="G43">
+      <c r="G48">
         <v>303</v>
       </c>
     </row>
-    <row r="44" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C44" s="1">
+    <row r="49" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C49" s="1">
         <v>45754</v>
       </c>
-      <c r="D44">
+      <c r="D49">
         <v>330</v>
       </c>
-      <c r="F44" s="1">
+      <c r="F49" s="1">
         <v>45754</v>
       </c>
-      <c r="G44">
+      <c r="G49">
         <v>302</v>
       </c>
     </row>
-    <row r="45" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C45" s="1">
+    <row r="50" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C50" s="1">
         <v>45747</v>
       </c>
-      <c r="D45">
+      <c r="D50">
         <v>325</v>
       </c>
-      <c r="F45" s="1">
+      <c r="F50" s="1">
         <v>45747</v>
       </c>
-      <c r="G45">
+      <c r="G50">
         <v>302</v>
       </c>
     </row>
-    <row r="46" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C46" s="1">
+    <row r="51" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C51" s="1">
         <v>45740</v>
       </c>
-      <c r="D46">
+      <c r="D51">
         <v>316</v>
       </c>
-      <c r="F46" s="1">
+      <c r="F51" s="1">
         <v>45740</v>
       </c>
-      <c r="G46">
+      <c r="G51">
         <v>296</v>
       </c>
     </row>
-    <row r="47" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C47" s="1">
+    <row r="52" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C52" s="1">
         <v>45733</v>
       </c>
-      <c r="D47">
+      <c r="D52">
         <v>310</v>
       </c>
-      <c r="F47" s="1">
+      <c r="F52" s="1">
         <v>45733</v>
       </c>
-      <c r="G47">
+      <c r="G52">
         <v>296</v>
       </c>
     </row>
-    <row r="48" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C48" s="1">
+    <row r="53" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C53" s="1">
         <v>45726</v>
       </c>
-      <c r="D48">
+      <c r="D53">
         <v>309</v>
       </c>
-      <c r="F48" s="1">
+      <c r="F53" s="1">
         <v>45726</v>
       </c>
-      <c r="G48">
+      <c r="G53">
         <v>294</v>
       </c>
     </row>
-    <row r="49" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C49" s="1">
+    <row r="54" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C54" s="1">
         <v>45719</v>
       </c>
-      <c r="D49">
+      <c r="D54">
         <v>308</v>
       </c>
-      <c r="F49" s="1">
+      <c r="F54" s="1">
         <v>45719</v>
       </c>
-      <c r="G49">
+      <c r="G54">
         <v>286</v>
       </c>
     </row>
-    <row r="50" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C50" s="1">
+    <row r="55" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C55" s="1">
         <v>45712</v>
       </c>
-      <c r="D50">
+      <c r="D55">
         <v>306</v>
       </c>
-      <c r="F50" s="1">
+      <c r="F55" s="1">
         <v>45712</v>
       </c>
-      <c r="G50">
+      <c r="G55">
         <v>286</v>
       </c>
     </row>
-    <row r="51" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C51" s="1">
+    <row r="56" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C56" s="1">
         <v>45705</v>
       </c>
-      <c r="D51">
+      <c r="D56">
         <v>301</v>
       </c>
-      <c r="F51" s="1">
+      <c r="F56" s="1">
         <v>45705</v>
       </c>
-      <c r="G51">
+      <c r="G56">
         <v>267</v>
       </c>
     </row>
-    <row r="52" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C52" s="1">
+    <row r="57" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C57" s="1">
         <v>45698</v>
       </c>
-      <c r="D52">
+      <c r="D57">
         <v>295</v>
       </c>
-      <c r="F52" s="1">
+      <c r="F57" s="1">
         <v>45698</v>
       </c>
-      <c r="G52">
+      <c r="G57">
         <v>267</v>
       </c>
     </row>
-    <row r="53" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C53" s="1">
+    <row r="58" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C58" s="1">
         <v>45691</v>
       </c>
-      <c r="D53">
+      <c r="D58">
         <v>289</v>
       </c>
-      <c r="F53" s="1">
+      <c r="F58" s="1">
         <v>45691</v>
       </c>
-      <c r="G53">
+      <c r="G58">
         <v>267</v>
       </c>
     </row>
-    <row r="54" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C54" s="1">
+    <row r="59" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C59" s="1">
         <v>45684</v>
       </c>
-      <c r="D54">
+      <c r="D59">
         <v>284</v>
       </c>
-      <c r="F54" s="1">
+      <c r="F59" s="1">
         <v>45684</v>
       </c>
-      <c r="G54">
+      <c r="G59">
         <v>262</v>
       </c>
     </row>
-    <row r="55" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C55" s="1">
+    <row r="60" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C60" s="1">
         <v>45677</v>
       </c>
-      <c r="D55">
+      <c r="D60">
         <v>273</v>
       </c>
-      <c r="F55" s="1">
+      <c r="F60" s="1">
         <v>45677</v>
       </c>
-      <c r="G55">
+      <c r="G60">
         <v>254</v>
       </c>
     </row>
-    <row r="56" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C56" s="1">
+    <row r="61" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C61" s="1">
         <v>45670</v>
       </c>
-      <c r="D56">
+      <c r="D61">
         <v>264</v>
       </c>
-      <c r="F56" s="1">
+      <c r="F61" s="1">
         <v>45670</v>
       </c>
-      <c r="G56">
+      <c r="G61">
         <v>250</v>
       </c>
     </row>
-    <row r="57" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C57" s="1">
+    <row r="62" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C62" s="1">
         <v>45663</v>
       </c>
-      <c r="D57">
+      <c r="D62">
         <v>256</v>
       </c>
-      <c r="F57" s="1">
+      <c r="F62" s="1">
         <v>45663</v>
       </c>
-      <c r="G57">
+      <c r="G62">
         <v>250</v>
       </c>
     </row>
-    <row r="58" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C58" s="1">
+    <row r="63" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C63" s="1">
         <v>45642</v>
       </c>
-      <c r="D58">
+      <c r="D63">
         <v>256</v>
       </c>
-      <c r="F58" s="1">
+      <c r="F63" s="1">
         <v>45642</v>
       </c>
-      <c r="G58">
+      <c r="G63">
         <v>245</v>
       </c>
     </row>
-    <row r="59" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C59" s="1">
+    <row r="64" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C64" s="1">
         <v>45635</v>
       </c>
-      <c r="D59">
+      <c r="D64">
         <v>251</v>
       </c>
-      <c r="F59" s="1">
+      <c r="F64" s="1">
         <v>45635</v>
       </c>
-      <c r="G59">
+      <c r="G64">
         <v>243</v>
       </c>
     </row>
-    <row r="60" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C60" s="1">
+    <row r="65" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C65" s="1">
         <v>45628</v>
       </c>
-      <c r="D60">
+      <c r="D65">
         <v>251</v>
       </c>
-      <c r="F60" s="1">
+      <c r="F65" s="1">
         <v>45628</v>
       </c>
-      <c r="G60">
+      <c r="G65">
         <v>239</v>
       </c>
     </row>
-    <row r="61" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C61" s="1">
+    <row r="66" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C66" s="1">
         <v>45621</v>
       </c>
-      <c r="D61">
+      <c r="D66">
         <v>247</v>
       </c>
-      <c r="F61" s="1">
+      <c r="F66" s="1">
         <v>45621</v>
       </c>
-      <c r="G61">
+      <c r="G66">
         <v>234</v>
       </c>
     </row>
-    <row r="62" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C62" s="1">
+    <row r="67" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C67" s="1">
         <v>45614</v>
       </c>
-      <c r="D62">
+      <c r="D67">
         <v>241</v>
       </c>
-      <c r="F62" s="1">
+      <c r="F67" s="1">
         <v>45614</v>
       </c>
-      <c r="G62">
+      <c r="G67">
         <v>234</v>
       </c>
     </row>
-    <row r="63" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C63" s="1">
+    <row r="68" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C68" s="1">
         <v>45607</v>
       </c>
-      <c r="D63">
+      <c r="D68">
         <v>239</v>
       </c>
-      <c r="F63" s="1">
+      <c r="F68" s="1">
         <v>45607</v>
       </c>
-      <c r="G63">
+      <c r="G68">
         <v>230</v>
       </c>
     </row>
-    <row r="64" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C64" s="1">
+    <row r="69" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C69" s="1">
         <v>45600</v>
       </c>
-      <c r="D64">
+      <c r="D69">
         <v>232</v>
       </c>
-      <c r="F64" s="1">
+      <c r="F69" s="1">
         <v>45600</v>
       </c>
-      <c r="G64">
+      <c r="G69">
         <v>227</v>
       </c>
     </row>
-    <row r="65" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C65" s="1">
+    <row r="70" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C70" s="1">
         <v>45579</v>
       </c>
-      <c r="D65">
+      <c r="D70">
         <v>231</v>
       </c>
-      <c r="F65" s="1">
+      <c r="F70" s="1">
         <v>45579</v>
       </c>
-      <c r="G65">
+      <c r="G70">
         <v>222</v>
       </c>
     </row>
-    <row r="66" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C66" s="1">
+    <row r="71" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C71" s="1">
         <v>45572</v>
       </c>
-      <c r="D66">
+      <c r="D71">
         <v>227</v>
       </c>
-      <c r="F66" s="1">
+      <c r="F71" s="1">
         <v>45572</v>
       </c>
-      <c r="G66">
+      <c r="G71">
         <v>216</v>
       </c>
     </row>
-    <row r="67" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C67" s="1">
+    <row r="72" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C72" s="1">
         <v>45565</v>
       </c>
-      <c r="D67">
+      <c r="D72">
         <v>223</v>
       </c>
-      <c r="F67" s="1">
+      <c r="F72" s="1">
         <v>45565</v>
       </c>
-      <c r="G67">
+      <c r="G72">
         <v>216</v>
       </c>
     </row>
-    <row r="68" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C68" s="1">
+    <row r="73" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C73" s="1">
         <v>45537</v>
       </c>
-      <c r="D68">
+      <c r="D73">
         <v>218</v>
       </c>
-      <c r="F68" s="1">
+      <c r="F73" s="1">
         <v>45537</v>
       </c>
-      <c r="G68">
+      <c r="G73">
         <v>207</v>
       </c>
     </row>
-    <row r="69" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C69" s="1">
+    <row r="74" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C74" s="1">
         <v>45530</v>
       </c>
-      <c r="D69">
+      <c r="D74">
         <v>217</v>
       </c>
-      <c r="F69" s="1">
+      <c r="F74" s="1">
         <v>45530</v>
       </c>
-      <c r="G69">
+      <c r="G74">
         <v>207</v>
       </c>
     </row>
-    <row r="70" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C70" s="1">
+    <row r="75" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C75" s="1">
         <v>45523</v>
       </c>
-      <c r="D70">
+      <c r="D75">
         <v>216</v>
       </c>
-      <c r="F70" s="1">
+      <c r="F75" s="1">
         <v>45523</v>
       </c>
-      <c r="G70">
+      <c r="G75">
         <v>200</v>
       </c>
     </row>
-    <row r="71" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C71" s="1">
+    <row r="76" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C76" s="1">
         <v>45516</v>
       </c>
-      <c r="D71">
+      <c r="D76">
         <v>212</v>
       </c>
-      <c r="F71" s="1">
+      <c r="F76" s="1">
         <v>45516</v>
       </c>
-      <c r="G71">
+      <c r="G76">
         <v>190</v>
       </c>
     </row>
-    <row r="72" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C72" s="1">
+    <row r="77" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C77" s="1">
         <v>45509</v>
       </c>
-      <c r="D72">
+      <c r="D77">
         <v>210</v>
       </c>
-      <c r="F72" s="1">
+      <c r="F77" s="1">
         <v>45509</v>
       </c>
-      <c r="G72">
+      <c r="G77">
         <v>189</v>
       </c>
     </row>
-    <row r="73" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C73" s="1">
+    <row r="78" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C78" s="1">
         <v>45502</v>
       </c>
-      <c r="D73">
+      <c r="D78">
         <v>210</v>
       </c>
-      <c r="F73" s="1">
+      <c r="F78" s="1">
         <v>45502</v>
       </c>
-      <c r="G73">
+      <c r="G78">
         <v>189</v>
       </c>
     </row>
-    <row r="74" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C74" s="1">
+    <row r="79" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C79" s="1">
         <v>45495</v>
       </c>
-      <c r="D74">
+      <c r="D79">
         <v>201</v>
       </c>
-      <c r="F74" s="1">
+      <c r="F79" s="1">
         <v>45495</v>
       </c>
-      <c r="G74">
+      <c r="G79">
         <v>183</v>
       </c>
     </row>
-    <row r="75" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C75" s="1">
+    <row r="80" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C80" s="1">
         <v>45488</v>
       </c>
-      <c r="D75">
+      <c r="D80">
         <v>199</v>
       </c>
-      <c r="F75" s="1">
+      <c r="F80" s="1">
         <v>45488</v>
       </c>
-      <c r="G75">
+      <c r="G80">
         <v>182</v>
       </c>
     </row>
-    <row r="76" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C76" s="1">
+    <row r="81" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C81" s="1">
         <v>45481</v>
       </c>
-      <c r="D76">
+      <c r="D81">
         <v>188</v>
       </c>
-      <c r="F76" s="1">
+      <c r="F81" s="1">
         <v>45481</v>
       </c>
-      <c r="G76">
+      <c r="G81">
         <v>180</v>
       </c>
     </row>
-    <row r="77" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C77" s="1">
+    <row r="82" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C82" s="1">
         <v>45474</v>
       </c>
-      <c r="D77">
+      <c r="D82">
         <v>187</v>
       </c>
-      <c r="F77" s="1">
+      <c r="F82" s="1">
         <v>45474</v>
       </c>
-      <c r="G77">
+      <c r="G82">
         <v>172</v>
       </c>
     </row>
-    <row r="78" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C78" s="1">
+    <row r="83" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C83" s="1">
         <v>45467</v>
       </c>
-      <c r="D78">
+      <c r="D83">
         <v>187</v>
       </c>
-      <c r="F78" s="1">
+      <c r="F83" s="1">
         <v>45467</v>
       </c>
-      <c r="G78">
+      <c r="G83">
         <v>172</v>
       </c>
     </row>
-    <row r="79" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C79" s="1">
+    <row r="84" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C84" s="1">
         <v>45460</v>
       </c>
-      <c r="D79">
+      <c r="D84">
         <v>185</v>
       </c>
-      <c r="F79" s="1">
+      <c r="F84" s="1">
         <v>45460</v>
       </c>
-      <c r="G79">
+      <c r="G84">
         <v>165</v>
       </c>
     </row>
-    <row r="80" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C80" s="1">
+    <row r="85" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C85" s="1">
         <v>45453</v>
       </c>
-      <c r="D80">
+      <c r="D85">
         <v>180</v>
       </c>
-      <c r="F80" s="1">
+      <c r="F85" s="1">
         <v>45453</v>
       </c>
-      <c r="G80">
+      <c r="G85">
         <v>164</v>
       </c>
     </row>
-    <row r="81" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C81" s="1">
+    <row r="86" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C86" s="1">
         <v>45446</v>
       </c>
-      <c r="D81">
+      <c r="D86">
         <v>177</v>
       </c>
-      <c r="F81" s="1">
+      <c r="F86" s="1">
         <v>45446</v>
       </c>
-      <c r="G81">
+      <c r="G86">
         <v>161</v>
       </c>
     </row>
-    <row r="82" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C82" s="1">
+    <row r="87" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C87" s="1">
         <v>45439</v>
       </c>
-      <c r="D82">
+      <c r="D87">
         <v>174</v>
       </c>
-      <c r="F82" s="1">
+      <c r="F87" s="1">
         <v>45439</v>
       </c>
-      <c r="G82">
+      <c r="G87">
         <v>161</v>
       </c>
     </row>
-    <row r="83" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C83" s="1">
+    <row r="88" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C88" s="1">
         <v>45432</v>
       </c>
-      <c r="D83">
+      <c r="D88">
         <v>173</v>
       </c>
-      <c r="F83" s="1">
+      <c r="F88" s="1">
         <v>45432</v>
       </c>
-      <c r="G83">
+      <c r="G88">
         <v>159</v>
       </c>
     </row>
-    <row r="84" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C84" s="1">
+    <row r="89" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C89" s="1">
         <v>45425</v>
       </c>
-      <c r="D84">
+      <c r="D89">
         <v>170</v>
       </c>
-      <c r="F84" s="1">
+      <c r="F89" s="1">
         <v>45425</v>
       </c>
-      <c r="G84">
+      <c r="G89">
         <v>157</v>
       </c>
     </row>
-    <row r="85" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C85" s="1">
+    <row r="90" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C90" s="1">
         <v>45418</v>
       </c>
-      <c r="D85">
+      <c r="D90">
         <v>170</v>
       </c>
-      <c r="F85" s="1">
+      <c r="F90" s="1">
         <v>45418</v>
       </c>
-      <c r="G85">
+      <c r="G90">
         <v>141</v>
       </c>
     </row>
-    <row r="86" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C86" s="1">
+    <row r="91" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C91" s="1">
         <v>45411</v>
       </c>
-      <c r="D86">
+      <c r="D91">
         <v>166</v>
       </c>
-      <c r="F86" s="1">
+      <c r="F91" s="1">
         <v>45411</v>
       </c>
-      <c r="G86">
+      <c r="G91">
         <v>141</v>
       </c>
     </row>
-    <row r="87" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C87" s="1">
+    <row r="92" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C92" s="1">
         <v>45404</v>
       </c>
-      <c r="D87">
+      <c r="D92">
         <v>166</v>
       </c>
-      <c r="F87" s="1">
+      <c r="F92" s="1">
         <v>45404</v>
       </c>
-      <c r="G87">
+      <c r="G92">
         <v>141</v>
       </c>
     </row>
-    <row r="88" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C88" s="1">
+    <row r="93" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C93" s="1">
         <v>45397</v>
       </c>
-      <c r="D88">
+      <c r="D93">
         <v>157</v>
       </c>
-      <c r="F88" s="1">
+      <c r="F93" s="1">
         <v>45397</v>
       </c>
-      <c r="G88">
+      <c r="G93">
         <v>132</v>
       </c>
     </row>
-    <row r="89" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C89" s="1">
+    <row r="94" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C94" s="1">
         <v>45390</v>
       </c>
-      <c r="D89">
+      <c r="D94">
         <v>146</v>
       </c>
-      <c r="F89" s="1">
+      <c r="F94" s="1">
         <v>45390</v>
       </c>
-      <c r="G89">
+      <c r="G94">
         <v>132</v>
       </c>
     </row>
-    <row r="90" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C90" s="1">
+    <row r="95" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C95" s="1">
         <v>45383</v>
       </c>
-      <c r="D90">
+      <c r="D95">
         <v>138</v>
       </c>
-      <c r="F90" s="1">
+      <c r="F95" s="1">
         <v>45383</v>
       </c>
-      <c r="G90">
+      <c r="G95">
         <v>119</v>
       </c>
     </row>
-    <row r="91" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C91" s="1">
+    <row r="96" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C96" s="1">
         <v>45376</v>
       </c>
-      <c r="D91">
+      <c r="D96">
         <v>129</v>
       </c>
-      <c r="F91" s="1">
+      <c r="F96" s="1">
         <v>45376</v>
       </c>
-      <c r="G91">
+      <c r="G96">
         <v>114</v>
       </c>
     </row>
-    <row r="92" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C92" s="1">
+    <row r="97" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C97" s="1">
         <v>45369</v>
       </c>
-      <c r="D92">
+      <c r="D97">
         <v>123</v>
       </c>
-      <c r="F92" s="1">
+      <c r="F97" s="1">
         <v>45369</v>
       </c>
-      <c r="G92">
+      <c r="G97">
         <v>97</v>
       </c>
     </row>
-    <row r="93" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C93" s="1">
+    <row r="98" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C98" s="1">
         <v>45362</v>
       </c>
-      <c r="D93">
+      <c r="D98">
         <v>113</v>
       </c>
-      <c r="F93" s="1"/>
-    </row>
-    <row r="94" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C94" s="1">
+      <c r="F98" s="1"/>
+    </row>
+    <row r="99" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C99" s="1">
         <v>45355</v>
       </c>
-      <c r="D94">
+      <c r="D99">
         <v>108</v>
       </c>
     </row>
-    <row r="95" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C95" s="1">
+    <row r="100" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C100" s="1">
         <v>45348</v>
       </c>
-      <c r="D95">
+      <c r="D100">
         <v>102</v>
       </c>
     </row>
-    <row r="96" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C96" s="1">
+    <row r="101" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C101" s="1">
         <v>45341</v>
       </c>
-      <c r="D96">
+      <c r="D101">
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C97" s="1">
+    <row r="102" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C102" s="1">
         <v>45334</v>
       </c>
-      <c r="D97">
+      <c r="D102">
         <v>80</v>
       </c>
     </row>
-    <row r="98" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C98" s="1">
+    <row r="103" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C103" s="1">
         <v>45327</v>
       </c>
-      <c r="D98">
+      <c r="D103">
         <v>66</v>
       </c>
     </row>
-    <row r="99" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C99" s="1">
+    <row r="104" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C104" s="1">
         <v>45320</v>
       </c>
-      <c r="D99">
+      <c r="D104">
         <v>55</v>
       </c>
     </row>
-    <row r="100" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C100" s="1">
+    <row r="105" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C105" s="1">
         <v>45313</v>
       </c>
-      <c r="D100">
+      <c r="D105">
         <v>53</v>
       </c>
     </row>
-    <row r="101" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C101" s="1">
+    <row r="106" spans="3:17" x14ac:dyDescent="0.35">
+      <c r="C106" s="1">
         <v>45306</v>
       </c>
-      <c r="D101">
+      <c r="D106">
         <v>52</v>
       </c>
     </row>
-    <row r="105" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="D105" s="2"/>
-      <c r="E105" s="2"/>
-      <c r="F105" s="2"/>
-      <c r="G105" s="2"/>
-      <c r="H105" s="2"/>
-      <c r="I105" s="2"/>
-      <c r="J105" s="2"/>
-      <c r="K105" s="2"/>
-      <c r="L105" s="2"/>
-      <c r="M105" s="2"/>
-      <c r="N105" s="2"/>
-      <c r="O105" s="2"/>
-      <c r="P105" s="2"/>
-      <c r="Q105" s="2"/>
-    </row>
-    <row r="106" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="D106" s="2"/>
-      <c r="E106" s="2"/>
-      <c r="F106" s="2"/>
-      <c r="G106" s="2"/>
-      <c r="H106" s="2"/>
-      <c r="I106" s="2"/>
-      <c r="J106" s="2"/>
-      <c r="K106" s="2"/>
-      <c r="L106" s="2"/>
-      <c r="M106" s="2"/>
-      <c r="N106" s="2"/>
-      <c r="O106" s="2"/>
-      <c r="P106" s="2"/>
-      <c r="Q106" s="2"/>
-    </row>
-    <row r="107" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="D107" s="2"/>
-      <c r="E107" s="2"/>
-      <c r="F107" s="2"/>
-      <c r="G107" s="2"/>
-      <c r="H107" s="2"/>
-      <c r="I107" s="2"/>
-      <c r="J107" s="2"/>
-      <c r="K107" s="2"/>
-      <c r="L107" s="2"/>
-      <c r="M107" s="2"/>
-      <c r="N107" s="2"/>
-      <c r="O107" s="2"/>
-      <c r="P107" s="2"/>
-      <c r="Q107" s="2"/>
-    </row>
-    <row r="108" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="D108" s="2"/>
-      <c r="E108" s="2"/>
-      <c r="F108" s="2"/>
-      <c r="G108" s="2"/>
-      <c r="H108" s="2"/>
-      <c r="I108" s="2"/>
-      <c r="J108" s="2"/>
-      <c r="K108" s="2"/>
-      <c r="L108" s="2"/>
-      <c r="M108" s="2"/>
-      <c r="N108" s="2"/>
-      <c r="O108" s="2"/>
-      <c r="P108" s="2"/>
-      <c r="Q108" s="2"/>
-    </row>
-    <row r="109" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="D109" s="2"/>
-      <c r="E109" s="2"/>
-      <c r="F109" s="2"/>
-      <c r="G109" s="2"/>
-      <c r="H109" s="2"/>
-      <c r="I109" s="2"/>
-      <c r="J109" s="2"/>
-      <c r="K109" s="2"/>
-      <c r="L109" s="2"/>
-      <c r="M109" s="2"/>
-      <c r="N109" s="2"/>
-      <c r="O109" s="2"/>
-      <c r="P109" s="2"/>
-      <c r="Q109" s="2"/>
-    </row>
-    <row r="110" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="110" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D110" s="2"/>
       <c r="E110" s="2"/>
       <c r="F110" s="2"/>
@@ -6102,7 +6037,7 @@
       <c r="P110" s="2"/>
       <c r="Q110" s="2"/>
     </row>
-    <row r="111" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="111" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D111" s="2"/>
       <c r="E111" s="2"/>
       <c r="F111" s="2"/>
@@ -6118,7 +6053,7 @@
       <c r="P111" s="2"/>
       <c r="Q111" s="2"/>
     </row>
-    <row r="112" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="112" spans="3:17" x14ac:dyDescent="0.35">
       <c r="D112" s="2"/>
       <c r="E112" s="2"/>
       <c r="F112" s="2"/>
@@ -6134,7 +6069,7 @@
       <c r="P112" s="2"/>
       <c r="Q112" s="2"/>
     </row>
-    <row r="113" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="113" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D113" s="2"/>
       <c r="E113" s="2"/>
       <c r="F113" s="2"/>
@@ -6150,7 +6085,7 @@
       <c r="P113" s="2"/>
       <c r="Q113" s="2"/>
     </row>
-    <row r="114" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="114" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D114" s="2"/>
       <c r="E114" s="2"/>
       <c r="F114" s="2"/>
@@ -6166,7 +6101,7 @@
       <c r="P114" s="2"/>
       <c r="Q114" s="2"/>
     </row>
-    <row r="115" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="115" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D115" s="2"/>
       <c r="E115" s="2"/>
       <c r="F115" s="2"/>
@@ -6182,7 +6117,7 @@
       <c r="P115" s="2"/>
       <c r="Q115" s="2"/>
     </row>
-    <row r="116" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="116" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D116" s="2"/>
       <c r="E116" s="2"/>
       <c r="F116" s="2"/>
@@ -6198,7 +6133,7 @@
       <c r="P116" s="2"/>
       <c r="Q116" s="2"/>
     </row>
-    <row r="117" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="117" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D117" s="2"/>
       <c r="E117" s="2"/>
       <c r="F117" s="2"/>
@@ -6214,7 +6149,7 @@
       <c r="P117" s="2"/>
       <c r="Q117" s="2"/>
     </row>
-    <row r="118" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="118" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D118" s="2"/>
       <c r="E118" s="2"/>
       <c r="F118" s="2"/>
@@ -6230,7 +6165,7 @@
       <c r="P118" s="2"/>
       <c r="Q118" s="2"/>
     </row>
-    <row r="119" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="119" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D119" s="2"/>
       <c r="E119" s="2"/>
       <c r="F119" s="2"/>
@@ -6246,7 +6181,7 @@
       <c r="P119" s="2"/>
       <c r="Q119" s="2"/>
     </row>
-    <row r="120" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="120" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D120" s="2"/>
       <c r="E120" s="2"/>
       <c r="F120" s="2"/>
@@ -6262,7 +6197,7 @@
       <c r="P120" s="2"/>
       <c r="Q120" s="2"/>
     </row>
-    <row r="121" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="121" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D121" s="2"/>
       <c r="E121" s="2"/>
       <c r="F121" s="2"/>
@@ -6278,7 +6213,7 @@
       <c r="P121" s="2"/>
       <c r="Q121" s="2"/>
     </row>
-    <row r="122" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="122" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D122" s="2"/>
       <c r="E122" s="2"/>
       <c r="F122" s="2"/>
@@ -6294,7 +6229,7 @@
       <c r="P122" s="2"/>
       <c r="Q122" s="2"/>
     </row>
-    <row r="123" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="123" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D123" s="2"/>
       <c r="E123" s="2"/>
       <c r="F123" s="2"/>
@@ -6310,7 +6245,7 @@
       <c r="P123" s="2"/>
       <c r="Q123" s="2"/>
     </row>
-    <row r="124" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="124" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D124" s="2"/>
       <c r="E124" s="2"/>
       <c r="F124" s="2"/>
@@ -6326,7 +6261,7 @@
       <c r="P124" s="2"/>
       <c r="Q124" s="2"/>
     </row>
-    <row r="125" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="125" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D125" s="2"/>
       <c r="E125" s="2"/>
       <c r="F125" s="2"/>
@@ -6342,7 +6277,7 @@
       <c r="P125" s="2"/>
       <c r="Q125" s="2"/>
     </row>
-    <row r="126" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="126" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D126" s="2"/>
       <c r="E126" s="2"/>
       <c r="F126" s="2"/>
@@ -6358,7 +6293,7 @@
       <c r="P126" s="2"/>
       <c r="Q126" s="2"/>
     </row>
-    <row r="127" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="127" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D127" s="2"/>
       <c r="E127" s="2"/>
       <c r="F127" s="2"/>
@@ -6374,7 +6309,7 @@
       <c r="P127" s="2"/>
       <c r="Q127" s="2"/>
     </row>
-    <row r="128" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="128" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D128" s="2"/>
       <c r="E128" s="2"/>
       <c r="F128" s="2"/>
@@ -6390,7 +6325,7 @@
       <c r="P128" s="2"/>
       <c r="Q128" s="2"/>
     </row>
-    <row r="129" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="129" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D129" s="2"/>
       <c r="E129" s="2"/>
       <c r="F129" s="2"/>
@@ -6406,7 +6341,7 @@
       <c r="P129" s="2"/>
       <c r="Q129" s="2"/>
     </row>
-    <row r="130" spans="4:17" x14ac:dyDescent="0.25">
+    <row r="130" spans="4:17" x14ac:dyDescent="0.35">
       <c r="D130" s="2"/>
       <c r="E130" s="2"/>
       <c r="F130" s="2"/>
@@ -6422,9 +6357,89 @@
       <c r="P130" s="2"/>
       <c r="Q130" s="2"/>
     </row>
+    <row r="131" spans="4:17" x14ac:dyDescent="0.35">
+      <c r="D131" s="2"/>
+      <c r="E131" s="2"/>
+      <c r="F131" s="2"/>
+      <c r="G131" s="2"/>
+      <c r="H131" s="2"/>
+      <c r="I131" s="2"/>
+      <c r="J131" s="2"/>
+      <c r="K131" s="2"/>
+      <c r="L131" s="2"/>
+      <c r="M131" s="2"/>
+      <c r="N131" s="2"/>
+      <c r="O131" s="2"/>
+      <c r="P131" s="2"/>
+      <c r="Q131" s="2"/>
+    </row>
+    <row r="132" spans="4:17" x14ac:dyDescent="0.35">
+      <c r="D132" s="2"/>
+      <c r="E132" s="2"/>
+      <c r="F132" s="2"/>
+      <c r="G132" s="2"/>
+      <c r="H132" s="2"/>
+      <c r="I132" s="2"/>
+      <c r="J132" s="2"/>
+      <c r="K132" s="2"/>
+      <c r="L132" s="2"/>
+      <c r="M132" s="2"/>
+      <c r="N132" s="2"/>
+      <c r="O132" s="2"/>
+      <c r="P132" s="2"/>
+      <c r="Q132" s="2"/>
+    </row>
+    <row r="133" spans="4:17" x14ac:dyDescent="0.35">
+      <c r="D133" s="2"/>
+      <c r="E133" s="2"/>
+      <c r="F133" s="2"/>
+      <c r="G133" s="2"/>
+      <c r="H133" s="2"/>
+      <c r="I133" s="2"/>
+      <c r="J133" s="2"/>
+      <c r="K133" s="2"/>
+      <c r="L133" s="2"/>
+      <c r="M133" s="2"/>
+      <c r="N133" s="2"/>
+      <c r="O133" s="2"/>
+      <c r="P133" s="2"/>
+      <c r="Q133" s="2"/>
+    </row>
+    <row r="134" spans="4:17" x14ac:dyDescent="0.35">
+      <c r="D134" s="2"/>
+      <c r="E134" s="2"/>
+      <c r="F134" s="2"/>
+      <c r="G134" s="2"/>
+      <c r="H134" s="2"/>
+      <c r="I134" s="2"/>
+      <c r="J134" s="2"/>
+      <c r="K134" s="2"/>
+      <c r="L134" s="2"/>
+      <c r="M134" s="2"/>
+      <c r="N134" s="2"/>
+      <c r="O134" s="2"/>
+      <c r="P134" s="2"/>
+      <c r="Q134" s="2"/>
+    </row>
+    <row r="135" spans="4:17" x14ac:dyDescent="0.35">
+      <c r="D135" s="2"/>
+      <c r="E135" s="2"/>
+      <c r="F135" s="2"/>
+      <c r="G135" s="2"/>
+      <c r="H135" s="2"/>
+      <c r="I135" s="2"/>
+      <c r="J135" s="2"/>
+      <c r="K135" s="2"/>
+      <c r="L135" s="2"/>
+      <c r="M135" s="2"/>
+      <c r="N135" s="2"/>
+      <c r="O135" s="2"/>
+      <c r="P135" s="2"/>
+      <c r="Q135" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D105:Q130"/>
+    <mergeCell ref="D110:Q135"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
LGHUB 2025/11/5 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
- 网站错误 & 本地化问题详见 LGHUB/WebLoc/README.md
</commit_message>
<xml_diff>
--- a/Documents/Graph_PC.xlsx
+++ b/Documents/Graph_PC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29417"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC8AC63B-2553-4096-AE26-327A677FA4AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E3DC4A4-786A-422F-B6AD-83C5CD4BDD0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="19954" windowHeight="12652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="2" r:id="rId1"/>
@@ -50,7 +50,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -64,6 +64,12 @@
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -86,12 +92,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -574,13 +581,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>67</c:v>
+                  <c:v>71</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -917,72 +924,72 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$20:$C$28</c:f>
+              <c:f>Sheet1!$C$19:$C$27</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45964</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45957</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45950</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45943</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45936</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45929</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45922</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45915</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45908</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45901</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$20:$D$28</c:f>
+              <c:f>Sheet1!$D$19:$D$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>523</c:v>
+                  <c:v>530</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>523</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>523</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>514</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>509</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>499</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>496</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>488</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>485</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>471</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1086,72 +1093,72 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$20:$C$28</c:f>
+              <c:f>Sheet1!$C$19:$C$27</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45964</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45957</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45950</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45943</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45936</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45929</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45922</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45915</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45908</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45901</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$20:$G$28</c:f>
+              <c:f>Sheet1!$G$19:$G$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>489</c:v>
+                  <c:v>493</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>482</c:v>
+                  <c:v>489</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>482</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>472</c:v>
+                  <c:v>482</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>455</c:v>
+                  <c:v>472</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>455</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>455</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>450</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>444</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>426</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1287,11 +1294,11 @@
         <c:axId val="1374569007"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="530"/>
-          <c:min val="410"/>
+          <c:max val="540"/>
+          <c:min val="440"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="r"/>
+        <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -1393,7 +1400,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="1374558447"/>
-        <c:crosses val="autoZero"/>
+        <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -1795,13 +1802,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>67</c:v>
+                  <c:v>71</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4812,51 +4819,65 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D108" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L109" sqref="L109"/>
+    <sheetView tabSelected="1" topLeftCell="B108" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="K109" sqref="K109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.35">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C19" s="1">
+        <v>45964</v>
+      </c>
+      <c r="D19">
+        <v>530</v>
+      </c>
+      <c r="F19" s="1">
+        <v>45964</v>
+      </c>
+      <c r="G19" s="3">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C20" s="1">
         <v>45957</v>
       </c>
@@ -4870,7 +4891,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C21" s="1">
         <v>45950</v>
       </c>
@@ -4884,7 +4905,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C22" s="1">
         <v>45943</v>
       </c>
@@ -4898,7 +4919,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C23" s="1">
         <v>45936</v>
       </c>
@@ -4912,7 +4933,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C24" s="1">
         <v>45929</v>
       </c>
@@ -4926,7 +4947,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C25" s="1">
         <v>45922</v>
       </c>
@@ -4940,7 +4961,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C26" s="1">
         <v>45915</v>
       </c>
@@ -4954,7 +4975,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C27" s="1">
         <v>45908</v>
       </c>
@@ -4968,7 +4989,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C28" s="1">
         <v>45901</v>
       </c>
@@ -4982,7 +5003,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C29" s="1">
         <v>45894</v>
       </c>
@@ -4996,7 +5017,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C30" s="1">
         <v>45887</v>
       </c>
@@ -5010,7 +5031,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C31" s="1">
         <v>45880</v>
       </c>
@@ -5024,7 +5045,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C32" s="1">
         <v>45873</v>
       </c>
@@ -5038,7 +5059,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C33" s="1">
         <v>45866</v>
       </c>
@@ -5052,7 +5073,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="34" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C34" s="1">
         <v>45859</v>
       </c>
@@ -5066,7 +5087,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="35" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C35" s="1">
         <v>45852</v>
       </c>
@@ -5080,7 +5101,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="36" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C36" s="1">
         <v>45845</v>
       </c>
@@ -5094,7 +5115,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="37" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C37" s="1">
         <v>45838</v>
       </c>
@@ -5108,7 +5129,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="38" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C38" s="1">
         <v>45831</v>
       </c>
@@ -5122,7 +5143,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="39" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C39" s="1">
         <v>45824</v>
       </c>
@@ -5136,7 +5157,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="40" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C40" s="1">
         <v>45817</v>
       </c>
@@ -5150,7 +5171,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="41" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C41" s="1">
         <v>45810</v>
       </c>
@@ -5164,7 +5185,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="42" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C42" s="1">
         <v>45803</v>
       </c>
@@ -5178,7 +5199,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="43" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C43" s="1">
         <v>45796</v>
       </c>
@@ -5192,7 +5213,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="44" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C44" s="1">
         <v>45789</v>
       </c>
@@ -5206,7 +5227,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="45" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C45" s="1">
         <v>45782</v>
       </c>
@@ -5220,7 +5241,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="46" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C46" s="1">
         <v>45775</v>
       </c>
@@ -5234,7 +5255,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="47" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C47" s="1">
         <v>45768</v>
       </c>
@@ -5248,7 +5269,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="48" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C48" s="1">
         <v>45761</v>
       </c>
@@ -5262,7 +5283,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="49" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="49" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C49" s="1">
         <v>45754</v>
       </c>
@@ -5276,7 +5297,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="50" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="50" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C50" s="1">
         <v>45747</v>
       </c>
@@ -5290,7 +5311,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="51" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="51" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C51" s="1">
         <v>45740</v>
       </c>
@@ -5304,7 +5325,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="52" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="52" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C52" s="1">
         <v>45733</v>
       </c>
@@ -5318,7 +5339,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="53" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="53" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C53" s="1">
         <v>45726</v>
       </c>
@@ -5332,7 +5353,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="54" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="54" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C54" s="1">
         <v>45719</v>
       </c>
@@ -5346,7 +5367,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="55" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="55" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C55" s="1">
         <v>45712</v>
       </c>
@@ -5360,7 +5381,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="56" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="56" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C56" s="1">
         <v>45705</v>
       </c>
@@ -5374,7 +5395,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="57" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="57" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C57" s="1">
         <v>45698</v>
       </c>
@@ -5388,7 +5409,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="58" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="58" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C58" s="1">
         <v>45691</v>
       </c>
@@ -5402,7 +5423,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="59" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="59" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C59" s="1">
         <v>45684</v>
       </c>
@@ -5416,7 +5437,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="60" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="60" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C60" s="1">
         <v>45677</v>
       </c>
@@ -5430,7 +5451,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="61" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="61" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C61" s="1">
         <v>45670</v>
       </c>
@@ -5444,7 +5465,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="62" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="62" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C62" s="1">
         <v>45663</v>
       </c>
@@ -5458,7 +5479,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="63" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="63" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C63" s="1">
         <v>45642</v>
       </c>
@@ -5472,7 +5493,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="64" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="64" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C64" s="1">
         <v>45635</v>
       </c>
@@ -5486,7 +5507,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="65" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="65" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C65" s="1">
         <v>45628</v>
       </c>
@@ -5500,7 +5521,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="66" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="66" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C66" s="1">
         <v>45621</v>
       </c>
@@ -5514,7 +5535,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="67" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="67" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C67" s="1">
         <v>45614</v>
       </c>
@@ -5528,7 +5549,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="68" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="68" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C68" s="1">
         <v>45607</v>
       </c>
@@ -5542,7 +5563,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="69" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="69" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C69" s="1">
         <v>45600</v>
       </c>
@@ -5556,7 +5577,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="70" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="70" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C70" s="1">
         <v>45579</v>
       </c>
@@ -5570,7 +5591,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="71" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="71" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C71" s="1">
         <v>45572</v>
       </c>
@@ -5584,7 +5605,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="72" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="72" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C72" s="1">
         <v>45565</v>
       </c>
@@ -5598,7 +5619,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="73" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="73" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C73" s="1">
         <v>45537</v>
       </c>
@@ -5612,7 +5633,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="74" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="74" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C74" s="1">
         <v>45530</v>
       </c>
@@ -5626,7 +5647,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="75" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="75" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C75" s="1">
         <v>45523</v>
       </c>
@@ -5640,7 +5661,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="76" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="76" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C76" s="1">
         <v>45516</v>
       </c>
@@ -5654,7 +5675,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="77" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="77" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C77" s="1">
         <v>45509</v>
       </c>
@@ -5668,7 +5689,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="78" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="78" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C78" s="1">
         <v>45502</v>
       </c>
@@ -5682,7 +5703,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="79" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="79" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C79" s="1">
         <v>45495</v>
       </c>
@@ -5696,7 +5717,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="80" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="80" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C80" s="1">
         <v>45488</v>
       </c>
@@ -5710,7 +5731,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="81" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="81" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C81" s="1">
         <v>45481</v>
       </c>
@@ -5724,7 +5745,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="82" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="82" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C82" s="1">
         <v>45474</v>
       </c>
@@ -5738,7 +5759,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="83" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="83" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C83" s="1">
         <v>45467</v>
       </c>
@@ -5752,7 +5773,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="84" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="84" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C84" s="1">
         <v>45460</v>
       </c>
@@ -5766,7 +5787,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="85" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="85" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C85" s="1">
         <v>45453</v>
       </c>
@@ -5780,7 +5801,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="86" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="86" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C86" s="1">
         <v>45446</v>
       </c>
@@ -5794,7 +5815,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="87" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="87" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C87" s="1">
         <v>45439</v>
       </c>
@@ -5808,7 +5829,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="88" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="88" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C88" s="1">
         <v>45432</v>
       </c>
@@ -5822,7 +5843,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="89" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="89" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C89" s="1">
         <v>45425</v>
       </c>
@@ -5836,7 +5857,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="90" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="90" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C90" s="1">
         <v>45418</v>
       </c>
@@ -5850,7 +5871,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="91" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="91" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C91" s="1">
         <v>45411</v>
       </c>
@@ -5864,7 +5885,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="92" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="92" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C92" s="1">
         <v>45404</v>
       </c>
@@ -5878,7 +5899,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="93" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="93" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C93" s="1">
         <v>45397</v>
       </c>
@@ -5892,7 +5913,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="94" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="94" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C94" s="1">
         <v>45390</v>
       </c>
@@ -5906,7 +5927,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="95" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="95" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C95" s="1">
         <v>45383</v>
       </c>
@@ -5920,7 +5941,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="96" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="96" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C96" s="1">
         <v>45376</v>
       </c>
@@ -5934,7 +5955,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="97" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="97" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C97" s="1">
         <v>45369</v>
       </c>
@@ -5948,7 +5969,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="98" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="98" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C98" s="1">
         <v>45362</v>
       </c>
@@ -5957,7 +5978,7 @@
       </c>
       <c r="F98" s="1"/>
     </row>
-    <row r="99" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="99" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C99" s="1">
         <v>45355</v>
       </c>
@@ -5965,7 +5986,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="100" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="100" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C100" s="1">
         <v>45348</v>
       </c>
@@ -5973,7 +5994,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="101" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="101" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C101" s="1">
         <v>45341</v>
       </c>
@@ -5981,7 +6002,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="102" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="102" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C102" s="1">
         <v>45334</v>
       </c>
@@ -5989,7 +6010,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="103" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="103" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C103" s="1">
         <v>45327</v>
       </c>
@@ -5997,7 +6018,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="104" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="104" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C104" s="1">
         <v>45320</v>
       </c>
@@ -6005,7 +6026,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="105" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="105" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C105" s="1">
         <v>45313</v>
       </c>
@@ -6013,7 +6034,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="106" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="106" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C106" s="1">
         <v>45306</v>
       </c>
@@ -6021,7 +6042,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="110" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="110" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D110" s="2"/>
       <c r="E110" s="2"/>
       <c r="F110" s="2"/>
@@ -6037,7 +6058,7 @@
       <c r="P110" s="2"/>
       <c r="Q110" s="2"/>
     </row>
-    <row r="111" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="111" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D111" s="2"/>
       <c r="E111" s="2"/>
       <c r="F111" s="2"/>
@@ -6053,7 +6074,7 @@
       <c r="P111" s="2"/>
       <c r="Q111" s="2"/>
     </row>
-    <row r="112" spans="3:17" x14ac:dyDescent="0.35">
+    <row r="112" spans="3:17" x14ac:dyDescent="0.25">
       <c r="D112" s="2"/>
       <c r="E112" s="2"/>
       <c r="F112" s="2"/>
@@ -6069,7 +6090,7 @@
       <c r="P112" s="2"/>
       <c r="Q112" s="2"/>
     </row>
-    <row r="113" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="113" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D113" s="2"/>
       <c r="E113" s="2"/>
       <c r="F113" s="2"/>
@@ -6085,7 +6106,7 @@
       <c r="P113" s="2"/>
       <c r="Q113" s="2"/>
     </row>
-    <row r="114" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="114" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D114" s="2"/>
       <c r="E114" s="2"/>
       <c r="F114" s="2"/>
@@ -6101,7 +6122,7 @@
       <c r="P114" s="2"/>
       <c r="Q114" s="2"/>
     </row>
-    <row r="115" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="115" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D115" s="2"/>
       <c r="E115" s="2"/>
       <c r="F115" s="2"/>
@@ -6117,7 +6138,7 @@
       <c r="P115" s="2"/>
       <c r="Q115" s="2"/>
     </row>
-    <row r="116" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="116" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D116" s="2"/>
       <c r="E116" s="2"/>
       <c r="F116" s="2"/>
@@ -6133,7 +6154,7 @@
       <c r="P116" s="2"/>
       <c r="Q116" s="2"/>
     </row>
-    <row r="117" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="117" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D117" s="2"/>
       <c r="E117" s="2"/>
       <c r="F117" s="2"/>
@@ -6149,7 +6170,7 @@
       <c r="P117" s="2"/>
       <c r="Q117" s="2"/>
     </row>
-    <row r="118" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="118" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D118" s="2"/>
       <c r="E118" s="2"/>
       <c r="F118" s="2"/>
@@ -6165,7 +6186,7 @@
       <c r="P118" s="2"/>
       <c r="Q118" s="2"/>
     </row>
-    <row r="119" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="119" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D119" s="2"/>
       <c r="E119" s="2"/>
       <c r="F119" s="2"/>
@@ -6181,7 +6202,7 @@
       <c r="P119" s="2"/>
       <c r="Q119" s="2"/>
     </row>
-    <row r="120" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="120" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D120" s="2"/>
       <c r="E120" s="2"/>
       <c r="F120" s="2"/>
@@ -6197,7 +6218,7 @@
       <c r="P120" s="2"/>
       <c r="Q120" s="2"/>
     </row>
-    <row r="121" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="121" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D121" s="2"/>
       <c r="E121" s="2"/>
       <c r="F121" s="2"/>
@@ -6213,7 +6234,7 @@
       <c r="P121" s="2"/>
       <c r="Q121" s="2"/>
     </row>
-    <row r="122" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="122" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D122" s="2"/>
       <c r="E122" s="2"/>
       <c r="F122" s="2"/>
@@ -6229,7 +6250,7 @@
       <c r="P122" s="2"/>
       <c r="Q122" s="2"/>
     </row>
-    <row r="123" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="123" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D123" s="2"/>
       <c r="E123" s="2"/>
       <c r="F123" s="2"/>
@@ -6245,7 +6266,7 @@
       <c r="P123" s="2"/>
       <c r="Q123" s="2"/>
     </row>
-    <row r="124" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="124" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D124" s="2"/>
       <c r="E124" s="2"/>
       <c r="F124" s="2"/>
@@ -6261,7 +6282,7 @@
       <c r="P124" s="2"/>
       <c r="Q124" s="2"/>
     </row>
-    <row r="125" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="125" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D125" s="2"/>
       <c r="E125" s="2"/>
       <c r="F125" s="2"/>
@@ -6277,7 +6298,7 @@
       <c r="P125" s="2"/>
       <c r="Q125" s="2"/>
     </row>
-    <row r="126" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="126" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D126" s="2"/>
       <c r="E126" s="2"/>
       <c r="F126" s="2"/>
@@ -6293,7 +6314,7 @@
       <c r="P126" s="2"/>
       <c r="Q126" s="2"/>
     </row>
-    <row r="127" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="127" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D127" s="2"/>
       <c r="E127" s="2"/>
       <c r="F127" s="2"/>
@@ -6309,7 +6330,7 @@
       <c r="P127" s="2"/>
       <c r="Q127" s="2"/>
     </row>
-    <row r="128" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="128" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D128" s="2"/>
       <c r="E128" s="2"/>
       <c r="F128" s="2"/>
@@ -6325,7 +6346,7 @@
       <c r="P128" s="2"/>
       <c r="Q128" s="2"/>
     </row>
-    <row r="129" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="129" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D129" s="2"/>
       <c r="E129" s="2"/>
       <c r="F129" s="2"/>
@@ -6341,7 +6362,7 @@
       <c r="P129" s="2"/>
       <c r="Q129" s="2"/>
     </row>
-    <row r="130" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="130" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D130" s="2"/>
       <c r="E130" s="2"/>
       <c r="F130" s="2"/>
@@ -6357,7 +6378,7 @@
       <c r="P130" s="2"/>
       <c r="Q130" s="2"/>
     </row>
-    <row r="131" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="131" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D131" s="2"/>
       <c r="E131" s="2"/>
       <c r="F131" s="2"/>
@@ -6373,7 +6394,7 @@
       <c r="P131" s="2"/>
       <c r="Q131" s="2"/>
     </row>
-    <row r="132" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="132" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D132" s="2"/>
       <c r="E132" s="2"/>
       <c r="F132" s="2"/>
@@ -6389,7 +6410,7 @@
       <c r="P132" s="2"/>
       <c r="Q132" s="2"/>
     </row>
-    <row r="133" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="133" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D133" s="2"/>
       <c r="E133" s="2"/>
       <c r="F133" s="2"/>
@@ -6405,7 +6426,7 @@
       <c r="P133" s="2"/>
       <c r="Q133" s="2"/>
     </row>
-    <row r="134" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="134" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D134" s="2"/>
       <c r="E134" s="2"/>
       <c r="F134" s="2"/>
@@ -6421,7 +6442,7 @@
       <c r="P134" s="2"/>
       <c r="Q134" s="2"/>
     </row>
-    <row r="135" spans="4:17" x14ac:dyDescent="0.35">
+    <row r="135" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D135" s="2"/>
       <c r="E135" s="2"/>
       <c r="F135" s="2"/>

</xml_diff>

<commit_message>
LGHUB 2025/11/11 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
- 网站错误 & 本地化问题详见 LGHUB/WebLoc/README.md
</commit_message>
<xml_diff>
--- a/Documents/Graph_PC.xlsx
+++ b/Documents/Graph_PC.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29504"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E3DC4A4-786A-422F-B6AD-83C5CD4BDD0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{107E7346-D8A2-4E11-9D84-FBCFDBFDD861}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -64,12 +64,6 @@
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -92,13 +86,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -581,13 +574,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>71</c:v>
+                  <c:v>79</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -924,43 +917,43 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$19:$C$27</c:f>
+              <c:f>Sheet1!$C$18:$C$26</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45971</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45964</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45957</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45950</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45943</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45936</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45929</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45922</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45915</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45908</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$19:$D$27</c:f>
+              <c:f>Sheet1!$D$18:$D$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -968,28 +961,28 @@
                   <c:v>530</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>523</c:v>
+                  <c:v>530</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>523</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>523</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>514</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>509</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>499</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>496</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>488</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>485</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1093,72 +1086,72 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$19:$C$27</c:f>
+              <c:f>Sheet1!$C$18:$C$26</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45971</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45964</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45957</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45950</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45943</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45936</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45929</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45922</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45915</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45908</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$19:$G$27</c:f>
+              <c:f>Sheet1!$G$18:$G$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>503</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>493</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>489</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>482</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>482</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>472</c:v>
+                  <c:v>482</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>455</c:v>
+                  <c:v>472</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>455</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>450</c:v>
+                  <c:v>455</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>444</c:v>
+                  <c:v>450</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1802,13 +1795,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>71</c:v>
+                  <c:v>79</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4820,7 +4813,7 @@
   <dimension ref="B2:Q135"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B108" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="K109" sqref="K109"/>
+      <selection activeCell="L109" sqref="L109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -4844,7 +4837,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
@@ -4860,7 +4853,21 @@
         <v>4</v>
       </c>
       <c r="C7">
-        <v>71</v>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C18" s="1">
+        <v>45971</v>
+      </c>
+      <c r="D18">
+        <v>530</v>
+      </c>
+      <c r="F18" s="1">
+        <v>45971</v>
+      </c>
+      <c r="G18">
+        <v>503</v>
       </c>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.25">
@@ -4873,7 +4880,7 @@
       <c r="F19" s="1">
         <v>45964</v>
       </c>
-      <c r="G19" s="3">
+      <c r="G19">
         <v>493</v>
       </c>
     </row>

</xml_diff>

<commit_message>
LGHUB 2025/11/22 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
- 网站错误 & 本地化问题详见 LGHUB/WebLoc/README.md
</commit_message>
<xml_diff>
--- a/Documents/Graph_PC.xlsx
+++ b/Documents/Graph_PC.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29504"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29517"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{107E7346-D8A2-4E11-9D84-FBCFDBFDD861}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8DE833A-A55A-489B-B510-ACAC85572D7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,13 +574,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>79</c:v>
+                  <c:v>82</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -917,72 +917,72 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$18:$C$26</c:f>
+              <c:f>Sheet1!$C$17:$C$25</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45978</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45971</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45964</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45957</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45950</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45943</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45936</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45929</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45922</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45915</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$18:$D$26</c:f>
+              <c:f>Sheet1!$D$17:$D$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>530</c:v>
+                  <c:v>540</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>530</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>523</c:v>
+                  <c:v>530</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>523</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>523</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>514</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>509</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>499</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>496</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>488</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1086,72 +1086,72 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$18:$C$26</c:f>
+              <c:f>Sheet1!$C$17:$C$25</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45978</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45971</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45964</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45957</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45950</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45943</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45936</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45929</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45922</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45915</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$18:$G$26</c:f>
+              <c:f>Sheet1!$G$17:$G$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>506</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>503</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>493</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>489</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>482</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>482</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>472</c:v>
+                  <c:v>482</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>455</c:v>
+                  <c:v>472</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>455</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>450</c:v>
+                  <c:v>455</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1287,8 +1287,8 @@
         <c:axId val="1374569007"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="540"/>
-          <c:min val="440"/>
+          <c:max val="550"/>
+          <c:min val="450"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1795,13 +1795,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>79</c:v>
+                  <c:v>82</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4812,7 +4812,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B108" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B109" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="L109" sqref="L109"/>
     </sheetView>
   </sheetViews>
@@ -4837,7 +4837,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
@@ -4853,7 +4853,21 @@
         <v>4</v>
       </c>
       <c r="C7">
-        <v>79</v>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C17" s="1">
+        <v>45978</v>
+      </c>
+      <c r="D17">
+        <v>540</v>
+      </c>
+      <c r="F17" s="1">
+        <v>45978</v>
+      </c>
+      <c r="G17">
+        <v>506</v>
       </c>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
LGHUB 2025/12/10 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
- 网站错误 & 本地化问题详见 LGHUB/WebLoc/README.md
</commit_message>
<xml_diff>
--- a/Documents/Graph_PC.xlsx
+++ b/Documents/Graph_PC.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29517"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8DE833A-A55A-489B-B510-ACAC85572D7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{572B1542-900E-4F50-8656-5D6591BF901A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,13 +574,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>82</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -917,72 +917,72 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$17:$C$25</c:f>
+              <c:f>Sheet1!$C$20:$C$28</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45992</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45985</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>45978</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
                   <c:v>45971</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
                   <c:v>45964</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="6">
                   <c:v>45957</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="7">
                   <c:v>45950</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>45943</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>45936</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>45929</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45922</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$17:$D$25</c:f>
+              <c:f>Sheet1!$D$20:$D$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>549</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>540</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
+                  <c:v>540</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>540</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>530</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
                   <c:v>530</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="6">
                   <c:v>523</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="7">
                   <c:v>523</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>514</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>509</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>499</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>496</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1086,72 +1086,72 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$17:$C$25</c:f>
+              <c:f>Sheet1!$C$20:$C$28</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>45999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45992</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>45985</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>45978</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
                   <c:v>45971</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
                   <c:v>45964</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="6">
                   <c:v>45957</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="7">
                   <c:v>45950</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>45943</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>45936</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>45929</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45922</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$17:$G$25</c:f>
+              <c:f>Sheet1!$G$20:$G$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>506</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
+                  <c:v>506</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>506</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>503</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
                   <c:v>493</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="6">
                   <c:v>489</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="7">
                   <c:v>482</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>482</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>472</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>455</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>455</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1287,8 +1287,8 @@
         <c:axId val="1374569007"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="550"/>
-          <c:min val="450"/>
+          <c:max val="560"/>
+          <c:min val="470"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1795,13 +1795,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>82</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4224,13 +4224,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>106422</xdr:colOff>
-      <xdr:row>110</xdr:row>
+      <xdr:row>116</xdr:row>
       <xdr:rowOff>165023</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>125</xdr:row>
+      <xdr:row>131</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4260,13 +4260,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>190501</xdr:colOff>
-      <xdr:row>110</xdr:row>
+      <xdr:row>116</xdr:row>
       <xdr:rowOff>162248</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>124495</xdr:colOff>
-      <xdr:row>125</xdr:row>
+      <xdr:row>131</xdr:row>
       <xdr:rowOff>163286</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4810,10 +4810,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:Q135"/>
+  <dimension ref="B2:Q141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B109" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="L109" sqref="L109"/>
+    <sheetView tabSelected="1" topLeftCell="C114" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="L115" sqref="L115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -4837,7 +4837,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
@@ -4853,1311 +4853,1257 @@
         <v>4</v>
       </c>
       <c r="C7">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C17" s="1">
-        <v>45978</v>
-      </c>
-      <c r="D17">
-        <v>540</v>
-      </c>
-      <c r="F17" s="1">
-        <v>45978</v>
-      </c>
-      <c r="G17">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C18" s="1">
-        <v>45971</v>
-      </c>
-      <c r="D18">
-        <v>530</v>
-      </c>
-      <c r="F18" s="1">
-        <v>45971</v>
-      </c>
-      <c r="G18">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C19" s="1">
-        <v>45964</v>
-      </c>
-      <c r="D19">
-        <v>530</v>
-      </c>
-      <c r="F19" s="1">
-        <v>45964</v>
-      </c>
-      <c r="G19">
-        <v>493</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C20" s="1">
-        <v>45957</v>
+        <v>45999</v>
       </c>
       <c r="D20">
-        <v>523</v>
+        <v>549</v>
       </c>
       <c r="F20" s="1">
-        <v>45957</v>
+        <v>45999</v>
       </c>
       <c r="G20">
-        <v>489</v>
+        <v>512</v>
       </c>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C21" s="1">
-        <v>45950</v>
+        <v>45992</v>
       </c>
       <c r="D21">
-        <v>523</v>
+        <v>540</v>
       </c>
       <c r="F21" s="1">
-        <v>45950</v>
+        <v>45992</v>
       </c>
       <c r="G21">
-        <v>482</v>
+        <v>506</v>
       </c>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C22" s="1">
-        <v>45943</v>
+        <v>45985</v>
       </c>
       <c r="D22">
-        <v>514</v>
+        <v>540</v>
       </c>
       <c r="F22" s="1">
-        <v>45943</v>
+        <v>45985</v>
       </c>
       <c r="G22">
-        <v>482</v>
+        <v>506</v>
       </c>
     </row>
     <row r="23" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C23" s="1">
-        <v>45936</v>
+        <v>45978</v>
       </c>
       <c r="D23">
-        <v>509</v>
+        <v>540</v>
       </c>
       <c r="F23" s="1">
-        <v>45936</v>
+        <v>45978</v>
       </c>
       <c r="G23">
-        <v>472</v>
+        <v>506</v>
       </c>
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C24" s="1">
-        <v>45929</v>
+        <v>45971</v>
       </c>
       <c r="D24">
-        <v>499</v>
+        <v>530</v>
       </c>
       <c r="F24" s="1">
-        <v>45929</v>
+        <v>45971</v>
       </c>
       <c r="G24">
-        <v>455</v>
+        <v>503</v>
       </c>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C25" s="1">
-        <v>45922</v>
+        <v>45964</v>
       </c>
       <c r="D25">
-        <v>496</v>
+        <v>530</v>
       </c>
       <c r="F25" s="1">
-        <v>45922</v>
+        <v>45964</v>
       </c>
       <c r="G25">
-        <v>455</v>
+        <v>493</v>
       </c>
     </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C26" s="1">
-        <v>45915</v>
+        <v>45957</v>
       </c>
       <c r="D26">
-        <v>488</v>
+        <v>523</v>
       </c>
       <c r="F26" s="1">
-        <v>45915</v>
+        <v>45957</v>
       </c>
       <c r="G26">
-        <v>450</v>
+        <v>489</v>
       </c>
     </row>
     <row r="27" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C27" s="1">
-        <v>45908</v>
+        <v>45950</v>
       </c>
       <c r="D27">
-        <v>485</v>
+        <v>523</v>
       </c>
       <c r="F27" s="1">
-        <v>45908</v>
+        <v>45950</v>
       </c>
       <c r="G27">
-        <v>444</v>
+        <v>482</v>
       </c>
     </row>
     <row r="28" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C28" s="1">
-        <v>45901</v>
+        <v>45943</v>
       </c>
       <c r="D28">
-        <v>471</v>
+        <v>514</v>
       </c>
       <c r="F28" s="1">
-        <v>45901</v>
+        <v>45943</v>
       </c>
       <c r="G28">
-        <v>426</v>
+        <v>482</v>
       </c>
     </row>
     <row r="29" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C29" s="1">
-        <v>45894</v>
+        <v>45936</v>
       </c>
       <c r="D29">
-        <v>456</v>
+        <v>509</v>
       </c>
       <c r="F29" s="1">
-        <v>45894</v>
+        <v>45936</v>
       </c>
       <c r="G29">
-        <v>421</v>
+        <v>472</v>
       </c>
     </row>
     <row r="30" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C30" s="1">
-        <v>45887</v>
+        <v>45929</v>
       </c>
       <c r="D30">
-        <v>446</v>
+        <v>499</v>
       </c>
       <c r="F30" s="1">
-        <v>45887</v>
+        <v>45929</v>
       </c>
       <c r="G30">
-        <v>415</v>
+        <v>455</v>
       </c>
     </row>
     <row r="31" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C31" s="1">
-        <v>45880</v>
+        <v>45922</v>
       </c>
       <c r="D31">
-        <v>443</v>
+        <v>496</v>
       </c>
       <c r="F31" s="1">
-        <v>45880</v>
+        <v>45922</v>
       </c>
       <c r="G31">
-        <v>406</v>
+        <v>455</v>
       </c>
     </row>
     <row r="32" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C32" s="1">
-        <v>45873</v>
+        <v>45915</v>
       </c>
       <c r="D32">
-        <v>440</v>
+        <v>488</v>
       </c>
       <c r="F32" s="1">
-        <v>45873</v>
+        <v>45915</v>
       </c>
       <c r="G32">
-        <v>405</v>
+        <v>450</v>
       </c>
     </row>
     <row r="33" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C33" s="1">
-        <v>45866</v>
+        <v>45908</v>
       </c>
       <c r="D33">
-        <v>432</v>
+        <v>485</v>
       </c>
       <c r="F33" s="1">
-        <v>45866</v>
+        <v>45908</v>
       </c>
       <c r="G33">
-        <v>406</v>
+        <v>444</v>
       </c>
     </row>
     <row r="34" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C34" s="1">
-        <v>45859</v>
+        <v>45901</v>
       </c>
       <c r="D34">
-        <v>430</v>
+        <v>471</v>
       </c>
       <c r="F34" s="1">
-        <v>45859</v>
+        <v>45901</v>
       </c>
       <c r="G34">
-        <v>389</v>
+        <v>426</v>
       </c>
     </row>
     <row r="35" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C35" s="1">
-        <v>45852</v>
+        <v>45894</v>
       </c>
       <c r="D35">
-        <v>419</v>
+        <v>456</v>
       </c>
       <c r="F35" s="1">
-        <v>45852</v>
+        <v>45894</v>
       </c>
       <c r="G35">
-        <v>386</v>
+        <v>421</v>
       </c>
     </row>
     <row r="36" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C36" s="1">
-        <v>45845</v>
+        <v>45887</v>
       </c>
       <c r="D36">
-        <v>418</v>
+        <v>446</v>
       </c>
       <c r="F36" s="1">
-        <v>45845</v>
+        <v>45887</v>
       </c>
       <c r="G36">
-        <v>386</v>
+        <v>415</v>
       </c>
     </row>
     <row r="37" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C37" s="1">
-        <v>45838</v>
+        <v>45880</v>
       </c>
       <c r="D37">
-        <v>416</v>
+        <v>443</v>
       </c>
       <c r="F37" s="1">
-        <v>45838</v>
+        <v>45880</v>
       </c>
       <c r="G37">
-        <v>370</v>
+        <v>406</v>
       </c>
     </row>
     <row r="38" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C38" s="1">
-        <v>45831</v>
+        <v>45873</v>
       </c>
       <c r="D38">
-        <v>416</v>
+        <v>440</v>
       </c>
       <c r="F38" s="1">
-        <v>45831</v>
+        <v>45873</v>
       </c>
       <c r="G38">
-        <v>370</v>
+        <v>405</v>
       </c>
     </row>
     <row r="39" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C39" s="1">
-        <v>45824</v>
+        <v>45866</v>
       </c>
       <c r="D39">
-        <v>407</v>
+        <v>432</v>
       </c>
       <c r="F39" s="1">
-        <v>45824</v>
+        <v>45866</v>
       </c>
       <c r="G39">
-        <v>369</v>
+        <v>406</v>
       </c>
     </row>
     <row r="40" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C40" s="1">
-        <v>45817</v>
+        <v>45859</v>
       </c>
       <c r="D40">
-        <v>404</v>
+        <v>430</v>
       </c>
       <c r="F40" s="1">
-        <v>45817</v>
+        <v>45859</v>
       </c>
       <c r="G40">
-        <v>359</v>
+        <v>389</v>
       </c>
     </row>
     <row r="41" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C41" s="1">
-        <v>45810</v>
+        <v>45852</v>
       </c>
       <c r="D41">
-        <v>395</v>
+        <v>419</v>
       </c>
       <c r="F41" s="1">
-        <v>45810</v>
+        <v>45852</v>
       </c>
       <c r="G41">
-        <v>360</v>
+        <v>386</v>
       </c>
     </row>
     <row r="42" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C42" s="1">
-        <v>45803</v>
+        <v>45845</v>
       </c>
       <c r="D42">
+        <v>418</v>
+      </c>
+      <c r="F42" s="1">
+        <v>45845</v>
+      </c>
+      <c r="G42">
         <v>386</v>
-      </c>
-      <c r="F42" s="1">
-        <v>45803</v>
-      </c>
-      <c r="G42">
-        <v>354</v>
       </c>
     </row>
     <row r="43" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C43" s="1">
-        <v>45796</v>
+        <v>45838</v>
       </c>
       <c r="D43">
-        <v>379</v>
+        <v>416</v>
       </c>
       <c r="F43" s="1">
-        <v>45796</v>
+        <v>45838</v>
       </c>
       <c r="G43">
-        <v>349</v>
+        <v>370</v>
       </c>
     </row>
     <row r="44" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C44" s="1">
-        <v>45789</v>
+        <v>45831</v>
       </c>
       <c r="D44">
-        <v>365</v>
+        <v>416</v>
       </c>
       <c r="F44" s="1">
-        <v>45789</v>
+        <v>45831</v>
       </c>
       <c r="G44">
-        <v>320</v>
+        <v>370</v>
       </c>
     </row>
     <row r="45" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C45" s="1">
-        <v>45782</v>
+        <v>45824</v>
       </c>
       <c r="D45">
-        <v>356</v>
+        <v>407</v>
       </c>
       <c r="F45" s="1">
-        <v>45782</v>
+        <v>45824</v>
       </c>
       <c r="G45">
-        <v>320</v>
+        <v>369</v>
       </c>
     </row>
     <row r="46" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C46" s="1">
-        <v>45775</v>
+        <v>45817</v>
       </c>
       <c r="D46">
-        <v>348</v>
+        <v>404</v>
       </c>
       <c r="F46" s="1">
-        <v>45775</v>
+        <v>45817</v>
       </c>
       <c r="G46">
-        <v>320</v>
+        <v>359</v>
       </c>
     </row>
     <row r="47" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C47" s="1">
-        <v>45768</v>
+        <v>45810</v>
       </c>
       <c r="D47">
-        <v>343</v>
+        <v>395</v>
       </c>
       <c r="F47" s="1">
-        <v>45768</v>
+        <v>45810</v>
       </c>
       <c r="G47">
-        <v>319</v>
+        <v>360</v>
       </c>
     </row>
     <row r="48" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C48" s="1">
-        <v>45761</v>
+        <v>45803</v>
       </c>
       <c r="D48">
-        <v>334</v>
+        <v>386</v>
       </c>
       <c r="F48" s="1">
-        <v>45761</v>
+        <v>45803</v>
       </c>
       <c r="G48">
-        <v>303</v>
+        <v>354</v>
       </c>
     </row>
     <row r="49" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C49" s="1">
-        <v>45754</v>
+        <v>45796</v>
       </c>
       <c r="D49">
-        <v>330</v>
+        <v>379</v>
       </c>
       <c r="F49" s="1">
-        <v>45754</v>
+        <v>45796</v>
       </c>
       <c r="G49">
-        <v>302</v>
+        <v>349</v>
       </c>
     </row>
     <row r="50" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C50" s="1">
-        <v>45747</v>
+        <v>45789</v>
       </c>
       <c r="D50">
-        <v>325</v>
+        <v>365</v>
       </c>
       <c r="F50" s="1">
-        <v>45747</v>
+        <v>45789</v>
       </c>
       <c r="G50">
-        <v>302</v>
+        <v>320</v>
       </c>
     </row>
     <row r="51" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C51" s="1">
-        <v>45740</v>
+        <v>45782</v>
       </c>
       <c r="D51">
-        <v>316</v>
+        <v>356</v>
       </c>
       <c r="F51" s="1">
-        <v>45740</v>
+        <v>45782</v>
       </c>
       <c r="G51">
-        <v>296</v>
+        <v>320</v>
       </c>
     </row>
     <row r="52" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C52" s="1">
-        <v>45733</v>
+        <v>45775</v>
       </c>
       <c r="D52">
-        <v>310</v>
+        <v>348</v>
       </c>
       <c r="F52" s="1">
-        <v>45733</v>
+        <v>45775</v>
       </c>
       <c r="G52">
-        <v>296</v>
+        <v>320</v>
       </c>
     </row>
     <row r="53" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C53" s="1">
-        <v>45726</v>
+        <v>45768</v>
       </c>
       <c r="D53">
-        <v>309</v>
+        <v>343</v>
       </c>
       <c r="F53" s="1">
-        <v>45726</v>
+        <v>45768</v>
       </c>
       <c r="G53">
-        <v>294</v>
+        <v>319</v>
       </c>
     </row>
     <row r="54" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C54" s="1">
-        <v>45719</v>
+        <v>45761</v>
       </c>
       <c r="D54">
-        <v>308</v>
+        <v>334</v>
       </c>
       <c r="F54" s="1">
-        <v>45719</v>
+        <v>45761</v>
       </c>
       <c r="G54">
-        <v>286</v>
+        <v>303</v>
       </c>
     </row>
     <row r="55" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C55" s="1">
-        <v>45712</v>
+        <v>45754</v>
       </c>
       <c r="D55">
-        <v>306</v>
+        <v>330</v>
       </c>
       <c r="F55" s="1">
-        <v>45712</v>
+        <v>45754</v>
       </c>
       <c r="G55">
-        <v>286</v>
+        <v>302</v>
       </c>
     </row>
     <row r="56" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C56" s="1">
-        <v>45705</v>
+        <v>45747</v>
       </c>
       <c r="D56">
-        <v>301</v>
+        <v>325</v>
       </c>
       <c r="F56" s="1">
-        <v>45705</v>
+        <v>45747</v>
       </c>
       <c r="G56">
-        <v>267</v>
+        <v>302</v>
       </c>
     </row>
     <row r="57" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C57" s="1">
-        <v>45698</v>
+        <v>45740</v>
       </c>
       <c r="D57">
-        <v>295</v>
+        <v>316</v>
       </c>
       <c r="F57" s="1">
-        <v>45698</v>
+        <v>45740</v>
       </c>
       <c r="G57">
-        <v>267</v>
+        <v>296</v>
       </c>
     </row>
     <row r="58" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C58" s="1">
-        <v>45691</v>
+        <v>45733</v>
       </c>
       <c r="D58">
-        <v>289</v>
+        <v>310</v>
       </c>
       <c r="F58" s="1">
-        <v>45691</v>
+        <v>45733</v>
       </c>
       <c r="G58">
-        <v>267</v>
+        <v>296</v>
       </c>
     </row>
     <row r="59" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C59" s="1">
-        <v>45684</v>
+        <v>45726</v>
       </c>
       <c r="D59">
-        <v>284</v>
+        <v>309</v>
       </c>
       <c r="F59" s="1">
-        <v>45684</v>
+        <v>45726</v>
       </c>
       <c r="G59">
-        <v>262</v>
+        <v>294</v>
       </c>
     </row>
     <row r="60" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C60" s="1">
-        <v>45677</v>
+        <v>45719</v>
       </c>
       <c r="D60">
-        <v>273</v>
+        <v>308</v>
       </c>
       <c r="F60" s="1">
-        <v>45677</v>
+        <v>45719</v>
       </c>
       <c r="G60">
-        <v>254</v>
+        <v>286</v>
       </c>
     </row>
     <row r="61" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C61" s="1">
-        <v>45670</v>
+        <v>45712</v>
       </c>
       <c r="D61">
-        <v>264</v>
+        <v>306</v>
       </c>
       <c r="F61" s="1">
-        <v>45670</v>
+        <v>45712</v>
       </c>
       <c r="G61">
-        <v>250</v>
+        <v>286</v>
       </c>
     </row>
     <row r="62" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C62" s="1">
-        <v>45663</v>
+        <v>45705</v>
       </c>
       <c r="D62">
-        <v>256</v>
+        <v>301</v>
       </c>
       <c r="F62" s="1">
-        <v>45663</v>
+        <v>45705</v>
       </c>
       <c r="G62">
-        <v>250</v>
+        <v>267</v>
       </c>
     </row>
     <row r="63" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C63" s="1">
-        <v>45642</v>
+        <v>45698</v>
       </c>
       <c r="D63">
-        <v>256</v>
+        <v>295</v>
       </c>
       <c r="F63" s="1">
-        <v>45642</v>
+        <v>45698</v>
       </c>
       <c r="G63">
-        <v>245</v>
+        <v>267</v>
       </c>
     </row>
     <row r="64" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C64" s="1">
-        <v>45635</v>
+        <v>45691</v>
       </c>
       <c r="D64">
-        <v>251</v>
+        <v>289</v>
       </c>
       <c r="F64" s="1">
-        <v>45635</v>
+        <v>45691</v>
       </c>
       <c r="G64">
-        <v>243</v>
+        <v>267</v>
       </c>
     </row>
     <row r="65" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C65" s="1">
-        <v>45628</v>
+        <v>45684</v>
       </c>
       <c r="D65">
-        <v>251</v>
+        <v>284</v>
       </c>
       <c r="F65" s="1">
-        <v>45628</v>
+        <v>45684</v>
       </c>
       <c r="G65">
-        <v>239</v>
+        <v>262</v>
       </c>
     </row>
     <row r="66" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C66" s="1">
-        <v>45621</v>
+        <v>45677</v>
       </c>
       <c r="D66">
-        <v>247</v>
+        <v>273</v>
       </c>
       <c r="F66" s="1">
-        <v>45621</v>
+        <v>45677</v>
       </c>
       <c r="G66">
-        <v>234</v>
+        <v>254</v>
       </c>
     </row>
     <row r="67" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C67" s="1">
-        <v>45614</v>
+        <v>45670</v>
       </c>
       <c r="D67">
-        <v>241</v>
+        <v>264</v>
       </c>
       <c r="F67" s="1">
-        <v>45614</v>
+        <v>45670</v>
       </c>
       <c r="G67">
-        <v>234</v>
+        <v>250</v>
       </c>
     </row>
     <row r="68" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C68" s="1">
-        <v>45607</v>
+        <v>45663</v>
       </c>
       <c r="D68">
-        <v>239</v>
+        <v>256</v>
       </c>
       <c r="F68" s="1">
-        <v>45607</v>
+        <v>45663</v>
       </c>
       <c r="G68">
-        <v>230</v>
+        <v>250</v>
       </c>
     </row>
     <row r="69" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C69" s="1">
-        <v>45600</v>
+        <v>45642</v>
       </c>
       <c r="D69">
-        <v>232</v>
+        <v>256</v>
       </c>
       <c r="F69" s="1">
-        <v>45600</v>
+        <v>45642</v>
       </c>
       <c r="G69">
-        <v>227</v>
+        <v>245</v>
       </c>
     </row>
     <row r="70" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C70" s="1">
-        <v>45579</v>
+        <v>45635</v>
       </c>
       <c r="D70">
-        <v>231</v>
+        <v>251</v>
       </c>
       <c r="F70" s="1">
-        <v>45579</v>
+        <v>45635</v>
       </c>
       <c r="G70">
-        <v>222</v>
+        <v>243</v>
       </c>
     </row>
     <row r="71" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C71" s="1">
-        <v>45572</v>
+        <v>45628</v>
       </c>
       <c r="D71">
-        <v>227</v>
+        <v>251</v>
       </c>
       <c r="F71" s="1">
-        <v>45572</v>
+        <v>45628</v>
       </c>
       <c r="G71">
-        <v>216</v>
+        <v>239</v>
       </c>
     </row>
     <row r="72" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C72" s="1">
-        <v>45565</v>
+        <v>45621</v>
       </c>
       <c r="D72">
-        <v>223</v>
+        <v>247</v>
       </c>
       <c r="F72" s="1">
-        <v>45565</v>
+        <v>45621</v>
       </c>
       <c r="G72">
-        <v>216</v>
+        <v>234</v>
       </c>
     </row>
     <row r="73" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C73" s="1">
-        <v>45537</v>
+        <v>45614</v>
       </c>
       <c r="D73">
-        <v>218</v>
+        <v>241</v>
       </c>
       <c r="F73" s="1">
-        <v>45537</v>
+        <v>45614</v>
       </c>
       <c r="G73">
-        <v>207</v>
+        <v>234</v>
       </c>
     </row>
     <row r="74" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C74" s="1">
-        <v>45530</v>
+        <v>45607</v>
       </c>
       <c r="D74">
-        <v>217</v>
+        <v>239</v>
       </c>
       <c r="F74" s="1">
-        <v>45530</v>
+        <v>45607</v>
       </c>
       <c r="G74">
-        <v>207</v>
+        <v>230</v>
       </c>
     </row>
     <row r="75" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C75" s="1">
-        <v>45523</v>
+        <v>45600</v>
       </c>
       <c r="D75">
-        <v>216</v>
+        <v>232</v>
       </c>
       <c r="F75" s="1">
-        <v>45523</v>
+        <v>45600</v>
       </c>
       <c r="G75">
-        <v>200</v>
+        <v>227</v>
       </c>
     </row>
     <row r="76" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C76" s="1">
-        <v>45516</v>
+        <v>45579</v>
       </c>
       <c r="D76">
-        <v>212</v>
+        <v>231</v>
       </c>
       <c r="F76" s="1">
-        <v>45516</v>
+        <v>45579</v>
       </c>
       <c r="G76">
-        <v>190</v>
+        <v>222</v>
       </c>
     </row>
     <row r="77" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C77" s="1">
-        <v>45509</v>
+        <v>45572</v>
       </c>
       <c r="D77">
-        <v>210</v>
+        <v>227</v>
       </c>
       <c r="F77" s="1">
-        <v>45509</v>
+        <v>45572</v>
       </c>
       <c r="G77">
-        <v>189</v>
+        <v>216</v>
       </c>
     </row>
     <row r="78" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C78" s="1">
-        <v>45502</v>
+        <v>45565</v>
       </c>
       <c r="D78">
-        <v>210</v>
+        <v>223</v>
       </c>
       <c r="F78" s="1">
-        <v>45502</v>
+        <v>45565</v>
       </c>
       <c r="G78">
-        <v>189</v>
+        <v>216</v>
       </c>
     </row>
     <row r="79" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C79" s="1">
-        <v>45495</v>
+        <v>45537</v>
       </c>
       <c r="D79">
-        <v>201</v>
+        <v>218</v>
       </c>
       <c r="F79" s="1">
-        <v>45495</v>
+        <v>45537</v>
       </c>
       <c r="G79">
-        <v>183</v>
+        <v>207</v>
       </c>
     </row>
     <row r="80" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C80" s="1">
-        <v>45488</v>
+        <v>45530</v>
       </c>
       <c r="D80">
-        <v>199</v>
+        <v>217</v>
       </c>
       <c r="F80" s="1">
-        <v>45488</v>
+        <v>45530</v>
       </c>
       <c r="G80">
-        <v>182</v>
+        <v>207</v>
       </c>
     </row>
     <row r="81" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C81" s="1">
-        <v>45481</v>
+        <v>45523</v>
       </c>
       <c r="D81">
-        <v>188</v>
+        <v>216</v>
       </c>
       <c r="F81" s="1">
-        <v>45481</v>
+        <v>45523</v>
       </c>
       <c r="G81">
-        <v>180</v>
+        <v>200</v>
       </c>
     </row>
     <row r="82" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C82" s="1">
-        <v>45474</v>
+        <v>45516</v>
       </c>
       <c r="D82">
-        <v>187</v>
+        <v>212</v>
       </c>
       <c r="F82" s="1">
-        <v>45474</v>
+        <v>45516</v>
       </c>
       <c r="G82">
-        <v>172</v>
+        <v>190</v>
       </c>
     </row>
     <row r="83" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C83" s="1">
-        <v>45467</v>
+        <v>45509</v>
       </c>
       <c r="D83">
-        <v>187</v>
+        <v>210</v>
       </c>
       <c r="F83" s="1">
-        <v>45467</v>
+        <v>45509</v>
       </c>
       <c r="G83">
-        <v>172</v>
+        <v>189</v>
       </c>
     </row>
     <row r="84" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C84" s="1">
-        <v>45460</v>
+        <v>45502</v>
       </c>
       <c r="D84">
-        <v>185</v>
+        <v>210</v>
       </c>
       <c r="F84" s="1">
-        <v>45460</v>
+        <v>45502</v>
       </c>
       <c r="G84">
-        <v>165</v>
+        <v>189</v>
       </c>
     </row>
     <row r="85" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C85" s="1">
-        <v>45453</v>
+        <v>45495</v>
       </c>
       <c r="D85">
-        <v>180</v>
+        <v>201</v>
       </c>
       <c r="F85" s="1">
-        <v>45453</v>
+        <v>45495</v>
       </c>
       <c r="G85">
-        <v>164</v>
+        <v>183</v>
       </c>
     </row>
     <row r="86" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C86" s="1">
-        <v>45446</v>
+        <v>45488</v>
       </c>
       <c r="D86">
-        <v>177</v>
+        <v>199</v>
       </c>
       <c r="F86" s="1">
-        <v>45446</v>
+        <v>45488</v>
       </c>
       <c r="G86">
-        <v>161</v>
+        <v>182</v>
       </c>
     </row>
     <row r="87" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C87" s="1">
-        <v>45439</v>
+        <v>45481</v>
       </c>
       <c r="D87">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="F87" s="1">
-        <v>45439</v>
+        <v>45481</v>
       </c>
       <c r="G87">
-        <v>161</v>
+        <v>180</v>
       </c>
     </row>
     <row r="88" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C88" s="1">
-        <v>45432</v>
+        <v>45474</v>
       </c>
       <c r="D88">
-        <v>173</v>
+        <v>187</v>
       </c>
       <c r="F88" s="1">
-        <v>45432</v>
+        <v>45474</v>
       </c>
       <c r="G88">
-        <v>159</v>
+        <v>172</v>
       </c>
     </row>
     <row r="89" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C89" s="1">
-        <v>45425</v>
+        <v>45467</v>
       </c>
       <c r="D89">
-        <v>170</v>
+        <v>187</v>
       </c>
       <c r="F89" s="1">
-        <v>45425</v>
+        <v>45467</v>
       </c>
       <c r="G89">
-        <v>157</v>
+        <v>172</v>
       </c>
     </row>
     <row r="90" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C90" s="1">
-        <v>45418</v>
+        <v>45460</v>
       </c>
       <c r="D90">
-        <v>170</v>
+        <v>185</v>
       </c>
       <c r="F90" s="1">
-        <v>45418</v>
+        <v>45460</v>
       </c>
       <c r="G90">
-        <v>141</v>
+        <v>165</v>
       </c>
     </row>
     <row r="91" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C91" s="1">
-        <v>45411</v>
+        <v>45453</v>
       </c>
       <c r="D91">
-        <v>166</v>
+        <v>180</v>
       </c>
       <c r="F91" s="1">
-        <v>45411</v>
+        <v>45453</v>
       </c>
       <c r="G91">
-        <v>141</v>
+        <v>164</v>
       </c>
     </row>
     <row r="92" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C92" s="1">
-        <v>45404</v>
+        <v>45446</v>
       </c>
       <c r="D92">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="F92" s="1">
-        <v>45404</v>
+        <v>45446</v>
       </c>
       <c r="G92">
-        <v>141</v>
+        <v>161</v>
       </c>
     </row>
     <row r="93" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C93" s="1">
-        <v>45397</v>
+        <v>45439</v>
       </c>
       <c r="D93">
-        <v>157</v>
+        <v>174</v>
       </c>
       <c r="F93" s="1">
-        <v>45397</v>
+        <v>45439</v>
       </c>
       <c r="G93">
-        <v>132</v>
+        <v>161</v>
       </c>
     </row>
     <row r="94" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C94" s="1">
-        <v>45390</v>
+        <v>45432</v>
       </c>
       <c r="D94">
-        <v>146</v>
+        <v>173</v>
       </c>
       <c r="F94" s="1">
-        <v>45390</v>
+        <v>45432</v>
       </c>
       <c r="G94">
-        <v>132</v>
+        <v>159</v>
       </c>
     </row>
     <row r="95" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C95" s="1">
-        <v>45383</v>
+        <v>45425</v>
       </c>
       <c r="D95">
-        <v>138</v>
+        <v>170</v>
       </c>
       <c r="F95" s="1">
-        <v>45383</v>
+        <v>45425</v>
       </c>
       <c r="G95">
-        <v>119</v>
+        <v>157</v>
       </c>
     </row>
     <row r="96" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C96" s="1">
+        <v>45418</v>
+      </c>
+      <c r="D96">
+        <v>170</v>
+      </c>
+      <c r="F96" s="1">
+        <v>45418</v>
+      </c>
+      <c r="G96">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="97" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C97" s="1">
+        <v>45411</v>
+      </c>
+      <c r="D97">
+        <v>166</v>
+      </c>
+      <c r="F97" s="1">
+        <v>45411</v>
+      </c>
+      <c r="G97">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="98" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C98" s="1">
+        <v>45404</v>
+      </c>
+      <c r="D98">
+        <v>166</v>
+      </c>
+      <c r="F98" s="1">
+        <v>45404</v>
+      </c>
+      <c r="G98">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="99" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C99" s="1">
+        <v>45397</v>
+      </c>
+      <c r="D99">
+        <v>157</v>
+      </c>
+      <c r="F99" s="1">
+        <v>45397</v>
+      </c>
+      <c r="G99">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="100" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C100" s="1">
+        <v>45390</v>
+      </c>
+      <c r="D100">
+        <v>146</v>
+      </c>
+      <c r="F100" s="1">
+        <v>45390</v>
+      </c>
+      <c r="G100">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="101" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C101" s="1">
+        <v>45383</v>
+      </c>
+      <c r="D101">
+        <v>138</v>
+      </c>
+      <c r="F101" s="1">
+        <v>45383</v>
+      </c>
+      <c r="G101">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="102" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C102" s="1">
         <v>45376</v>
       </c>
-      <c r="D96">
+      <c r="D102">
         <v>129</v>
       </c>
-      <c r="F96" s="1">
+      <c r="F102" s="1">
         <v>45376</v>
       </c>
-      <c r="G96">
+      <c r="G102">
         <v>114</v>
       </c>
     </row>
-    <row r="97" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C97" s="1">
+    <row r="103" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C103" s="1">
         <v>45369</v>
       </c>
-      <c r="D97">
+      <c r="D103">
         <v>123</v>
       </c>
-      <c r="F97" s="1">
+      <c r="F103" s="1">
         <v>45369</v>
       </c>
-      <c r="G97">
+      <c r="G103">
         <v>97</v>
       </c>
     </row>
-    <row r="98" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C98" s="1">
+    <row r="104" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C104" s="1">
         <v>45362</v>
       </c>
-      <c r="D98">
+      <c r="D104">
         <v>113</v>
       </c>
-      <c r="F98" s="1"/>
-    </row>
-    <row r="99" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C99" s="1">
+      <c r="F104" s="1"/>
+    </row>
+    <row r="105" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C105" s="1">
         <v>45355</v>
       </c>
-      <c r="D99">
+      <c r="D105">
         <v>108</v>
       </c>
     </row>
-    <row r="100" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C100" s="1">
+    <row r="106" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C106" s="1">
         <v>45348</v>
       </c>
-      <c r="D100">
+      <c r="D106">
         <v>102</v>
       </c>
     </row>
-    <row r="101" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C101" s="1">
+    <row r="107" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C107" s="1">
         <v>45341</v>
       </c>
-      <c r="D101">
+      <c r="D107">
         <v>95</v>
       </c>
     </row>
-    <row r="102" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C102" s="1">
+    <row r="108" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C108" s="1">
         <v>45334</v>
       </c>
-      <c r="D102">
+      <c r="D108">
         <v>80</v>
       </c>
     </row>
-    <row r="103" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C103" s="1">
+    <row r="109" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C109" s="1">
         <v>45327</v>
       </c>
-      <c r="D103">
+      <c r="D109">
         <v>66</v>
       </c>
     </row>
-    <row r="104" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C104" s="1">
+    <row r="110" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C110" s="1">
         <v>45320</v>
       </c>
-      <c r="D104">
+      <c r="D110">
         <v>55</v>
       </c>
     </row>
-    <row r="105" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C105" s="1">
+    <row r="111" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C111" s="1">
         <v>45313</v>
       </c>
-      <c r="D105">
+      <c r="D111">
         <v>53</v>
       </c>
     </row>
-    <row r="106" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C106" s="1">
+    <row r="112" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C112" s="1">
         <v>45306</v>
       </c>
-      <c r="D106">
+      <c r="D112">
         <v>52</v>
       </c>
-    </row>
-    <row r="110" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="D110" s="2"/>
-      <c r="E110" s="2"/>
-      <c r="F110" s="2"/>
-      <c r="G110" s="2"/>
-      <c r="H110" s="2"/>
-      <c r="I110" s="2"/>
-      <c r="J110" s="2"/>
-      <c r="K110" s="2"/>
-      <c r="L110" s="2"/>
-      <c r="M110" s="2"/>
-      <c r="N110" s="2"/>
-      <c r="O110" s="2"/>
-      <c r="P110" s="2"/>
-      <c r="Q110" s="2"/>
-    </row>
-    <row r="111" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="D111" s="2"/>
-      <c r="E111" s="2"/>
-      <c r="F111" s="2"/>
-      <c r="G111" s="2"/>
-      <c r="H111" s="2"/>
-      <c r="I111" s="2"/>
-      <c r="J111" s="2"/>
-      <c r="K111" s="2"/>
-      <c r="L111" s="2"/>
-      <c r="M111" s="2"/>
-      <c r="N111" s="2"/>
-      <c r="O111" s="2"/>
-      <c r="P111" s="2"/>
-      <c r="Q111" s="2"/>
-    </row>
-    <row r="112" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="D112" s="2"/>
-      <c r="E112" s="2"/>
-      <c r="F112" s="2"/>
-      <c r="G112" s="2"/>
-      <c r="H112" s="2"/>
-      <c r="I112" s="2"/>
-      <c r="J112" s="2"/>
-      <c r="K112" s="2"/>
-      <c r="L112" s="2"/>
-      <c r="M112" s="2"/>
-      <c r="N112" s="2"/>
-      <c r="O112" s="2"/>
-      <c r="P112" s="2"/>
-      <c r="Q112" s="2"/>
-    </row>
-    <row r="113" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D113" s="2"/>
-      <c r="E113" s="2"/>
-      <c r="F113" s="2"/>
-      <c r="G113" s="2"/>
-      <c r="H113" s="2"/>
-      <c r="I113" s="2"/>
-      <c r="J113" s="2"/>
-      <c r="K113" s="2"/>
-      <c r="L113" s="2"/>
-      <c r="M113" s="2"/>
-      <c r="N113" s="2"/>
-      <c r="O113" s="2"/>
-      <c r="P113" s="2"/>
-      <c r="Q113" s="2"/>
-    </row>
-    <row r="114" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D114" s="2"/>
-      <c r="E114" s="2"/>
-      <c r="F114" s="2"/>
-      <c r="G114" s="2"/>
-      <c r="H114" s="2"/>
-      <c r="I114" s="2"/>
-      <c r="J114" s="2"/>
-      <c r="K114" s="2"/>
-      <c r="L114" s="2"/>
-      <c r="M114" s="2"/>
-      <c r="N114" s="2"/>
-      <c r="O114" s="2"/>
-      <c r="P114" s="2"/>
-      <c r="Q114" s="2"/>
-    </row>
-    <row r="115" spans="4:17" x14ac:dyDescent="0.25">
-      <c r="D115" s="2"/>
-      <c r="E115" s="2"/>
-      <c r="F115" s="2"/>
-      <c r="G115" s="2"/>
-      <c r="H115" s="2"/>
-      <c r="I115" s="2"/>
-      <c r="J115" s="2"/>
-      <c r="K115" s="2"/>
-      <c r="L115" s="2"/>
-      <c r="M115" s="2"/>
-      <c r="N115" s="2"/>
-      <c r="O115" s="2"/>
-      <c r="P115" s="2"/>
-      <c r="Q115" s="2"/>
     </row>
     <row r="116" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D116" s="2"/>
@@ -6479,9 +6425,105 @@
       <c r="P135" s="2"/>
       <c r="Q135" s="2"/>
     </row>
+    <row r="136" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D136" s="2"/>
+      <c r="E136" s="2"/>
+      <c r="F136" s="2"/>
+      <c r="G136" s="2"/>
+      <c r="H136" s="2"/>
+      <c r="I136" s="2"/>
+      <c r="J136" s="2"/>
+      <c r="K136" s="2"/>
+      <c r="L136" s="2"/>
+      <c r="M136" s="2"/>
+      <c r="N136" s="2"/>
+      <c r="O136" s="2"/>
+      <c r="P136" s="2"/>
+      <c r="Q136" s="2"/>
+    </row>
+    <row r="137" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D137" s="2"/>
+      <c r="E137" s="2"/>
+      <c r="F137" s="2"/>
+      <c r="G137" s="2"/>
+      <c r="H137" s="2"/>
+      <c r="I137" s="2"/>
+      <c r="J137" s="2"/>
+      <c r="K137" s="2"/>
+      <c r="L137" s="2"/>
+      <c r="M137" s="2"/>
+      <c r="N137" s="2"/>
+      <c r="O137" s="2"/>
+      <c r="P137" s="2"/>
+      <c r="Q137" s="2"/>
+    </row>
+    <row r="138" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D138" s="2"/>
+      <c r="E138" s="2"/>
+      <c r="F138" s="2"/>
+      <c r="G138" s="2"/>
+      <c r="H138" s="2"/>
+      <c r="I138" s="2"/>
+      <c r="J138" s="2"/>
+      <c r="K138" s="2"/>
+      <c r="L138" s="2"/>
+      <c r="M138" s="2"/>
+      <c r="N138" s="2"/>
+      <c r="O138" s="2"/>
+      <c r="P138" s="2"/>
+      <c r="Q138" s="2"/>
+    </row>
+    <row r="139" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D139" s="2"/>
+      <c r="E139" s="2"/>
+      <c r="F139" s="2"/>
+      <c r="G139" s="2"/>
+      <c r="H139" s="2"/>
+      <c r="I139" s="2"/>
+      <c r="J139" s="2"/>
+      <c r="K139" s="2"/>
+      <c r="L139" s="2"/>
+      <c r="M139" s="2"/>
+      <c r="N139" s="2"/>
+      <c r="O139" s="2"/>
+      <c r="P139" s="2"/>
+      <c r="Q139" s="2"/>
+    </row>
+    <row r="140" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D140" s="2"/>
+      <c r="E140" s="2"/>
+      <c r="F140" s="2"/>
+      <c r="G140" s="2"/>
+      <c r="H140" s="2"/>
+      <c r="I140" s="2"/>
+      <c r="J140" s="2"/>
+      <c r="K140" s="2"/>
+      <c r="L140" s="2"/>
+      <c r="M140" s="2"/>
+      <c r="N140" s="2"/>
+      <c r="O140" s="2"/>
+      <c r="P140" s="2"/>
+      <c r="Q140" s="2"/>
+    </row>
+    <row r="141" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D141" s="2"/>
+      <c r="E141" s="2"/>
+      <c r="F141" s="2"/>
+      <c r="G141" s="2"/>
+      <c r="H141" s="2"/>
+      <c r="I141" s="2"/>
+      <c r="J141" s="2"/>
+      <c r="K141" s="2"/>
+      <c r="L141" s="2"/>
+      <c r="M141" s="2"/>
+      <c r="N141" s="2"/>
+      <c r="O141" s="2"/>
+      <c r="P141" s="2"/>
+      <c r="Q141" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D110:Q135"/>
+    <mergeCell ref="D116:Q141"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
LGHUB 2025/12/19 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
- 网站错误 & 本地化问题详见 LGHUB/WebLoc/README.md
</commit_message>
<xml_diff>
--- a/Documents/Graph_PC.xlsx
+++ b/Documents/Graph_PC.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29611"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{572B1542-900E-4F50-8656-5D6591BF901A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FE34C87-EF78-4C7C-B4DA-2BF09A3D1B1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,13 +574,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>88</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -917,43 +917,43 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$20:$C$28</c:f>
+              <c:f>Sheet1!$C$19:$C$27</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>46006</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45999</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45992</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45985</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45978</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45971</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45964</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45957</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45950</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45943</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$20:$D$28</c:f>
+              <c:f>Sheet1!$D$19:$D$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -961,7 +961,7 @@
                   <c:v>549</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>540</c:v>
+                  <c:v>549</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>540</c:v>
@@ -970,19 +970,19 @@
                   <c:v>540</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>530</c:v>
+                  <c:v>540</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>530</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>523</c:v>
+                  <c:v>530</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>523</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>514</c:v>
+                  <c:v>523</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1086,51 +1086,51 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$20:$C$28</c:f>
+              <c:f>Sheet1!$C$19:$C$27</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>46006</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>45999</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45992</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45985</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45978</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45971</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45964</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45957</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45950</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45943</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$20:$G$28</c:f>
+              <c:f>Sheet1!$G$19:$G$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>512</c:v>
+                  <c:v>521</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>506</c:v>
+                  <c:v>512</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>506</c:v>
@@ -1139,16 +1139,16 @@
                   <c:v>506</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>506</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>503</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>493</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>489</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>482</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>482</c:v>
@@ -1795,13 +1795,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>88</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4812,8 +4812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C114" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="L115" sqref="L115"/>
+    <sheetView tabSelected="1" topLeftCell="C115" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="N115" sqref="N115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -4837,7 +4837,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
@@ -4853,7 +4853,21 @@
         <v>4</v>
       </c>
       <c r="C7">
-        <v>88</v>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C19" s="1">
+        <v>46006</v>
+      </c>
+      <c r="D19">
+        <v>549</v>
+      </c>
+      <c r="F19" s="1">
+        <v>46006</v>
+      </c>
+      <c r="G19">
+        <v>521</v>
       </c>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
LGHUB 2026/1/15 更新 1
签发：Ling Gao
- 反馈更新详见 Documents/Update_Feedback.md
- 平台更新详见 Documents/Update_Platform.md
- 更新简报详见 LGHUB/Canary.md
- 网站错误 & 本地化问题详见 LGHUB/WebLoc/README.md
</commit_message>
<xml_diff>
--- a/Documents/Graph_PC.xlsx
+++ b/Documents/Graph_PC.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29711"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hnist\Desktop\LGHUB\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FE34C87-EF78-4C7C-B4DA-2BF09A3D1B1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64D11FFF-01BD-4031-B346-124281E7CCAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -574,13 +574,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>96</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -917,54 +917,54 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$19:$C$27</c:f>
+              <c:f>Sheet1!$C$18:$C$26</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>46034</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>46006</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45999</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45992</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45985</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45978</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45971</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45964</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45957</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45950</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$19:$D$27</c:f>
+              <c:f>Sheet1!$D$18:$D$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>549</c:v>
+                  <c:v>550</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>549</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>540</c:v>
+                  <c:v>549</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>540</c:v>
@@ -973,13 +973,13 @@
                   <c:v>540</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>530</c:v>
+                  <c:v>540</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>530</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>523</c:v>
+                  <c:v>530</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>523</c:v>
@@ -1086,54 +1086,54 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$19:$C$27</c:f>
+              <c:f>Sheet1!$C$18:$C$26</c:f>
               <c:numCache>
                 <c:formatCode>m"月"d"日"</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>46034</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>46006</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>45999</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45992</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45985</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>45978</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>45971</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>45964</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>45957</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>45950</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$19:$G$27</c:f>
+              <c:f>Sheet1!$G$18:$G$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>526</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>521</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>512</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>506</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>506</c:v>
@@ -1142,16 +1142,16 @@
                   <c:v>506</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>506</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>503</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>493</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>489</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>482</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1288,7 +1288,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="560"/>
-          <c:min val="470"/>
+          <c:min val="480"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1530,7 +1530,7 @@
                 <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
                 <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
               </a:rPr>
-              <a:t>(9</a:t>
+              <a:t>(1</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="zh-CN" altLang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
@@ -1556,7 +1556,7 @@
                 <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
                 <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
               </a:rPr>
-              <a:t>- 12</a:t>
+              <a:t>- 4</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="zh-CN" altLang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
@@ -1795,13 +1795,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>96</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4812,8 +4812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C115" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="N115" sqref="N115"/>
+    <sheetView tabSelected="1" topLeftCell="B117" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="K115" sqref="K115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -4837,7 +4837,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
@@ -4845,7 +4845,7 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
@@ -4853,7 +4853,21 @@
         <v>4</v>
       </c>
       <c r="C7">
-        <v>96</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C18" s="1">
+        <v>46034</v>
+      </c>
+      <c r="D18">
+        <v>550</v>
+      </c>
+      <c r="F18" s="1">
+        <v>46034</v>
+      </c>
+      <c r="G18">
+        <v>526</v>
       </c>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.25">

</xml_diff>